<commit_message>
Commented the Menu System
Commented the Menu System.
Need to start work on writing necessary variables to the EEPROM and
getting factory defaults setup.  Need to change a bunch of variables
declared as integers to bytes.  Outlined variables in the excel file.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="15300" windowHeight="10080"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="15300" windowHeight="10080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
     <sheet name="User Settings" sheetId="2" r:id="rId2"/>
     <sheet name="Alarm Settings" sheetId="4" r:id="rId3"/>
+    <sheet name="Menu Variables" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="154">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -241,13 +242,250 @@
   </si>
   <si>
     <t>Turns the Serial debugging ON or OFF;  0 = ON and 1 =OFF</t>
+  </si>
+  <si>
+    <t>Calibrate Flow Sens</t>
+  </si>
+  <si>
+    <t>Flow Sensor Calib</t>
+  </si>
+  <si>
+    <t>Calibrate Sensor 4</t>
+  </si>
+  <si>
+    <t>Temp 4 Calib</t>
+  </si>
+  <si>
+    <t>char* M2Items34[]={"", "Calibrate Flow Sens", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Calibrate Sensor 3</t>
+  </si>
+  <si>
+    <t>Temp 3 Calib</t>
+  </si>
+  <si>
+    <t>char* M2Items33[]={"", "Calibrate Sensor 4", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>char* M2Items32[]={"", "Calibrate Sensor 3", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Calibrate Sensor 2</t>
+  </si>
+  <si>
+    <t>Temp 2 Calib</t>
+  </si>
+  <si>
+    <t>char* M2Items31[]={"", "Calibrate Sensor 2", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>char* M2Items30[]={"", "Calibrate Sensor 1", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Calibrate Sensor 1</t>
+  </si>
+  <si>
+    <t>Temp 1 Calib</t>
+  </si>
+  <si>
+    <t>char* M1Items3[]={"", "Temp 1 Calib", "Temp 2 Calib", "Temp 3 Calib", "Temp 4 Calib", "Flow Calib", ""};  //  setup menu item 4 for Timer Setup Min 0 Max 4</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>char* M2Items23[]={"", "Set Sens 4 Addr", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>char* M2Items22[]={"", "Set Sens 3 Addr", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Set Sen 4 Addr</t>
+  </si>
+  <si>
+    <t>Temp Sens 4 Addr</t>
+  </si>
+  <si>
+    <t>char* M2Items21[]={"", "Set Sens 2 Addr", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>char* M2Items20[]={"", "Set Sens 1 Addr", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Set Sen 3 Addr</t>
+  </si>
+  <si>
+    <t>Temp Sens 3 Addr</t>
+  </si>
+  <si>
+    <t>char* M1Items2[]={"", "Temp Sens 1 Addr", "Temp Sens 2 Addr", "Temp Sens 3 Addr", "Temp Sens 4 Addr", ""};  //  setup menu item 3 for Timer Setup Min 0 Max 3</t>
+  </si>
+  <si>
+    <t>Set Sen 2 Addr</t>
+  </si>
+  <si>
+    <t>Temp Sens 2 Addr</t>
+  </si>
+  <si>
+    <t>Set Sen 1 Addr</t>
+  </si>
+  <si>
+    <t>Temp Sens 1 Addr</t>
+  </si>
+  <si>
+    <t>Sensor Addr Config</t>
+  </si>
+  <si>
+    <t>char* M2Items13[]={"", "Set Timer 4", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Set Timer 4</t>
+  </si>
+  <si>
+    <t>char* M2Items12[]={"", "Set Timer 3", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Set Timer 3</t>
+  </si>
+  <si>
+    <t>char* M2Items11[]={"", "Set Timer 2", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Set Timer 2</t>
+  </si>
+  <si>
+    <t>char* M2Items10[]={"", "Set Timer 1", "Exit", ""};</t>
+  </si>
+  <si>
+    <t>Set Timer 1</t>
+  </si>
+  <si>
+    <t>char* M1Items1[]={"", "Set Timer 1", "Set Timer 2", "Set Timer 3", "Set Timer 4", ""};  //  setup menu item 2 for Timer Setup Min 0 Max 3</t>
+  </si>
+  <si>
+    <t>Timers Setup</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>char* M2Items05[]={"", "On", "Off", ""};</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Serial Debugging</t>
+  </si>
+  <si>
+    <t>char* M2Items04[]={"", "Need Date/Time Here", ""};</t>
+  </si>
+  <si>
+    <t>Need this one too</t>
+  </si>
+  <si>
+    <t>Set Date/Time</t>
+  </si>
+  <si>
+    <t>char* M2Items03[]={"", "B Light Brightness", ""};</t>
+  </si>
+  <si>
+    <t>Need this one</t>
+  </si>
+  <si>
+    <t>B Light Brightnes</t>
+  </si>
+  <si>
+    <t>24 Hour</t>
+  </si>
+  <si>
+    <t>char* M2Items02[]={"", "12 Hour", "24 Hour", ""};</t>
+  </si>
+  <si>
+    <t>12 Hour</t>
+  </si>
+  <si>
+    <t>Time Format</t>
+  </si>
+  <si>
+    <t>1 Decimal</t>
+  </si>
+  <si>
+    <t>char* M2Items01[]={"", "No Decimal", "1 Decimal", ""};</t>
+  </si>
+  <si>
+    <t>No Decimal</t>
+  </si>
+  <si>
+    <t>Temp Precision</t>
+  </si>
+  <si>
+    <t>Fahrenheit</t>
+  </si>
+  <si>
+    <t>char* M2Items00[]={"", "Celsius", "Fahrenheit", ""};</t>
+  </si>
+  <si>
+    <t>Celsius</t>
+  </si>
+  <si>
+    <t>Temp Type</t>
+  </si>
+  <si>
+    <t>char* M1Items0[]={"", "Temp Type", "Temp Precision", "Time Format", "B Light Brightness", "Set Date/Time", "Serial Debugging", ""};  //  setup menu item 1 for System Config Min 0 Max 6</t>
+  </si>
+  <si>
+    <t>System Config</t>
+  </si>
+  <si>
+    <t>M3Sel</t>
+  </si>
+  <si>
+    <t>M2Sel</t>
+  </si>
+  <si>
+    <t>M1Sel</t>
+  </si>
+  <si>
+    <t>M0Sel</t>
+  </si>
+  <si>
+    <t>char* M0Items[]={"", "System Config", "Timers Setup", "Sensor Addr Config","Calibration",""};  //  setup menu items here  Min Cursor = 0 and Max Cursor = 3</t>
+  </si>
+  <si>
+    <t>M3Start</t>
+  </si>
+  <si>
+    <t>M2Start</t>
+  </si>
+  <si>
+    <t>M1Start</t>
+  </si>
+  <si>
+    <t>M0Start</t>
+  </si>
+  <si>
+    <t>Mlevel</t>
+  </si>
+  <si>
+    <t>MLevel3</t>
+  </si>
+  <si>
+    <t>MLevel2</t>
+  </si>
+  <si>
+    <t>MLevel1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,8 +500,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +577,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -331,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -343,6 +626,21 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,4 +1911,1584 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="2.33203125" customWidth="1"/>
+    <col min="16" max="16" width="155.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="17">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12">
+        <v>1</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="O5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="13">
+        <v>2</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0</v>
+      </c>
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="10">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="13">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>2</v>
+      </c>
+      <c r="J7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0</v>
+      </c>
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>1</v>
+      </c>
+      <c r="M8" s="14">
+        <v>0</v>
+      </c>
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13">
+        <v>2</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>1</v>
+      </c>
+      <c r="L9" s="12">
+        <v>1</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0</v>
+      </c>
+      <c r="N9" s="14">
+        <v>0</v>
+      </c>
+      <c r="O9" s="10">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13">
+        <v>2</v>
+      </c>
+      <c r="J10" s="13">
+        <v>1</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1</v>
+      </c>
+      <c r="L10" s="12">
+        <v>1</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0</v>
+      </c>
+      <c r="N10" s="14">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="12">
+        <v>2</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12">
+        <v>1</v>
+      </c>
+      <c r="J11" s="12">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>2</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0</v>
+      </c>
+      <c r="N11" s="14">
+        <v>0</v>
+      </c>
+      <c r="O11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13">
+        <v>2</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>2</v>
+      </c>
+      <c r="L12" s="12">
+        <v>2</v>
+      </c>
+      <c r="M12" s="14">
+        <v>0</v>
+      </c>
+      <c r="N12" s="14">
+        <v>0</v>
+      </c>
+      <c r="O12" s="10">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13">
+        <v>2</v>
+      </c>
+      <c r="J13" s="13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12">
+        <v>2</v>
+      </c>
+      <c r="L13" s="12">
+        <v>2</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0</v>
+      </c>
+      <c r="N13" s="14">
+        <v>0</v>
+      </c>
+      <c r="O13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="12">
+        <v>3</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12">
+        <v>1</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>3</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13">
+        <v>2</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>3</v>
+      </c>
+      <c r="L15" s="12">
+        <v>3</v>
+      </c>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="10">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="13">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13">
+        <v>2</v>
+      </c>
+      <c r="J16" s="13">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>3</v>
+      </c>
+      <c r="L16" s="12">
+        <v>3</v>
+      </c>
+      <c r="M16" s="14">
+        <v>0</v>
+      </c>
+      <c r="N16" s="14">
+        <v>0</v>
+      </c>
+      <c r="O16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="12">
+        <v>4</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>4</v>
+      </c>
+      <c r="M17" s="14">
+        <v>0</v>
+      </c>
+      <c r="N17" s="14">
+        <v>0</v>
+      </c>
+      <c r="O17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13">
+        <v>2</v>
+      </c>
+      <c r="J18" s="13">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>4</v>
+      </c>
+      <c r="L18" s="12">
+        <v>4</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
+      <c r="N18" s="14">
+        <v>0</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="13">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13">
+        <v>2</v>
+      </c>
+      <c r="J19" s="13">
+        <v>1</v>
+      </c>
+      <c r="K19" s="12">
+        <v>4</v>
+      </c>
+      <c r="L19" s="12">
+        <v>4</v>
+      </c>
+      <c r="M19" s="14">
+        <v>0</v>
+      </c>
+      <c r="N19" s="14">
+        <v>0</v>
+      </c>
+      <c r="O19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="12">
+        <v>5</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12">
+        <v>1</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>5</v>
+      </c>
+      <c r="M20" s="14">
+        <v>0</v>
+      </c>
+      <c r="N20" s="14">
+        <v>0</v>
+      </c>
+      <c r="O20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13">
+        <v>2</v>
+      </c>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <v>5</v>
+      </c>
+      <c r="L21" s="12">
+        <v>5</v>
+      </c>
+      <c r="M21" s="14">
+        <v>0</v>
+      </c>
+      <c r="N21" s="14">
+        <v>0</v>
+      </c>
+      <c r="O21" s="10">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="13">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13">
+        <v>2</v>
+      </c>
+      <c r="J22" s="13">
+        <v>1</v>
+      </c>
+      <c r="K22" s="12">
+        <v>5</v>
+      </c>
+      <c r="L22" s="12">
+        <v>5</v>
+      </c>
+      <c r="M22" s="14">
+        <v>0</v>
+      </c>
+      <c r="N22" s="14">
+        <v>0</v>
+      </c>
+      <c r="O22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>1</v>
+      </c>
+      <c r="B23" s="11">
+        <v>1</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11">
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
+        <v>0</v>
+      </c>
+      <c r="K23" s="11">
+        <v>0</v>
+      </c>
+      <c r="L23" s="11">
+        <v>0</v>
+      </c>
+      <c r="M23" s="11">
+        <v>0</v>
+      </c>
+      <c r="N23" s="11">
+        <v>1</v>
+      </c>
+      <c r="O23" s="10">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="12">
+        <v>0</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12">
+        <v>1</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0</v>
+      </c>
+      <c r="M24" s="11">
+        <v>1</v>
+      </c>
+      <c r="N24" s="11">
+        <v>1</v>
+      </c>
+      <c r="O24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="13">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13">
+        <v>2</v>
+      </c>
+      <c r="J25" s="13">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
+        <v>0</v>
+      </c>
+      <c r="M25" s="11">
+        <v>1</v>
+      </c>
+      <c r="N25" s="11">
+        <v>1</v>
+      </c>
+      <c r="O25" s="10">
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="13">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13">
+        <v>2</v>
+      </c>
+      <c r="J26" s="13">
+        <v>1</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0</v>
+      </c>
+      <c r="M26" s="11">
+        <v>1</v>
+      </c>
+      <c r="N26" s="11">
+        <v>1</v>
+      </c>
+      <c r="O26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="12">
+        <v>1</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12">
+        <v>1</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0</v>
+      </c>
+      <c r="K27" s="12">
+        <v>0</v>
+      </c>
+      <c r="L27" s="12">
+        <v>1</v>
+      </c>
+      <c r="M27" s="11">
+        <v>1</v>
+      </c>
+      <c r="N27" s="11">
+        <v>1</v>
+      </c>
+      <c r="O27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="13">
+        <v>0</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13">
+        <v>2</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0</v>
+      </c>
+      <c r="K28" s="12">
+        <v>1</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1</v>
+      </c>
+      <c r="M28" s="11">
+        <v>1</v>
+      </c>
+      <c r="N28" s="11">
+        <v>1</v>
+      </c>
+      <c r="O28" s="10">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="13">
+        <v>1</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13">
+        <v>2</v>
+      </c>
+      <c r="J29" s="13">
+        <v>1</v>
+      </c>
+      <c r="K29" s="12">
+        <v>1</v>
+      </c>
+      <c r="L29" s="12">
+        <v>1</v>
+      </c>
+      <c r="M29" s="11">
+        <v>1</v>
+      </c>
+      <c r="N29" s="11">
+        <v>1</v>
+      </c>
+      <c r="O29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="12">
+        <v>2</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12">
+        <v>1</v>
+      </c>
+      <c r="J30" s="12">
+        <v>0</v>
+      </c>
+      <c r="K30" s="12">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <v>2</v>
+      </c>
+      <c r="M30" s="11">
+        <v>1</v>
+      </c>
+      <c r="N30" s="11">
+        <v>1</v>
+      </c>
+      <c r="O30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="13">
+        <v>0</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13">
+        <v>2</v>
+      </c>
+      <c r="J31" s="13">
+        <v>0</v>
+      </c>
+      <c r="K31" s="12">
+        <v>2</v>
+      </c>
+      <c r="L31" s="12">
+        <v>2</v>
+      </c>
+      <c r="M31" s="11">
+        <v>1</v>
+      </c>
+      <c r="N31" s="11">
+        <v>1</v>
+      </c>
+      <c r="O31" s="10">
+        <v>0</v>
+      </c>
+      <c r="P31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="13">
+        <v>1</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13">
+        <v>2</v>
+      </c>
+      <c r="J32" s="13">
+        <v>1</v>
+      </c>
+      <c r="K32" s="12">
+        <v>2</v>
+      </c>
+      <c r="L32" s="12">
+        <v>2</v>
+      </c>
+      <c r="M32" s="11">
+        <v>1</v>
+      </c>
+      <c r="N32" s="11">
+        <v>1</v>
+      </c>
+      <c r="O32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="12">
+        <v>3</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12">
+        <v>1</v>
+      </c>
+      <c r="J33" s="12">
+        <v>1</v>
+      </c>
+      <c r="K33" s="12">
+        <v>0</v>
+      </c>
+      <c r="L33" s="12">
+        <v>3</v>
+      </c>
+      <c r="M33" s="11">
+        <v>1</v>
+      </c>
+      <c r="N33" s="11">
+        <v>1</v>
+      </c>
+      <c r="O33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="13">
+        <v>0</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13">
+        <v>2</v>
+      </c>
+      <c r="J34" s="13">
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
+        <v>3</v>
+      </c>
+      <c r="L34" s="12">
+        <v>3</v>
+      </c>
+      <c r="M34" s="11">
+        <v>1</v>
+      </c>
+      <c r="N34" s="11">
+        <v>1</v>
+      </c>
+      <c r="O34" s="10">
+        <v>0</v>
+      </c>
+      <c r="P34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="13">
+        <v>1</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13">
+        <v>2</v>
+      </c>
+      <c r="J35" s="13">
+        <v>1</v>
+      </c>
+      <c r="K35" s="12">
+        <v>3</v>
+      </c>
+      <c r="L35" s="12">
+        <v>3</v>
+      </c>
+      <c r="M35" s="11">
+        <v>1</v>
+      </c>
+      <c r="N35" s="11">
+        <v>1</v>
+      </c>
+      <c r="O35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
+        <v>2</v>
+      </c>
+      <c r="B36" s="10">
+        <v>2</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10">
+        <v>0</v>
+      </c>
+      <c r="J36" s="10">
+        <v>0</v>
+      </c>
+      <c r="K36" s="10">
+        <v>0</v>
+      </c>
+      <c r="L36" s="10">
+        <v>0</v>
+      </c>
+      <c r="M36" s="10">
+        <v>0</v>
+      </c>
+      <c r="N36" s="10">
+        <v>2</v>
+      </c>
+      <c r="O36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>93</v>
+      </c>
+      <c r="P40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>99</v>
+      </c>
+      <c r="P41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>93</v>
+      </c>
+      <c r="P42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>95</v>
+      </c>
+      <c r="P43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>93</v>
+      </c>
+      <c r="P44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>3</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>88</v>
+      </c>
+      <c r="P46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="P47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>84</v>
+      </c>
+      <c r="P48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="P49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>80</v>
+      </c>
+      <c r="P50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="J1:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refining of EEProm Variables and Menu System
I do not remember what all I have done lol
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="168">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Data Type</t>
   </si>
   <si>
-    <t>Serial_Debug</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Bytes Used</t>
   </si>
   <si>
-    <t>Temp_Type</t>
-  </si>
-  <si>
     <t>Info</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>Defines if there are setting stored in the EEPROM for the current config setup</t>
   </si>
   <si>
-    <t>ConfigID</t>
-  </si>
-  <si>
     <t>AlarmHourA_ON</t>
   </si>
   <si>
@@ -487,9 +478,6 @@
     <t>Byte</t>
   </si>
   <si>
-    <t>Backlight Brightness</t>
-  </si>
-  <si>
     <t>Flow Sensor 100%</t>
   </si>
   <si>
@@ -512,6 +500,27 @@
   </si>
   <si>
     <t>Ending Address =99</t>
+  </si>
+  <si>
+    <t>tempReadDelay</t>
+  </si>
+  <si>
+    <t>tempType</t>
+  </si>
+  <si>
+    <t>tempPrecision</t>
+  </si>
+  <si>
+    <t>timeFormat</t>
+  </si>
+  <si>
+    <t>backlightLevel</t>
+  </si>
+  <si>
+    <t>serialDebug</t>
+  </si>
+  <si>
+    <t>configID</t>
   </si>
 </sst>
 </file>
@@ -657,9 +666,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -668,14 +674,17 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,7 +989,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,17 +1001,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1016,13 +1025,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,16 +1039,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1047,10 +1056,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1059,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1067,10 +1076,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>155</v>
+        <v>33</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1079,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1087,10 +1096,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>155</v>
+        <v>34</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1099,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1107,10 +1116,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>154</v>
+        <v>166</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1119,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1127,10 +1136,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>154</v>
+        <v>31</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1139,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1168,17 +1177,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1192,13 +1201,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1206,13 +1215,13 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>154</v>
+        <v>162</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1220,10 +1229,10 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>154</v>
+        <v>163</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1231,10 +1240,10 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>154</v>
+        <v>164</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1242,10 +1251,10 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>155</v>
+        <v>165</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1253,10 +1262,10 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1264,29 +1273,35 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>26</v>
       </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1314,17 +1329,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="A1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1338,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,10 +1367,10 @@
         <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>154</v>
+        <v>57</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1369,10 +1384,10 @@
         <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>154</v>
+        <v>55</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1386,10 +1401,10 @@
         <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>155</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1403,10 +1418,10 @@
         <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>155</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1420,10 +1435,10 @@
         <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>155</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1437,10 +1452,10 @@
         <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>155</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1454,10 +1469,10 @@
         <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>154</v>
+        <v>58</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1471,10 +1486,10 @@
         <v>57</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>154</v>
+        <v>56</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1488,10 +1503,10 @@
         <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>155</v>
+        <v>16</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1505,10 +1520,10 @@
         <v>59</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>155</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1522,10 +1537,10 @@
         <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>155</v>
+        <v>18</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1539,10 +1554,10 @@
         <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>155</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1556,10 +1571,10 @@
         <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>154</v>
+        <v>59</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1573,10 +1588,10 @@
         <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>154</v>
+        <v>61</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1590,10 +1605,10 @@
         <v>64</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>155</v>
+        <v>20</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1607,10 +1622,10 @@
         <v>65</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>155</v>
+        <v>22</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1624,10 +1639,10 @@
         <v>66</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>155</v>
+        <v>23</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1641,10 +1656,10 @@
         <v>67</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>155</v>
+        <v>24</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1658,10 +1673,10 @@
         <v>68</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>154</v>
+        <v>60</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1675,10 +1690,10 @@
         <v>69</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>154</v>
+        <v>62</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1692,10 +1707,10 @@
         <v>70</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>155</v>
+        <v>25</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1709,10 +1724,10 @@
         <v>71</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>155</v>
+        <v>21</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1726,10 +1741,10 @@
         <v>72</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>155</v>
+        <v>26</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1743,10 +1758,10 @@
         <v>73</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>155</v>
+        <v>27</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1760,10 +1775,10 @@
         <v>74</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>154</v>
+        <v>63</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1777,10 +1792,10 @@
         <v>75</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>154</v>
+        <v>64</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1794,10 +1809,10 @@
         <v>76</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>155</v>
+        <v>39</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1811,10 +1826,10 @@
         <v>77</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>155</v>
+        <v>40</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1828,10 +1843,10 @@
         <v>78</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>155</v>
+        <v>41</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1845,10 +1860,10 @@
         <v>79</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>155</v>
+        <v>42</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1862,10 +1877,10 @@
         <v>80</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>154</v>
+        <v>65</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1879,10 +1894,10 @@
         <v>81</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>154</v>
+        <v>67</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1896,10 +1911,10 @@
         <v>82</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>155</v>
+        <v>43</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1913,10 +1928,10 @@
         <v>83</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>155</v>
+        <v>44</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1930,10 +1945,10 @@
         <v>84</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>155</v>
+        <v>45</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1947,10 +1962,10 @@
         <v>85</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>155</v>
+        <v>46</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1964,10 +1979,10 @@
         <v>86</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>154</v>
+        <v>66</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1981,10 +1996,10 @@
         <v>87</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>154</v>
+        <v>68</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1998,10 +2013,10 @@
         <v>88</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>155</v>
+        <v>47</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2015,10 +2030,10 @@
         <v>89</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>155</v>
+        <v>48</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2032,10 +2047,10 @@
         <v>90</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>155</v>
+        <v>49</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2049,10 +2064,10 @@
         <v>91</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>155</v>
+        <v>50</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2066,10 +2081,10 @@
         <v>92</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>154</v>
+        <v>69</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2083,10 +2098,10 @@
         <v>93</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>154</v>
+        <v>70</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>151</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2100,10 +2115,10 @@
         <v>94</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>155</v>
+        <v>51</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2117,10 +2132,10 @@
         <v>95</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>155</v>
+        <v>52</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2134,10 +2149,10 @@
         <v>96</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>155</v>
+        <v>53</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -2151,10 +2166,10 @@
         <v>97</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>155</v>
+        <v>54</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>152</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -2194,60 +2209,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19" t="s">
-        <v>151</v>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17" t="s">
+        <v>148</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M1" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19" t="s">
-        <v>146</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
@@ -2257,1258 +2272,1258 @@
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
       <c r="P2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
-        <v>0</v>
-      </c>
-      <c r="B4" s="14">
-        <v>0</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14">
-        <v>0</v>
-      </c>
-      <c r="J4" s="14">
-        <v>0</v>
-      </c>
-      <c r="K4" s="14">
-        <v>0</v>
-      </c>
-      <c r="L4" s="14">
-        <v>0</v>
-      </c>
-      <c r="M4" s="14">
-        <v>0</v>
-      </c>
-      <c r="N4" s="14">
-        <v>0</v>
-      </c>
-      <c r="O4" s="17">
+      <c r="A4" s="13">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="13">
+        <v>0</v>
+      </c>
+      <c r="O4" s="16">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12">
-        <v>1</v>
-      </c>
-      <c r="J5" s="12">
-        <v>0</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12">
-        <v>0</v>
-      </c>
-      <c r="M5" s="14">
-        <v>0</v>
-      </c>
-      <c r="N5" s="14">
-        <v>0</v>
-      </c>
-      <c r="O5" s="10">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11">
+        <v>1</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="16">
-        <v>0</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="13">
-        <v>2</v>
-      </c>
-      <c r="J6" s="13">
-        <v>0</v>
-      </c>
-      <c r="K6" s="12">
-        <v>0</v>
-      </c>
-      <c r="L6" s="12">
-        <v>0</v>
-      </c>
-      <c r="M6" s="14">
-        <v>0</v>
-      </c>
-      <c r="N6" s="14">
-        <v>0</v>
-      </c>
-      <c r="O6" s="10">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="15">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="12">
+        <v>2</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0</v>
+      </c>
+      <c r="O6" s="9">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="13">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13">
-        <v>2</v>
-      </c>
-      <c r="J7" s="13">
-        <v>1</v>
-      </c>
-      <c r="K7" s="12">
-        <v>0</v>
-      </c>
-      <c r="L7" s="12">
-        <v>0</v>
-      </c>
-      <c r="M7" s="14">
-        <v>0</v>
-      </c>
-      <c r="N7" s="14">
-        <v>0</v>
-      </c>
-      <c r="O7" s="10">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="12">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12">
+        <v>2</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0</v>
+      </c>
+      <c r="N7" s="13">
+        <v>0</v>
+      </c>
+      <c r="O7" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12">
-        <v>1</v>
-      </c>
-      <c r="J8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12">
-        <v>1</v>
-      </c>
-      <c r="M8" s="14">
-        <v>0</v>
-      </c>
-      <c r="N8" s="14">
-        <v>0</v>
-      </c>
-      <c r="O8" s="10">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11">
+        <v>1</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <v>1</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0</v>
+      </c>
+      <c r="N8" s="13">
+        <v>0</v>
+      </c>
+      <c r="O8" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="13">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13">
-        <v>2</v>
-      </c>
-      <c r="J9" s="13">
-        <v>0</v>
-      </c>
-      <c r="K9" s="12">
-        <v>1</v>
-      </c>
-      <c r="L9" s="12">
-        <v>1</v>
-      </c>
-      <c r="M9" s="14">
-        <v>0</v>
-      </c>
-      <c r="N9" s="14">
-        <v>0</v>
-      </c>
-      <c r="O9" s="10">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12">
+        <v>2</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11">
+        <v>1</v>
+      </c>
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
+      <c r="M9" s="13">
+        <v>0</v>
+      </c>
+      <c r="N9" s="13">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
-        <v>2</v>
-      </c>
-      <c r="J10" s="13">
-        <v>1</v>
-      </c>
-      <c r="K10" s="12">
-        <v>1</v>
-      </c>
-      <c r="L10" s="12">
-        <v>1</v>
-      </c>
-      <c r="M10" s="14">
-        <v>0</v>
-      </c>
-      <c r="N10" s="14">
-        <v>0</v>
-      </c>
-      <c r="O10" s="10">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12">
+        <v>2</v>
+      </c>
+      <c r="J10" s="12">
+        <v>1</v>
+      </c>
+      <c r="K10" s="11">
+        <v>1</v>
+      </c>
+      <c r="L10" s="11">
+        <v>1</v>
+      </c>
+      <c r="M10" s="13">
+        <v>0</v>
+      </c>
+      <c r="N10" s="13">
+        <v>0</v>
+      </c>
+      <c r="O10" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="12">
-        <v>2</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12">
-        <v>1</v>
-      </c>
-      <c r="J11" s="12">
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="12">
-        <v>2</v>
-      </c>
-      <c r="M11" s="14">
-        <v>0</v>
-      </c>
-      <c r="N11" s="14">
-        <v>0</v>
-      </c>
-      <c r="O11" s="10">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
+        <v>2</v>
+      </c>
+      <c r="M11" s="13">
+        <v>0</v>
+      </c>
+      <c r="N11" s="13">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13">
-        <v>2</v>
-      </c>
-      <c r="J12" s="13">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>2</v>
-      </c>
-      <c r="L12" s="12">
-        <v>2</v>
-      </c>
-      <c r="M12" s="14">
-        <v>0</v>
-      </c>
-      <c r="N12" s="14">
-        <v>0</v>
-      </c>
-      <c r="O12" s="10">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12">
+        <v>2</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11">
+        <v>2</v>
+      </c>
+      <c r="L12" s="11">
+        <v>2</v>
+      </c>
+      <c r="M12" s="13">
+        <v>0</v>
+      </c>
+      <c r="N12" s="13">
+        <v>0</v>
+      </c>
+      <c r="O12" s="9">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13">
-        <v>2</v>
-      </c>
-      <c r="J13" s="13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="12">
-        <v>2</v>
-      </c>
-      <c r="L13" s="12">
-        <v>2</v>
-      </c>
-      <c r="M13" s="14">
-        <v>0</v>
-      </c>
-      <c r="N13" s="14">
-        <v>0</v>
-      </c>
-      <c r="O13" s="10">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12">
+        <v>2</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="K13" s="11">
+        <v>2</v>
+      </c>
+      <c r="L13" s="11">
+        <v>2</v>
+      </c>
+      <c r="M13" s="13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="12">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="11">
         <v>3</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <v>0</v>
-      </c>
-      <c r="L14" s="12">
+      <c r="E14" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
         <v>3</v>
       </c>
-      <c r="M14" s="14">
-        <v>0</v>
-      </c>
-      <c r="N14" s="14">
-        <v>0</v>
-      </c>
-      <c r="O14" s="10">
+      <c r="M14" s="13">
+        <v>0</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0</v>
+      </c>
+      <c r="O14" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="13">
-        <v>0</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13">
-        <v>2</v>
-      </c>
-      <c r="J15" s="13">
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12">
+        <v>2</v>
+      </c>
+      <c r="J15" s="12">
+        <v>0</v>
+      </c>
+      <c r="K15" s="11">
         <v>3</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="11">
         <v>3</v>
       </c>
-      <c r="M15" s="14">
-        <v>0</v>
-      </c>
-      <c r="N15" s="14">
-        <v>0</v>
-      </c>
-      <c r="O15" s="10">
+      <c r="M15" s="13">
+        <v>0</v>
+      </c>
+      <c r="N15" s="13">
+        <v>0</v>
+      </c>
+      <c r="O15" s="9">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="13">
-        <v>1</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13">
-        <v>2</v>
-      </c>
-      <c r="J16" s="13">
-        <v>1</v>
-      </c>
-      <c r="K16" s="12">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="12">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12">
+        <v>2</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="11">
         <v>3</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="11">
         <v>3</v>
       </c>
-      <c r="M16" s="14">
-        <v>0</v>
-      </c>
-      <c r="N16" s="14">
-        <v>0</v>
-      </c>
-      <c r="O16" s="10">
+      <c r="M16" s="13">
+        <v>0</v>
+      </c>
+      <c r="N16" s="13">
+        <v>0</v>
+      </c>
+      <c r="O16" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="12">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="11">
         <v>4</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12">
-        <v>1</v>
-      </c>
-      <c r="J17" s="12">
-        <v>0</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
+      <c r="E17" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11">
+        <v>1</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
         <v>4</v>
       </c>
-      <c r="M17" s="14">
-        <v>0</v>
-      </c>
-      <c r="N17" s="14">
-        <v>0</v>
-      </c>
-      <c r="O17" s="10">
+      <c r="M17" s="13">
+        <v>0</v>
+      </c>
+      <c r="N17" s="13">
+        <v>0</v>
+      </c>
+      <c r="O17" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="13">
-        <v>0</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13">
-        <v>2</v>
-      </c>
-      <c r="J18" s="13">
-        <v>0</v>
-      </c>
-      <c r="K18" s="12">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12">
+        <v>2</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="11">
         <v>4</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="11">
         <v>4</v>
       </c>
-      <c r="M18" s="14">
-        <v>0</v>
-      </c>
-      <c r="N18" s="14">
-        <v>0</v>
-      </c>
-      <c r="O18" s="10">
+      <c r="M18" s="13">
+        <v>0</v>
+      </c>
+      <c r="N18" s="13">
+        <v>0</v>
+      </c>
+      <c r="O18" s="9">
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="13">
-        <v>1</v>
-      </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13">
-        <v>2</v>
-      </c>
-      <c r="J19" s="13">
-        <v>1</v>
-      </c>
-      <c r="K19" s="12">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="12">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12">
+        <v>2</v>
+      </c>
+      <c r="J19" s="12">
+        <v>1</v>
+      </c>
+      <c r="K19" s="11">
         <v>4</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="11">
         <v>4</v>
       </c>
-      <c r="M19" s="14">
-        <v>0</v>
-      </c>
-      <c r="N19" s="14">
-        <v>0</v>
-      </c>
-      <c r="O19" s="10">
+      <c r="M19" s="13">
+        <v>0</v>
+      </c>
+      <c r="N19" s="13">
+        <v>0</v>
+      </c>
+      <c r="O19" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="12">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="11">
         <v>5</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12">
-        <v>1</v>
-      </c>
-      <c r="J20" s="12">
-        <v>0</v>
-      </c>
-      <c r="K20" s="12">
-        <v>0</v>
-      </c>
-      <c r="L20" s="12">
+      <c r="E20" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11">
+        <v>1</v>
+      </c>
+      <c r="J20" s="11">
+        <v>0</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11">
         <v>5</v>
       </c>
-      <c r="M20" s="14">
-        <v>0</v>
-      </c>
-      <c r="N20" s="14">
-        <v>0</v>
-      </c>
-      <c r="O20" s="10">
+      <c r="M20" s="13">
+        <v>0</v>
+      </c>
+      <c r="N20" s="13">
+        <v>0</v>
+      </c>
+      <c r="O20" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="13">
-        <v>0</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13">
-        <v>2</v>
-      </c>
-      <c r="J21" s="13">
-        <v>0</v>
-      </c>
-      <c r="K21" s="12">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="12">
+        <v>0</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12">
+        <v>2</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="11">
         <v>5</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="11">
         <v>5</v>
       </c>
-      <c r="M21" s="14">
-        <v>0</v>
-      </c>
-      <c r="N21" s="14">
-        <v>0</v>
-      </c>
-      <c r="O21" s="10">
+      <c r="M21" s="13">
+        <v>0</v>
+      </c>
+      <c r="N21" s="13">
+        <v>0</v>
+      </c>
+      <c r="O21" s="9">
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="13">
-        <v>1</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13">
-        <v>2</v>
-      </c>
-      <c r="J22" s="13">
-        <v>1</v>
-      </c>
-      <c r="K22" s="12">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="12">
+        <v>1</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12">
+        <v>2</v>
+      </c>
+      <c r="J22" s="12">
+        <v>1</v>
+      </c>
+      <c r="K22" s="11">
         <v>5</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="11">
         <v>5</v>
       </c>
-      <c r="M22" s="14">
-        <v>0</v>
-      </c>
-      <c r="N22" s="14">
-        <v>0</v>
-      </c>
-      <c r="O22" s="10">
+      <c r="M22" s="13">
+        <v>0</v>
+      </c>
+      <c r="N22" s="13">
+        <v>0</v>
+      </c>
+      <c r="O22" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="11">
-        <v>1</v>
-      </c>
-      <c r="B23" s="11">
-        <v>1</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11">
-        <v>0</v>
-      </c>
-      <c r="J23" s="11">
-        <v>0</v>
-      </c>
-      <c r="K23" s="11">
-        <v>0</v>
-      </c>
-      <c r="L23" s="11">
-        <v>0</v>
-      </c>
-      <c r="M23" s="11">
-        <v>0</v>
-      </c>
-      <c r="N23" s="11">
-        <v>1</v>
-      </c>
-      <c r="O23" s="10">
+      <c r="A23" s="10">
+        <v>1</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="J23" s="10">
+        <v>0</v>
+      </c>
+      <c r="K23" s="10">
+        <v>0</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0</v>
+      </c>
+      <c r="M23" s="10">
+        <v>0</v>
+      </c>
+      <c r="N23" s="10">
+        <v>1</v>
+      </c>
+      <c r="O23" s="9">
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="12">
-        <v>0</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12">
-        <v>1</v>
-      </c>
-      <c r="J24" s="12">
-        <v>0</v>
-      </c>
-      <c r="K24" s="12">
-        <v>0</v>
-      </c>
-      <c r="L24" s="12">
-        <v>0</v>
-      </c>
-      <c r="M24" s="11">
-        <v>1</v>
-      </c>
-      <c r="N24" s="11">
-        <v>1</v>
-      </c>
-      <c r="O24" s="10">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="11">
+        <v>0</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11">
+        <v>1</v>
+      </c>
+      <c r="J24" s="11">
+        <v>0</v>
+      </c>
+      <c r="K24" s="11">
+        <v>0</v>
+      </c>
+      <c r="L24" s="11">
+        <v>0</v>
+      </c>
+      <c r="M24" s="10">
+        <v>1</v>
+      </c>
+      <c r="N24" s="10">
+        <v>1</v>
+      </c>
+      <c r="O24" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="13">
-        <v>0</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13">
-        <v>2</v>
-      </c>
-      <c r="J25" s="13">
-        <v>0</v>
-      </c>
-      <c r="K25" s="12">
-        <v>0</v>
-      </c>
-      <c r="L25" s="12">
-        <v>0</v>
-      </c>
-      <c r="M25" s="11">
-        <v>1</v>
-      </c>
-      <c r="N25" s="11">
-        <v>1</v>
-      </c>
-      <c r="O25" s="10">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12">
+        <v>2</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="11">
+        <v>0</v>
+      </c>
+      <c r="L25" s="11">
+        <v>0</v>
+      </c>
+      <c r="M25" s="10">
+        <v>1</v>
+      </c>
+      <c r="N25" s="10">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9">
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="13">
-        <v>1</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13">
-        <v>2</v>
-      </c>
-      <c r="J26" s="13">
-        <v>1</v>
-      </c>
-      <c r="K26" s="12">
-        <v>0</v>
-      </c>
-      <c r="L26" s="12">
-        <v>0</v>
-      </c>
-      <c r="M26" s="11">
-        <v>1</v>
-      </c>
-      <c r="N26" s="11">
-        <v>1</v>
-      </c>
-      <c r="O26" s="10">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="12">
+        <v>1</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12">
+        <v>2</v>
+      </c>
+      <c r="J26" s="12">
+        <v>1</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0</v>
+      </c>
+      <c r="L26" s="11">
+        <v>0</v>
+      </c>
+      <c r="M26" s="10">
+        <v>1</v>
+      </c>
+      <c r="N26" s="10">
+        <v>1</v>
+      </c>
+      <c r="O26" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="12">
-        <v>1</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12">
-        <v>1</v>
-      </c>
-      <c r="J27" s="12">
-        <v>0</v>
-      </c>
-      <c r="K27" s="12">
-        <v>0</v>
-      </c>
-      <c r="L27" s="12">
-        <v>1</v>
-      </c>
-      <c r="M27" s="11">
-        <v>1</v>
-      </c>
-      <c r="N27" s="11">
-        <v>1</v>
-      </c>
-      <c r="O27" s="10">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="11">
+        <v>1</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11">
+        <v>1</v>
+      </c>
+      <c r="J27" s="11">
+        <v>0</v>
+      </c>
+      <c r="K27" s="11">
+        <v>0</v>
+      </c>
+      <c r="L27" s="11">
+        <v>1</v>
+      </c>
+      <c r="M27" s="10">
+        <v>1</v>
+      </c>
+      <c r="N27" s="10">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="13">
-        <v>0</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13">
-        <v>2</v>
-      </c>
-      <c r="J28" s="13">
-        <v>0</v>
-      </c>
-      <c r="K28" s="12">
-        <v>1</v>
-      </c>
-      <c r="L28" s="12">
-        <v>1</v>
-      </c>
-      <c r="M28" s="11">
-        <v>1</v>
-      </c>
-      <c r="N28" s="11">
-        <v>1</v>
-      </c>
-      <c r="O28" s="10">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12">
+        <v>2</v>
+      </c>
+      <c r="J28" s="12">
+        <v>0</v>
+      </c>
+      <c r="K28" s="11">
+        <v>1</v>
+      </c>
+      <c r="L28" s="11">
+        <v>1</v>
+      </c>
+      <c r="M28" s="10">
+        <v>1</v>
+      </c>
+      <c r="N28" s="10">
+        <v>1</v>
+      </c>
+      <c r="O28" s="9">
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="13">
-        <v>1</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13">
-        <v>2</v>
-      </c>
-      <c r="J29" s="13">
-        <v>1</v>
-      </c>
-      <c r="K29" s="12">
-        <v>1</v>
-      </c>
-      <c r="L29" s="12">
-        <v>1</v>
-      </c>
-      <c r="M29" s="11">
-        <v>1</v>
-      </c>
-      <c r="N29" s="11">
-        <v>1</v>
-      </c>
-      <c r="O29" s="10">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="12">
+        <v>1</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12">
+        <v>2</v>
+      </c>
+      <c r="J29" s="12">
+        <v>1</v>
+      </c>
+      <c r="K29" s="11">
+        <v>1</v>
+      </c>
+      <c r="L29" s="11">
+        <v>1</v>
+      </c>
+      <c r="M29" s="10">
+        <v>1</v>
+      </c>
+      <c r="N29" s="10">
+        <v>1</v>
+      </c>
+      <c r="O29" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="12">
-        <v>2</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12">
-        <v>1</v>
-      </c>
-      <c r="J30" s="12">
-        <v>0</v>
-      </c>
-      <c r="K30" s="12">
-        <v>0</v>
-      </c>
-      <c r="L30" s="12">
-        <v>2</v>
-      </c>
-      <c r="M30" s="11">
-        <v>1</v>
-      </c>
-      <c r="N30" s="11">
-        <v>1</v>
-      </c>
-      <c r="O30" s="10">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="11">
+        <v>2</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11">
+        <v>1</v>
+      </c>
+      <c r="J30" s="11">
+        <v>0</v>
+      </c>
+      <c r="K30" s="11">
+        <v>0</v>
+      </c>
+      <c r="L30" s="11">
+        <v>2</v>
+      </c>
+      <c r="M30" s="10">
+        <v>1</v>
+      </c>
+      <c r="N30" s="10">
+        <v>1</v>
+      </c>
+      <c r="O30" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="13">
-        <v>0</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13">
-        <v>2</v>
-      </c>
-      <c r="J31" s="13">
-        <v>0</v>
-      </c>
-      <c r="K31" s="12">
-        <v>2</v>
-      </c>
-      <c r="L31" s="12">
-        <v>2</v>
-      </c>
-      <c r="M31" s="11">
-        <v>1</v>
-      </c>
-      <c r="N31" s="11">
-        <v>1</v>
-      </c>
-      <c r="O31" s="10">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="12">
+        <v>0</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12">
+        <v>2</v>
+      </c>
+      <c r="J31" s="12">
+        <v>0</v>
+      </c>
+      <c r="K31" s="11">
+        <v>2</v>
+      </c>
+      <c r="L31" s="11">
+        <v>2</v>
+      </c>
+      <c r="M31" s="10">
+        <v>1</v>
+      </c>
+      <c r="N31" s="10">
+        <v>1</v>
+      </c>
+      <c r="O31" s="9">
         <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="13">
-        <v>1</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13">
-        <v>2</v>
-      </c>
-      <c r="J32" s="13">
-        <v>1</v>
-      </c>
-      <c r="K32" s="12">
-        <v>2</v>
-      </c>
-      <c r="L32" s="12">
-        <v>2</v>
-      </c>
-      <c r="M32" s="11">
-        <v>1</v>
-      </c>
-      <c r="N32" s="11">
-        <v>1</v>
-      </c>
-      <c r="O32" s="10">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="12">
+        <v>1</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12">
+        <v>2</v>
+      </c>
+      <c r="J32" s="12">
+        <v>1</v>
+      </c>
+      <c r="K32" s="11">
+        <v>2</v>
+      </c>
+      <c r="L32" s="11">
+        <v>2</v>
+      </c>
+      <c r="M32" s="10">
+        <v>1</v>
+      </c>
+      <c r="N32" s="10">
+        <v>1</v>
+      </c>
+      <c r="O32" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="12">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="11">
         <v>3</v>
       </c>
-      <c r="E33" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12">
-        <v>1</v>
-      </c>
-      <c r="J33" s="12">
-        <v>1</v>
-      </c>
-      <c r="K33" s="12">
-        <v>0</v>
-      </c>
-      <c r="L33" s="12">
+      <c r="E33" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11">
+        <v>1</v>
+      </c>
+      <c r="J33" s="11">
+        <v>1</v>
+      </c>
+      <c r="K33" s="11">
+        <v>0</v>
+      </c>
+      <c r="L33" s="11">
         <v>3</v>
       </c>
-      <c r="M33" s="11">
-        <v>1</v>
-      </c>
-      <c r="N33" s="11">
-        <v>1</v>
-      </c>
-      <c r="O33" s="10">
+      <c r="M33" s="10">
+        <v>1</v>
+      </c>
+      <c r="N33" s="10">
+        <v>1</v>
+      </c>
+      <c r="O33" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="13">
-        <v>0</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13">
-        <v>2</v>
-      </c>
-      <c r="J34" s="13">
-        <v>0</v>
-      </c>
-      <c r="K34" s="12">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="12">
+        <v>0</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12">
+        <v>2</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0</v>
+      </c>
+      <c r="K34" s="11">
         <v>3</v>
       </c>
-      <c r="L34" s="12">
+      <c r="L34" s="11">
         <v>3</v>
       </c>
-      <c r="M34" s="11">
-        <v>1</v>
-      </c>
-      <c r="N34" s="11">
-        <v>1</v>
-      </c>
-      <c r="O34" s="10">
+      <c r="M34" s="10">
+        <v>1</v>
+      </c>
+      <c r="N34" s="10">
+        <v>1</v>
+      </c>
+      <c r="O34" s="9">
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="13">
-        <v>1</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13">
-        <v>2</v>
-      </c>
-      <c r="J35" s="13">
-        <v>1</v>
-      </c>
-      <c r="K35" s="12">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="12">
+        <v>1</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12">
+        <v>2</v>
+      </c>
+      <c r="J35" s="12">
+        <v>1</v>
+      </c>
+      <c r="K35" s="11">
         <v>3</v>
       </c>
-      <c r="L35" s="12">
+      <c r="L35" s="11">
         <v>3</v>
       </c>
-      <c r="M35" s="11">
-        <v>1</v>
-      </c>
-      <c r="N35" s="11">
-        <v>1</v>
-      </c>
-      <c r="O35" s="10">
+      <c r="M35" s="10">
+        <v>1</v>
+      </c>
+      <c r="N35" s="10">
+        <v>1</v>
+      </c>
+      <c r="O35" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="10">
-        <v>2</v>
-      </c>
-      <c r="B36" s="10">
-        <v>2</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10">
-        <v>0</v>
-      </c>
-      <c r="J36" s="10">
-        <v>0</v>
-      </c>
-      <c r="K36" s="10">
-        <v>0</v>
-      </c>
-      <c r="L36" s="10">
-        <v>0</v>
-      </c>
-      <c r="M36" s="10">
-        <v>0</v>
-      </c>
-      <c r="N36" s="10">
-        <v>2</v>
-      </c>
-      <c r="O36" s="10">
+      <c r="A36" s="9">
+        <v>2</v>
+      </c>
+      <c r="B36" s="9">
+        <v>2</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9">
+        <v>0</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0</v>
+      </c>
+      <c r="M36" s="9">
+        <v>0</v>
+      </c>
+      <c r="N36" s="9">
+        <v>2</v>
+      </c>
+      <c r="O36" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10">
-        <v>0</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" s="10">
-        <v>0</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -3516,13 +3531,13 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -3530,10 +3545,10 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -3541,16 +3556,16 @@
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="P41" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -3558,10 +3573,10 @@
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
@@ -3569,16 +3584,16 @@
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P43" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -3586,10 +3601,10 @@
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P44" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -3600,7 +3615,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -3624,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="P45" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -3632,16 +3647,16 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -3649,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="P47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -3657,16 +3672,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P48" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="4:16" x14ac:dyDescent="0.3">
@@ -3674,7 +3689,7 @@
         <v>1</v>
       </c>
       <c r="P49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="4:16" x14ac:dyDescent="0.3">
@@ -3682,16 +3697,16 @@
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="P50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="4:16" x14ac:dyDescent="0.3">
@@ -3704,13 +3719,13 @@
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="4:16" x14ac:dyDescent="0.3">
@@ -3723,13 +3738,13 @@
         <v>4</v>
       </c>
       <c r="E54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F54">
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="4:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
EEPROM and Alarm work
Got the EEPROM erasing and factory defaults to work correctly.  Also
started working on support to get the ids of the alarms I set so I can
change them later.  Have some working code on AlarmA on and off.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="191">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -499,9 +499,6 @@
     <t>Start Address = 50</t>
   </si>
   <si>
-    <t>Ending Address =99</t>
-  </si>
-  <si>
     <t>tempReadDelay</t>
   </si>
   <si>
@@ -521,6 +518,78 @@
   </si>
   <si>
     <t>configID</t>
+  </si>
+  <si>
+    <t>AlarmAPMA_ON</t>
+  </si>
+  <si>
+    <t>Alarm APMA_OFF</t>
+  </si>
+  <si>
+    <t>AlarmAPMB_ON</t>
+  </si>
+  <si>
+    <t>Alarm APMB_OFF</t>
+  </si>
+  <si>
+    <t>AlarmAPMC_ON</t>
+  </si>
+  <si>
+    <t>Alarm APMC_OFF</t>
+  </si>
+  <si>
+    <t>AlarmAPMD_ON</t>
+  </si>
+  <si>
+    <t>Alarm APMD_OFF</t>
+  </si>
+  <si>
+    <t>AlarmAPME_ON</t>
+  </si>
+  <si>
+    <t>AlarmAPMF_ON</t>
+  </si>
+  <si>
+    <t>Alarm APMF_OFF</t>
+  </si>
+  <si>
+    <t>AlarmAPMG_ON</t>
+  </si>
+  <si>
+    <t>Alarm APMG_OFF</t>
+  </si>
+  <si>
+    <t>AlarmAPMH_ON</t>
+  </si>
+  <si>
+    <t>Alarm APMH_OFF</t>
+  </si>
+  <si>
+    <t>Current state of the Alarm:  0=On, 1=Off</t>
+  </si>
+  <si>
+    <t>Enables the Alarm:  0=On, 1=Off</t>
+  </si>
+  <si>
+    <t>Sets the Minute for the Alarm On:  Valid numbers are 0-59</t>
+  </si>
+  <si>
+    <t>Sets the on Hour for the Alarm On:  Valid Numbers are If 24 hour = 0-23 and if 12 Hour = 1-12</t>
+  </si>
+  <si>
+    <t>Sets AM or PM for the Alarm On</t>
+  </si>
+  <si>
+    <t>Sets the on Hour for the Alarm Off:  Valid Numbers are If 24 hour = 0-23 and if 12 Hour = 1-12</t>
+  </si>
+  <si>
+    <t>Sets the Minute for the Alarm Off:  Valid numbers are 0-59</t>
+  </si>
+  <si>
+    <t>Sets AM or PM for the Alarm Off</t>
+  </si>
+  <si>
+    <t>Ending Address =113</t>
   </si>
 </sst>
 </file>
@@ -564,60 +633,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -656,23 +677,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -986,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,12 +1014,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" t="s">
         <v>156</v>
       </c>
@@ -1039,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1053,33 +1066,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>152</v>
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1088,17 +1101,17 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D6">
@@ -1108,47 +1121,52 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>151</v>
+        <v>34</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1183,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,12 +1195,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" t="s">
         <v>155</v>
       </c>
@@ -1215,9 +1233,9 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>151</v>
       </c>
       <c r="F3" t="s">
@@ -1229,9 +1247,9 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1240,9 +1258,9 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1251,9 +1269,9 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C6" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1264,7 +1282,7 @@
       <c r="B7" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1275,7 +1293,7 @@
       <c r="B8" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1284,9 +1302,9 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1314,39 +1332,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="9" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" t="s">
         <v>159</v>
       </c>
       <c r="F1" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -1366,10 +1385,10 @@
       <c r="A3">
         <v>50</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D3">
@@ -1377,16 +1396,19 @@
       </c>
       <c r="E3">
         <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>51</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D4">
@@ -1394,16 +1416,19 @@
       </c>
       <c r="E4">
         <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>52</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D5">
@@ -1411,16 +1436,19 @@
       </c>
       <c r="E5">
         <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>53</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D6">
@@ -1428,33 +1456,39 @@
       </c>
       <c r="E6">
         <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>54</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>152</v>
+      <c r="B7" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>55</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D8">
@@ -1462,33 +1496,39 @@
       </c>
       <c r="E8">
         <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>56</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>151</v>
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>57</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D10">
@@ -1496,50 +1536,59 @@
       </c>
       <c r="E10">
         <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>58</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>152</v>
+      <c r="B11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>59</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>152</v>
+      <c r="B12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>60</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D13">
@@ -1547,16 +1596,19 @@
       </c>
       <c r="E13">
         <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>61</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D14">
@@ -1564,16 +1616,19 @@
       </c>
       <c r="E14">
         <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>62</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D15">
@@ -1581,17 +1636,20 @@
       </c>
       <c r="E15">
         <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>63</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>151</v>
+      <c r="B16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1599,15 +1657,18 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>64</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D17">
@@ -1616,16 +1677,19 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>65</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>152</v>
+      <c r="B18" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1633,16 +1697,19 @@
       <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>66</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>152</v>
+      <c r="B19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1650,16 +1717,19 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>67</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>152</v>
+      <c r="B20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1667,16 +1737,19 @@
       <c r="E20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>68</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>151</v>
+      <c r="B21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1684,16 +1757,19 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>69</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>151</v>
+      <c r="B22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1701,16 +1777,19 @@
       <c r="E22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>70</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>152</v>
+      <c r="B23" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1718,15 +1797,18 @@
       <c r="E23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>71</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D24">
@@ -1735,15 +1817,18 @@
       <c r="E24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>72</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D25">
@@ -1752,16 +1837,19 @@
       <c r="E25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>73</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>152</v>
+      <c r="B26" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1769,15 +1857,18 @@
       <c r="E26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>74</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D27">
@@ -1786,15 +1877,18 @@
       <c r="E27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>75</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D28">
@@ -1803,15 +1897,18 @@
       <c r="E28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>76</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D29">
@@ -1820,15 +1917,18 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>77</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D30">
@@ -1837,16 +1937,19 @@
       <c r="E30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>78</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>152</v>
+      <c r="B31" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1854,15 +1957,18 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>79</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="18" t="s">
+      <c r="B32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D32">
@@ -1871,16 +1977,19 @@
       <c r="E32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>80</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>151</v>
+      <c r="B33" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1888,15 +1997,18 @@
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>81</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="18" t="s">
+      <c r="B34" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D34">
@@ -1905,16 +2017,19 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>82</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>152</v>
+      <c r="B35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1922,16 +2037,19 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>83</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>152</v>
+      <c r="B36" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1939,15 +2057,18 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>84</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="18" t="s">
+      <c r="B37" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D37">
@@ -1956,15 +2077,18 @@
       <c r="E37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>85</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="18" t="s">
+      <c r="B38" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D38">
@@ -1973,15 +2097,18 @@
       <c r="E38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>86</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="18" t="s">
+      <c r="B39" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>151</v>
       </c>
       <c r="D39">
@@ -1990,16 +2117,19 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>87</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>151</v>
+      <c r="B40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2007,15 +2137,18 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>88</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="18" t="s">
+      <c r="B41" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D41">
@@ -2024,16 +2157,19 @@
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>89</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>152</v>
+      <c r="B42" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2041,16 +2177,19 @@
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>90</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>152</v>
+      <c r="B43" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2058,16 +2197,19 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>91</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>152</v>
+      <c r="B44" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2075,16 +2217,19 @@
       <c r="E44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>92</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>151</v>
+      <c r="B45" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2092,16 +2237,19 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>93</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>151</v>
+      <c r="B46" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2109,16 +2257,19 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>94</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>152</v>
+      <c r="B47" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2126,15 +2277,18 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>95</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="18" t="s">
+      <c r="B48" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D48">
@@ -2143,15 +2297,18 @@
       <c r="E48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>96</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="18" t="s">
+      <c r="B49" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>152</v>
       </c>
       <c r="D49">
@@ -2160,22 +2317,348 @@
       <c r="E49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>97</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>98</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>99</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>100</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>101</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>102</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>103</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>104</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>105</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>106</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>107</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>108</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>109</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>110</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>111</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>112</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C65" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>113</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2209,131 +2692,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="12" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
       <c r="P2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
-        <v>0</v>
-      </c>
-      <c r="B4" s="13">
-        <v>0</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="A4" s="5">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13">
-        <v>0</v>
-      </c>
-      <c r="J4" s="13">
-        <v>0</v>
-      </c>
-      <c r="K4" s="13">
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <v>0</v>
-      </c>
-      <c r="M4" s="13">
-        <v>0</v>
-      </c>
-      <c r="N4" s="13">
-        <v>0</v>
-      </c>
-      <c r="O4" s="16">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="8">
         <v>0</v>
       </c>
       <c r="P4" t="s">
@@ -2341,72 +2824,72 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="11">
-        <v>0</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11">
-        <v>1</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0</v>
-      </c>
-      <c r="K5" s="11">
-        <v>0</v>
-      </c>
-      <c r="L5" s="11">
-        <v>0</v>
-      </c>
-      <c r="M5" s="13">
-        <v>0</v>
-      </c>
-      <c r="N5" s="13">
-        <v>0</v>
-      </c>
-      <c r="O5" s="9">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="15">
-        <v>0</v>
-      </c>
-      <c r="G6" s="15" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="12">
+      <c r="H6" s="6"/>
+      <c r="I6" s="4">
         <v>2</v>
       </c>
-      <c r="J6" s="12">
-        <v>0</v>
-      </c>
-      <c r="K6" s="11">
-        <v>0</v>
-      </c>
-      <c r="L6" s="11">
-        <v>0</v>
-      </c>
-      <c r="M6" s="13">
-        <v>0</v>
-      </c>
-      <c r="N6" s="13">
-        <v>0</v>
-      </c>
-      <c r="O6" s="9">
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
         <v>0</v>
       </c>
       <c r="P6" t="s">
@@ -2414,107 +2897,107 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12">
+      <c r="H7" s="4"/>
+      <c r="I7" s="4">
         <v>2</v>
       </c>
-      <c r="J7" s="12">
-        <v>1</v>
-      </c>
-      <c r="K7" s="11">
-        <v>0</v>
-      </c>
-      <c r="L7" s="11">
-        <v>0</v>
-      </c>
-      <c r="M7" s="13">
-        <v>0</v>
-      </c>
-      <c r="N7" s="13">
-        <v>0</v>
-      </c>
-      <c r="O7" s="9">
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="11">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11">
-        <v>1</v>
-      </c>
-      <c r="J8" s="11">
-        <v>0</v>
-      </c>
-      <c r="K8" s="11">
-        <v>0</v>
-      </c>
-      <c r="L8" s="11">
-        <v>1</v>
-      </c>
-      <c r="M8" s="13">
-        <v>0</v>
-      </c>
-      <c r="N8" s="13">
-        <v>0</v>
-      </c>
-      <c r="O8" s="9">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12">
+      <c r="H9" s="4"/>
+      <c r="I9" s="4">
         <v>2</v>
       </c>
-      <c r="J9" s="12">
-        <v>0</v>
-      </c>
-      <c r="K9" s="11">
-        <v>1</v>
-      </c>
-      <c r="L9" s="11">
-        <v>1</v>
-      </c>
-      <c r="M9" s="13">
-        <v>0</v>
-      </c>
-      <c r="N9" s="13">
-        <v>0</v>
-      </c>
-      <c r="O9" s="9">
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
         <v>0</v>
       </c>
       <c r="P9" t="s">
@@ -2522,107 +3005,107 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12">
+      <c r="H10" s="4"/>
+      <c r="I10" s="4">
         <v>2</v>
       </c>
-      <c r="J10" s="12">
-        <v>1</v>
-      </c>
-      <c r="K10" s="11">
-        <v>1</v>
-      </c>
-      <c r="L10" s="11">
-        <v>1</v>
-      </c>
-      <c r="M10" s="13">
-        <v>0</v>
-      </c>
-      <c r="N10" s="13">
-        <v>0</v>
-      </c>
-      <c r="O10" s="9">
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="11">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11">
-        <v>1</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0</v>
-      </c>
-      <c r="K11" s="11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="11">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
         <v>2</v>
       </c>
-      <c r="M11" s="13">
-        <v>0</v>
-      </c>
-      <c r="N11" s="13">
-        <v>0</v>
-      </c>
-      <c r="O11" s="9">
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="12" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
         <v>2</v>
       </c>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="11">
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
         <v>2</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="3">
         <v>2</v>
       </c>
-      <c r="M12" s="13">
-        <v>0</v>
-      </c>
-      <c r="N12" s="13">
-        <v>0</v>
-      </c>
-      <c r="O12" s="9">
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
         <v>0</v>
       </c>
       <c r="P12" t="s">
@@ -2630,107 +3113,107 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="12">
-        <v>1</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4">
         <v>2</v>
       </c>
-      <c r="J13" s="12">
-        <v>1</v>
-      </c>
-      <c r="K13" s="11">
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="3">
         <v>2</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="3">
         <v>2</v>
       </c>
-      <c r="M13" s="13">
-        <v>0</v>
-      </c>
-      <c r="N13" s="13">
-        <v>0</v>
-      </c>
-      <c r="O13" s="9">
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="3">
         <v>3</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11">
-        <v>1</v>
-      </c>
-      <c r="J14" s="11">
-        <v>0</v>
-      </c>
-      <c r="K14" s="11">
-        <v>0</v>
-      </c>
-      <c r="L14" s="11">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
         <v>3</v>
       </c>
-      <c r="M14" s="13">
-        <v>0</v>
-      </c>
-      <c r="N14" s="13">
-        <v>0</v>
-      </c>
-      <c r="O14" s="9">
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="12" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12">
+      <c r="H15" s="4"/>
+      <c r="I15" s="4">
         <v>2</v>
       </c>
-      <c r="J15" s="12">
-        <v>0</v>
-      </c>
-      <c r="K15" s="11">
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
         <v>3</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="3">
         <v>3</v>
       </c>
-      <c r="M15" s="13">
-        <v>0</v>
-      </c>
-      <c r="N15" s="13">
-        <v>0</v>
-      </c>
-      <c r="O15" s="9">
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
         <v>0</v>
       </c>
       <c r="P15" t="s">
@@ -2738,105 +3221,105 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="12">
-        <v>1</v>
-      </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
         <v>2</v>
       </c>
-      <c r="J16" s="12">
-        <v>1</v>
-      </c>
-      <c r="K16" s="11">
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3">
         <v>3</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="3">
         <v>3</v>
       </c>
-      <c r="M16" s="13">
-        <v>0</v>
-      </c>
-      <c r="N16" s="13">
-        <v>0</v>
-      </c>
-      <c r="O16" s="9">
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="11">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="3">
         <v>4</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11">
-        <v>1</v>
-      </c>
-      <c r="J17" s="11">
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
-        <v>0</v>
-      </c>
-      <c r="L17" s="11">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
         <v>4</v>
       </c>
-      <c r="M17" s="13">
-        <v>0</v>
-      </c>
-      <c r="N17" s="13">
-        <v>0</v>
-      </c>
-      <c r="O17" s="9">
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="12">
-        <v>0</v>
-      </c>
-      <c r="G18" s="12" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12">
+      <c r="H18" s="4"/>
+      <c r="I18" s="4">
         <v>2</v>
       </c>
-      <c r="J18" s="12">
-        <v>0</v>
-      </c>
-      <c r="K18" s="11">
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
         <v>4</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="3">
         <v>4</v>
       </c>
-      <c r="M18" s="13">
-        <v>0</v>
-      </c>
-      <c r="N18" s="13">
-        <v>0</v>
-      </c>
-      <c r="O18" s="9">
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
         <v>0</v>
       </c>
       <c r="P18" t="s">
@@ -2844,105 +3327,105 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="12">
-        <v>1</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4">
         <v>2</v>
       </c>
-      <c r="J19" s="12">
-        <v>1</v>
-      </c>
-      <c r="K19" s="11">
+      <c r="J19" s="4">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
         <v>4</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="3">
         <v>4</v>
       </c>
-      <c r="M19" s="13">
-        <v>0</v>
-      </c>
-      <c r="N19" s="13">
-        <v>0</v>
-      </c>
-      <c r="O19" s="9">
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="11">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="3">
         <v>5</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11">
-        <v>1</v>
-      </c>
-      <c r="J20" s="11">
-        <v>0</v>
-      </c>
-      <c r="K20" s="11">
-        <v>0</v>
-      </c>
-      <c r="L20" s="11">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
         <v>5</v>
       </c>
-      <c r="M20" s="13">
-        <v>0</v>
-      </c>
-      <c r="N20" s="13">
-        <v>0</v>
-      </c>
-      <c r="O20" s="9">
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="12">
-        <v>0</v>
-      </c>
-      <c r="G21" s="12" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12">
+      <c r="H21" s="4"/>
+      <c r="I21" s="4">
         <v>2</v>
       </c>
-      <c r="J21" s="12">
-        <v>0</v>
-      </c>
-      <c r="K21" s="11">
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
         <v>5</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="3">
         <v>5</v>
       </c>
-      <c r="M21" s="13">
-        <v>0</v>
-      </c>
-      <c r="N21" s="13">
-        <v>0</v>
-      </c>
-      <c r="O21" s="9">
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
         <v>0</v>
       </c>
       <c r="P21" t="s">
@@ -2950,74 +3433,74 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="12">
-        <v>1</v>
-      </c>
-      <c r="G22" s="12" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12">
+      <c r="H22" s="4"/>
+      <c r="I22" s="4">
         <v>2</v>
       </c>
-      <c r="J22" s="12">
-        <v>1</v>
-      </c>
-      <c r="K22" s="11">
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3">
         <v>5</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="3">
         <v>5</v>
       </c>
-      <c r="M22" s="13">
-        <v>0</v>
-      </c>
-      <c r="N22" s="13">
-        <v>0</v>
-      </c>
-      <c r="O22" s="9">
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
-        <v>1</v>
-      </c>
-      <c r="B23" s="10">
-        <v>1</v>
-      </c>
-      <c r="C23" s="10" t="s">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10">
-        <v>0</v>
-      </c>
-      <c r="J23" s="10">
-        <v>0</v>
-      </c>
-      <c r="K23" s="10">
-        <v>0</v>
-      </c>
-      <c r="L23" s="10">
-        <v>0</v>
-      </c>
-      <c r="M23" s="10">
-        <v>0</v>
-      </c>
-      <c r="N23" s="10">
-        <v>1</v>
-      </c>
-      <c r="O23" s="9">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1">
         <v>0</v>
       </c>
       <c r="P23" t="s">
@@ -3025,72 +3508,72 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11">
-        <v>1</v>
-      </c>
-      <c r="J24" s="11">
-        <v>0</v>
-      </c>
-      <c r="K24" s="11">
-        <v>0</v>
-      </c>
-      <c r="L24" s="11">
-        <v>0</v>
-      </c>
-      <c r="M24" s="10">
-        <v>1</v>
-      </c>
-      <c r="N24" s="10">
-        <v>1</v>
-      </c>
-      <c r="O24" s="9">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="12">
-        <v>0</v>
-      </c>
-      <c r="G25" s="12" t="s">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12">
+      <c r="H25" s="4"/>
+      <c r="I25" s="4">
         <v>2</v>
       </c>
-      <c r="J25" s="12">
-        <v>0</v>
-      </c>
-      <c r="K25" s="11">
-        <v>0</v>
-      </c>
-      <c r="L25" s="11">
-        <v>0</v>
-      </c>
-      <c r="M25" s="10">
-        <v>1</v>
-      </c>
-      <c r="N25" s="10">
-        <v>1</v>
-      </c>
-      <c r="O25" s="9">
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1</v>
+      </c>
+      <c r="N25" s="2">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1">
         <v>0</v>
       </c>
       <c r="P25" t="s">
@@ -3098,107 +3581,107 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="12">
-        <v>1</v>
-      </c>
-      <c r="G26" s="12" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12">
+      <c r="H26" s="4"/>
+      <c r="I26" s="4">
         <v>2</v>
       </c>
-      <c r="J26" s="12">
-        <v>1</v>
-      </c>
-      <c r="K26" s="11">
-        <v>0</v>
-      </c>
-      <c r="L26" s="11">
-        <v>0</v>
-      </c>
-      <c r="M26" s="10">
-        <v>1</v>
-      </c>
-      <c r="N26" s="10">
-        <v>1</v>
-      </c>
-      <c r="O26" s="9">
+      <c r="J26" s="4">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="11">
-        <v>1</v>
-      </c>
-      <c r="E27" s="11" t="s">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11">
-        <v>1</v>
-      </c>
-      <c r="J27" s="11">
-        <v>0</v>
-      </c>
-      <c r="K27" s="11">
-        <v>0</v>
-      </c>
-      <c r="L27" s="11">
-        <v>1</v>
-      </c>
-      <c r="M27" s="10">
-        <v>1</v>
-      </c>
-      <c r="N27" s="10">
-        <v>1</v>
-      </c>
-      <c r="O27" s="9">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
+      <c r="M27" s="2">
+        <v>1</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="12">
-        <v>0</v>
-      </c>
-      <c r="G28" s="12" t="s">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12">
+      <c r="H28" s="4"/>
+      <c r="I28" s="4">
         <v>2</v>
       </c>
-      <c r="J28" s="12">
-        <v>0</v>
-      </c>
-      <c r="K28" s="11">
-        <v>1</v>
-      </c>
-      <c r="L28" s="11">
-        <v>1</v>
-      </c>
-      <c r="M28" s="10">
-        <v>1</v>
-      </c>
-      <c r="N28" s="10">
-        <v>1</v>
-      </c>
-      <c r="O28" s="9">
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1">
         <v>0</v>
       </c>
       <c r="P28" t="s">
@@ -3206,107 +3689,107 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="12">
-        <v>1</v>
-      </c>
-      <c r="G29" s="12" t="s">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12">
+      <c r="H29" s="4"/>
+      <c r="I29" s="4">
         <v>2</v>
       </c>
-      <c r="J29" s="12">
-        <v>1</v>
-      </c>
-      <c r="K29" s="11">
-        <v>1</v>
-      </c>
-      <c r="L29" s="11">
-        <v>1</v>
-      </c>
-      <c r="M29" s="10">
-        <v>1</v>
-      </c>
-      <c r="N29" s="10">
-        <v>1</v>
-      </c>
-      <c r="O29" s="9">
+      <c r="J29" s="4">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="11">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="3">
         <v>2</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11">
-        <v>1</v>
-      </c>
-      <c r="J30" s="11">
-        <v>0</v>
-      </c>
-      <c r="K30" s="11">
-        <v>0</v>
-      </c>
-      <c r="L30" s="11">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
         <v>2</v>
       </c>
-      <c r="M30" s="10">
-        <v>1</v>
-      </c>
-      <c r="N30" s="10">
-        <v>1</v>
-      </c>
-      <c r="O30" s="9">
+      <c r="M30" s="2">
+        <v>1</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="12">
-        <v>0</v>
-      </c>
-      <c r="G31" s="12" t="s">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12">
+      <c r="H31" s="4"/>
+      <c r="I31" s="4">
         <v>2</v>
       </c>
-      <c r="J31" s="12">
-        <v>0</v>
-      </c>
-      <c r="K31" s="11">
+      <c r="J31" s="4">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
         <v>2</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="3">
         <v>2</v>
       </c>
-      <c r="M31" s="10">
-        <v>1</v>
-      </c>
-      <c r="N31" s="10">
-        <v>1</v>
-      </c>
-      <c r="O31" s="9">
+      <c r="M31" s="2">
+        <v>1</v>
+      </c>
+      <c r="N31" s="2">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
         <v>0</v>
       </c>
       <c r="P31" t="s">
@@ -3314,107 +3797,107 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="12">
-        <v>1</v>
-      </c>
-      <c r="G32" s="12" t="s">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12">
+      <c r="H32" s="4"/>
+      <c r="I32" s="4">
         <v>2</v>
       </c>
-      <c r="J32" s="12">
-        <v>1</v>
-      </c>
-      <c r="K32" s="11">
+      <c r="J32" s="4">
+        <v>1</v>
+      </c>
+      <c r="K32" s="3">
         <v>2</v>
       </c>
-      <c r="L32" s="11">
+      <c r="L32" s="3">
         <v>2</v>
       </c>
-      <c r="M32" s="10">
-        <v>1</v>
-      </c>
-      <c r="N32" s="10">
-        <v>1</v>
-      </c>
-      <c r="O32" s="9">
+      <c r="M32" s="2">
+        <v>1</v>
+      </c>
+      <c r="N32" s="2">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="11">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="3">
         <v>3</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11">
-        <v>1</v>
-      </c>
-      <c r="J33" s="11">
-        <v>1</v>
-      </c>
-      <c r="K33" s="11">
-        <v>0</v>
-      </c>
-      <c r="L33" s="11">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>1</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0</v>
+      </c>
+      <c r="L33" s="3">
         <v>3</v>
       </c>
-      <c r="M33" s="10">
-        <v>1</v>
-      </c>
-      <c r="N33" s="10">
-        <v>1</v>
-      </c>
-      <c r="O33" s="9">
+      <c r="M33" s="2">
+        <v>1</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1</v>
+      </c>
+      <c r="O33" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="12">
-        <v>0</v>
-      </c>
-      <c r="G34" s="12" t="s">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12">
+      <c r="H34" s="4"/>
+      <c r="I34" s="4">
         <v>2</v>
       </c>
-      <c r="J34" s="12">
-        <v>0</v>
-      </c>
-      <c r="K34" s="11">
+      <c r="J34" s="4">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
         <v>3</v>
       </c>
-      <c r="L34" s="11">
+      <c r="L34" s="3">
         <v>3</v>
       </c>
-      <c r="M34" s="10">
-        <v>1</v>
-      </c>
-      <c r="N34" s="10">
-        <v>1</v>
-      </c>
-      <c r="O34" s="9">
+      <c r="M34" s="2">
+        <v>1</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1</v>
+      </c>
+      <c r="O34" s="1">
         <v>0</v>
       </c>
       <c r="P34" t="s">
@@ -3422,101 +3905,101 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="12">
-        <v>1</v>
-      </c>
-      <c r="G35" s="12" t="s">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12">
+      <c r="H35" s="4"/>
+      <c r="I35" s="4">
         <v>2</v>
       </c>
-      <c r="J35" s="12">
-        <v>1</v>
-      </c>
-      <c r="K35" s="11">
+      <c r="J35" s="4">
+        <v>1</v>
+      </c>
+      <c r="K35" s="3">
         <v>3</v>
       </c>
-      <c r="L35" s="11">
+      <c r="L35" s="3">
         <v>3</v>
       </c>
-      <c r="M35" s="10">
-        <v>1</v>
-      </c>
-      <c r="N35" s="10">
-        <v>1</v>
-      </c>
-      <c r="O35" s="9">
+      <c r="M35" s="2">
+        <v>1</v>
+      </c>
+      <c r="N35" s="2">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="9">
+      <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="1">
         <v>2</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9">
-        <v>0</v>
-      </c>
-      <c r="J36" s="9">
-        <v>0</v>
-      </c>
-      <c r="K36" s="9">
-        <v>0</v>
-      </c>
-      <c r="L36" s="9">
-        <v>0</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
-      <c r="N36" s="9">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
         <v>2</v>
       </c>
-      <c r="O36" s="9">
+      <c r="O36" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9">
-        <v>0</v>
-      </c>
-      <c r="E37" s="9" t="s">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F37" s="9">
-        <v>0</v>
-      </c>
-      <c r="G37" s="9" t="s">
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F38">

</xml_diff>

<commit_message>
LCD timer setup now working, except for the 12 hour 12 to 1 rollover that occures at 1pm.  Need to work on that in the MenuNumSel function.  Started working on getting rid of all of the old timer variables and all references to _0.  Still need to test alarm setting as well.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="242">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -435,9 +435,6 @@
     <t>Alarm 7</t>
   </si>
   <si>
-    <t>Alarm 8</t>
-  </si>
-  <si>
     <t>AlarmEnable</t>
   </si>
   <si>
@@ -751,6 +748,9 @@
   </si>
   <si>
     <t>Alarmid</t>
+  </si>
+  <si>
+    <t>Time format 0 = 24 hour, 1 = 12 hour</t>
   </si>
 </sst>
 </file>
@@ -1654,13 +1654,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1671,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1687,7 +1687,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1695,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1703,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1711,7 +1711,7 @@
         <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1728,7 +1728,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1819,6 +1819,9 @@
       </c>
       <c r="C6" s="10" t="s">
         <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1945,7 +1948,7 @@
         <v>100</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>103</v>
@@ -1957,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1966,7 +1969,7 @@
         <v>101</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>103</v>
@@ -1978,18 +1981,18 @@
         <v>0</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="30">
         <v>102</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>103</v>
@@ -2010,7 +2013,7 @@
         <v>103</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>103</v>
@@ -2022,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2031,7 +2034,7 @@
         <v>104</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>103</v>
@@ -2043,7 +2046,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2052,7 +2055,7 @@
         <v>105</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>103</v>
@@ -2073,7 +2076,7 @@
         <v>106</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>103</v>
@@ -2085,7 +2088,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2094,7 +2097,7 @@
         <v>107</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>103</v>
@@ -2111,13 +2114,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" s="30">
         <v>108</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>103</v>
@@ -2138,7 +2141,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>103</v>
@@ -2150,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2159,7 +2162,7 @@
         <v>110</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>103</v>
@@ -2171,7 +2174,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2180,7 +2183,7 @@
         <v>111</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>103</v>
@@ -2201,7 +2204,7 @@
         <v>112</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>103</v>
@@ -2213,7 +2216,7 @@
         <v>12</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2222,7 +2225,7 @@
         <v>113</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>103</v>
@@ -2239,13 +2242,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B17" s="34">
         <v>114</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>103</v>
@@ -2266,7 +2269,7 @@
         <v>115</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>103</v>
@@ -2278,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2287,7 +2290,7 @@
         <v>116</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>103</v>
@@ -2299,7 +2302,7 @@
         <v>12</v>
       </c>
       <c r="G19" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2308,7 +2311,7 @@
         <v>117</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>103</v>
@@ -2329,7 +2332,7 @@
         <v>118</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>103</v>
@@ -2341,7 +2344,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2350,7 +2353,7 @@
         <v>119</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>103</v>
@@ -2367,13 +2370,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B23" s="30">
         <v>120</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>103</v>
@@ -2394,7 +2397,7 @@
         <v>121</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>103</v>
@@ -2406,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2415,7 +2418,7 @@
         <v>122</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>103</v>
@@ -2427,7 +2430,7 @@
         <v>12</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2436,7 +2439,7 @@
         <v>123</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>103</v>
@@ -2457,7 +2460,7 @@
         <v>124</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>103</v>
@@ -2469,7 +2472,7 @@
         <v>12</v>
       </c>
       <c r="G27" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2478,7 +2481,7 @@
         <v>125</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D28" s="36" t="s">
         <v>103</v>
@@ -2495,13 +2498,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B29" s="34">
         <v>126</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>103</v>
@@ -2522,7 +2525,7 @@
         <v>127</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>103</v>
@@ -2534,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2543,7 +2546,7 @@
         <v>128</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>103</v>
@@ -2555,7 +2558,7 @@
         <v>12</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2564,7 +2567,7 @@
         <v>129</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>103</v>
@@ -2585,7 +2588,7 @@
         <v>130</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D33" s="23" t="s">
         <v>103</v>
@@ -2597,7 +2600,7 @@
         <v>12</v>
       </c>
       <c r="G33" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2606,7 +2609,7 @@
         <v>131</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>103</v>
@@ -2623,13 +2626,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B35" s="30">
         <v>132</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>103</v>
@@ -2650,7 +2653,7 @@
         <v>133</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>103</v>
@@ -2662,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2671,7 +2674,7 @@
         <v>134</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>103</v>
@@ -2683,7 +2686,7 @@
         <v>12</v>
       </c>
       <c r="G37" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2692,7 +2695,7 @@
         <v>135</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D38" s="23" t="s">
         <v>103</v>
@@ -2713,7 +2716,7 @@
         <v>136</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" s="23" t="s">
         <v>103</v>
@@ -2725,7 +2728,7 @@
         <v>12</v>
       </c>
       <c r="G39" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2734,7 +2737,7 @@
         <v>137</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D40" s="36" t="s">
         <v>103</v>
@@ -2751,13 +2754,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B41" s="34">
         <v>138</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>103</v>
@@ -2778,7 +2781,7 @@
         <v>139</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D42" s="23" t="s">
         <v>103</v>
@@ -2790,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2799,7 +2802,7 @@
         <v>140</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D43" s="23" t="s">
         <v>103</v>
@@ -2811,7 +2814,7 @@
         <v>12</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2820,7 +2823,7 @@
         <v>141</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D44" s="23" t="s">
         <v>103</v>
@@ -2841,7 +2844,7 @@
         <v>142</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>103</v>
@@ -2853,7 +2856,7 @@
         <v>12</v>
       </c>
       <c r="G45" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2862,7 +2865,7 @@
         <v>143</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>103</v>
@@ -2879,13 +2882,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B47" s="30">
         <v>144</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D47" s="31" t="s">
         <v>103</v>
@@ -2906,7 +2909,7 @@
         <v>145</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>103</v>
@@ -2918,7 +2921,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2927,7 +2930,7 @@
         <v>146</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D49" s="23" t="s">
         <v>103</v>
@@ -2939,7 +2942,7 @@
         <v>12</v>
       </c>
       <c r="G49" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2948,7 +2951,7 @@
         <v>147</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D50" s="23" t="s">
         <v>103</v>
@@ -2969,7 +2972,7 @@
         <v>148</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D51" s="23" t="s">
         <v>103</v>
@@ -2981,7 +2984,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2990,7 +2993,7 @@
         <v>149</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D52" s="36" t="s">
         <v>103</v>
@@ -3025,49 +3028,46 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="21"/>
-    <col min="2" max="10" width="2.77734375" customWidth="1"/>
+    <col min="2" max="9" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="20"/>
       <c r="B1" s="19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1" s="19">
-        <v>1</v>
-      </c>
-      <c r="J1" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>128</v>
       </c>
@@ -3093,13 +3093,13 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>129</v>
       </c>
@@ -3122,16 +3122,16 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>130</v>
       </c>
@@ -3151,19 +3151,19 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>131</v>
       </c>
@@ -3180,10 +3180,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3191,11 +3191,11 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>132</v>
       </c>
@@ -3209,10 +3209,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -3223,11 +3223,11 @@
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>133</v>
       </c>
@@ -3238,10 +3238,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -3255,11 +3255,11 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>134</v>
       </c>
@@ -3267,10 +3267,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3287,19 +3287,19 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>135</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3319,40 +3319,8 @@
       <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
+      <c r="K9">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3362,15 +3330,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AT25"/>
+  <dimension ref="A1:AT25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AT2" sqref="AT2:AT9"/>
+      <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.109375" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
     <col min="2" max="21" width="2.21875" style="41" customWidth="1"/>
     <col min="23" max="42" width="2.21875" customWidth="1"/>
     <col min="44" max="46" width="8.88671875" style="45"/>
@@ -3378,7 +3346,7 @@
     <col min="50" max="50" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:46" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B1" s="44">
         <v>0</v>
       </c>
@@ -3500,31 +3468,34 @@
         <v>19</v>
       </c>
       <c r="AR1" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS1" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="AS1" s="45" t="s">
-        <v>241</v>
-      </c>
       <c r="AT1" s="45" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="2:46" x14ac:dyDescent="0.35">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="E2" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="F2" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>213</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>214</v>
       </c>
       <c r="H2" s="42"/>
       <c r="I2" s="42">
@@ -3532,49 +3503,52 @@
       </c>
       <c r="J2" s="42"/>
       <c r="K2" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L2" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M2" s="42"/>
       <c r="N2" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="O2" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="P2" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q2" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="R2" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="S2" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="T2" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="O2" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="P2" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q2" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="R2" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="S2" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="T2" s="42" t="s">
-        <v>220</v>
-      </c>
       <c r="U2" s="42"/>
+      <c r="V2">
+        <v>0</v>
+      </c>
       <c r="W2" s="42"/>
       <c r="X2" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y2" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="Y2" s="42" t="s">
+      <c r="Z2" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="Z2" s="42" t="s">
+      <c r="AA2" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB2" s="42" t="s">
         <v>213</v>
-      </c>
-      <c r="AA2" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="AB2" s="42" t="s">
-        <v>214</v>
       </c>
       <c r="AC2" s="42"/>
       <c r="AD2" s="42">
@@ -3582,35 +3556,35 @@
       </c>
       <c r="AE2" s="42"/>
       <c r="AF2" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AG2" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AH2" s="42"/>
       <c r="AI2" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="AJ2" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK2" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="AJ2" s="42" t="s">
-        <v>212</v>
-      </c>
-      <c r="AK2" s="42" t="s">
-        <v>237</v>
-      </c>
       <c r="AL2" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="AM2" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="AM2" s="42" t="s">
+      <c r="AN2" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="AN2" s="42" t="s">
-        <v>233</v>
-      </c>
       <c r="AO2" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AP2" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AR2" s="45">
         <v>0</v>
@@ -3623,7 +3597,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
@@ -3634,13 +3611,13 @@
       <c r="I3" s="42"/>
       <c r="J3" s="42"/>
       <c r="K3" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M3" s="43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N3" s="42">
         <v>1</v>
@@ -3649,7 +3626,7 @@
         <v>2</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q3" s="42">
         <v>5</v>
@@ -3659,10 +3636,13 @@
       </c>
       <c r="S3" s="42"/>
       <c r="T3" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="U3" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="U3" s="42" t="s">
-        <v>217</v>
+      <c r="V3">
+        <v>1</v>
       </c>
       <c r="W3" s="42"/>
       <c r="X3" s="42"/>
@@ -3677,13 +3657,13 @@
       <c r="AG3" s="42"/>
       <c r="AH3" s="42"/>
       <c r="AI3" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AJ3" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AK3" s="43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AL3" s="42">
         <v>1</v>
@@ -3692,7 +3672,7 @@
         <v>2</v>
       </c>
       <c r="AN3" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AO3" s="42">
         <v>5</v>
@@ -3711,36 +3691,39 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="D4" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>220</v>
-      </c>
       <c r="E4" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G4" s="42"/>
       <c r="H4" s="42"/>
       <c r="I4" s="42"/>
       <c r="J4" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="K4" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="K4" s="42" t="s">
-        <v>230</v>
-      </c>
       <c r="L4" s="42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M4" s="43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N4" s="42">
         <v>1</v>
@@ -3749,7 +3732,7 @@
         <v>2</v>
       </c>
       <c r="P4" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q4" s="42">
         <v>5</v>
@@ -3759,25 +3742,28 @@
       </c>
       <c r="S4" s="42"/>
       <c r="T4" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U4" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="W4" s="42" t="s">
+      <c r="X4" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="X4" s="42" t="s">
+      <c r="Y4" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="Y4" s="42" t="s">
-        <v>220</v>
-      </c>
       <c r="Z4" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AA4" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB4" s="42"/>
       <c r="AC4" s="42"/>
@@ -3786,16 +3772,16 @@
       <c r="AF4" s="42"/>
       <c r="AG4" s="42"/>
       <c r="AH4" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI4" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="AI4" s="42" t="s">
-        <v>230</v>
-      </c>
       <c r="AJ4" s="42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AK4" s="43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AL4" s="42">
         <v>1</v>
@@ -3804,7 +3790,7 @@
         <v>2</v>
       </c>
       <c r="AN4" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AO4" s="42">
         <v>5</v>
@@ -3823,19 +3809,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" s="42"/>
       <c r="C5" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G5" s="42"/>
       <c r="H5" s="42"/>
@@ -3846,36 +3835,39 @@
       <c r="M5" s="42"/>
       <c r="N5" s="42"/>
       <c r="O5" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="P5" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q5" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="R5" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="S5" s="42" t="s">
         <v>234</v>
-      </c>
-      <c r="P5" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q5" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="R5" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="S5" s="42" t="s">
-        <v>235</v>
       </c>
       <c r="T5" s="42"/>
       <c r="U5" s="42">
         <v>1</v>
       </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
       <c r="W5" s="42"/>
       <c r="X5" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y5" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z5" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AA5" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB5" s="42"/>
       <c r="AC5" s="42"/>
@@ -3886,19 +3878,19 @@
       <c r="AH5" s="42"/>
       <c r="AI5" s="42"/>
       <c r="AJ5" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="AK5" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="AL5" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="AM5" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="AN5" s="42" t="s">
         <v>234</v>
-      </c>
-      <c r="AK5" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="AL5" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="AM5" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="AN5" s="42" t="s">
-        <v>235</v>
       </c>
       <c r="AO5" s="42"/>
       <c r="AP5" s="42">
@@ -3915,27 +3907,127 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:46" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="41"/>
-      <c r="AE6" s="41"/>
-      <c r="AF6" s="41"/>
-      <c r="AG6" s="41"/>
-      <c r="AH6" s="41"/>
-      <c r="AI6" s="41"/>
-      <c r="AJ6" s="41"/>
-      <c r="AK6" s="41"/>
-      <c r="AL6" s="41"/>
-      <c r="AM6" s="41"/>
-      <c r="AN6" s="41"/>
-      <c r="AO6" s="41"/>
-      <c r="AP6" s="41"/>
+    <row r="6" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="44">
+        <v>0</v>
+      </c>
+      <c r="C6" s="44">
+        <v>1</v>
+      </c>
+      <c r="D6" s="44">
+        <v>2</v>
+      </c>
+      <c r="E6" s="44">
+        <v>3</v>
+      </c>
+      <c r="F6" s="44">
+        <v>4</v>
+      </c>
+      <c r="G6" s="44">
+        <v>5</v>
+      </c>
+      <c r="H6" s="44">
+        <v>6</v>
+      </c>
+      <c r="I6" s="44">
+        <v>7</v>
+      </c>
+      <c r="J6" s="44">
+        <v>8</v>
+      </c>
+      <c r="K6" s="44">
+        <v>9</v>
+      </c>
+      <c r="L6" s="44">
+        <v>10</v>
+      </c>
+      <c r="M6" s="44">
+        <v>11</v>
+      </c>
+      <c r="N6" s="44">
+        <v>12</v>
+      </c>
+      <c r="O6" s="44">
+        <v>13</v>
+      </c>
+      <c r="P6" s="44">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="44">
+        <v>15</v>
+      </c>
+      <c r="R6" s="44">
+        <v>16</v>
+      </c>
+      <c r="S6" s="44">
+        <v>17</v>
+      </c>
+      <c r="T6" s="44">
+        <v>18</v>
+      </c>
+      <c r="U6" s="44">
+        <v>19</v>
+      </c>
+      <c r="W6" s="44">
+        <v>0</v>
+      </c>
+      <c r="X6" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="44">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="44">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="44">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="44">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="44">
+        <v>6</v>
+      </c>
+      <c r="AD6" s="44">
+        <v>7</v>
+      </c>
+      <c r="AE6" s="44">
+        <v>8</v>
+      </c>
+      <c r="AF6" s="44">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="44">
+        <v>10</v>
+      </c>
+      <c r="AH6" s="44">
+        <v>11</v>
+      </c>
+      <c r="AI6" s="44">
+        <v>12</v>
+      </c>
+      <c r="AJ6" s="44">
+        <v>13</v>
+      </c>
+      <c r="AK6" s="44">
+        <v>14</v>
+      </c>
+      <c r="AL6" s="44">
+        <v>15</v>
+      </c>
+      <c r="AM6" s="44">
+        <v>16</v>
+      </c>
+      <c r="AN6" s="44">
+        <v>17</v>
+      </c>
+      <c r="AO6" s="44">
+        <v>18</v>
+      </c>
+      <c r="AP6" s="44">
+        <v>19</v>
+      </c>
       <c r="AR6" s="45">
         <v>4</v>
       </c>
@@ -3947,9 +4039,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0</v>
+      </c>
       <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="C7" s="42" t="s">
+        <v>210</v>
+      </c>
       <c r="D7" s="42" t="s">
         <v>211</v>
       </c>
@@ -3957,43 +4054,48 @@
         <v>212</v>
       </c>
       <c r="F7" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="G7" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42">
-        <v>1</v>
-      </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42" t="s">
-        <v>229</v>
-      </c>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42">
+        <v>1</v>
+      </c>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="L7" s="42"/>
       <c r="M7" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q7" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="P7" s="42" t="s">
+      <c r="R7" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="Q7" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="R7" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="S7" s="42"/>
+      <c r="S7" s="42" t="s">
+        <v>208</v>
+      </c>
       <c r="T7" s="42"/>
       <c r="U7" s="42"/>
+      <c r="V7">
+        <v>0</v>
+      </c>
       <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
+      <c r="X7" s="42" t="s">
+        <v>210</v>
+      </c>
       <c r="Y7" s="42" t="s">
         <v>211</v>
       </c>
@@ -4001,39 +4103,39 @@
         <v>212</v>
       </c>
       <c r="AA7" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB7" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="AB7" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="AC7" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD7" s="42"/>
-      <c r="AE7" s="42">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="42"/>
-      <c r="AG7" s="42" t="s">
-        <v>229</v>
-      </c>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="42"/>
+      <c r="AF7" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="AG7" s="42"/>
       <c r="AH7" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI7" s="42"/>
-      <c r="AJ7" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI7" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="AJ7" s="42"/>
+      <c r="AK7" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL7" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="AK7" s="42" t="s">
+      <c r="AM7" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="AL7" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="AM7" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="AN7" s="42"/>
+      <c r="AN7" s="42" t="s">
+        <v>208</v>
+      </c>
       <c r="AO7" s="42"/>
       <c r="AP7" s="42"/>
       <c r="AR7" s="45">
@@ -4047,7 +4149,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
       <c r="B8" s="42"/>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
@@ -4061,7 +4166,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K8" s="42">
         <v>5</v>
@@ -4071,10 +4176,10 @@
       </c>
       <c r="M8" s="42"/>
       <c r="N8" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="O8" s="42" t="s">
         <v>216</v>
-      </c>
-      <c r="O8" s="42" t="s">
-        <v>217</v>
       </c>
       <c r="P8" s="42"/>
       <c r="Q8" s="42"/>
@@ -4082,6 +4187,9 @@
       <c r="S8" s="42"/>
       <c r="T8" s="42"/>
       <c r="U8" s="42"/>
+      <c r="V8">
+        <v>1</v>
+      </c>
       <c r="W8" s="42"/>
       <c r="X8" s="42"/>
       <c r="Y8" s="42"/>
@@ -4096,7 +4204,7 @@
         <v>4</v>
       </c>
       <c r="AF8" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AG8" s="42">
         <v>5</v>
@@ -4123,24 +4231,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="D9" s="42" t="s">
         <v>209</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>210</v>
       </c>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I9" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J9" s="42"/>
       <c r="K9" s="42"/>
@@ -4154,24 +4265,27 @@
       <c r="S9" s="42"/>
       <c r="T9" s="42"/>
       <c r="U9" s="42"/>
+      <c r="V9">
+        <v>2</v>
+      </c>
       <c r="W9" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="X9" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="X9" s="42" t="s">
+      <c r="Y9" s="42" t="s">
         <v>209</v>
-      </c>
-      <c r="Y9" s="42" t="s">
-        <v>210</v>
       </c>
       <c r="Z9" s="42"/>
       <c r="AA9" s="42"/>
       <c r="AB9" s="42"/>
       <c r="AC9" s="42"/>
       <c r="AD9" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AE9" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF9" s="42"/>
       <c r="AG9" s="42"/>
@@ -4195,18 +4309,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3</v>
+      </c>
       <c r="B10" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="D10" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>224</v>
-      </c>
       <c r="E10" s="42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
@@ -4224,17 +4341,20 @@
       <c r="S10" s="42"/>
       <c r="T10" s="42"/>
       <c r="U10" s="42"/>
+      <c r="V10">
+        <v>3</v>
+      </c>
       <c r="W10" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="X10" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="X10" s="42" t="s">
+      <c r="Y10" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="Y10" s="42" t="s">
-        <v>224</v>
-      </c>
       <c r="Z10" s="42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AA10" s="42"/>
       <c r="AB10" s="42"/>
@@ -4253,31 +4373,136 @@
       <c r="AO10" s="42"/>
       <c r="AP10" s="42"/>
     </row>
-    <row r="11" spans="2:46" x14ac:dyDescent="0.35">
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="41"/>
-      <c r="AC11" s="41"/>
-      <c r="AD11" s="41"/>
-      <c r="AE11" s="41"/>
-      <c r="AF11" s="41"/>
-      <c r="AG11" s="41"/>
-      <c r="AH11" s="41"/>
-      <c r="AI11" s="41"/>
-      <c r="AJ11" s="41"/>
-      <c r="AK11" s="41"/>
-      <c r="AL11" s="41"/>
-      <c r="AM11" s="41"/>
-      <c r="AN11" s="41"/>
-      <c r="AO11" s="41"/>
-      <c r="AP11" s="41"/>
-    </row>
-    <row r="12" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B11" s="44">
+        <v>0</v>
+      </c>
+      <c r="C11" s="44">
+        <v>1</v>
+      </c>
+      <c r="D11" s="44">
+        <v>2</v>
+      </c>
+      <c r="E11" s="44">
+        <v>3</v>
+      </c>
+      <c r="F11" s="44">
+        <v>4</v>
+      </c>
+      <c r="G11" s="44">
+        <v>5</v>
+      </c>
+      <c r="H11" s="44">
+        <v>6</v>
+      </c>
+      <c r="I11" s="44">
+        <v>7</v>
+      </c>
+      <c r="J11" s="44">
+        <v>8</v>
+      </c>
+      <c r="K11" s="44">
+        <v>9</v>
+      </c>
+      <c r="L11" s="44">
+        <v>10</v>
+      </c>
+      <c r="M11" s="44">
+        <v>11</v>
+      </c>
+      <c r="N11" s="44">
+        <v>12</v>
+      </c>
+      <c r="O11" s="44">
+        <v>13</v>
+      </c>
+      <c r="P11" s="44">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="44">
+        <v>15</v>
+      </c>
+      <c r="R11" s="44">
+        <v>16</v>
+      </c>
+      <c r="S11" s="44">
+        <v>17</v>
+      </c>
+      <c r="T11" s="44">
+        <v>18</v>
+      </c>
+      <c r="U11" s="44">
+        <v>19</v>
+      </c>
+      <c r="W11" s="44">
+        <v>0</v>
+      </c>
+      <c r="X11" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="44">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="44">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="44">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="44">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="44">
+        <v>6</v>
+      </c>
+      <c r="AD11" s="44">
+        <v>7</v>
+      </c>
+      <c r="AE11" s="44">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="44">
+        <v>9</v>
+      </c>
+      <c r="AG11" s="44">
+        <v>10</v>
+      </c>
+      <c r="AH11" s="44">
+        <v>11</v>
+      </c>
+      <c r="AI11" s="44">
+        <v>12</v>
+      </c>
+      <c r="AJ11" s="44">
+        <v>13</v>
+      </c>
+      <c r="AK11" s="44">
+        <v>14</v>
+      </c>
+      <c r="AL11" s="44">
+        <v>15</v>
+      </c>
+      <c r="AM11" s="44">
+        <v>16</v>
+      </c>
+      <c r="AN11" s="44">
+        <v>17</v>
+      </c>
+      <c r="AO11" s="44">
+        <v>18</v>
+      </c>
+      <c r="AP11" s="44">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0</v>
+      </c>
       <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="C12" s="42" t="s">
+        <v>210</v>
+      </c>
       <c r="D12" s="42" t="s">
         <v>211</v>
       </c>
@@ -4285,45 +4510,50 @@
         <v>212</v>
       </c>
       <c r="F12" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="G12" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="G12" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="H12" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42">
-        <v>1</v>
-      </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42" t="s">
+      <c r="H12" s="42"/>
+      <c r="I12" s="42">
+        <v>1</v>
+      </c>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="N12" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="M12" s="42" t="s">
-        <v>230</v>
-      </c>
-      <c r="N12" s="42" t="s">
-        <v>230</v>
-      </c>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42" t="s">
+      <c r="O12" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="R12" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="Q12" s="42" t="s">
+      <c r="S12" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="R12" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="S12" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="T12" s="42"/>
+      <c r="T12" s="42" t="s">
+        <v>208</v>
+      </c>
       <c r="U12" s="42"/>
+      <c r="V12">
+        <v>0</v>
+      </c>
       <c r="W12" s="42"/>
-      <c r="X12" s="42"/>
+      <c r="X12" s="42" t="s">
+        <v>210</v>
+      </c>
       <c r="Y12" s="42" t="s">
         <v>211</v>
       </c>
@@ -4331,43 +4561,48 @@
         <v>212</v>
       </c>
       <c r="AA12" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB12" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="AB12" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="AC12" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD12" s="42"/>
-      <c r="AE12" s="42">
-        <v>1</v>
-      </c>
-      <c r="AF12" s="42"/>
-      <c r="AG12" s="42" t="s">
+      <c r="AC12" s="42"/>
+      <c r="AD12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="42"/>
+      <c r="AF12" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="AG12" s="42"/>
+      <c r="AH12" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI12" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="AH12" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI12" s="42"/>
       <c r="AJ12" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="AK12" s="42"/>
+      <c r="AL12" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="AM12" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="AK12" s="42" t="s">
+      <c r="AN12" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="AL12" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="AM12" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="AN12" s="42"/>
-      <c r="AO12" s="42"/>
+      <c r="AO12" s="42" t="s">
+        <v>208</v>
+      </c>
       <c r="AP12" s="42"/>
     </row>
-    <row r="13" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1</v>
+      </c>
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
@@ -4381,7 +4616,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K13" s="42">
         <v>5</v>
@@ -4391,10 +4626,10 @@
       </c>
       <c r="M13" s="42"/>
       <c r="N13" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="O13" s="42" t="s">
         <v>216</v>
-      </c>
-      <c r="O13" s="42" t="s">
-        <v>217</v>
       </c>
       <c r="P13" s="42"/>
       <c r="Q13" s="42"/>
@@ -4402,6 +4637,9 @@
       <c r="S13" s="42"/>
       <c r="T13" s="42"/>
       <c r="U13" s="42"/>
+      <c r="V13">
+        <v>1</v>
+      </c>
       <c r="W13" s="42"/>
       <c r="X13" s="42"/>
       <c r="Y13" s="42"/>
@@ -4416,7 +4654,7 @@
         <v>4</v>
       </c>
       <c r="AF13" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AG13" s="42">
         <v>5</v>
@@ -4433,15 +4671,18 @@
       <c r="AO13" s="42"/>
       <c r="AP13" s="42"/>
     </row>
-    <row r="14" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2</v>
+      </c>
       <c r="B14" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="D14" s="42" t="s">
         <v>209</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>210</v>
       </c>
       <c r="E14" s="42"/>
       <c r="F14" s="42"/>
@@ -4450,10 +4691,10 @@
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
       <c r="K14" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L14" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M14" s="42"/>
       <c r="N14" s="42"/>
@@ -4464,14 +4705,17 @@
       <c r="S14" s="42"/>
       <c r="T14" s="42"/>
       <c r="U14" s="42"/>
+      <c r="V14">
+        <v>2</v>
+      </c>
       <c r="W14" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="X14" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="X14" s="42" t="s">
+      <c r="Y14" s="42" t="s">
         <v>209</v>
-      </c>
-      <c r="Y14" s="42" t="s">
-        <v>210</v>
       </c>
       <c r="Z14" s="42"/>
       <c r="AA14" s="42"/>
@@ -4481,10 +4725,10 @@
       <c r="AE14" s="42"/>
       <c r="AF14" s="42"/>
       <c r="AG14" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AH14" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AI14" s="42"/>
       <c r="AJ14" s="42"/>
@@ -4495,24 +4739,27 @@
       <c r="AO14" s="42"/>
       <c r="AP14" s="42"/>
     </row>
-    <row r="15" spans="2:46" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3</v>
+      </c>
       <c r="B15" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
@@ -4528,23 +4775,26 @@
       <c r="S15" s="42"/>
       <c r="T15" s="42"/>
       <c r="U15" s="42"/>
+      <c r="V15">
+        <v>3</v>
+      </c>
       <c r="W15" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X15" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y15" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z15" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AA15" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB15" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AC15" s="42"/>
       <c r="AD15" s="42"/>
@@ -4561,10 +4811,137 @@
       <c r="AO15" s="42"/>
       <c r="AP15" s="42"/>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="44">
+        <v>0</v>
+      </c>
+      <c r="C16" s="44">
+        <v>1</v>
+      </c>
+      <c r="D16" s="44">
+        <v>2</v>
+      </c>
+      <c r="E16" s="44">
+        <v>3</v>
+      </c>
+      <c r="F16" s="44">
+        <v>4</v>
+      </c>
+      <c r="G16" s="44">
+        <v>5</v>
+      </c>
+      <c r="H16" s="44">
+        <v>6</v>
+      </c>
+      <c r="I16" s="44">
+        <v>7</v>
+      </c>
+      <c r="J16" s="44">
+        <v>8</v>
+      </c>
+      <c r="K16" s="44">
+        <v>9</v>
+      </c>
+      <c r="L16" s="44">
+        <v>10</v>
+      </c>
+      <c r="M16" s="44">
+        <v>11</v>
+      </c>
+      <c r="N16" s="44">
+        <v>12</v>
+      </c>
+      <c r="O16" s="44">
+        <v>13</v>
+      </c>
+      <c r="P16" s="44">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="44">
+        <v>15</v>
+      </c>
+      <c r="R16" s="44">
+        <v>16</v>
+      </c>
+      <c r="S16" s="44">
+        <v>17</v>
+      </c>
+      <c r="T16" s="44">
+        <v>18</v>
+      </c>
+      <c r="U16" s="44">
+        <v>19</v>
+      </c>
+      <c r="W16" s="44">
+        <v>0</v>
+      </c>
+      <c r="X16" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="44">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="44">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="44">
+        <v>4</v>
+      </c>
+      <c r="AB16" s="44">
+        <v>5</v>
+      </c>
+      <c r="AC16" s="44">
+        <v>6</v>
+      </c>
+      <c r="AD16" s="44">
+        <v>7</v>
+      </c>
+      <c r="AE16" s="44">
+        <v>8</v>
+      </c>
+      <c r="AF16" s="44">
+        <v>9</v>
+      </c>
+      <c r="AG16" s="44">
+        <v>10</v>
+      </c>
+      <c r="AH16" s="44">
+        <v>11</v>
+      </c>
+      <c r="AI16" s="44">
+        <v>12</v>
+      </c>
+      <c r="AJ16" s="44">
+        <v>13</v>
+      </c>
+      <c r="AK16" s="44">
+        <v>14</v>
+      </c>
+      <c r="AL16" s="44">
+        <v>15</v>
+      </c>
+      <c r="AM16" s="44">
+        <v>16</v>
+      </c>
+      <c r="AN16" s="44">
+        <v>17</v>
+      </c>
+      <c r="AO16" s="44">
+        <v>18</v>
+      </c>
+      <c r="AP16" s="44">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0</v>
+      </c>
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
+      <c r="D17" s="42" t="s">
+        <v>210</v>
+      </c>
       <c r="E17" s="42" t="s">
         <v>211</v>
       </c>
@@ -4572,40 +4949,86 @@
         <v>212</v>
       </c>
       <c r="G17" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="H17" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="H17" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42">
-        <v>1</v>
-      </c>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42" t="s">
+      <c r="I17" s="42"/>
+      <c r="J17" s="42">
+        <v>1</v>
+      </c>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="O17" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="P17" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q17" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="R17" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="N17" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="O17" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="P17" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q17" s="42" t="s">
-        <v>235</v>
-      </c>
-      <c r="R17" s="42"/>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
       <c r="U17" s="42"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17" s="42"/>
+      <c r="X17" s="42"/>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42"/>
+      <c r="AA17" s="42"/>
+      <c r="AB17" s="42"/>
+      <c r="AC17" s="42"/>
+      <c r="AD17" s="42"/>
+      <c r="AE17" s="42"/>
+      <c r="AF17" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG17" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH17" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="42">
+        <v>2</v>
+      </c>
+      <c r="AK17" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="AL17" s="42">
+        <v>5</v>
+      </c>
+      <c r="AM17" s="42">
+        <v>9</v>
+      </c>
+      <c r="AN17" s="42"/>
+      <c r="AO17" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="AP17" s="42" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1</v>
+      </c>
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
       <c r="D18" s="42"/>
@@ -4628,31 +5051,73 @@
       <c r="S18" s="42"/>
       <c r="T18" s="42"/>
       <c r="U18" s="42"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18" s="42"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="42"/>
+      <c r="AC18" s="42"/>
+      <c r="AD18" s="42"/>
+      <c r="AE18" s="42"/>
+      <c r="AF18" s="42"/>
+      <c r="AG18" s="42"/>
+      <c r="AH18" s="42"/>
+      <c r="AI18" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="AJ18" s="42">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="42">
+        <v>2</v>
+      </c>
+      <c r="AL18" s="42">
+        <v>3</v>
+      </c>
+      <c r="AM18" s="42">
+        <v>4</v>
+      </c>
+      <c r="AN18" s="42">
+        <v>5</v>
+      </c>
+      <c r="AO18" s="42">
+        <v>6</v>
+      </c>
+      <c r="AP18" s="42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2</v>
+      </c>
       <c r="B19" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="D19" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="G19" s="42" t="s">
         <v>209</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>210</v>
       </c>
       <c r="H19" s="42"/>
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
       <c r="K19" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L19" s="42"/>
       <c r="M19" s="42"/>
@@ -4664,22 +5129,64 @@
       <c r="S19" s="42"/>
       <c r="T19" s="42"/>
       <c r="U19" s="42"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="V19">
+        <v>2</v>
+      </c>
+      <c r="W19" s="42"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="42"/>
+      <c r="AC19" s="42"/>
+      <c r="AD19" s="42"/>
+      <c r="AE19" s="42"/>
+      <c r="AF19" s="42"/>
+      <c r="AG19" s="42"/>
+      <c r="AH19" s="42"/>
+      <c r="AI19" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ19" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK19" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="AL19" s="42">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="42">
+        <v>2</v>
+      </c>
+      <c r="AN19" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="AO19" s="42">
+        <v>5</v>
+      </c>
+      <c r="AP19" s="42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>3</v>
+      </c>
       <c r="B20" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="F20" s="42" t="s">
         <v>234</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>235</v>
       </c>
       <c r="G20" s="42"/>
       <c r="H20" s="42"/>
@@ -4696,24 +5203,169 @@
       <c r="S20" s="42"/>
       <c r="T20" s="42"/>
       <c r="U20" s="42"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="V20">
+        <v>3</v>
+      </c>
+      <c r="W20" s="42"/>
+      <c r="X20" s="42"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
+      <c r="AA20" s="42"/>
+      <c r="AB20" s="42"/>
+      <c r="AC20" s="42"/>
+      <c r="AD20" s="42"/>
+      <c r="AE20" s="42"/>
+      <c r="AF20" s="42"/>
+      <c r="AG20" s="42"/>
+      <c r="AH20" s="42"/>
+      <c r="AI20" s="42"/>
+      <c r="AJ20" s="42"/>
+      <c r="AK20" s="42"/>
+      <c r="AL20" s="42"/>
+      <c r="AM20" s="42"/>
+      <c r="AN20" s="42"/>
+      <c r="AO20" s="42"/>
+      <c r="AP20" s="42"/>
+    </row>
+    <row r="21" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B21" s="44">
+        <v>0</v>
+      </c>
+      <c r="C21" s="44">
+        <v>1</v>
+      </c>
+      <c r="D21" s="44">
+        <v>2</v>
+      </c>
+      <c r="E21" s="44">
+        <v>3</v>
+      </c>
+      <c r="F21" s="44">
+        <v>4</v>
+      </c>
+      <c r="G21" s="44">
+        <v>5</v>
+      </c>
+      <c r="H21" s="44">
+        <v>6</v>
+      </c>
+      <c r="I21" s="44">
+        <v>7</v>
+      </c>
+      <c r="J21" s="44">
+        <v>8</v>
+      </c>
+      <c r="K21" s="44">
+        <v>9</v>
+      </c>
+      <c r="L21" s="44">
+        <v>10</v>
+      </c>
+      <c r="M21" s="44">
+        <v>11</v>
+      </c>
+      <c r="N21" s="44">
+        <v>12</v>
+      </c>
+      <c r="O21" s="44">
+        <v>13</v>
+      </c>
+      <c r="P21" s="44">
+        <v>14</v>
+      </c>
+      <c r="Q21" s="44">
+        <v>15</v>
+      </c>
+      <c r="R21" s="44">
+        <v>16</v>
+      </c>
+      <c r="S21" s="44">
+        <v>17</v>
+      </c>
+      <c r="T21" s="44">
+        <v>18</v>
+      </c>
+      <c r="U21" s="44">
+        <v>19</v>
+      </c>
+      <c r="W21" s="44">
+        <v>0</v>
+      </c>
+      <c r="X21" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="44">
+        <v>2</v>
+      </c>
+      <c r="Z21" s="44">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="44">
+        <v>4</v>
+      </c>
+      <c r="AB21" s="44">
+        <v>5</v>
+      </c>
+      <c r="AC21" s="44">
+        <v>6</v>
+      </c>
+      <c r="AD21" s="44">
+        <v>7</v>
+      </c>
+      <c r="AE21" s="44">
+        <v>8</v>
+      </c>
+      <c r="AF21" s="44">
+        <v>9</v>
+      </c>
+      <c r="AG21" s="44">
+        <v>10</v>
+      </c>
+      <c r="AH21" s="44">
+        <v>11</v>
+      </c>
+      <c r="AI21" s="44">
+        <v>12</v>
+      </c>
+      <c r="AJ21" s="44">
+        <v>13</v>
+      </c>
+      <c r="AK21" s="44">
+        <v>14</v>
+      </c>
+      <c r="AL21" s="44">
+        <v>15</v>
+      </c>
+      <c r="AM21" s="44">
+        <v>16</v>
+      </c>
+      <c r="AN21" s="44">
+        <v>17</v>
+      </c>
+      <c r="AO21" s="44">
+        <v>18</v>
+      </c>
+      <c r="AP21" s="44">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="F22" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="G22" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="42" t="s">
         <v>213</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="H22" s="42" t="s">
-        <v>214</v>
       </c>
       <c r="I22" s="42"/>
       <c r="J22" s="42">
@@ -4721,31 +5373,31 @@
       </c>
       <c r="K22" s="42"/>
       <c r="L22" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="M22" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="N22" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="O22" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="P22" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q22" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="R22" s="42" t="s">
         <v>219</v>
-      </c>
-      <c r="M22" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="N22" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="O22" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="P22" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q22" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="R22" s="42" t="s">
-        <v>220</v>
       </c>
       <c r="S22" s="42"/>
       <c r="T22" s="42"/>
       <c r="U22" s="42"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B23" s="42"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42"/>
@@ -4755,13 +5407,13 @@
       <c r="H23" s="42"/>
       <c r="I23" s="42"/>
       <c r="J23" s="42" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K23" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L23" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M23" s="42"/>
       <c r="N23" s="42"/>
@@ -4773,35 +5425,35 @@
       <c r="T23" s="42"/>
       <c r="U23" s="42"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B24" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D24" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="E24" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="F24" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="F24" s="42" t="s">
-        <v>233</v>
-      </c>
       <c r="G24" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K24" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L24" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M24" s="42"/>
       <c r="N24" s="42"/>
@@ -4813,21 +5465,21 @@
       <c r="T24" s="42"/>
       <c r="U24" s="42"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B25" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="D25" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="E25" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="42" t="s">
         <v>213</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="F25" s="42" t="s">
-        <v>214</v>
       </c>
       <c r="G25" s="42"/>
       <c r="H25" s="42"/>

</xml_diff>

<commit_message>
Added support for all 8 timers.  Cleaned up old timer variables.  Cleaned up Serial debugging for the alarms.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="242">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -822,7 +822,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +856,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1092,7 +1098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1153,6 +1159,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1507,12 +1516,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="A1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="E1" t="s">
         <v>107</v>
       </c>
@@ -1741,12 +1750,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="E1" t="s">
         <v>106</v>
       </c>
@@ -1907,13 +1916,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
       <c r="F1" s="24" t="s">
         <v>119</v>
       </c>
@@ -1943,7 +1952,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="30">
         <v>100</v>
       </c>
@@ -1964,7 +1973,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="34">
         <v>101</v>
       </c>
@@ -1985,7 +1994,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="48" t="s">
         <v>191</v>
       </c>
       <c r="B5" s="30">
@@ -2008,7 +2017,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="48"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="34">
         <v>103</v>
       </c>
@@ -2029,7 +2038,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="34">
         <v>104</v>
       </c>
@@ -2050,7 +2059,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="34">
         <v>105</v>
       </c>
@@ -2071,7 +2080,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="34">
         <v>106</v>
       </c>
@@ -2092,7 +2101,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="49"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="27">
         <v>107</v>
       </c>
@@ -2113,7 +2122,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>192</v>
       </c>
       <c r="B11" s="30">
@@ -2136,7 +2145,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="34">
         <v>109</v>
       </c>
@@ -2157,7 +2166,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="34">
         <v>110</v>
       </c>
@@ -2178,7 +2187,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="34">
         <v>111</v>
       </c>
@@ -2199,7 +2208,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="34">
         <v>112</v>
       </c>
@@ -2220,7 +2229,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="27">
         <v>113</v>
       </c>
@@ -2241,7 +2250,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="48" t="s">
         <v>193</v>
       </c>
       <c r="B17" s="34">
@@ -2264,7 +2273,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="34">
         <v>115</v>
       </c>
@@ -2285,7 +2294,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="34">
         <v>116</v>
       </c>
@@ -2306,7 +2315,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="34">
         <v>117</v>
       </c>
@@ -2327,7 +2336,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="34">
         <v>118</v>
       </c>
@@ -2348,7 +2357,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="34">
         <v>119</v>
       </c>
@@ -2369,7 +2378,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="48" t="s">
         <v>194</v>
       </c>
       <c r="B23" s="30">
@@ -2392,7 +2401,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="48"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="34">
         <v>121</v>
       </c>
@@ -2413,7 +2422,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="48"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="34">
         <v>122</v>
       </c>
@@ -2434,7 +2443,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="48"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="34">
         <v>123</v>
       </c>
@@ -2455,7 +2464,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="34">
         <v>124</v>
       </c>
@@ -2476,7 +2485,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="49"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="27">
         <v>125</v>
       </c>
@@ -2497,7 +2506,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="48" t="s">
         <v>195</v>
       </c>
       <c r="B29" s="34">
@@ -2520,7 +2529,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="34">
         <v>127</v>
       </c>
@@ -2541,7 +2550,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="48"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="34">
         <v>128</v>
       </c>
@@ -2562,7 +2571,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="48"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="34">
         <v>129</v>
       </c>
@@ -2583,7 +2592,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="48"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="34">
         <v>130</v>
       </c>
@@ -2604,7 +2613,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="49"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="34">
         <v>131</v>
       </c>
@@ -2625,7 +2634,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="48" t="s">
         <v>196</v>
       </c>
       <c r="B35" s="30">
@@ -2648,7 +2657,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="48"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="34">
         <v>133</v>
       </c>
@@ -2669,7 +2678,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="48"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="34">
         <v>134</v>
       </c>
@@ -2690,7 +2699,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="48"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="34">
         <v>135</v>
       </c>
@@ -2711,7 +2720,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="48"/>
+      <c r="A39" s="49"/>
       <c r="B39" s="34">
         <v>136</v>
       </c>
@@ -2732,7 +2741,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="49"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="27">
         <v>137</v>
       </c>
@@ -2753,7 +2762,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="48" t="s">
         <v>197</v>
       </c>
       <c r="B41" s="34">
@@ -2776,7 +2785,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="48"/>
+      <c r="A42" s="49"/>
       <c r="B42" s="34">
         <v>139</v>
       </c>
@@ -2797,7 +2806,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="48"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="34">
         <v>140</v>
       </c>
@@ -2818,7 +2827,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="48"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="34">
         <v>141</v>
       </c>
@@ -2839,7 +2848,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="48"/>
+      <c r="A45" s="49"/>
       <c r="B45" s="34">
         <v>142</v>
       </c>
@@ -2860,7 +2869,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="49"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="34">
         <v>143</v>
       </c>
@@ -2881,7 +2890,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="47" t="s">
+      <c r="A47" s="48" t="s">
         <v>198</v>
       </c>
       <c r="B47" s="30">
@@ -2904,7 +2913,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="48"/>
+      <c r="A48" s="49"/>
       <c r="B48" s="34">
         <v>145</v>
       </c>
@@ -2925,7 +2934,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="48"/>
+      <c r="A49" s="49"/>
       <c r="B49" s="34">
         <v>146</v>
       </c>
@@ -2946,7 +2955,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="48"/>
+      <c r="A50" s="49"/>
       <c r="B50" s="34">
         <v>147</v>
       </c>
@@ -2967,7 +2976,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="48"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="34">
         <v>148</v>
       </c>
@@ -2988,7 +2997,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="49"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="27">
         <v>149</v>
       </c>
@@ -3330,10 +3339,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT25"/>
+  <dimension ref="A1:AW25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI18" sqref="AI18"/>
+      <selection activeCell="AW3" sqref="AW3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3346,7 +3355,7 @@
     <col min="50" max="50" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B1" s="44">
         <v>0</v>
       </c>
@@ -3477,7 +3486,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3590,14 +3599,21 @@
         <v>0</v>
       </c>
       <c r="AS2" s="45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT2" s="45">
-        <f>AR2+8</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="AV2">
+        <f>(AS2-1)/2</f>
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <f t="shared" ref="AW2:AW9" si="0">(AT2-2)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3684,14 +3700,21 @@
         <v>1</v>
       </c>
       <c r="AS3" s="45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT3" s="45">
-        <f t="shared" ref="AT3:AT9" si="0">AR3+8</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="AV3">
+        <f>(AS3-1)/2</f>
+        <v>1</v>
+      </c>
+      <c r="AW3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3802,14 +3825,21 @@
         <v>2</v>
       </c>
       <c r="AS4" s="45">
+        <v>5</v>
+      </c>
+      <c r="AT4" s="45">
+        <v>6</v>
+      </c>
+      <c r="AV4">
+        <f t="shared" ref="AV4:AW9" si="1">(AS4-1)/2</f>
         <v>2</v>
       </c>
-      <c r="AT4" s="45">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.35">
+      <c r="AW4">
+        <f>(AT4-2)/2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3900,14 +3930,21 @@
         <v>3</v>
       </c>
       <c r="AS5" s="45">
+        <v>7</v>
+      </c>
+      <c r="AT5" s="45">
+        <v>8</v>
+      </c>
+      <c r="AV5">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="AT5" s="45">
+      <c r="AW5">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="44">
         <v>0</v>
       </c>
@@ -4032,14 +4069,21 @@
         <v>4</v>
       </c>
       <c r="AS6" s="45">
+        <v>9</v>
+      </c>
+      <c r="AT6" s="45">
+        <v>10</v>
+      </c>
+      <c r="AV6">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AT6" s="45">
+      <c r="AW6">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4142,14 +4186,21 @@
         <v>5</v>
       </c>
       <c r="AS7" s="45">
+        <v>11</v>
+      </c>
+      <c r="AT7" s="45">
+        <v>12</v>
+      </c>
+      <c r="AV7">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="AT7" s="45">
+      <c r="AW7">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4224,14 +4275,21 @@
         <v>6</v>
       </c>
       <c r="AS8" s="45">
+        <v>13</v>
+      </c>
+      <c r="AT8" s="45">
+        <v>14</v>
+      </c>
+      <c r="AV8">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="AT8" s="45">
+      <c r="AW8">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4302,14 +4360,21 @@
         <v>7</v>
       </c>
       <c r="AS9" s="45">
+        <v>15</v>
+      </c>
+      <c r="AT9" s="45">
+        <v>16</v>
+      </c>
+      <c r="AV9">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="AT9" s="45">
+      <c r="AW9">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
@@ -4373,7 +4438,7 @@
       <c r="AO10" s="42"/>
       <c r="AP10" s="42"/>
     </row>
-    <row r="11" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="44">
         <v>0</v>
       </c>
@@ -4495,7 +4560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -4599,7 +4664,7 @@
       </c>
       <c r="AP12" s="42"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4671,7 +4736,7 @@
       <c r="AO13" s="42"/>
       <c r="AP13" s="42"/>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4739,7 +4804,7 @@
       <c r="AO14" s="42"/>
       <c r="AP14" s="42"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3</v>
       </c>
@@ -4811,7 +4876,7 @@
       <c r="AO15" s="42"/>
       <c r="AP15" s="42"/>
     </row>
-    <row r="16" spans="1:46" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:49" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="44">
         <v>0</v>
       </c>
@@ -5396,6 +5461,52 @@
       <c r="S22" s="42"/>
       <c r="T22" s="42"/>
       <c r="U22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y22" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z22" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA22" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB22" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC22" s="42"/>
+      <c r="AD22" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="42"/>
+      <c r="AF22" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="AG22" s="42"/>
+      <c r="AH22" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI22" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="AJ22" s="42"/>
+      <c r="AK22" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL22" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="AM22" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="AN22" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="AO22" s="42"/>
+      <c r="AP22" s="42"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B23" s="42"/>
@@ -5424,6 +5535,40 @@
       <c r="S23" s="42"/>
       <c r="T23" s="42"/>
       <c r="U23" s="42"/>
+      <c r="W23" s="42"/>
+      <c r="X23" s="42"/>
+      <c r="Y23" s="42"/>
+      <c r="Z23" s="42"/>
+      <c r="AA23" s="42"/>
+      <c r="AB23" s="42"/>
+      <c r="AC23" s="46">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="42">
+        <v>2</v>
+      </c>
+      <c r="AE23" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="AF23" s="42">
+        <v>5</v>
+      </c>
+      <c r="AG23" s="42">
+        <v>9</v>
+      </c>
+      <c r="AH23" s="42"/>
+      <c r="AI23" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="AJ23" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="AK23" s="42"/>
+      <c r="AL23" s="42"/>
+      <c r="AM23" s="42"/>
+      <c r="AN23" s="42"/>
+      <c r="AO23" s="42"/>
+      <c r="AP23" s="42"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B24" s="42" t="s">
@@ -5464,6 +5609,36 @@
       <c r="S24" s="42"/>
       <c r="T24" s="42"/>
       <c r="U24" s="42"/>
+      <c r="W24" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="X24" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y24" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="42"/>
+      <c r="AC24" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD24" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="AE24" s="42"/>
+      <c r="AF24" s="42"/>
+      <c r="AG24" s="42"/>
+      <c r="AH24" s="42"/>
+      <c r="AI24" s="42"/>
+      <c r="AJ24" s="42"/>
+      <c r="AK24" s="42"/>
+      <c r="AL24" s="42"/>
+      <c r="AM24" s="42"/>
+      <c r="AN24" s="42"/>
+      <c r="AO24" s="42"/>
+      <c r="AP24" s="42"/>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B25" s="42" t="s">
@@ -5496,6 +5671,34 @@
       <c r="S25" s="42"/>
       <c r="T25" s="42"/>
       <c r="U25" s="42"/>
+      <c r="W25" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="X25" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y25" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z25" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA25" s="42"/>
+      <c r="AB25" s="42"/>
+      <c r="AC25" s="42"/>
+      <c r="AD25" s="42"/>
+      <c r="AE25" s="42"/>
+      <c r="AF25" s="42"/>
+      <c r="AG25" s="42"/>
+      <c r="AH25" s="42"/>
+      <c r="AI25" s="42"/>
+      <c r="AJ25" s="42"/>
+      <c r="AK25" s="42"/>
+      <c r="AL25" s="42"/>
+      <c r="AM25" s="42"/>
+      <c r="AN25" s="42"/>
+      <c r="AO25" s="42"/>
+      <c r="AP25" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9094,25 +9297,25 @@
       <c r="H1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="55" t="s">
+      <c r="N1" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="55" t="s">
+      <c r="O1" s="56" t="s">
         <v>92</v>
       </c>
     </row>
@@ -9133,13 +9336,13 @@
       <c r="H2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
       <c r="P2" t="s">
         <v>93</v>
       </c>
@@ -9161,13 +9364,13 @@
       <c r="H3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">

</xml_diff>

<commit_message>
Tagging as v0.16 AlarmEnableing via the LCD menu is now complete.  Added the enable flag to the startup alarm settings display.  There is still no support for this feature, but will be comming in future builds.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="238">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -735,9 +735,6 @@
   </si>
   <si>
     <t>Time format 0 = 24 hour, 1 = 12 hour</t>
-  </si>
-  <si>
-    <t>EEPROM Suppress</t>
   </si>
   <si>
     <t>EEPROM read/write</t>
@@ -1459,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1804,7 +1801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
@@ -2944,7 +2941,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3130,7 +3127,7 @@
         <v>5</v>
       </c>
       <c r="N5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -3166,9 +3163,6 @@
       </c>
       <c r="M6">
         <v>6</v>
-      </c>
-      <c r="N6" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -3296,10 +3290,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW25"/>
+  <dimension ref="A1:AW30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AR14" sqref="AR14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27:W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -3788,7 +3782,7 @@
         <v>6</v>
       </c>
       <c r="AV4">
-        <f t="shared" ref="AV4:AW9" si="1">(AS4-1)/2</f>
+        <f t="shared" ref="AV4:AV9" si="1">(AS4-1)/2</f>
         <v>2</v>
       </c>
       <c r="AW4">
@@ -5372,50 +5366,55 @@
       </c>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0</v>
+      </c>
       <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
+      <c r="C22" s="37" t="s">
+        <v>205</v>
+      </c>
       <c r="D22" s="37" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G22" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37">
+        <v>1</v>
+      </c>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="N22" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="O22" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="P22" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q22" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="R22" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="H22" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37">
-        <v>1</v>
-      </c>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37" t="s">
-        <v>213</v>
-      </c>
-      <c r="M22" s="37" t="s">
-        <v>221</v>
-      </c>
-      <c r="N22" s="37" t="s">
-        <v>225</v>
-      </c>
-      <c r="O22" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="P22" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q22" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="R22" s="37" t="s">
+      <c r="S22" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="S22" s="37"/>
       <c r="T22" s="37"/>
       <c r="U22" s="37"/>
       <c r="W22" s="37"/>
@@ -5466,6 +5465,9 @@
       <c r="AP22" s="37"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1</v>
+      </c>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
       <c r="D23" s="37"/>
@@ -5528,6 +5530,9 @@
       <c r="AP23" s="37"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2</v>
+      </c>
       <c r="B24" s="37" t="s">
         <v>213</v>
       </c>
@@ -5598,6 +5603,9 @@
       <c r="AP24" s="37"/>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>3</v>
+      </c>
       <c r="B25" s="37" t="s">
         <v>205</v>
       </c>
@@ -5656,6 +5664,232 @@
       <c r="AN25" s="37"/>
       <c r="AO25" s="37"/>
       <c r="AP25" s="37"/>
+    </row>
+    <row r="26" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="39">
+        <v>0</v>
+      </c>
+      <c r="C26" s="39">
+        <v>1</v>
+      </c>
+      <c r="D26" s="39">
+        <v>2</v>
+      </c>
+      <c r="E26" s="39">
+        <v>3</v>
+      </c>
+      <c r="F26" s="39">
+        <v>4</v>
+      </c>
+      <c r="G26" s="39">
+        <v>5</v>
+      </c>
+      <c r="H26" s="39">
+        <v>6</v>
+      </c>
+      <c r="I26" s="39">
+        <v>7</v>
+      </c>
+      <c r="J26" s="39">
+        <v>8</v>
+      </c>
+      <c r="K26" s="39">
+        <v>9</v>
+      </c>
+      <c r="L26" s="39">
+        <v>10</v>
+      </c>
+      <c r="M26" s="39">
+        <v>11</v>
+      </c>
+      <c r="N26" s="39">
+        <v>12</v>
+      </c>
+      <c r="O26" s="39">
+        <v>13</v>
+      </c>
+      <c r="P26" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q26" s="39">
+        <v>15</v>
+      </c>
+      <c r="R26" s="39">
+        <v>16</v>
+      </c>
+      <c r="S26" s="39">
+        <v>17</v>
+      </c>
+      <c r="T26" s="39">
+        <v>18</v>
+      </c>
+      <c r="U26" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37">
+        <v>1</v>
+      </c>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="N27" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="O27" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="P27" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q27" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="R27" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="S27" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="T27" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="U27" s="37"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="K28" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="L28" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="G29" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="K29" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="L29" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="M29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="37"/>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tagging as v0.19 Added NumSel types to the MenuNumSel function.  0=normal numbers, 1=time, 2=yes/no, 3=enable/disable.  If the 7th bit is set you will supress the saving or exit without save message.  If you set the 8th bit to 1, you will disable eeprom writing at the end of the function.  Fixed a small bug that if the hour was >22, it was displaying it 1 digit to the right.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,15 @@
     <sheet name="Bit Shift" sheetId="8" r:id="rId4"/>
     <sheet name="LCD Setups" sheetId="9" r:id="rId5"/>
     <sheet name="Menu Variables" sheetId="6" r:id="rId6"/>
+    <sheet name="12 Hour" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="282">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -738,13 +740,145 @@
   </si>
   <si>
     <t>EEPROM read/write</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>1 digit</t>
+  </si>
+  <si>
+    <t>2 digit</t>
+  </si>
+  <si>
+    <t>col +1</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>start -12</t>
+  </si>
+  <si>
+    <t>start = start</t>
+  </si>
+  <si>
+    <t>if &lt;12</t>
+  </si>
+  <si>
+    <t>if = 0 start + 12</t>
+  </si>
+  <si>
+    <t>if &gt; =12</t>
+  </si>
+  <si>
+    <t>Roadmap Generalized</t>
+  </si>
+  <si>
+    <t>Add a type to MenuNumSel and possibly rename it ot MenuSel since it wont just be dealing with Numbers</t>
+  </si>
+  <si>
+    <t>Finish out the Alarm functions</t>
+  </si>
+  <si>
+    <t>Add in Alarm Type</t>
+  </si>
+  <si>
+    <t>Make this usefull</t>
+  </si>
+  <si>
+    <t>Add in AlarmEnable/Disable to the AlarmOn/Off functions</t>
+  </si>
+  <si>
+    <t>Menu System Timeout</t>
+  </si>
+  <si>
+    <t>Add the ability for the menu system to timeout after being in it for a certain ammount of time</t>
+  </si>
+  <si>
+    <t>Add Alarm State reading and functionality</t>
+  </si>
+  <si>
+    <t>Continue to log sensors while in the menu</t>
+  </si>
+  <si>
+    <t>Set the date and time using the LCD screen</t>
+  </si>
+  <si>
+    <t>Add hardware and software support for Backlight brightness</t>
+  </si>
+  <si>
+    <t>Be able to address the sensors</t>
+  </si>
+  <si>
+    <t>Be able to calibrate the sensors</t>
+  </si>
+  <si>
+    <t>Add a flow meter to the project</t>
+  </si>
+  <si>
+    <t>calibrate the flow meter</t>
+  </si>
+  <si>
+    <t>display the flow on the LCD screen</t>
+  </si>
+  <si>
+    <t>be able to name the sensors according to the address</t>
+  </si>
+  <si>
+    <t>Assign the Alarms a relay to triger</t>
+  </si>
+  <si>
+    <t>Assign names to the alarms and make the display be able to select the alarms by name</t>
+  </si>
+  <si>
+    <t>Split the sysconfig menu and add a User Settings Menu</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Time breakpoints brainstorming and visualization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,8 +928,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -829,6 +970,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,7 +1236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1149,6 +1320,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1801,7 +1993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
@@ -2940,7 +3132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N267"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -11739,10 +11931,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW30"/>
+  <dimension ref="A1:AW40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27:W27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -14175,6 +14367,66 @@
       <c r="U26" s="39">
         <v>19</v>
       </c>
+      <c r="W26" s="39">
+        <v>0</v>
+      </c>
+      <c r="X26" s="39">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="39">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="39">
+        <v>3</v>
+      </c>
+      <c r="AA26" s="39">
+        <v>4</v>
+      </c>
+      <c r="AB26" s="39">
+        <v>5</v>
+      </c>
+      <c r="AC26" s="39">
+        <v>6</v>
+      </c>
+      <c r="AD26" s="39">
+        <v>7</v>
+      </c>
+      <c r="AE26" s="39">
+        <v>8</v>
+      </c>
+      <c r="AF26" s="39">
+        <v>9</v>
+      </c>
+      <c r="AG26" s="39">
+        <v>10</v>
+      </c>
+      <c r="AH26" s="39">
+        <v>11</v>
+      </c>
+      <c r="AI26" s="39">
+        <v>12</v>
+      </c>
+      <c r="AJ26" s="39">
+        <v>13</v>
+      </c>
+      <c r="AK26" s="39">
+        <v>14</v>
+      </c>
+      <c r="AL26" s="39">
+        <v>15</v>
+      </c>
+      <c r="AM26" s="39">
+        <v>16</v>
+      </c>
+      <c r="AN26" s="39">
+        <v>17</v>
+      </c>
+      <c r="AO26" s="39">
+        <v>18</v>
+      </c>
+      <c r="AP26" s="39">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -14230,6 +14482,61 @@
         <v>214</v>
       </c>
       <c r="U27" s="37"/>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="X27" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y27" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="Z27" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA27" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB27" s="37"/>
+      <c r="AC27" s="37">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="37"/>
+      <c r="AE27" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF27" s="37"/>
+      <c r="AG27" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH27" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI27" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ27" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="AK27" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="AL27" s="37"/>
+      <c r="AM27" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN27" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="AO27" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="AP27" s="37" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A28">
@@ -14261,6 +14568,31 @@
       <c r="S28" s="37"/>
       <c r="T28" s="37"/>
       <c r="U28" s="37"/>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28" s="37"/>
+      <c r="X28" s="37"/>
+      <c r="Y28" s="37"/>
+      <c r="Z28" s="37"/>
+      <c r="AA28" s="37"/>
+      <c r="AB28" s="37"/>
+      <c r="AC28" s="37"/>
+      <c r="AD28" s="37"/>
+      <c r="AE28" s="37"/>
+      <c r="AF28" s="37">
+        <v>1</v>
+      </c>
+      <c r="AG28" s="37"/>
+      <c r="AH28" s="37"/>
+      <c r="AI28" s="37"/>
+      <c r="AJ28" s="37"/>
+      <c r="AK28" s="37"/>
+      <c r="AL28" s="37"/>
+      <c r="AM28" s="37"/>
+      <c r="AN28" s="37"/>
+      <c r="AO28" s="37"/>
+      <c r="AP28" s="37"/>
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A29">
@@ -14304,6 +14636,51 @@
       <c r="S29" s="37"/>
       <c r="T29" s="37"/>
       <c r="U29" s="37"/>
+      <c r="V29">
+        <v>2</v>
+      </c>
+      <c r="W29" s="37">
+        <v>0</v>
+      </c>
+      <c r="X29" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y29" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z29" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA29" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB29" s="37"/>
+      <c r="AC29" s="37"/>
+      <c r="AD29" s="37"/>
+      <c r="AE29" s="37"/>
+      <c r="AF29" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="AG29" s="37"/>
+      <c r="AH29" s="37"/>
+      <c r="AI29" s="37"/>
+      <c r="AJ29" s="37">
+        <v>2</v>
+      </c>
+      <c r="AK29" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="AL29" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="AM29" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="AN29" s="37">
+        <v>2</v>
+      </c>
+      <c r="AO29" s="37"/>
+      <c r="AP29" s="37"/>
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A30">
@@ -14339,6 +14716,1113 @@
       <c r="S30" s="37"/>
       <c r="T30" s="37"/>
       <c r="U30" s="37"/>
+      <c r="V30">
+        <v>3</v>
+      </c>
+      <c r="W30" s="37">
+        <v>1</v>
+      </c>
+      <c r="X30" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="Y30" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z30" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA30" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB30" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="AC30" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD30" s="37"/>
+      <c r="AE30" s="37"/>
+      <c r="AF30" s="37"/>
+      <c r="AG30" s="37"/>
+      <c r="AH30" s="37"/>
+      <c r="AI30" s="37"/>
+      <c r="AJ30" s="37">
+        <v>3</v>
+      </c>
+      <c r="AK30" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="AL30" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="AM30" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN30" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="AO30" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="AP30" s="37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B31" s="39">
+        <v>0</v>
+      </c>
+      <c r="C31" s="39">
+        <v>1</v>
+      </c>
+      <c r="D31" s="39">
+        <v>2</v>
+      </c>
+      <c r="E31" s="39">
+        <v>3</v>
+      </c>
+      <c r="F31" s="39">
+        <v>4</v>
+      </c>
+      <c r="G31" s="39">
+        <v>5</v>
+      </c>
+      <c r="H31" s="39">
+        <v>6</v>
+      </c>
+      <c r="I31" s="39">
+        <v>7</v>
+      </c>
+      <c r="J31" s="39">
+        <v>8</v>
+      </c>
+      <c r="K31" s="39">
+        <v>9</v>
+      </c>
+      <c r="L31" s="39">
+        <v>10</v>
+      </c>
+      <c r="M31" s="39">
+        <v>11</v>
+      </c>
+      <c r="N31" s="39">
+        <v>12</v>
+      </c>
+      <c r="O31" s="39">
+        <v>13</v>
+      </c>
+      <c r="P31" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q31" s="39">
+        <v>15</v>
+      </c>
+      <c r="R31" s="39">
+        <v>16</v>
+      </c>
+      <c r="S31" s="39">
+        <v>17</v>
+      </c>
+      <c r="T31" s="39">
+        <v>18</v>
+      </c>
+      <c r="U31" s="39">
+        <v>19</v>
+      </c>
+      <c r="W31" s="39">
+        <v>0</v>
+      </c>
+      <c r="X31" s="39">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="39">
+        <v>2</v>
+      </c>
+      <c r="Z31" s="39">
+        <v>3</v>
+      </c>
+      <c r="AA31" s="39">
+        <v>4</v>
+      </c>
+      <c r="AB31" s="39">
+        <v>5</v>
+      </c>
+      <c r="AC31" s="39">
+        <v>6</v>
+      </c>
+      <c r="AD31" s="39">
+        <v>7</v>
+      </c>
+      <c r="AE31" s="39">
+        <v>8</v>
+      </c>
+      <c r="AF31" s="39">
+        <v>9</v>
+      </c>
+      <c r="AG31" s="39">
+        <v>10</v>
+      </c>
+      <c r="AH31" s="39">
+        <v>11</v>
+      </c>
+      <c r="AI31" s="39">
+        <v>12</v>
+      </c>
+      <c r="AJ31" s="39">
+        <v>13</v>
+      </c>
+      <c r="AK31" s="39">
+        <v>14</v>
+      </c>
+      <c r="AL31" s="39">
+        <v>15</v>
+      </c>
+      <c r="AM31" s="39">
+        <v>16</v>
+      </c>
+      <c r="AN31" s="39">
+        <v>17</v>
+      </c>
+      <c r="AO31" s="39">
+        <v>18</v>
+      </c>
+      <c r="AP31" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32" s="37">
+        <v>1</v>
+      </c>
+      <c r="C32" s="37">
+        <v>1</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="E32" s="37">
+        <v>2</v>
+      </c>
+      <c r="F32" s="37">
+        <v>0</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="H32" s="37">
+        <v>4</v>
+      </c>
+      <c r="I32" s="37">
+        <v>4</v>
+      </c>
+      <c r="J32" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="K32" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N32" s="37">
+        <v>1</v>
+      </c>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q32" s="37">
+        <v>4</v>
+      </c>
+      <c r="R32" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S32" s="37">
+        <v>3</v>
+      </c>
+      <c r="T32" s="37"/>
+      <c r="U32" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32" s="37"/>
+      <c r="X32" s="37">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z32" s="37">
+        <v>2</v>
+      </c>
+      <c r="AA32" s="37">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC32" s="37">
+        <v>4</v>
+      </c>
+      <c r="AD32" s="37">
+        <v>4</v>
+      </c>
+      <c r="AE32" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF32" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG32" s="37"/>
+      <c r="AH32" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI32" s="37">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="37"/>
+      <c r="AK32" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL32" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM32" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN32" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO32" s="37"/>
+      <c r="AP32" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37">
+        <v>1</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E33" s="37">
+        <v>2</v>
+      </c>
+      <c r="F33" s="37">
+        <v>8</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="H33" s="37">
+        <v>2</v>
+      </c>
+      <c r="I33" s="37">
+        <v>0</v>
+      </c>
+      <c r="J33" s="37">
+        <v>1</v>
+      </c>
+      <c r="K33" s="37">
+        <v>5</v>
+      </c>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N33" s="37">
+        <v>2</v>
+      </c>
+      <c r="O33" s="37"/>
+      <c r="P33" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q33" s="37">
+        <v>4</v>
+      </c>
+      <c r="R33" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S33" s="37">
+        <v>3</v>
+      </c>
+      <c r="T33" s="37"/>
+      <c r="U33" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33" s="37"/>
+      <c r="X33" s="37">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="Z33" s="37">
+        <v>2</v>
+      </c>
+      <c r="AA33" s="37">
+        <v>8</v>
+      </c>
+      <c r="AB33" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC33" s="37">
+        <v>2</v>
+      </c>
+      <c r="AD33" s="37">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="37">
+        <v>1</v>
+      </c>
+      <c r="AF33" s="37">
+        <v>5</v>
+      </c>
+      <c r="AG33" s="37"/>
+      <c r="AH33" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI33" s="37">
+        <v>2</v>
+      </c>
+      <c r="AJ33" s="37"/>
+      <c r="AK33" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL33" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM33" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN33" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO33" s="37"/>
+      <c r="AP33" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N34" s="37">
+        <v>3</v>
+      </c>
+      <c r="O34" s="37"/>
+      <c r="P34" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q34" s="37">
+        <v>4</v>
+      </c>
+      <c r="R34" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S34" s="37">
+        <v>3</v>
+      </c>
+      <c r="T34" s="37"/>
+      <c r="U34" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V34">
+        <v>2</v>
+      </c>
+      <c r="W34" s="37"/>
+      <c r="X34" s="37"/>
+      <c r="Y34" s="37"/>
+      <c r="Z34" s="37"/>
+      <c r="AA34" s="37"/>
+      <c r="AB34" s="37"/>
+      <c r="AC34" s="37"/>
+      <c r="AD34" s="37"/>
+      <c r="AE34" s="37"/>
+      <c r="AF34" s="37"/>
+      <c r="AG34" s="37"/>
+      <c r="AH34" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI34" s="37">
+        <v>3</v>
+      </c>
+      <c r="AJ34" s="37"/>
+      <c r="AK34" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL34" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM34" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN34" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO34" s="37"/>
+      <c r="AP34" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="H35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="I35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N35" s="37">
+        <v>4</v>
+      </c>
+      <c r="O35" s="37"/>
+      <c r="P35" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q35" s="37">
+        <v>4</v>
+      </c>
+      <c r="R35" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S35" s="37">
+        <v>3</v>
+      </c>
+      <c r="T35" s="37"/>
+      <c r="U35" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V35">
+        <v>3</v>
+      </c>
+      <c r="W35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="X35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AB35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD35" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE35" s="37"/>
+      <c r="AF35" s="37"/>
+      <c r="AG35" s="37"/>
+      <c r="AH35" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI35" s="37">
+        <v>4</v>
+      </c>
+      <c r="AJ35" s="37"/>
+      <c r="AK35" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL35" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM35" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN35" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO35" s="37"/>
+      <c r="AP35" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B36" s="39">
+        <v>0</v>
+      </c>
+      <c r="C36" s="39">
+        <v>1</v>
+      </c>
+      <c r="D36" s="39">
+        <v>2</v>
+      </c>
+      <c r="E36" s="39">
+        <v>3</v>
+      </c>
+      <c r="F36" s="39">
+        <v>4</v>
+      </c>
+      <c r="G36" s="39">
+        <v>5</v>
+      </c>
+      <c r="H36" s="39">
+        <v>6</v>
+      </c>
+      <c r="I36" s="39">
+        <v>7</v>
+      </c>
+      <c r="J36" s="39">
+        <v>8</v>
+      </c>
+      <c r="K36" s="39">
+        <v>9</v>
+      </c>
+      <c r="L36" s="39">
+        <v>10</v>
+      </c>
+      <c r="M36" s="39">
+        <v>11</v>
+      </c>
+      <c r="N36" s="39">
+        <v>12</v>
+      </c>
+      <c r="O36" s="39">
+        <v>13</v>
+      </c>
+      <c r="P36" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q36" s="39">
+        <v>15</v>
+      </c>
+      <c r="R36" s="39">
+        <v>16</v>
+      </c>
+      <c r="S36" s="39">
+        <v>17</v>
+      </c>
+      <c r="T36" s="39">
+        <v>18</v>
+      </c>
+      <c r="U36" s="39">
+        <v>19</v>
+      </c>
+      <c r="W36" s="39">
+        <v>0</v>
+      </c>
+      <c r="X36" s="39">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="39">
+        <v>2</v>
+      </c>
+      <c r="Z36" s="39">
+        <v>3</v>
+      </c>
+      <c r="AA36" s="39">
+        <v>4</v>
+      </c>
+      <c r="AB36" s="39">
+        <v>5</v>
+      </c>
+      <c r="AC36" s="39">
+        <v>6</v>
+      </c>
+      <c r="AD36" s="39">
+        <v>7</v>
+      </c>
+      <c r="AE36" s="39">
+        <v>8</v>
+      </c>
+      <c r="AF36" s="39">
+        <v>9</v>
+      </c>
+      <c r="AG36" s="39">
+        <v>10</v>
+      </c>
+      <c r="AH36" s="39">
+        <v>11</v>
+      </c>
+      <c r="AI36" s="39">
+        <v>12</v>
+      </c>
+      <c r="AJ36" s="39">
+        <v>13</v>
+      </c>
+      <c r="AK36" s="39">
+        <v>14</v>
+      </c>
+      <c r="AL36" s="39">
+        <v>15</v>
+      </c>
+      <c r="AM36" s="39">
+        <v>16</v>
+      </c>
+      <c r="AN36" s="39">
+        <v>17</v>
+      </c>
+      <c r="AO36" s="39">
+        <v>18</v>
+      </c>
+      <c r="AP36" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37">
+        <v>2</v>
+      </c>
+      <c r="D37" s="37">
+        <v>3</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="F37" s="37">
+        <v>2</v>
+      </c>
+      <c r="G37" s="37">
+        <v>0</v>
+      </c>
+      <c r="H37" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="I37" s="37">
+        <v>4</v>
+      </c>
+      <c r="J37" s="37">
+        <v>4</v>
+      </c>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N37" s="37">
+        <v>1</v>
+      </c>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q37" s="37">
+        <v>4</v>
+      </c>
+      <c r="R37" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S37" s="37">
+        <v>3</v>
+      </c>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37" s="37"/>
+      <c r="X37" s="37"/>
+      <c r="Y37" s="37">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA37" s="37">
+        <v>2</v>
+      </c>
+      <c r="AB37" s="37">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD37" s="37">
+        <v>4</v>
+      </c>
+      <c r="AE37" s="37">
+        <v>4</v>
+      </c>
+      <c r="AF37" s="37"/>
+      <c r="AG37" s="37"/>
+      <c r="AH37" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI37" s="37">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="37"/>
+      <c r="AK37" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL37" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM37" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN37" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO37" s="37"/>
+      <c r="AP37" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37">
+        <v>1</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E38" s="37">
+        <v>2</v>
+      </c>
+      <c r="F38" s="37">
+        <v>8</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="H38" s="37">
+        <v>2</v>
+      </c>
+      <c r="I38" s="37">
+        <v>0</v>
+      </c>
+      <c r="J38" s="37">
+        <v>1</v>
+      </c>
+      <c r="K38" s="37">
+        <v>5</v>
+      </c>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N38" s="37">
+        <v>2</v>
+      </c>
+      <c r="O38" s="37"/>
+      <c r="P38" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q38" s="37">
+        <v>4</v>
+      </c>
+      <c r="R38" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S38" s="37">
+        <v>3</v>
+      </c>
+      <c r="T38" s="37"/>
+      <c r="U38" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
+      </c>
+      <c r="W38" s="37"/>
+      <c r="X38" s="37">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="Z38" s="37">
+        <v>2</v>
+      </c>
+      <c r="AA38" s="37">
+        <v>8</v>
+      </c>
+      <c r="AB38" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC38" s="37">
+        <v>2</v>
+      </c>
+      <c r="AD38" s="37">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="37">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="37">
+        <v>5</v>
+      </c>
+      <c r="AG38" s="37"/>
+      <c r="AH38" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI38" s="37">
+        <v>2</v>
+      </c>
+      <c r="AJ38" s="37"/>
+      <c r="AK38" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL38" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM38" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN38" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO38" s="37"/>
+      <c r="AP38" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N39" s="37">
+        <v>3</v>
+      </c>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q39" s="37">
+        <v>4</v>
+      </c>
+      <c r="R39" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S39" s="37">
+        <v>3</v>
+      </c>
+      <c r="T39" s="37"/>
+      <c r="U39" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V39">
+        <v>2</v>
+      </c>
+      <c r="W39" s="37"/>
+      <c r="X39" s="37"/>
+      <c r="Y39" s="37"/>
+      <c r="Z39" s="37"/>
+      <c r="AA39" s="37"/>
+      <c r="AB39" s="37"/>
+      <c r="AC39" s="37"/>
+      <c r="AD39" s="37"/>
+      <c r="AE39" s="37"/>
+      <c r="AF39" s="37"/>
+      <c r="AG39" s="37"/>
+      <c r="AH39" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI39" s="37">
+        <v>3</v>
+      </c>
+      <c r="AJ39" s="37"/>
+      <c r="AK39" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL39" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM39" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN39" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO39" s="37"/>
+      <c r="AP39" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="G40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="H40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="I40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N40" s="37">
+        <v>4</v>
+      </c>
+      <c r="O40" s="37"/>
+      <c r="P40" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q40" s="37">
+        <v>4</v>
+      </c>
+      <c r="R40" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S40" s="37">
+        <v>3</v>
+      </c>
+      <c r="T40" s="37"/>
+      <c r="U40" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V40">
+        <v>3</v>
+      </c>
+      <c r="W40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="X40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AD40" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE40" s="37"/>
+      <c r="AF40" s="37"/>
+      <c r="AG40" s="37"/>
+      <c r="AH40" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI40" s="37">
+        <v>4</v>
+      </c>
+      <c r="AJ40" s="37"/>
+      <c r="AK40" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL40" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM40" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN40" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO40" s="37"/>
+      <c r="AP40" s="37" t="s">
+        <v>239</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16033,4 +17517,437 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="61" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="B1" s="62"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="52"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="58"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="52"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="58"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="52"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="52"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="52"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="52"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D12" s="52"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="58"/>
+      <c r="C13" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" s="53"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="59"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="53"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="53"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="53"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="53"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" s="53"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>252</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="59"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="53"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="59"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="53"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="59"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="53"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="59"/>
+      <c r="C23" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D23" s="53"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="59"/>
+      <c r="C24" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D24" s="53"/>
+    </row>
+    <row r="25" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="C25" s="56"/>
+      <c r="D25" s="52"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Attempted to fix some errors with displaying 12 hour time.  Added support to display seconds on the LCD.  Need to add a menu function to do this, but will probably wait till I split the Menu up a little bit more.  Still need to figure out the initial cursor position for displaying seconds or not.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="4"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="293">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -872,6 +872,39 @@
   </si>
   <si>
     <t>Time breakpoints brainstorming and visualization</t>
+  </si>
+  <si>
+    <t>Serial debugging bits</t>
+  </si>
+  <si>
+    <t>MenuNumSel types</t>
+  </si>
+  <si>
+    <t>Normal numbers</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Enable/Disable</t>
+  </si>
+  <si>
+    <t>No write to EEPROM</t>
+  </si>
+  <si>
+    <t>Any number higher than 128 will be no write</t>
+  </si>
+  <si>
+    <t>For Hours</t>
+  </si>
+  <si>
+    <t>Minutes should work fine with Normal numbers</t>
+  </si>
+  <si>
+    <t>Suppress the save or exit saving message</t>
   </si>
 </sst>
 </file>
@@ -1288,6 +1321,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1320,27 +1374,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1661,12 +1694,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
       <c r="E1" t="s">
         <v>107</v>
       </c>
@@ -1843,12 +1876,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
       <c r="E1" t="s">
         <v>106</v>
       </c>
@@ -1993,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,13 +2042,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="19" t="s">
         <v>119</v>
       </c>
@@ -2045,7 +2078,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -2066,7 +2099,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -2087,7 +2120,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="53" t="s">
         <v>187</v>
       </c>
       <c r="B5" s="25">
@@ -2110,7 +2143,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -2131,7 +2164,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -2152,7 +2185,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -2173,7 +2206,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -2194,7 +2227,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="44"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -2215,7 +2248,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="53" t="s">
         <v>188</v>
       </c>
       <c r="B11" s="25">
@@ -2238,7 +2271,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -2259,7 +2292,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -2280,7 +2313,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -2301,7 +2334,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="43"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -2322,7 +2355,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -2343,7 +2376,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="53" t="s">
         <v>189</v>
       </c>
       <c r="B17" s="29">
@@ -2366,7 +2399,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -2387,7 +2420,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -2408,7 +2441,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -2429,7 +2462,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -2450,7 +2483,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="44"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -2471,7 +2504,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="53" t="s">
         <v>190</v>
       </c>
       <c r="B23" s="25">
@@ -2494,7 +2527,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="43"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -2515,7 +2548,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="43"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -2536,7 +2569,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="43"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -2557,7 +2590,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -2578,7 +2611,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="44"/>
+      <c r="A28" s="55"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -2599,7 +2632,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="53" t="s">
         <v>191</v>
       </c>
       <c r="B29" s="29">
@@ -2622,7 +2655,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="43"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -2643,7 +2676,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="43"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -2664,7 +2697,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="43"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -2685,7 +2718,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="43"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -2706,7 +2739,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="44"/>
+      <c r="A34" s="55"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -2727,7 +2760,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="53" t="s">
         <v>192</v>
       </c>
       <c r="B35" s="25">
@@ -2750,7 +2783,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="43"/>
+      <c r="A36" s="54"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -2771,7 +2804,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="43"/>
+      <c r="A37" s="54"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -2792,7 +2825,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="43"/>
+      <c r="A38" s="54"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -2813,7 +2846,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="43"/>
+      <c r="A39" s="54"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -2834,7 +2867,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="44"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -2855,7 +2888,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="53" t="s">
         <v>193</v>
       </c>
       <c r="B41" s="29">
@@ -2878,7 +2911,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="43"/>
+      <c r="A42" s="54"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -2899,7 +2932,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="43"/>
+      <c r="A43" s="54"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -2920,7 +2953,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="43"/>
+      <c r="A44" s="54"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -2941,7 +2974,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="43"/>
+      <c r="A45" s="54"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -2962,7 +2995,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="44"/>
+      <c r="A46" s="55"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -2983,7 +3016,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="53" t="s">
         <v>194</v>
       </c>
       <c r="B47" s="25">
@@ -3006,7 +3039,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="43"/>
+      <c r="A48" s="54"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -3027,7 +3060,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="43"/>
+      <c r="A49" s="54"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -3048,7 +3081,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="43"/>
+      <c r="A50" s="54"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -3069,7 +3102,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="43"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -3090,7 +3123,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="44"/>
+      <c r="A52" s="55"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -3130,10 +3163,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N267"/>
+  <dimension ref="A1:P267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3143,7 +3176,7 @@
     <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="15"/>
       <c r="B1" s="14">
         <v>7</v>
@@ -3169,8 +3202,11 @@
       <c r="I1" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>124</v>
       </c>
@@ -3208,7 +3244,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>125</v>
       </c>
@@ -3246,7 +3282,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>126</v>
       </c>
@@ -3284,7 +3320,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>127</v>
       </c>
@@ -3322,7 +3358,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>128</v>
       </c>
@@ -3357,7 +3393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>129</v>
       </c>
@@ -3395,7 +3431,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>130</v>
       </c>
@@ -3427,7 +3463,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>131</v>
       </c>
@@ -3465,7 +3501,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M10">
         <v>1</v>
       </c>
@@ -3473,7 +3509,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>132</v>
       </c>
@@ -3508,8 +3544,11 @@
         <f>DEC2BIN(J12)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0</v>
       </c>
@@ -3541,8 +3580,14 @@
         <f t="shared" ref="K13:K76" si="0">DEC2BIN(J13)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0</v>
       </c>
@@ -3574,8 +3619,20 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>285</v>
+      </c>
+      <c r="O14" t="s">
+        <v>290</v>
+      </c>
+      <c r="P14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>0</v>
       </c>
@@ -3607,8 +3664,14 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0</v>
       </c>
@@ -3640,8 +3703,14 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0</v>
       </c>
@@ -3673,8 +3742,11 @@
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>0</v>
       </c>
@@ -3706,8 +3778,11 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>0</v>
       </c>
@@ -3739,8 +3814,11 @@
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>0</v>
       </c>
@@ -3772,8 +3850,14 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M20">
+        <v>64</v>
+      </c>
+      <c r="N20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>0</v>
       </c>
@@ -3805,8 +3889,17 @@
         <f t="shared" si="0"/>
         <v>1001</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M21">
+        <v>128</v>
+      </c>
+      <c r="N21" t="s">
+        <v>288</v>
+      </c>
+      <c r="O21" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0</v>
       </c>
@@ -3839,7 +3932,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>0</v>
       </c>
@@ -3872,7 +3965,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>0</v>
       </c>
@@ -3905,7 +3998,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0</v>
       </c>
@@ -3938,7 +4031,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0</v>
       </c>
@@ -3971,7 +4064,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>0</v>
       </c>
@@ -4004,7 +4097,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0</v>
       </c>
@@ -4037,7 +4130,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>0</v>
       </c>
@@ -4070,7 +4163,7 @@
         <v>10001</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>0</v>
       </c>
@@ -4103,7 +4196,7 @@
         <v>10010</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>0</v>
       </c>
@@ -4136,7 +4229,7 @@
         <v>10011</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>0</v>
       </c>
@@ -11931,10 +12024,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW40"/>
+  <dimension ref="A1:AW51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -14551,14 +14644,12 @@
       <c r="H28" s="37"/>
       <c r="I28" s="37"/>
       <c r="J28" s="37" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="K28" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="L28" s="37" t="s">
-        <v>231</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="L28" s="37"/>
       <c r="M28" s="37"/>
       <c r="N28" s="37"/>
       <c r="O28" s="37"/>
@@ -14624,9 +14715,7 @@
       <c r="K29" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="L29" s="37" t="s">
-        <v>220</v>
-      </c>
+      <c r="L29" s="37"/>
       <c r="M29" s="37"/>
       <c r="N29" s="37"/>
       <c r="O29" s="37"/>
@@ -15824,6 +15913,518 @@
         <v>239</v>
       </c>
     </row>
+    <row r="41" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B41" s="39">
+        <v>0</v>
+      </c>
+      <c r="C41" s="39">
+        <v>1</v>
+      </c>
+      <c r="D41" s="39">
+        <v>2</v>
+      </c>
+      <c r="E41" s="39">
+        <v>3</v>
+      </c>
+      <c r="F41" s="39">
+        <v>4</v>
+      </c>
+      <c r="G41" s="39">
+        <v>5</v>
+      </c>
+      <c r="H41" s="39">
+        <v>6</v>
+      </c>
+      <c r="I41" s="39">
+        <v>7</v>
+      </c>
+      <c r="J41" s="39">
+        <v>8</v>
+      </c>
+      <c r="K41" s="39">
+        <v>9</v>
+      </c>
+      <c r="L41" s="39">
+        <v>10</v>
+      </c>
+      <c r="M41" s="39">
+        <v>11</v>
+      </c>
+      <c r="N41" s="39">
+        <v>12</v>
+      </c>
+      <c r="O41" s="39">
+        <v>13</v>
+      </c>
+      <c r="P41" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q41" s="39">
+        <v>15</v>
+      </c>
+      <c r="R41" s="39">
+        <v>16</v>
+      </c>
+      <c r="S41" s="39">
+        <v>17</v>
+      </c>
+      <c r="T41" s="39">
+        <v>18</v>
+      </c>
+      <c r="U41" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37">
+        <v>1</v>
+      </c>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="O42" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="P42" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q42" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="R42" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="S42" s="37"/>
+      <c r="T42" s="37"/>
+      <c r="U42" s="37"/>
+    </row>
+    <row r="43" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="J43" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="K43" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="L43" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="M43" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="N43" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="O43" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="37"/>
+    </row>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="L44" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
+      <c r="O44" s="37"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="37"/>
+    </row>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E45" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+    </row>
+    <row r="46" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B46" s="39">
+        <v>0</v>
+      </c>
+      <c r="C46" s="39">
+        <v>1</v>
+      </c>
+      <c r="D46" s="39">
+        <v>2</v>
+      </c>
+      <c r="E46" s="39">
+        <v>3</v>
+      </c>
+      <c r="F46" s="39">
+        <v>4</v>
+      </c>
+      <c r="G46" s="39">
+        <v>5</v>
+      </c>
+      <c r="H46" s="39">
+        <v>6</v>
+      </c>
+      <c r="I46" s="39">
+        <v>7</v>
+      </c>
+      <c r="J46" s="39">
+        <v>8</v>
+      </c>
+      <c r="K46" s="39">
+        <v>9</v>
+      </c>
+      <c r="L46" s="39">
+        <v>10</v>
+      </c>
+      <c r="M46" s="39">
+        <v>11</v>
+      </c>
+      <c r="N46" s="39">
+        <v>12</v>
+      </c>
+      <c r="O46" s="39">
+        <v>13</v>
+      </c>
+      <c r="P46" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q46" s="39">
+        <v>15</v>
+      </c>
+      <c r="R46" s="39">
+        <v>16</v>
+      </c>
+      <c r="S46" s="39">
+        <v>17</v>
+      </c>
+      <c r="T46" s="39">
+        <v>18</v>
+      </c>
+      <c r="U46" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E47" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37">
+        <v>1</v>
+      </c>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="O47" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="P47" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q47" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="R47" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37"/>
+      <c r="U47" s="37"/>
+    </row>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="J48" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="K48" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="L48" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="M48" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="N48" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="37"/>
+      <c r="U48" s="37"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E49" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F49" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="L49" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37"/>
+      <c r="U49" s="37"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="F50" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="37"/>
+      <c r="U50" s="37"/>
+    </row>
+    <row r="51" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B51" s="39">
+        <v>0</v>
+      </c>
+      <c r="C51" s="39">
+        <v>1</v>
+      </c>
+      <c r="D51" s="39">
+        <v>2</v>
+      </c>
+      <c r="E51" s="39">
+        <v>3</v>
+      </c>
+      <c r="F51" s="39">
+        <v>4</v>
+      </c>
+      <c r="G51" s="39">
+        <v>5</v>
+      </c>
+      <c r="H51" s="39">
+        <v>6</v>
+      </c>
+      <c r="I51" s="39">
+        <v>7</v>
+      </c>
+      <c r="J51" s="39">
+        <v>8</v>
+      </c>
+      <c r="K51" s="39">
+        <v>9</v>
+      </c>
+      <c r="L51" s="39">
+        <v>10</v>
+      </c>
+      <c r="M51" s="39">
+        <v>11</v>
+      </c>
+      <c r="N51" s="39">
+        <v>12</v>
+      </c>
+      <c r="O51" s="39">
+        <v>13</v>
+      </c>
+      <c r="P51" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q51" s="39">
+        <v>15</v>
+      </c>
+      <c r="R51" s="39">
+        <v>16</v>
+      </c>
+      <c r="S51" s="39">
+        <v>17</v>
+      </c>
+      <c r="T51" s="39">
+        <v>18</v>
+      </c>
+      <c r="U51" s="39">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15836,7 +16437,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P21" sqref="P21"/>
+      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15869,25 +16470,25 @@
       <c r="H1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="N1" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="50" t="s">
+      <c r="O1" s="61" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15908,13 +16509,13 @@
       <c r="H2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
       <c r="P2" t="s">
         <v>93</v>
       </c>
@@ -15936,13 +16537,13 @@
       <c r="H3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -17529,59 +18130,59 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="61" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:4" s="50" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="62"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="52"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="41"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="52"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="52"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="41" t="s">
         <v>248</v>
       </c>
     </row>
@@ -17589,121 +18190,121 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="41"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="52"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="52"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="52"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="41"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="52"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="56" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="D12" s="52"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="56" t="s">
+      <c r="B13" s="47"/>
+      <c r="C13" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="D13" s="53"/>
+      <c r="D13" s="42"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="53"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="42"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="53"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="42"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="53"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="42"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="53"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="48" t="s">
         <v>258</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="D18" s="53"/>
+      <c r="D18" s="42"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="42" t="s">
         <v>249</v>
       </c>
     </row>
@@ -17711,55 +18312,55 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="53"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="42"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="53"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="42"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="53"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="42"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="56" t="s">
+      <c r="B23" s="48"/>
+      <c r="C23" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="D23" s="53"/>
+      <c r="D23" s="42"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="56" t="s">
+      <c r="B24" s="48"/>
+      <c r="C24" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="D24" s="53"/>
+      <c r="D24" s="42"/>
     </row>
     <row r="25" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="49" t="s">
         <v>257</v>
       </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="52"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Transitioning from double to single hour digits should be fixed now.  Will wait and see.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="295">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -905,6 +905,12 @@
   </si>
   <si>
     <t>Suppress the save or exit saving message</t>
+  </si>
+  <si>
+    <t>secondsDisplay</t>
+  </si>
+  <si>
+    <t>Display of the seconds: 0 = No; 1 = Yes</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1869,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A4" sqref="A4:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,10 +1970,13 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>293</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>103</v>
+      </c>
+      <c r="F7" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1975,7 +1984,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>103</v>
@@ -1986,7 +1995,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>103</v>
@@ -1997,9 +2006,20 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2026,7 +2046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -12024,10 +12044,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW51"/>
+  <dimension ref="A1:AW56"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -15516,29 +15536,27 @@
         <v>0</v>
       </c>
       <c r="B37" s="37"/>
-      <c r="C37" s="37">
+      <c r="C37" s="37"/>
+      <c r="D37" s="37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="37">
+        <v>1</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="G37" s="37">
         <v>2</v>
       </c>
-      <c r="D37" s="37">
-        <v>3</v>
-      </c>
-      <c r="E37" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="F37" s="37">
-        <v>2</v>
-      </c>
-      <c r="G37" s="37">
-        <v>0</v>
-      </c>
-      <c r="H37" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="I37" s="37">
-        <v>4</v>
-      </c>
-      <c r="J37" s="37">
-        <v>4</v>
+      <c r="H37" s="37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="J37" s="37" t="s">
+        <v>211</v>
       </c>
       <c r="K37" s="37"/>
       <c r="L37" s="37"/>
@@ -15570,27 +15588,21 @@
       </c>
       <c r="W37" s="37"/>
       <c r="X37" s="37"/>
-      <c r="Y37" s="37">
-        <v>1</v>
-      </c>
-      <c r="Z37" s="37" t="s">
+      <c r="Y37" s="37"/>
+      <c r="Z37" s="37"/>
+      <c r="AA37" s="37">
+        <v>1</v>
+      </c>
+      <c r="AB37" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="AA37" s="37">
+      <c r="AC37" s="37">
         <v>2</v>
       </c>
-      <c r="AB37" s="37">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="37" t="s">
-        <v>209</v>
-      </c>
       <c r="AD37" s="37">
-        <v>4</v>
-      </c>
-      <c r="AE37" s="37">
-        <v>4</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AE37" s="37"/>
       <c r="AF37" s="37"/>
       <c r="AG37" s="37"/>
       <c r="AH37" s="37" t="s">
@@ -15810,28 +15822,28 @@
         <v>3</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="E40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="F40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="G40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="H40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="I40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="J40" s="37"/>
       <c r="K40" s="37"/>
@@ -15863,28 +15875,28 @@
         <v>3</v>
       </c>
       <c r="W40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="X40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="Y40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="Z40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="AA40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="AB40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="AC40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="AD40" s="37" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="AE40" s="37"/>
       <c r="AF40" s="37"/>
@@ -15974,170 +15986,468 @@
       <c r="U41" s="39">
         <v>19</v>
       </c>
+      <c r="W41" s="39">
+        <v>0</v>
+      </c>
+      <c r="X41" s="39">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="39">
+        <v>2</v>
+      </c>
+      <c r="Z41" s="39">
+        <v>3</v>
+      </c>
+      <c r="AA41" s="39">
+        <v>4</v>
+      </c>
+      <c r="AB41" s="39">
+        <v>5</v>
+      </c>
+      <c r="AC41" s="39">
+        <v>6</v>
+      </c>
+      <c r="AD41" s="39">
+        <v>7</v>
+      </c>
+      <c r="AE41" s="39">
+        <v>8</v>
+      </c>
+      <c r="AF41" s="39">
+        <v>9</v>
+      </c>
+      <c r="AG41" s="39">
+        <v>10</v>
+      </c>
+      <c r="AH41" s="39">
+        <v>11</v>
+      </c>
+      <c r="AI41" s="39">
+        <v>12</v>
+      </c>
+      <c r="AJ41" s="39">
+        <v>13</v>
+      </c>
+      <c r="AK41" s="39">
+        <v>14</v>
+      </c>
+      <c r="AL41" s="39">
+        <v>15</v>
+      </c>
+      <c r="AM41" s="39">
+        <v>16</v>
+      </c>
+      <c r="AN41" s="39">
+        <v>17</v>
+      </c>
+      <c r="AO41" s="39">
+        <v>18</v>
+      </c>
+      <c r="AP41" s="39">
+        <v>19</v>
+      </c>
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0</v>
       </c>
       <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37" t="s">
-        <v>205</v>
+      <c r="C42" s="37">
+        <v>2</v>
+      </c>
+      <c r="D42" s="37">
+        <v>3</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="F42" s="37" t="s">
-        <v>207</v>
-      </c>
-      <c r="G42" s="37" t="s">
-        <v>203</v>
+        <v>209</v>
+      </c>
+      <c r="F42" s="37">
+        <v>2</v>
+      </c>
+      <c r="G42" s="37">
+        <v>0</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="I42" s="37"/>
+        <v>209</v>
+      </c>
+      <c r="I42" s="37">
+        <v>4</v>
+      </c>
       <c r="J42" s="37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K42" s="37"/>
-      <c r="L42" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="O42" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="P42" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q42" s="37" t="s">
-        <v>225</v>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N42" s="37">
+        <v>1</v>
+      </c>
+      <c r="O42" s="37"/>
+      <c r="P42" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q42" s="37">
+        <v>4</v>
       </c>
       <c r="R42" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="S42" s="37"/>
+        <v>238</v>
+      </c>
+      <c r="S42" s="37">
+        <v>3</v>
+      </c>
       <c r="T42" s="37"/>
-      <c r="U42" s="37"/>
+      <c r="U42" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42" s="37"/>
+      <c r="X42" s="37"/>
+      <c r="Y42" s="37">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA42" s="37">
+        <v>2</v>
+      </c>
+      <c r="AB42" s="37">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD42" s="37">
+        <v>4</v>
+      </c>
+      <c r="AE42" s="37">
+        <v>4</v>
+      </c>
+      <c r="AF42" s="37"/>
+      <c r="AG42" s="37"/>
+      <c r="AH42" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI42" s="37">
+        <v>1</v>
+      </c>
+      <c r="AJ42" s="37"/>
+      <c r="AK42" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL42" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM42" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN42" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO42" s="37"/>
+      <c r="AP42" s="37" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="43" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37" t="s">
-        <v>230</v>
-      </c>
-      <c r="J43" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="K43" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="L43" s="37" t="s">
-        <v>225</v>
-      </c>
+      <c r="C43" s="37">
+        <v>1</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E43" s="37">
+        <v>2</v>
+      </c>
+      <c r="F43" s="37">
+        <v>8</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="H43" s="37">
+        <v>2</v>
+      </c>
+      <c r="I43" s="37">
+        <v>0</v>
+      </c>
+      <c r="J43" s="37">
+        <v>1</v>
+      </c>
+      <c r="K43" s="37">
+        <v>5</v>
+      </c>
+      <c r="L43" s="37"/>
       <c r="M43" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="N43" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="O43" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="P43" s="37"/>
-      <c r="Q43" s="37"/>
-      <c r="R43" s="37"/>
-      <c r="S43" s="37"/>
+        <v>202</v>
+      </c>
+      <c r="N43" s="37">
+        <v>2</v>
+      </c>
+      <c r="O43" s="37"/>
+      <c r="P43" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q43" s="37">
+        <v>4</v>
+      </c>
+      <c r="R43" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S43" s="37">
+        <v>3</v>
+      </c>
       <c r="T43" s="37"/>
-      <c r="U43" s="37"/>
+      <c r="U43" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="Z43" s="37">
+        <v>2</v>
+      </c>
+      <c r="AA43" s="37">
+        <v>8</v>
+      </c>
+      <c r="AB43" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC43" s="37">
+        <v>2</v>
+      </c>
+      <c r="AD43" s="37">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="37">
+        <v>1</v>
+      </c>
+      <c r="AF43" s="37">
+        <v>5</v>
+      </c>
+      <c r="AG43" s="37"/>
+      <c r="AH43" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI43" s="37">
+        <v>2</v>
+      </c>
+      <c r="AJ43" s="37"/>
+      <c r="AK43" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL43" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM43" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN43" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO43" s="37"/>
+      <c r="AP43" s="37" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="44" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2</v>
       </c>
-      <c r="B44" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="C44" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E44" s="37" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="G44" s="37" t="s">
-        <v>204</v>
-      </c>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
       <c r="H44" s="37"/>
       <c r="I44" s="37"/>
       <c r="J44" s="37"/>
-      <c r="K44" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="L44" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="M44" s="37"/>
-      <c r="N44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N44" s="37">
+        <v>3</v>
+      </c>
       <c r="O44" s="37"/>
-      <c r="P44" s="37"/>
-      <c r="Q44" s="37"/>
-      <c r="R44" s="37"/>
-      <c r="S44" s="37"/>
+      <c r="P44" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q44" s="37">
+        <v>4</v>
+      </c>
+      <c r="R44" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S44" s="37">
+        <v>3</v>
+      </c>
       <c r="T44" s="37"/>
-      <c r="U44" s="37"/>
+      <c r="U44" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V44">
+        <v>2</v>
+      </c>
+      <c r="W44" s="37"/>
+      <c r="X44" s="37"/>
+      <c r="Y44" s="37"/>
+      <c r="Z44" s="37"/>
+      <c r="AA44" s="37"/>
+      <c r="AB44" s="37"/>
+      <c r="AC44" s="37"/>
+      <c r="AD44" s="37"/>
+      <c r="AE44" s="37"/>
+      <c r="AF44" s="37"/>
+      <c r="AG44" s="37"/>
+      <c r="AH44" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI44" s="37">
+        <v>3</v>
+      </c>
+      <c r="AJ44" s="37"/>
+      <c r="AK44" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL44" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM44" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN44" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO44" s="37"/>
+      <c r="AP44" s="37" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="45" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>3</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="E45" s="37" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F45" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
+        <v>241</v>
+      </c>
+      <c r="G45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="H45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="I45" s="37" t="s">
+        <v>241</v>
+      </c>
       <c r="J45" s="37"/>
       <c r="K45" s="37"/>
       <c r="L45" s="37"/>
-      <c r="M45" s="37"/>
-      <c r="N45" s="37"/>
+      <c r="M45" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N45" s="37">
+        <v>4</v>
+      </c>
       <c r="O45" s="37"/>
-      <c r="P45" s="37"/>
-      <c r="Q45" s="37"/>
-      <c r="R45" s="37"/>
-      <c r="S45" s="37"/>
+      <c r="P45" s="37">
+        <v>7</v>
+      </c>
+      <c r="Q45" s="37">
+        <v>4</v>
+      </c>
+      <c r="R45" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="S45" s="37">
+        <v>3</v>
+      </c>
       <c r="T45" s="37"/>
-      <c r="U45" s="37"/>
+      <c r="U45" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="V45">
+        <v>3</v>
+      </c>
+      <c r="W45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="X45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AD45" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE45" s="37"/>
+      <c r="AF45" s="37"/>
+      <c r="AG45" s="37"/>
+      <c r="AH45" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI45" s="37">
+        <v>4</v>
+      </c>
+      <c r="AJ45" s="37"/>
+      <c r="AK45" s="37">
+        <v>7</v>
+      </c>
+      <c r="AL45" s="37">
+        <v>4</v>
+      </c>
+      <c r="AM45" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="AN45" s="37">
+        <v>3</v>
+      </c>
+      <c r="AO45" s="37"/>
+      <c r="AP45" s="37" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="46" spans="1:42" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B46" s="39">
@@ -16262,24 +16572,26 @@
       <c r="G48" s="37"/>
       <c r="H48" s="37"/>
       <c r="I48" s="37" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="J48" s="37" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="K48" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="L48" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="L48" s="37" t="s">
+      <c r="M48" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="M48" s="37" t="s">
+      <c r="N48" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="N48" s="37" t="s">
+      <c r="O48" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="O48" s="37"/>
       <c r="P48" s="37"/>
       <c r="Q48" s="37"/>
       <c r="R48" s="37"/>
@@ -16422,6 +16734,230 @@
         <v>18</v>
       </c>
       <c r="U51" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="E52" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="G52" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="H52" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37">
+        <v>1</v>
+      </c>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="O52" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="P52" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q52" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="R52" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="S52" s="37"/>
+      <c r="T52" s="37"/>
+      <c r="U52" s="37"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="J53" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="K53" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="L53" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="M53" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="N53" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="O53" s="37"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="37"/>
+      <c r="S53" s="37"/>
+      <c r="T53" s="37"/>
+      <c r="U53" s="37"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="D54" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E54" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F54" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="L54" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
+      <c r="O54" s="37"/>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="37"/>
+      <c r="S54" s="37"/>
+      <c r="T54" s="37"/>
+      <c r="U54" s="37"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="E55" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="F55" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="37"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
+      <c r="S55" s="37"/>
+      <c r="T55" s="37"/>
+      <c r="U55" s="37"/>
+    </row>
+    <row r="56" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B56" s="39">
+        <v>0</v>
+      </c>
+      <c r="C56" s="39">
+        <v>1</v>
+      </c>
+      <c r="D56" s="39">
+        <v>2</v>
+      </c>
+      <c r="E56" s="39">
+        <v>3</v>
+      </c>
+      <c r="F56" s="39">
+        <v>4</v>
+      </c>
+      <c r="G56" s="39">
+        <v>5</v>
+      </c>
+      <c r="H56" s="39">
+        <v>6</v>
+      </c>
+      <c r="I56" s="39">
+        <v>7</v>
+      </c>
+      <c r="J56" s="39">
+        <v>8</v>
+      </c>
+      <c r="K56" s="39">
+        <v>9</v>
+      </c>
+      <c r="L56" s="39">
+        <v>10</v>
+      </c>
+      <c r="M56" s="39">
+        <v>11</v>
+      </c>
+      <c r="N56" s="39">
+        <v>12</v>
+      </c>
+      <c r="O56" s="39">
+        <v>13</v>
+      </c>
+      <c r="P56" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q56" s="39">
+        <v>15</v>
+      </c>
+      <c r="R56" s="39">
+        <v>16</v>
+      </c>
+      <c r="S56" s="39">
+        <v>17</v>
+      </c>
+      <c r="T56" s="39">
+        <v>18</v>
+      </c>
+      <c r="U56" s="39">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tagging as v0.23  Added menu options to support enabling or disabling multiple relays per alarm event.  Still need to add the activation of the relays via the AlarmON/OFF functions.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="313">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -959,6 +959,12 @@
   </si>
   <si>
     <t>char* m2Items42[]={"", "Exit", "Restore Defaults", ""};</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>+/-</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1408,6 +1414,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1441,12 +1453,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1766,12 +1773,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" t="s">
         <v>98</v>
       </c>
@@ -1948,12 +1955,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
       <c r="E1" t="s">
         <v>97</v>
       </c>
@@ -2128,13 +2135,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="19" t="s">
         <v>110</v>
       </c>
@@ -2164,7 +2171,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="56"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -2185,7 +2192,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="57"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -2206,7 +2213,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="59" t="s">
         <v>178</v>
       </c>
       <c r="B5" s="25">
@@ -2229,7 +2236,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -2250,7 +2257,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -2271,7 +2278,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -2292,7 +2299,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -2313,7 +2320,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="55"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -2334,7 +2341,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="59" t="s">
         <v>179</v>
       </c>
       <c r="B11" s="25">
@@ -2357,7 +2364,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -2378,7 +2385,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -2399,7 +2406,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -2420,7 +2427,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -2441,7 +2448,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -2462,7 +2469,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="59" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="29">
@@ -2485,7 +2492,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -2506,7 +2513,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -2527,7 +2534,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -2548,7 +2555,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -2569,7 +2576,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="55"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -2590,7 +2597,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="59" t="s">
         <v>181</v>
       </c>
       <c r="B23" s="25">
@@ -2613,7 +2620,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -2634,7 +2641,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -2655,7 +2662,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -2676,7 +2683,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -2697,7 +2704,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="55"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -2718,7 +2725,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="59" t="s">
         <v>182</v>
       </c>
       <c r="B29" s="29">
@@ -2741,7 +2748,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -2762,7 +2769,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -2783,7 +2790,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -2804,7 +2811,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="54"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -2825,7 +2832,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="55"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -2846,7 +2853,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="59" t="s">
         <v>183</v>
       </c>
       <c r="B35" s="25">
@@ -2869,7 +2876,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="54"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -2890,7 +2897,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="54"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -2911,7 +2918,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="54"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -2932,7 +2939,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="54"/>
+      <c r="A39" s="60"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -2953,7 +2960,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="55"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -2974,7 +2981,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="59" t="s">
         <v>184</v>
       </c>
       <c r="B41" s="29">
@@ -2997,7 +3004,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="54"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -3018,7 +3025,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="54"/>
+      <c r="A43" s="60"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -3039,7 +3046,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="54"/>
+      <c r="A44" s="60"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -3060,7 +3067,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="54"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -3081,7 +3088,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="55"/>
+      <c r="A46" s="61"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -3102,7 +3109,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="59" t="s">
         <v>185</v>
       </c>
       <c r="B47" s="25">
@@ -3125,7 +3132,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="54"/>
+      <c r="A48" s="60"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -3146,7 +3153,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="54"/>
+      <c r="A49" s="60"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -3167,7 +3174,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="54"/>
+      <c r="A50" s="60"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -3188,7 +3195,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="54"/>
+      <c r="A51" s="60"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -3209,7 +3216,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="55"/>
+      <c r="A52" s="61"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -3251,8 +3258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3976,6 +3983,9 @@
       <c r="M17">
         <v>8</v>
       </c>
+      <c r="N17" s="69" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18">
@@ -12257,8 +12267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AQ29" sqref="AQ29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -13306,7 +13316,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:84" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="39">
         <v>0</v>
       </c>
@@ -13695,7 +13705,9 @@
       <c r="BI7" s="37">
         <v>3</v>
       </c>
-      <c r="BJ7" s="37"/>
+      <c r="BJ7" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK7" s="37" t="s">
         <v>230</v>
       </c>
@@ -13740,7 +13752,9 @@
       <c r="CD7" s="37">
         <v>3</v>
       </c>
-      <c r="CE7" s="37"/>
+      <c r="CE7" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF7" s="37" t="s">
         <v>230</v>
       </c>
@@ -13867,7 +13881,9 @@
       <c r="BI8" s="37">
         <v>3</v>
       </c>
-      <c r="BJ8" s="37"/>
+      <c r="BJ8" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK8" s="37" t="s">
         <v>230</v>
       </c>
@@ -13922,7 +13938,9 @@
       <c r="CD8" s="37">
         <v>3</v>
       </c>
-      <c r="CE8" s="37"/>
+      <c r="CE8" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF8" s="37" t="s">
         <v>230</v>
       </c>
@@ -14027,7 +14045,9 @@
       <c r="BI9" s="37">
         <v>3</v>
       </c>
-      <c r="BJ9" s="37"/>
+      <c r="BJ9" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK9" s="37" t="s">
         <v>230</v>
       </c>
@@ -14064,7 +14084,9 @@
       <c r="CD9" s="37">
         <v>3</v>
       </c>
-      <c r="CE9" s="37"/>
+      <c r="CE9" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF9" s="37" t="s">
         <v>230</v>
       </c>
@@ -14181,7 +14203,9 @@
       <c r="BI10" s="37">
         <v>3</v>
       </c>
-      <c r="BJ10" s="37"/>
+      <c r="BJ10" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK10" s="37" t="s">
         <v>230</v>
       </c>
@@ -14234,7 +14258,9 @@
       <c r="CD10" s="37">
         <v>3</v>
       </c>
-      <c r="CE10" s="37"/>
+      <c r="CE10" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF10" s="37" t="s">
         <v>230</v>
       </c>
@@ -14634,7 +14660,9 @@
       <c r="BI12" s="37">
         <v>3</v>
       </c>
-      <c r="BJ12" s="37"/>
+      <c r="BJ12" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK12" s="37" t="s">
         <v>230</v>
       </c>
@@ -14685,7 +14713,9 @@
       <c r="CD12" s="37">
         <v>3</v>
       </c>
-      <c r="CE12" s="37"/>
+      <c r="CE12" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF12" s="37" t="s">
         <v>230</v>
       </c>
@@ -14812,7 +14842,9 @@
       <c r="BI13" s="37">
         <v>3</v>
       </c>
-      <c r="BJ13" s="37"/>
+      <c r="BJ13" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK13" s="37" t="s">
         <v>230</v>
       </c>
@@ -14867,7 +14899,9 @@
       <c r="CD13" s="37">
         <v>3</v>
       </c>
-      <c r="CE13" s="37"/>
+      <c r="CE13" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF13" s="37" t="s">
         <v>230</v>
       </c>
@@ -14972,7 +15006,9 @@
       <c r="BI14" s="37">
         <v>3</v>
       </c>
-      <c r="BJ14" s="37"/>
+      <c r="BJ14" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK14" s="37" t="s">
         <v>230</v>
       </c>
@@ -15009,7 +15045,9 @@
       <c r="CD14" s="37">
         <v>3</v>
       </c>
-      <c r="CE14" s="37"/>
+      <c r="CE14" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF14" s="37" t="s">
         <v>230</v>
       </c>
@@ -15134,7 +15172,9 @@
       <c r="BI15" s="37">
         <v>3</v>
       </c>
-      <c r="BJ15" s="37"/>
+      <c r="BJ15" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK15" s="37" t="s">
         <v>230</v>
       </c>
@@ -15187,7 +15227,9 @@
       <c r="CD15" s="37">
         <v>3</v>
       </c>
-      <c r="CE15" s="37"/>
+      <c r="CE15" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="CF15" s="37" t="s">
         <v>230</v>
       </c>
@@ -15480,7 +15522,9 @@
       <c r="R17" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="S17" s="37"/>
+      <c r="S17" s="37" t="s">
+        <v>222</v>
+      </c>
       <c r="T17" s="37"/>
       <c r="U17" s="37"/>
       <c r="V17">
@@ -15656,16 +15700,30 @@
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
       <c r="J18" s="37"/>
-      <c r="K18" s="37">
-        <v>1</v>
-      </c>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
+      <c r="K18" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="L18" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="M18" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="N18" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="O18" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="P18" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q18" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="R18" s="37" t="s">
+        <v>210</v>
+      </c>
       <c r="S18" s="37"/>
       <c r="T18" s="37"/>
       <c r="U18" s="37"/>
@@ -15776,16 +15834,30 @@
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
       <c r="J19" s="37"/>
-      <c r="K19" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
+      <c r="K19" s="37">
+        <v>1</v>
+      </c>
+      <c r="L19" s="37">
+        <v>2</v>
+      </c>
+      <c r="M19" s="37">
+        <v>3</v>
+      </c>
+      <c r="N19" s="37">
+        <v>4</v>
+      </c>
+      <c r="O19" s="37">
+        <v>5</v>
+      </c>
+      <c r="P19" s="37">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="37">
+        <v>7</v>
+      </c>
+      <c r="R19" s="37">
+        <v>8</v>
+      </c>
       <c r="S19" s="37"/>
       <c r="T19" s="37"/>
       <c r="U19" s="37"/>
@@ -15934,13 +16006,17 @@
       <c r="F20" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="G20" s="37"/>
+      <c r="G20" s="37" t="s">
+        <v>222</v>
+      </c>
       <c r="H20" s="37"/>
       <c r="I20" s="37"/>
       <c r="J20" s="37"/>
       <c r="K20" s="37"/>
       <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
+      <c r="M20" s="37" t="s">
+        <v>211</v>
+      </c>
       <c r="N20" s="37"/>
       <c r="O20" s="37"/>
       <c r="P20" s="37"/>
@@ -16364,7 +16440,9 @@
       <c r="S22" s="37">
         <v>3</v>
       </c>
-      <c r="T22" s="37"/>
+      <c r="T22" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U22" s="37" t="s">
         <v>230</v>
       </c>
@@ -16419,7 +16497,9 @@
       <c r="AN22" s="37">
         <v>3</v>
       </c>
-      <c r="AO22" s="37"/>
+      <c r="AO22" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP22" s="37" t="s">
         <v>230</v>
       </c>
@@ -16470,7 +16550,9 @@
       <c r="BI22" s="37">
         <v>3</v>
       </c>
-      <c r="BJ22" s="37"/>
+      <c r="BJ22" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK22" s="37" t="s">
         <v>230</v>
       </c>
@@ -16550,7 +16632,9 @@
       <c r="S23" s="37">
         <v>3</v>
       </c>
-      <c r="T23" s="37"/>
+      <c r="T23" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U23" s="37" t="s">
         <v>230</v>
       </c>
@@ -16605,7 +16689,9 @@
       <c r="AN23" s="37">
         <v>3</v>
       </c>
-      <c r="AO23" s="37"/>
+      <c r="AO23" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP23" s="37" t="s">
         <v>230</v>
       </c>
@@ -16660,7 +16746,9 @@
       <c r="BI23" s="37">
         <v>3</v>
       </c>
-      <c r="BJ23" s="37"/>
+      <c r="BJ23" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK23" s="37" t="s">
         <v>230</v>
       </c>
@@ -16722,7 +16810,9 @@
       <c r="S24" s="37">
         <v>3</v>
       </c>
-      <c r="T24" s="37"/>
+      <c r="T24" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U24" s="37" t="s">
         <v>230</v>
       </c>
@@ -16759,7 +16849,9 @@
       <c r="AN24" s="37">
         <v>3</v>
       </c>
-      <c r="AO24" s="37"/>
+      <c r="AO24" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP24" s="37" t="s">
         <v>230</v>
       </c>
@@ -16796,7 +16888,9 @@
       <c r="BI24" s="37">
         <v>3</v>
       </c>
-      <c r="BJ24" s="37"/>
+      <c r="BJ24" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK24" s="37" t="s">
         <v>230</v>
       </c>
@@ -16874,7 +16968,9 @@
       <c r="S25" s="37">
         <v>3</v>
       </c>
-      <c r="T25" s="37"/>
+      <c r="T25" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U25" s="37" t="s">
         <v>230</v>
       </c>
@@ -16927,7 +17023,9 @@
       <c r="AN25" s="37">
         <v>3</v>
       </c>
-      <c r="AO25" s="37"/>
+      <c r="AO25" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP25" s="37" t="s">
         <v>230</v>
       </c>
@@ -16980,7 +17078,9 @@
       <c r="BI25" s="37">
         <v>3</v>
       </c>
-      <c r="BJ25" s="37"/>
+      <c r="BJ25" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK25" s="37" t="s">
         <v>230</v>
       </c>
@@ -17301,7 +17401,9 @@
       <c r="S27" s="37">
         <v>3</v>
       </c>
-      <c r="T27" s="37"/>
+      <c r="T27" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U27" s="37" t="s">
         <v>230</v>
       </c>
@@ -17352,7 +17454,9 @@
       <c r="AN27" s="37">
         <v>3</v>
       </c>
-      <c r="AO27" s="37"/>
+      <c r="AO27" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP27" s="37" t="s">
         <v>230</v>
       </c>
@@ -17397,7 +17501,9 @@
       <c r="BI27" s="37">
         <v>3</v>
       </c>
-      <c r="BJ27" s="37"/>
+      <c r="BJ27" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK27" s="37" t="s">
         <v>230</v>
       </c>
@@ -17477,7 +17583,9 @@
       <c r="S28" s="37">
         <v>3</v>
       </c>
-      <c r="T28" s="37"/>
+      <c r="T28" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U28" s="37" t="s">
         <v>230</v>
       </c>
@@ -17532,7 +17640,9 @@
       <c r="AN28" s="37">
         <v>3</v>
       </c>
-      <c r="AO28" s="37"/>
+      <c r="AO28" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP28" s="37" t="s">
         <v>230</v>
       </c>
@@ -17587,7 +17697,9 @@
       <c r="BI28" s="37">
         <v>3</v>
       </c>
-      <c r="BJ28" s="37"/>
+      <c r="BJ28" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK28" s="37" t="s">
         <v>230</v>
       </c>
@@ -17649,7 +17761,9 @@
       <c r="S29" s="37">
         <v>3</v>
       </c>
-      <c r="T29" s="37"/>
+      <c r="T29" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U29" s="37" t="s">
         <v>230</v>
       </c>
@@ -17686,7 +17800,9 @@
       <c r="AN29" s="37">
         <v>3</v>
       </c>
-      <c r="AO29" s="37"/>
+      <c r="AO29" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP29" s="37" t="s">
         <v>230</v>
       </c>
@@ -17723,7 +17839,9 @@
       <c r="BI29" s="37">
         <v>3</v>
       </c>
-      <c r="BJ29" s="37"/>
+      <c r="BJ29" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK29" s="37" t="s">
         <v>230</v>
       </c>
@@ -17801,7 +17919,9 @@
       <c r="S30" s="37">
         <v>3</v>
       </c>
-      <c r="T30" s="37"/>
+      <c r="T30" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="U30" s="37" t="s">
         <v>230</v>
       </c>
@@ -17854,7 +17974,9 @@
       <c r="AN30" s="37">
         <v>3</v>
       </c>
-      <c r="AO30" s="37"/>
+      <c r="AO30" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="AP30" s="37" t="s">
         <v>230</v>
       </c>
@@ -17907,7 +18029,9 @@
       <c r="BI30" s="37">
         <v>3</v>
       </c>
-      <c r="BJ30" s="37"/>
+      <c r="BJ30" s="37" t="s">
+        <v>311</v>
+      </c>
       <c r="BK30" s="37" t="s">
         <v>230</v>
       </c>
@@ -19461,25 +19585,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="K1" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="61" t="s">
+      <c r="L1" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="61" t="s">
+      <c r="N1" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="61" t="s">
+      <c r="O1" s="67" t="s">
         <v>83</v>
       </c>
     </row>
@@ -19500,13 +19624,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -19528,13 +19652,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -21233,36 +21357,36 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="63">
-        <v>2</v>
-      </c>
-      <c r="B51" s="63">
-        <v>2</v>
-      </c>
-      <c r="C51" s="63" t="s">
+      <c r="A51" s="52">
+        <v>2</v>
+      </c>
+      <c r="B51" s="52">
+        <v>2</v>
+      </c>
+      <c r="C51" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="63"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="63">
-        <v>0</v>
-      </c>
-      <c r="J51" s="63">
-        <v>0</v>
-      </c>
-      <c r="K51" s="63">
-        <v>0</v>
-      </c>
-      <c r="L51" s="63">
-        <v>0</v>
-      </c>
-      <c r="M51" s="63">
-        <v>0</v>
-      </c>
-      <c r="N51" s="63">
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52">
+        <v>0</v>
+      </c>
+      <c r="J51" s="52">
+        <v>0</v>
+      </c>
+      <c r="K51" s="52">
+        <v>0</v>
+      </c>
+      <c r="L51" s="52">
+        <v>0</v>
+      </c>
+      <c r="M51" s="52">
+        <v>0</v>
+      </c>
+      <c r="N51" s="52">
         <v>2</v>
       </c>
       <c r="O51" s="1">
@@ -21297,10 +21421,10 @@
       <c r="L52" s="3">
         <v>0</v>
       </c>
-      <c r="M52" s="63">
-        <v>2</v>
-      </c>
-      <c r="N52" s="63">
+      <c r="M52" s="52">
+        <v>2</v>
+      </c>
+      <c r="N52" s="52">
         <v>2</v>
       </c>
       <c r="O52" s="1">
@@ -21329,10 +21453,10 @@
       <c r="L53" s="3">
         <v>0</v>
       </c>
-      <c r="M53" s="64">
-        <v>2</v>
-      </c>
-      <c r="N53" s="64">
+      <c r="M53" s="53">
+        <v>2</v>
+      </c>
+      <c r="N53" s="53">
         <v>2</v>
       </c>
       <c r="O53">
@@ -21364,10 +21488,10 @@
       <c r="L54" s="3">
         <v>0</v>
       </c>
-      <c r="M54" s="63">
-        <v>2</v>
-      </c>
-      <c r="N54" s="63">
+      <c r="M54" s="52">
+        <v>2</v>
+      </c>
+      <c r="N54" s="52">
         <v>2</v>
       </c>
       <c r="O54">
@@ -21396,10 +21520,10 @@
       <c r="L55" s="3">
         <v>1</v>
       </c>
-      <c r="M55" s="64">
-        <v>2</v>
-      </c>
-      <c r="N55" s="64">
+      <c r="M55" s="53">
+        <v>2</v>
+      </c>
+      <c r="N55" s="53">
         <v>2</v>
       </c>
       <c r="O55">
@@ -21428,10 +21552,10 @@
       <c r="L56" s="3">
         <v>1</v>
       </c>
-      <c r="M56" s="63">
-        <v>2</v>
-      </c>
-      <c r="N56" s="63">
+      <c r="M56" s="52">
+        <v>2</v>
+      </c>
+      <c r="N56" s="52">
         <v>2</v>
       </c>
       <c r="O56">
@@ -21463,10 +21587,10 @@
       <c r="L57" s="3">
         <v>1</v>
       </c>
-      <c r="M57" s="64">
-        <v>2</v>
-      </c>
-      <c r="N57" s="64">
+      <c r="M57" s="53">
+        <v>2</v>
+      </c>
+      <c r="N57" s="53">
         <v>2</v>
       </c>
       <c r="O57">
@@ -21495,10 +21619,10 @@
       <c r="L58" s="3">
         <v>2</v>
       </c>
-      <c r="M58" s="63">
-        <v>2</v>
-      </c>
-      <c r="N58" s="63">
+      <c r="M58" s="52">
+        <v>2</v>
+      </c>
+      <c r="N58" s="52">
         <v>2</v>
       </c>
       <c r="O58">
@@ -21527,10 +21651,10 @@
       <c r="L59" s="3">
         <v>2</v>
       </c>
-      <c r="M59" s="64">
-        <v>2</v>
-      </c>
-      <c r="N59" s="64">
+      <c r="M59" s="53">
+        <v>2</v>
+      </c>
+      <c r="N59" s="53">
         <v>2</v>
       </c>
       <c r="O59">
@@ -21562,10 +21686,10 @@
       <c r="L60" s="3">
         <v>2</v>
       </c>
-      <c r="M60" s="63">
-        <v>2</v>
-      </c>
-      <c r="N60" s="63">
+      <c r="M60" s="52">
+        <v>2</v>
+      </c>
+      <c r="N60" s="52">
         <v>2</v>
       </c>
       <c r="O60">
@@ -21594,10 +21718,10 @@
       <c r="L61" s="3">
         <v>3</v>
       </c>
-      <c r="M61" s="64">
-        <v>2</v>
-      </c>
-      <c r="N61" s="64">
+      <c r="M61" s="53">
+        <v>2</v>
+      </c>
+      <c r="N61" s="53">
         <v>2</v>
       </c>
       <c r="O61">
@@ -21626,10 +21750,10 @@
       <c r="L62" s="3">
         <v>3</v>
       </c>
-      <c r="M62" s="63">
-        <v>2</v>
-      </c>
-      <c r="N62" s="63">
+      <c r="M62" s="52">
+        <v>2</v>
+      </c>
+      <c r="N62" s="52">
         <v>2</v>
       </c>
       <c r="O62">
@@ -21661,10 +21785,10 @@
       <c r="L63" s="3">
         <v>3</v>
       </c>
-      <c r="M63" s="64">
-        <v>2</v>
-      </c>
-      <c r="N63" s="64">
+      <c r="M63" s="53">
+        <v>2</v>
+      </c>
+      <c r="N63" s="53">
         <v>2</v>
       </c>
       <c r="O63">
@@ -21672,36 +21796,36 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="66">
+      <c r="A64" s="55">
         <v>3</v>
       </c>
-      <c r="B64" s="66">
+      <c r="B64" s="55">
         <v>3</v>
       </c>
-      <c r="C64" s="66" t="s">
+      <c r="C64" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="D64" s="66"/>
-      <c r="E64" s="66"/>
-      <c r="F64" s="66"/>
-      <c r="G64" s="66"/>
-      <c r="H64" s="66"/>
-      <c r="I64" s="66">
-        <v>0</v>
-      </c>
-      <c r="J64" s="66">
-        <v>0</v>
-      </c>
-      <c r="K64" s="66">
-        <v>0</v>
-      </c>
-      <c r="L64" s="66">
-        <v>0</v>
-      </c>
-      <c r="M64" s="65">
-        <v>0</v>
-      </c>
-      <c r="N64" s="65">
+      <c r="D64" s="55"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="55">
+        <v>0</v>
+      </c>
+      <c r="J64" s="55">
+        <v>0</v>
+      </c>
+      <c r="K64" s="55">
+        <v>0</v>
+      </c>
+      <c r="L64" s="55">
+        <v>0</v>
+      </c>
+      <c r="M64" s="54">
+        <v>0</v>
+      </c>
+      <c r="N64" s="54">
         <v>3</v>
       </c>
       <c r="O64">
@@ -21733,10 +21857,10 @@
       <c r="L65" s="3">
         <v>0</v>
       </c>
-      <c r="M65" s="66">
+      <c r="M65" s="55">
         <v>3</v>
       </c>
-      <c r="N65" s="66">
+      <c r="N65" s="55">
         <v>3</v>
       </c>
     </row>
@@ -21762,10 +21886,10 @@
       <c r="L66" s="3">
         <v>0</v>
       </c>
-      <c r="M66" s="66">
+      <c r="M66" s="55">
         <v>3</v>
       </c>
-      <c r="N66" s="66">
+      <c r="N66" s="55">
         <v>3</v>
       </c>
       <c r="P66" t="s">
@@ -21792,10 +21916,10 @@
       <c r="L67" s="3">
         <v>0</v>
       </c>
-      <c r="M67" s="66">
+      <c r="M67" s="55">
         <v>3</v>
       </c>
-      <c r="N67" s="66">
+      <c r="N67" s="55">
         <v>3</v>
       </c>
     </row>
@@ -21821,10 +21945,10 @@
       <c r="L68" s="3">
         <v>1</v>
       </c>
-      <c r="M68" s="66">
+      <c r="M68" s="55">
         <v>3</v>
       </c>
-      <c r="N68" s="66">
+      <c r="N68" s="55">
         <v>3</v>
       </c>
     </row>
@@ -21850,10 +21974,10 @@
       <c r="L69" s="3">
         <v>1</v>
       </c>
-      <c r="M69" s="66">
+      <c r="M69" s="55">
         <v>3</v>
       </c>
-      <c r="N69" s="66">
+      <c r="N69" s="55">
         <v>3</v>
       </c>
       <c r="P69" t="s">
@@ -21880,10 +22004,10 @@
       <c r="L70" s="3">
         <v>1</v>
       </c>
-      <c r="M70" s="66">
+      <c r="M70" s="55">
         <v>3</v>
       </c>
-      <c r="N70" s="66">
+      <c r="N70" s="55">
         <v>3</v>
       </c>
     </row>
@@ -21909,10 +22033,10 @@
       <c r="L71" s="3">
         <v>2</v>
       </c>
-      <c r="M71" s="66">
+      <c r="M71" s="55">
         <v>3</v>
       </c>
-      <c r="N71" s="66">
+      <c r="N71" s="55">
         <v>3</v>
       </c>
     </row>
@@ -21938,10 +22062,10 @@
       <c r="L72" s="3">
         <v>2</v>
       </c>
-      <c r="M72" s="66">
+      <c r="M72" s="55">
         <v>3</v>
       </c>
-      <c r="N72" s="66">
+      <c r="N72" s="55">
         <v>3</v>
       </c>
       <c r="P72" t="s">
@@ -21968,10 +22092,10 @@
       <c r="L73" s="3">
         <v>2</v>
       </c>
-      <c r="M73" s="66">
+      <c r="M73" s="55">
         <v>3</v>
       </c>
-      <c r="N73" s="66">
+      <c r="N73" s="55">
         <v>3</v>
       </c>
     </row>
@@ -21997,10 +22121,10 @@
       <c r="L74" s="3">
         <v>3</v>
       </c>
-      <c r="M74" s="66">
+      <c r="M74" s="55">
         <v>3</v>
       </c>
-      <c r="N74" s="66">
+      <c r="N74" s="55">
         <v>3</v>
       </c>
     </row>
@@ -22026,10 +22150,10 @@
       <c r="L75" s="3">
         <v>3</v>
       </c>
-      <c r="M75" s="66">
+      <c r="M75" s="55">
         <v>3</v>
       </c>
-      <c r="N75" s="66">
+      <c r="N75" s="55">
         <v>3</v>
       </c>
       <c r="P75" t="s">
@@ -22056,10 +22180,10 @@
       <c r="L76" s="3">
         <v>3</v>
       </c>
-      <c r="M76" s="66">
+      <c r="M76" s="55">
         <v>3</v>
       </c>
-      <c r="N76" s="66">
+      <c r="N76" s="55">
         <v>3</v>
       </c>
     </row>
@@ -22085,10 +22209,10 @@
       <c r="L77" s="3">
         <v>3.86013986013986</v>
       </c>
-      <c r="M77" s="66">
+      <c r="M77" s="55">
         <v>3</v>
       </c>
-      <c r="N77" s="66">
+      <c r="N77" s="55">
         <v>3</v>
       </c>
     </row>
@@ -22114,10 +22238,10 @@
       <c r="L78" s="3">
         <v>4.1748251748251803</v>
       </c>
-      <c r="M78" s="66">
+      <c r="M78" s="55">
         <v>3</v>
       </c>
-      <c r="N78" s="66">
+      <c r="N78" s="55">
         <v>3</v>
       </c>
       <c r="P78" t="s">
@@ -22144,44 +22268,44 @@
       <c r="L79" s="3">
         <v>4.48951048951049</v>
       </c>
-      <c r="M79" s="66">
+      <c r="M79" s="55">
         <v>3</v>
       </c>
-      <c r="N79" s="66">
+      <c r="N79" s="55">
         <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A80" s="68">
+      <c r="A80" s="57">
         <v>4</v>
       </c>
-      <c r="B80" s="68">
+      <c r="B80" s="57">
         <v>4</v>
       </c>
-      <c r="C80" s="68" t="s">
+      <c r="C80" s="57" t="s">
         <v>303</v>
       </c>
-      <c r="D80" s="68"/>
-      <c r="E80" s="68"/>
-      <c r="F80" s="68"/>
-      <c r="G80" s="68"/>
-      <c r="H80" s="68"/>
-      <c r="I80" s="68">
-        <v>0</v>
-      </c>
-      <c r="J80" s="68">
-        <v>0</v>
-      </c>
-      <c r="K80" s="68">
-        <v>0</v>
-      </c>
-      <c r="L80" s="68">
-        <v>0</v>
-      </c>
-      <c r="M80" s="67">
-        <v>0</v>
-      </c>
-      <c r="N80" s="67">
+      <c r="D80" s="57"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="57"/>
+      <c r="H80" s="57"/>
+      <c r="I80" s="57">
+        <v>0</v>
+      </c>
+      <c r="J80" s="57">
+        <v>0</v>
+      </c>
+      <c r="K80" s="57">
+        <v>0</v>
+      </c>
+      <c r="L80" s="57">
+        <v>0</v>
+      </c>
+      <c r="M80" s="56">
+        <v>0</v>
+      </c>
+      <c r="N80" s="56">
         <v>4</v>
       </c>
     </row>
@@ -22207,10 +22331,10 @@
       <c r="L81" s="3">
         <v>0</v>
       </c>
-      <c r="M81" s="68">
+      <c r="M81" s="57">
         <v>4</v>
       </c>
-      <c r="N81" s="68">
+      <c r="N81" s="57">
         <v>4</v>
       </c>
       <c r="O81" s="1">
@@ -22239,10 +22363,10 @@
       <c r="L82" s="3">
         <v>0</v>
       </c>
-      <c r="M82" s="68">
+      <c r="M82" s="57">
         <v>4</v>
       </c>
-      <c r="N82" s="68">
+      <c r="N82" s="57">
         <v>4</v>
       </c>
       <c r="O82" s="1">
@@ -22274,10 +22398,10 @@
       <c r="L83" s="3">
         <v>0</v>
       </c>
-      <c r="M83" s="68">
+      <c r="M83" s="57">
         <v>4</v>
       </c>
-      <c r="N83" s="68">
+      <c r="N83" s="57">
         <v>4</v>
       </c>
       <c r="O83" s="1">
@@ -22306,10 +22430,10 @@
       <c r="L84" s="3">
         <v>1</v>
       </c>
-      <c r="M84" s="68">
+      <c r="M84" s="57">
         <v>4</v>
       </c>
-      <c r="N84" s="68">
+      <c r="N84" s="57">
         <v>4</v>
       </c>
       <c r="O84" s="1">
@@ -22338,10 +22462,10 @@
       <c r="L85" s="3">
         <v>1</v>
       </c>
-      <c r="M85" s="68">
+      <c r="M85" s="57">
         <v>4</v>
       </c>
-      <c r="N85" s="68">
+      <c r="N85" s="57">
         <v>4</v>
       </c>
       <c r="O85" s="1">
@@ -22373,10 +22497,10 @@
       <c r="L86" s="3">
         <v>1</v>
       </c>
-      <c r="M86" s="68">
+      <c r="M86" s="57">
         <v>4</v>
       </c>
-      <c r="N86" s="68">
+      <c r="N86" s="57">
         <v>4</v>
       </c>
       <c r="O86" s="1">
@@ -22405,10 +22529,10 @@
       <c r="L87" s="3">
         <v>2</v>
       </c>
-      <c r="M87" s="68">
+      <c r="M87" s="57">
         <v>4</v>
       </c>
-      <c r="N87" s="68">
+      <c r="N87" s="57">
         <v>4</v>
       </c>
       <c r="O87" s="1">
@@ -22437,10 +22561,10 @@
       <c r="L88" s="3">
         <v>2</v>
       </c>
-      <c r="M88" s="68">
+      <c r="M88" s="57">
         <v>4</v>
       </c>
-      <c r="N88" s="68">
+      <c r="N88" s="57">
         <v>4</v>
       </c>
       <c r="O88" s="1">
@@ -22472,10 +22596,10 @@
       <c r="L89" s="3">
         <v>2</v>
       </c>
-      <c r="M89" s="68">
+      <c r="M89" s="57">
         <v>4</v>
       </c>
-      <c r="N89" s="68">
+      <c r="N89" s="57">
         <v>4</v>
       </c>
       <c r="O89" s="1">
@@ -22502,10 +22626,10 @@
       <c r="L90" s="3">
         <v>3</v>
       </c>
-      <c r="M90" s="68">
+      <c r="M90" s="57">
         <v>4</v>
       </c>
-      <c r="N90" s="68">
+      <c r="N90" s="57">
         <v>4</v>
       </c>
     </row>
@@ -22529,10 +22653,10 @@
       <c r="L91" s="3">
         <v>3</v>
       </c>
-      <c r="M91" s="68">
+      <c r="M91" s="57">
         <v>4</v>
       </c>
-      <c r="N91" s="68">
+      <c r="N91" s="57">
         <v>4</v>
       </c>
     </row>
@@ -22556,10 +22680,10 @@
       <c r="L92" s="3">
         <v>3</v>
       </c>
-      <c r="M92" s="68">
+      <c r="M92" s="57">
         <v>4</v>
       </c>
-      <c r="N92" s="68">
+      <c r="N92" s="57">
         <v>4</v>
       </c>
     </row>
@@ -22583,10 +22707,10 @@
       <c r="L93" s="3">
         <v>3.86013986013986</v>
       </c>
-      <c r="M93" s="68">
+      <c r="M93" s="57">
         <v>4</v>
       </c>
-      <c r="N93" s="68">
+      <c r="N93" s="57">
         <v>4</v>
       </c>
     </row>
@@ -22610,10 +22734,10 @@
       <c r="L94" s="3">
         <v>4.1748251748251803</v>
       </c>
-      <c r="M94" s="68">
+      <c r="M94" s="57">
         <v>4</v>
       </c>
-      <c r="N94" s="68">
+      <c r="N94" s="57">
         <v>4</v>
       </c>
     </row>
@@ -22637,10 +22761,10 @@
       <c r="L95" s="3">
         <v>4.48951048951049</v>
       </c>
-      <c r="M95" s="68">
+      <c r="M95" s="57">
         <v>4</v>
       </c>
-      <c r="N95" s="68">
+      <c r="N95" s="57">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tagging as v0.24  Finished adding support for an alarm to trigger multiple relays through the use of AlarmRelay[id].  Also added RelayState to store which relays are turned on in case of power outage.  Also changed some of the delays on the alarm setting options to speed that up a bit.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="316">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -965,6 +965,15 @@
   </si>
   <si>
     <t>+/-</t>
+  </si>
+  <si>
+    <t>RelayState</t>
+  </si>
+  <si>
+    <t>Holds the current state of all alarms</t>
+  </si>
+  <si>
+    <t>Relays</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1420,6 +1429,10 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1453,7 +1466,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1761,7 +1773,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,12 +1785,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="A1" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" t="s">
         <v>98</v>
       </c>
@@ -1955,12 +1967,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
       <c r="E1" t="s">
         <v>97</v>
       </c>
@@ -2117,10 +2129,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2135,13 +2147,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
       <c r="F1" s="19" t="s">
         <v>110</v>
       </c>
@@ -2171,7 +2183,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -2192,7 +2204,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="63"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -2213,7 +2225,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="63" t="s">
         <v>178</v>
       </c>
       <c r="B5" s="25">
@@ -2236,7 +2248,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="60"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -2257,7 +2269,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="60"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -2278,7 +2290,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="60"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -2299,7 +2311,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="60"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -2320,7 +2332,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="61"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -2341,7 +2353,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="63" t="s">
         <v>179</v>
       </c>
       <c r="B11" s="25">
@@ -2364,7 +2376,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="60"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -2385,7 +2397,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="60"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -2406,7 +2418,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="60"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -2427,7 +2439,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="60"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -2448,7 +2460,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="61"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -2469,7 +2481,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="63" t="s">
         <v>180</v>
       </c>
       <c r="B17" s="29">
@@ -2492,7 +2504,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="60"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -2513,7 +2525,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="60"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -2534,7 +2546,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="60"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -2555,7 +2567,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="60"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -2576,7 +2588,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="61"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -2597,7 +2609,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="63" t="s">
         <v>181</v>
       </c>
       <c r="B23" s="25">
@@ -2620,7 +2632,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="60"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -2641,7 +2653,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="60"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -2662,7 +2674,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="60"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -2683,7 +2695,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="60"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -2704,7 +2716,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="61"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -2725,7 +2737,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="63" t="s">
         <v>182</v>
       </c>
       <c r="B29" s="29">
@@ -2748,7 +2760,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -2769,7 +2781,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="60"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -2790,7 +2802,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="60"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -2811,7 +2823,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="60"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -2832,7 +2844,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="61"/>
+      <c r="A34" s="65"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -2853,7 +2865,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="63" t="s">
         <v>183</v>
       </c>
       <c r="B35" s="25">
@@ -2876,7 +2888,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="60"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -2897,7 +2909,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="60"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -2918,7 +2930,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="60"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -2939,7 +2951,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -2960,7 +2972,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="61"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -2981,7 +2993,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="59" t="s">
+      <c r="A41" s="63" t="s">
         <v>184</v>
       </c>
       <c r="B41" s="29">
@@ -3004,7 +3016,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="60"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -3025,7 +3037,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="60"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -3046,7 +3058,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="60"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -3067,7 +3079,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="60"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -3088,7 +3100,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="61"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -3109,7 +3121,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="59" t="s">
+      <c r="A47" s="63" t="s">
         <v>185</v>
       </c>
       <c r="B47" s="25">
@@ -3132,7 +3144,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="60"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -3153,7 +3165,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="60"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -3174,7 +3186,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="60"/>
+      <c r="A50" s="64"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -3195,7 +3207,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="60"/>
+      <c r="A51" s="64"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -3216,7 +3228,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="61"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -3234,6 +3246,23 @@
       </c>
       <c r="G52" s="32" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="59">
+        <v>150</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="D53" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="E53" s="8">
+        <v>1</v>
+      </c>
+      <c r="G53" s="61" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -3258,8 +3287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z267"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3562,6 +3591,9 @@
       <c r="M6">
         <v>6</v>
       </c>
+      <c r="N6" t="s">
+        <v>315</v>
+      </c>
       <c r="U6" s="40">
         <v>4</v>
       </c>
@@ -3983,7 +4015,7 @@
       <c r="M17">
         <v>8</v>
       </c>
-      <c r="N17" s="69" t="s">
+      <c r="N17" s="58" t="s">
         <v>312</v>
       </c>
     </row>
@@ -12267,8 +12299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AB24" sqref="AB24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -13140,31 +13172,47 @@
         <v>195</v>
       </c>
       <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
+      <c r="H5" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>232</v>
+      </c>
       <c r="O5" s="37" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="P5" s="37" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="Q5" s="37" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="R5" s="37" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="S5" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37">
-        <v>1</v>
+        <v>210</v>
+      </c>
+      <c r="T5" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="U5" s="37" t="s">
+        <v>210</v>
       </c>
       <c r="V5">
         <v>4</v>
@@ -13183,31 +13231,47 @@
         <v>195</v>
       </c>
       <c r="AB5" s="37"/>
-      <c r="AC5" s="37"/>
-      <c r="AD5" s="37"/>
-      <c r="AE5" s="37"/>
-      <c r="AF5" s="37"/>
-      <c r="AG5" s="37"/>
-      <c r="AH5" s="37"/>
-      <c r="AI5" s="37"/>
+      <c r="AC5" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD5" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE5" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="AF5" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="AG5" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH5" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI5" s="37" t="s">
+        <v>232</v>
+      </c>
       <c r="AJ5" s="37" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="AK5" s="37" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="AL5" s="37" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="AM5" s="37" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="AN5" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="AO5" s="37"/>
-      <c r="AP5" s="37">
-        <v>8</v>
+        <v>210</v>
+      </c>
+      <c r="AO5" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="AP5" s="37" t="s">
+        <v>210</v>
       </c>
       <c r="AQ5">
         <v>3</v>
@@ -19585,25 +19649,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="67" t="s">
+      <c r="K1" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="71" t="s">
         <v>83</v>
       </c>
     </row>
@@ -19624,13 +19688,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -19652,13 +19716,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">

</xml_diff>

<commit_message>
Added compile date and time to the serial port at startup.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="-2148" yWindow="1596" windowWidth="23028" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="317">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -974,6 +974,9 @@
   </si>
   <si>
     <t>Relays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t </t>
   </si>
 </sst>
 </file>
@@ -3287,7 +3290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -12299,8 +12302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -18374,17 +18377,37 @@
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
+      <c r="F32" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="H32" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="J32" s="37" t="s">
+        <v>199</v>
+      </c>
       <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
+      <c r="L32" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="M32" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="N32" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="O32" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="P32" s="37" t="s">
+        <v>233</v>
+      </c>
       <c r="Q32" s="37"/>
       <c r="R32" s="37"/>
       <c r="S32" s="37"/>
@@ -18477,13 +18500,27 @@
       <c r="L33" s="37"/>
       <c r="M33" s="37"/>
       <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="37"/>
+      <c r="O33" s="37">
+        <v>1</v>
+      </c>
+      <c r="P33" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="R33" s="37">
+        <v>5</v>
+      </c>
+      <c r="S33" s="37">
+        <v>5</v>
+      </c>
+      <c r="T33" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="U33" s="37" t="s">
+        <v>202</v>
+      </c>
       <c r="V33">
         <v>2</v>
       </c>
@@ -18558,26 +18595,60 @@
       <c r="A34">
         <v>2</v>
       </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
+      <c r="B34" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>316</v>
+      </c>
       <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
+      <c r="G34" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="I34" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="J34" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="K34" s="37" t="s">
+        <v>199</v>
+      </c>
       <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
+      <c r="M34" s="37">
+        <v>1</v>
+      </c>
       <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="37"/>
-      <c r="R34" s="37"/>
-      <c r="S34" s="37"/>
-      <c r="T34" s="37"/>
-      <c r="U34" s="37"/>
+      <c r="O34" s="37">
+        <v>1</v>
+      </c>
+      <c r="P34" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="R34" s="37">
+        <v>5</v>
+      </c>
+      <c r="S34" s="37">
+        <v>5</v>
+      </c>
+      <c r="T34" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="U34" s="37" t="s">
+        <v>202</v>
+      </c>
       <c r="V34">
         <v>3</v>
       </c>
@@ -18653,17 +18724,35 @@
         <v>3</v>
       </c>
       <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
+      <c r="C35" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>316</v>
+      </c>
       <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
+      <c r="G35" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="H35" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="I35" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="J35" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="K35" s="37" t="s">
+        <v>199</v>
+      </c>
       <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
+      <c r="M35" s="37">
+        <v>2</v>
+      </c>
       <c r="N35" s="37"/>
       <c r="O35" s="37"/>
       <c r="P35" s="37"/>

</xml_diff>

<commit_message>
Fixed the bug with the read totalling.  Added some more things to the serial debugging.  Flow alarm display show shows "Flow Good" or  "Flow Alarm" depending on if the flow is restricted past the flowRateMin variable.  Fixed the flowRateMax variable to correctly store the 2 bytes necessary for an integer in the EEPROM.  Reorganized some of the initialization variables to make a bit more sense for the purpose that they serve.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="326">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1001,6 +1001,9 @@
   </si>
   <si>
     <t>byte to determine if the flow sensor is enabled.  0 = Disabled, 1 = Enabled.</t>
+  </si>
+  <si>
+    <t>Flow Sensor</t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3363,7 +3366,7 @@
   <dimension ref="A1:Z267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="M16" sqref="M16:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3371,6 +3374,7 @@
     <col min="1" max="1" width="8.88671875" style="16"/>
     <col min="2" max="9" width="2.77734375" customWidth="1"/>
     <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -3444,10 +3448,10 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U2" s="40">
         <v>0</v>
@@ -3499,10 +3503,10 @@
         <v>2</v>
       </c>
       <c r="M3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="U3" s="40">
         <v>1</v>
@@ -3554,10 +3558,10 @@
         <v>4</v>
       </c>
       <c r="M4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U4" s="40">
         <v>2</v>
@@ -3609,10 +3613,10 @@
         <v>8</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>226</v>
+        <v>186</v>
       </c>
       <c r="U5" s="40">
         <v>3</v>
@@ -3664,10 +3668,10 @@
         <v>16</v>
       </c>
       <c r="M6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N6" t="s">
-        <v>313</v>
+        <v>226</v>
       </c>
       <c r="U6" s="40">
         <v>4</v>
@@ -3719,10 +3723,10 @@
         <v>32</v>
       </c>
       <c r="M7">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>190</v>
+        <v>313</v>
       </c>
       <c r="U7" s="40">
         <v>5</v>
@@ -3773,6 +3777,12 @@
       <c r="K8">
         <v>64</v>
       </c>
+      <c r="M8">
+        <v>32</v>
+      </c>
+      <c r="N8" t="s">
+        <v>190</v>
+      </c>
       <c r="U8" s="40">
         <v>6</v>
       </c>
@@ -3823,10 +3833,10 @@
         <v>128</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>188</v>
+        <v>325</v>
       </c>
       <c r="U9" s="40">
         <v>7</v>
@@ -3848,9 +3858,14 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="M11">
+        <v>255</v>
+      </c>
+      <c r="N11" t="s">
         <v>184</v>
       </c>
     </row>
@@ -3889,9 +3904,6 @@
         <f>DEC2BIN(J12)</f>
         <v>0</v>
       </c>
-      <c r="M12" t="s">
-        <v>272</v>
-      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13">
@@ -3924,12 +3936,6 @@
       <c r="K13" t="str">
         <f t="shared" ref="K13:K76" si="2">DEC2BIN(J13)</f>
         <v>1</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
@@ -3964,17 +3970,8 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>274</v>
-      </c>
-      <c r="O14" t="s">
-        <v>279</v>
-      </c>
-      <c r="P14" t="s">
-        <v>280</v>
+      <c r="M14" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -4010,10 +4007,10 @@
         <v>11</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -4049,10 +4046,16 @@
         <v>100</v>
       </c>
       <c r="M16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>276</v>
+        <v>274</v>
+      </c>
+      <c r="O16" t="s">
+        <v>279</v>
+      </c>
+      <c r="P16" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -4088,10 +4091,10 @@
         <v>101</v>
       </c>
       <c r="M17">
-        <v>8</v>
-      </c>
-      <c r="N17" s="58" t="s">
-        <v>310</v>
+        <v>2</v>
+      </c>
+      <c r="N17" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -4127,7 +4130,10 @@
         <v>110</v>
       </c>
       <c r="M18">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
@@ -4163,7 +4169,10 @@
         <v>111</v>
       </c>
       <c r="M19">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="N19" s="58" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
@@ -4199,10 +4208,7 @@
         <v>1000</v>
       </c>
       <c r="M20">
-        <v>64</v>
-      </c>
-      <c r="N20" t="s">
-        <v>281</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -4238,13 +4244,7 @@
         <v>1001</v>
       </c>
       <c r="M21">
-        <v>128</v>
-      </c>
-      <c r="N21" t="s">
-        <v>277</v>
-      </c>
-      <c r="O21" t="s">
-        <v>278</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
@@ -4279,6 +4279,12 @@
         <f t="shared" si="2"/>
         <v>1010</v>
       </c>
+      <c r="M22">
+        <v>64</v>
+      </c>
+      <c r="N22" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23">
@@ -4312,6 +4318,15 @@
         <f t="shared" si="2"/>
         <v>1011</v>
       </c>
+      <c r="M23">
+        <v>128</v>
+      </c>
+      <c r="N23" t="s">
+        <v>277</v>
+      </c>
+      <c r="O23" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24">
@@ -4344,6 +4359,9 @@
       <c r="K24" t="str">
         <f t="shared" si="2"/>
         <v>1100</v>
+      </c>
+      <c r="M24">
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changed my mind about flow sensor Delay and Time needing to be user settable.  All things are easier if they are not and it will make much better use of time if they are not user settable.  Took out the menu entries,  but left the footprints to be able to easily find where to add the next menu items I may need.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="326">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1984,7 +1984,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2166,7 +2166,7 @@
         <v>317</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
         <v>318</v>
@@ -2177,12 +2177,23 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
+        <v>317</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
         <v>319</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>320</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tagging as v0.30  Finished adding support to enable and disable the flow sensor.   This is selectable in the user settings section of the menu and will enable or disable the alarm associated with the flowReadID.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="323">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -973,30 +973,15 @@
     <t xml:space="preserve">t </t>
   </si>
   <si>
-    <t>flowReadDelay</t>
-  </si>
-  <si>
-    <t>flowReadTime</t>
-  </si>
-  <si>
     <t>flowRateMax</t>
   </si>
   <si>
-    <t>maximum flow rate after a filter clean</t>
-  </si>
-  <si>
     <t>flowRateMin</t>
   </si>
   <si>
     <t>minimum flow rate to trigger an alarm</t>
   </si>
   <si>
-    <t>time to sample the flow rate in seconds</t>
-  </si>
-  <si>
-    <t>time between flow readings in seconds</t>
-  </si>
-  <si>
     <t>flowSensorEnable</t>
   </si>
   <si>
@@ -1004,6 +989,12 @@
   </si>
   <si>
     <t>Flow Sensor</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1975,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2121,13 +2112,13 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2138,10 +2129,7 @@
         <v>315</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" t="s">
-        <v>322</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2155,46 +2143,22 @@
         <v>94</v>
       </c>
       <c r="F12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
-        <v>317</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
-        <v>317</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>319</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
@@ -2220,7 +2184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3847,7 +3811,7 @@
         <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="U9" s="40">
         <v>7</v>
@@ -12403,8 +12367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="AI37" sqref="AI37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -19430,22 +19394,48 @@
       </c>
       <c r="B38" s="37"/>
       <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="37"/>
-      <c r="N38" s="37"/>
-      <c r="O38" s="37"/>
-      <c r="P38" s="37"/>
-      <c r="Q38" s="37"/>
-      <c r="R38" s="37"/>
-      <c r="S38" s="37"/>
+      <c r="D38" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="H38" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="I38" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="J38" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="K38" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="L38" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="M38" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="N38" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="P38" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q38" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="R38" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="S38" s="36" t="s">
+        <v>321</v>
+      </c>
       <c r="T38" s="37"/>
       <c r="U38" s="37"/>
       <c r="V38">
@@ -19533,10 +19523,18 @@
       <c r="G39" s="37"/>
       <c r="H39" s="37"/>
       <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
+      <c r="J39" s="37">
+        <v>1</v>
+      </c>
+      <c r="K39" s="37">
+        <v>0</v>
+      </c>
+      <c r="L39" s="37">
+        <v>0</v>
+      </c>
+      <c r="M39" s="37" t="s">
+        <v>322</v>
+      </c>
       <c r="N39" s="37"/>
       <c r="O39" s="37"/>
       <c r="P39" s="37"/>

</xml_diff>

<commit_message>
Started adding in the Set date and time menu editing.  Changed LCDDateDisplay to have options or col and row on the lcd printing and the display variable decides whether or not to refresh the date if the day has not changed.  This allows the use of the same funciton to display the date anywhere on the LCD.  Also finished adding the functions to change the time via the LCD menu system.  Still need to add the 12 hour format to this part in the Menu_system file.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="328">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -995,6 +995,21 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Day of the week</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -1974,7 +1989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3341,7 +3356,7 @@
   <dimension ref="A1:Z267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16:M24"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4185,6 +4200,9 @@
       <c r="M20">
         <v>16</v>
       </c>
+      <c r="N20" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21">
@@ -12365,10 +12383,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG41"/>
+  <dimension ref="A1:CG42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="Z19" workbookViewId="0">
+      <selection activeCell="AY31" sqref="AY31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -13982,7 +14000,9 @@
       <c r="AQ8">
         <v>1</v>
       </c>
-      <c r="AR8" s="37"/>
+      <c r="AR8" s="37">
+        <v>1</v>
+      </c>
       <c r="AS8" s="37">
         <v>1</v>
       </c>
@@ -16744,12 +16764,24 @@
       <c r="BP22" s="37"/>
       <c r="BQ22" s="37"/>
       <c r="BR22" s="37"/>
-      <c r="BS22" s="37"/>
-      <c r="BT22" s="37"/>
-      <c r="BU22" s="37"/>
-      <c r="BV22" s="37"/>
-      <c r="BW22" s="37"/>
-      <c r="BX22" s="37"/>
+      <c r="BS22" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BT22" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="BU22" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BV22" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW22" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BX22" s="37" t="s">
+        <v>218</v>
+      </c>
       <c r="BY22" s="37"/>
       <c r="BZ22" s="37"/>
       <c r="CA22" s="37"/>
@@ -16943,13 +16975,27 @@
       <c r="BP23" s="37"/>
       <c r="BQ23" s="37"/>
       <c r="BR23" s="37"/>
-      <c r="BS23" s="37"/>
-      <c r="BT23" s="37"/>
-      <c r="BU23" s="37"/>
-      <c r="BV23" s="37"/>
-      <c r="BW23" s="37"/>
-      <c r="BX23" s="37"/>
-      <c r="BY23" s="37"/>
+      <c r="BS23" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="BT23" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="BU23" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BV23" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BW23" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX23" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BY23" s="37" t="s">
+        <v>218</v>
+      </c>
       <c r="BZ23" s="37"/>
       <c r="CA23" s="37"/>
       <c r="CB23" s="37"/>
@@ -17088,15 +17134,33 @@
       <c r="BP24" s="37"/>
       <c r="BQ24" s="37"/>
       <c r="BR24" s="37"/>
-      <c r="BS24" s="37"/>
-      <c r="BT24" s="37"/>
-      <c r="BU24" s="37"/>
-      <c r="BV24" s="37"/>
-      <c r="BW24" s="37"/>
-      <c r="BX24" s="37"/>
-      <c r="BY24" s="37"/>
-      <c r="BZ24" s="37"/>
-      <c r="CA24" s="37"/>
+      <c r="BS24" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="BT24" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BU24" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV24" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BW24" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BX24" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BY24" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BZ24" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="CA24" s="37" t="s">
+        <v>218</v>
+      </c>
       <c r="CB24" s="37"/>
       <c r="CC24" s="37"/>
       <c r="CD24" s="37"/>
@@ -17281,14 +17345,30 @@
       <c r="BP25" s="37"/>
       <c r="BQ25" s="37"/>
       <c r="BR25" s="37"/>
-      <c r="BS25" s="37"/>
-      <c r="BT25" s="37"/>
-      <c r="BU25" s="37"/>
-      <c r="BV25" s="37"/>
-      <c r="BW25" s="37"/>
-      <c r="BX25" s="37"/>
-      <c r="BY25" s="37"/>
-      <c r="BZ25" s="37"/>
+      <c r="BS25" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="BT25" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BU25" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="BV25" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="BW25" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BX25" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY25" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BZ25" s="37" t="s">
+        <v>218</v>
+      </c>
       <c r="CA25" s="37"/>
       <c r="CB25" s="37"/>
       <c r="CC25" s="37"/>
@@ -17706,14 +17786,30 @@
       <c r="BP27" s="37"/>
       <c r="BQ27" s="37"/>
       <c r="BR27" s="37"/>
-      <c r="BS27" s="37"/>
-      <c r="BT27" s="37"/>
-      <c r="BU27" s="37"/>
-      <c r="BV27" s="37"/>
-      <c r="BW27" s="37"/>
-      <c r="BX27" s="37"/>
-      <c r="BY27" s="37"/>
-      <c r="BZ27" s="37"/>
+      <c r="BS27" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BT27" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BU27" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BV27" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="BW27" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="BX27" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY27" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BZ27" s="37" t="s">
+        <v>218</v>
+      </c>
       <c r="CA27" s="37"/>
       <c r="CB27" s="37"/>
       <c r="CC27" s="37"/>
@@ -18596,12 +18692,24 @@
       <c r="AV32" s="37"/>
       <c r="AW32" s="37"/>
       <c r="AX32" s="37"/>
-      <c r="AY32" s="37"/>
-      <c r="AZ32" s="37"/>
-      <c r="BA32" s="37"/>
-      <c r="BB32" s="37"/>
-      <c r="BC32" s="37"/>
-      <c r="BD32" s="37"/>
+      <c r="AY32" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AZ32" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BA32" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="BB32" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="BC32" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BD32" s="37" t="s">
+        <v>234</v>
+      </c>
       <c r="BE32" s="37"/>
       <c r="BF32" s="37"/>
       <c r="BG32" s="37"/>
@@ -18723,20 +18831,46 @@
       <c r="AR33" s="37"/>
       <c r="AS33" s="37"/>
       <c r="AT33" s="37"/>
-      <c r="AU33" s="37"/>
-      <c r="AV33" s="37"/>
-      <c r="AW33" s="37"/>
-      <c r="AX33" s="37"/>
-      <c r="AY33" s="37"/>
-      <c r="AZ33" s="37"/>
-      <c r="BA33" s="37"/>
+      <c r="AU33" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="AV33" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="AW33" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="AX33" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="AY33" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="AZ33" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="BA33" s="37" t="s">
+        <v>203</v>
+      </c>
       <c r="BB33" s="37"/>
-      <c r="BC33" s="37"/>
-      <c r="BD33" s="37"/>
-      <c r="BE33" s="37"/>
-      <c r="BF33" s="37"/>
-      <c r="BG33" s="37"/>
-      <c r="BH33" s="37"/>
+      <c r="BC33" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="BD33" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="BE33" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="BF33" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="BG33" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BH33" s="37" t="s">
+        <v>197</v>
+      </c>
       <c r="BI33" s="37"/>
       <c r="BJ33" s="37"/>
       <c r="BK33" s="37"/>
@@ -19322,18 +19456,40 @@
       <c r="X37" s="37"/>
       <c r="Y37" s="37"/>
       <c r="Z37" s="37"/>
-      <c r="AA37" s="37"/>
-      <c r="AB37" s="37"/>
-      <c r="AC37" s="37"/>
-      <c r="AD37" s="37"/>
-      <c r="AE37" s="37"/>
-      <c r="AF37" s="37"/>
-      <c r="AG37" s="37"/>
+      <c r="AA37" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB37" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD37" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AE37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF37" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG37" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="AH37" s="37"/>
-      <c r="AI37" s="37"/>
-      <c r="AJ37" s="37"/>
-      <c r="AK37" s="37"/>
-      <c r="AL37" s="37"/>
+      <c r="AI37" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AJ37" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="AK37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL37" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="AM37" s="37"/>
       <c r="AN37" s="37"/>
       <c r="AO37" s="37"/>
@@ -19345,18 +19501,40 @@
       <c r="AS37" s="37"/>
       <c r="AT37" s="37"/>
       <c r="AU37" s="37"/>
-      <c r="AV37" s="37"/>
-      <c r="AW37" s="37"/>
-      <c r="AX37" s="37"/>
-      <c r="AY37" s="37"/>
-      <c r="AZ37" s="37"/>
-      <c r="BA37" s="37"/>
-      <c r="BB37" s="37"/>
+      <c r="AV37" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW37" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AX37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AY37" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AZ37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BA37" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB37" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BC37" s="37"/>
-      <c r="BD37" s="37"/>
-      <c r="BE37" s="37"/>
-      <c r="BF37" s="37"/>
-      <c r="BG37" s="37"/>
+      <c r="BD37" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="BE37" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BF37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BG37" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BH37" s="37"/>
       <c r="BI37" s="37"/>
       <c r="BJ37" s="37"/>
@@ -19368,18 +19546,40 @@
       <c r="BN37" s="37"/>
       <c r="BO37" s="37"/>
       <c r="BP37" s="37"/>
-      <c r="BQ37" s="37"/>
-      <c r="BR37" s="37"/>
-      <c r="BS37" s="37"/>
-      <c r="BT37" s="37"/>
-      <c r="BU37" s="37"/>
-      <c r="BV37" s="37"/>
-      <c r="BW37" s="37"/>
+      <c r="BQ37" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BR37" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BS37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BT37" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="BU37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BV37" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BW37" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BX37" s="37"/>
-      <c r="BY37" s="37"/>
-      <c r="BZ37" s="37"/>
-      <c r="CA37" s="37"/>
-      <c r="CB37" s="37"/>
+      <c r="BY37" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="BZ37" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="CA37" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="CB37" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="CC37" s="37"/>
       <c r="CD37" s="37"/>
       <c r="CE37" s="37"/>
@@ -19446,16 +19646,36 @@
       <c r="Y38" s="37"/>
       <c r="Z38" s="37"/>
       <c r="AA38" s="37"/>
-      <c r="AB38" s="37"/>
-      <c r="AC38" s="37"/>
-      <c r="AD38" s="37"/>
-      <c r="AE38" s="37"/>
-      <c r="AF38" s="37"/>
-      <c r="AG38" s="37"/>
-      <c r="AH38" s="37"/>
-      <c r="AI38" s="37"/>
-      <c r="AJ38" s="37"/>
-      <c r="AK38" s="37"/>
+      <c r="AB38" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC38" s="37">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE38" s="37">
+        <v>2</v>
+      </c>
+      <c r="AF38" s="37">
+        <v>8</v>
+      </c>
+      <c r="AG38" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH38" s="37">
+        <v>2</v>
+      </c>
+      <c r="AI38" s="37">
+        <v>0</v>
+      </c>
+      <c r="AJ38" s="37">
+        <v>1</v>
+      </c>
+      <c r="AK38" s="37">
+        <v>5</v>
+      </c>
       <c r="AL38" s="37"/>
       <c r="AM38" s="37"/>
       <c r="AN38" s="37"/>
@@ -19469,16 +19689,36 @@
       <c r="AT38" s="37"/>
       <c r="AU38" s="37"/>
       <c r="AV38" s="37"/>
-      <c r="AW38" s="37"/>
-      <c r="AX38" s="37"/>
-      <c r="AY38" s="37"/>
-      <c r="AZ38" s="37"/>
-      <c r="BA38" s="37"/>
-      <c r="BB38" s="37"/>
-      <c r="BC38" s="37"/>
-      <c r="BD38" s="37"/>
-      <c r="BE38" s="37"/>
-      <c r="BF38" s="37"/>
+      <c r="AW38" s="37">
+        <v>1</v>
+      </c>
+      <c r="AX38" s="37">
+        <v>1</v>
+      </c>
+      <c r="AY38" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="AZ38" s="37">
+        <v>2</v>
+      </c>
+      <c r="BA38" s="37">
+        <v>8</v>
+      </c>
+      <c r="BB38" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="BC38" s="37">
+        <v>2</v>
+      </c>
+      <c r="BD38" s="37">
+        <v>0</v>
+      </c>
+      <c r="BE38" s="37">
+        <v>1</v>
+      </c>
+      <c r="BF38" s="37">
+        <v>5</v>
+      </c>
       <c r="BG38" s="37"/>
       <c r="BH38" s="37"/>
       <c r="BI38" s="37"/>
@@ -19492,16 +19732,36 @@
       <c r="BO38" s="37"/>
       <c r="BP38" s="37"/>
       <c r="BQ38" s="37"/>
-      <c r="BR38" s="37"/>
-      <c r="BS38" s="37"/>
-      <c r="BT38" s="37"/>
-      <c r="BU38" s="37"/>
-      <c r="BV38" s="37"/>
-      <c r="BW38" s="37"/>
-      <c r="BX38" s="37"/>
-      <c r="BY38" s="37"/>
-      <c r="BZ38" s="37"/>
-      <c r="CA38" s="37"/>
+      <c r="BR38" s="37">
+        <v>1</v>
+      </c>
+      <c r="BS38" s="37">
+        <v>1</v>
+      </c>
+      <c r="BT38" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="BU38" s="37">
+        <v>2</v>
+      </c>
+      <c r="BV38" s="37">
+        <v>8</v>
+      </c>
+      <c r="BW38" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="BX38" s="37">
+        <v>2</v>
+      </c>
+      <c r="BY38" s="37">
+        <v>0</v>
+      </c>
+      <c r="BZ38" s="37">
+        <v>1</v>
+      </c>
+      <c r="CA38" s="37">
+        <v>5</v>
+      </c>
       <c r="CB38" s="37"/>
       <c r="CC38" s="37"/>
       <c r="CD38" s="37"/>
@@ -19551,8 +19811,12 @@
       <c r="Y39" s="37"/>
       <c r="Z39" s="37"/>
       <c r="AA39" s="37"/>
-      <c r="AB39" s="37"/>
-      <c r="AC39" s="37"/>
+      <c r="AB39" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC39" s="37" t="s">
+        <v>209</v>
+      </c>
       <c r="AD39" s="37"/>
       <c r="AE39" s="37"/>
       <c r="AF39" s="37"/>
@@ -19577,8 +19841,12 @@
       <c r="AW39" s="37"/>
       <c r="AX39" s="37"/>
       <c r="AY39" s="37"/>
-      <c r="AZ39" s="37"/>
-      <c r="BA39" s="37"/>
+      <c r="AZ39" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="BA39" s="37" t="s">
+        <v>209</v>
+      </c>
       <c r="BB39" s="37"/>
       <c r="BC39" s="37"/>
       <c r="BD39" s="37"/>
@@ -19605,8 +19873,12 @@
       <c r="BW39" s="37"/>
       <c r="BX39" s="37"/>
       <c r="BY39" s="37"/>
-      <c r="BZ39" s="37"/>
-      <c r="CA39" s="37"/>
+      <c r="BZ39" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="CA39" s="37" t="s">
+        <v>209</v>
+      </c>
       <c r="CB39" s="37"/>
       <c r="CC39" s="37"/>
       <c r="CD39" s="37"/>
@@ -19646,19 +19918,41 @@
       <c r="W40" s="37"/>
       <c r="X40" s="37"/>
       <c r="Y40" s="37"/>
-      <c r="Z40" s="37"/>
-      <c r="AA40" s="37"/>
-      <c r="AB40" s="37"/>
+      <c r="Z40" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA40" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB40" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="AC40" s="37"/>
-      <c r="AD40" s="37"/>
-      <c r="AE40" s="37"/>
-      <c r="AF40" s="37"/>
+      <c r="AD40" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE40" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF40" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="AG40" s="37"/>
-      <c r="AH40" s="37"/>
-      <c r="AI40" s="37"/>
-      <c r="AJ40" s="37"/>
-      <c r="AK40" s="37"/>
-      <c r="AL40" s="37"/>
+      <c r="AH40" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI40" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="AJ40" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="AK40" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL40" s="37" t="s">
+        <v>235</v>
+      </c>
       <c r="AM40" s="37"/>
       <c r="AN40" s="37"/>
       <c r="AO40" s="37"/>
@@ -19670,17 +19964,35 @@
       <c r="AS40" s="37"/>
       <c r="AT40" s="37"/>
       <c r="AU40" s="37"/>
-      <c r="AV40" s="37"/>
-      <c r="AW40" s="37"/>
-      <c r="AX40" s="37"/>
+      <c r="AV40" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW40" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AX40" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="AY40" s="37"/>
-      <c r="AZ40" s="37"/>
-      <c r="BA40" s="37"/>
-      <c r="BB40" s="37"/>
+      <c r="AZ40" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BA40" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB40" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BC40" s="37"/>
-      <c r="BD40" s="37"/>
-      <c r="BE40" s="37"/>
-      <c r="BF40" s="37"/>
+      <c r="BD40" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="BE40" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BF40" s="37" t="s">
+        <v>218</v>
+      </c>
       <c r="BG40" s="37"/>
       <c r="BH40" s="37"/>
       <c r="BI40" s="37"/>
@@ -19692,18 +20004,38 @@
       <c r="BM40" s="37"/>
       <c r="BN40" s="37"/>
       <c r="BO40" s="37"/>
-      <c r="BP40" s="37"/>
-      <c r="BQ40" s="37"/>
-      <c r="BR40" s="37"/>
+      <c r="BP40" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BQ40" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BR40" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="BS40" s="37"/>
-      <c r="BT40" s="37"/>
-      <c r="BU40" s="37"/>
-      <c r="BV40" s="37"/>
+      <c r="BT40" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BU40" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BV40" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BW40" s="37"/>
-      <c r="BX40" s="37"/>
-      <c r="BY40" s="37"/>
-      <c r="BZ40" s="37"/>
-      <c r="CA40" s="37"/>
+      <c r="BX40" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="BY40" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BZ40" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="CA40" s="37" t="s">
+        <v>197</v>
+      </c>
       <c r="CB40" s="37"/>
       <c r="CC40" s="37"/>
       <c r="CD40" s="37"/>
@@ -19953,6 +20285,38 @@
       </c>
       <c r="CF41" s="39">
         <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="AW42">
+        <v>0</v>
+      </c>
+      <c r="AX42">
+        <v>1</v>
+      </c>
+      <c r="AY42">
+        <v>2</v>
+      </c>
+      <c r="AZ42">
+        <v>3</v>
+      </c>
+      <c r="BA42">
+        <v>4</v>
+      </c>
+      <c r="BB42">
+        <v>5</v>
+      </c>
+      <c r="BC42">
+        <v>6</v>
+      </c>
+      <c r="BD42">
+        <v>7</v>
+      </c>
+      <c r="BE42">
+        <v>8</v>
+      </c>
+      <c r="BF42">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got the 12 hour format for the time working somewhat.  The display of the AMPM indicator is not displaying accurately.  Also need to add 12 to the final number if it is PM before it is written to the RTC.  Need a overhaul on the LCDTimeDisplay function to get this working with the timer settings and the time display.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="328">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1386,7 +1386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1501,6 +1501,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12383,10 +12386,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG42"/>
+  <dimension ref="A1:CG51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z19" workbookViewId="0">
-      <selection activeCell="AY31" sqref="AY31"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="BR34" sqref="BR34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -18721,24 +18724,52 @@
         <v>0</v>
       </c>
       <c r="BM32" s="37"/>
-      <c r="BN32" s="37"/>
-      <c r="BO32" s="37"/>
+      <c r="BN32" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="BO32" s="37" t="s">
+        <v>206</v>
+      </c>
       <c r="BP32" s="37"/>
-      <c r="BQ32" s="37"/>
-      <c r="BR32" s="37"/>
-      <c r="BS32" s="37"/>
+      <c r="BQ32" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="BR32" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="BS32" s="37" t="s">
+        <v>207</v>
+      </c>
       <c r="BT32" s="37"/>
-      <c r="BU32" s="37"/>
-      <c r="BV32" s="37"/>
-      <c r="BW32" s="37"/>
-      <c r="BX32" s="37"/>
+      <c r="BU32" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="BV32" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BW32" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BX32" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="BY32" s="37"/>
-      <c r="BZ32" s="37"/>
-      <c r="CA32" s="37"/>
+      <c r="BZ32" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="CA32" s="37" t="s">
+        <v>206</v>
+      </c>
       <c r="CB32" s="37"/>
-      <c r="CC32" s="37"/>
-      <c r="CD32" s="37"/>
-      <c r="CE32" s="37"/>
+      <c r="CC32" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="CD32" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="CE32" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="CF32" s="37"/>
       <c r="CG32">
         <v>0</v>
@@ -18877,26 +18908,58 @@
       <c r="BL33">
         <v>1</v>
       </c>
-      <c r="BM33" s="37"/>
-      <c r="BN33" s="37"/>
-      <c r="BO33" s="37"/>
+      <c r="BM33" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BN33" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BO33" s="37" t="s">
+        <v>203</v>
+      </c>
       <c r="BP33" s="37"/>
-      <c r="BQ33" s="37"/>
-      <c r="BR33" s="37"/>
-      <c r="BS33" s="37"/>
-      <c r="BT33" s="37"/>
+      <c r="BQ33" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="BR33" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BS33" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BT33" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BU33" s="37"/>
-      <c r="BV33" s="37"/>
-      <c r="BW33" s="37"/>
-      <c r="BX33" s="37"/>
+      <c r="BV33" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="BW33" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BX33" s="37" t="s">
+        <v>203</v>
+      </c>
       <c r="BY33" s="37"/>
-      <c r="BZ33" s="37"/>
-      <c r="CA33" s="37"/>
-      <c r="CB33" s="37"/>
-      <c r="CC33" s="37"/>
+      <c r="BZ33" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="CA33" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="CB33" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="CC33" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="CD33" s="37"/>
-      <c r="CE33" s="37"/>
-      <c r="CF33" s="37"/>
+      <c r="CE33" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="CF33" s="37" t="s">
+        <v>206</v>
+      </c>
       <c r="CG33">
         <v>1</v>
       </c>
@@ -19001,48 +19064,84 @@
       <c r="AQ34">
         <v>2</v>
       </c>
-      <c r="AR34" s="37"/>
-      <c r="AS34" s="37"/>
-      <c r="AT34" s="37"/>
-      <c r="AU34" s="37"/>
-      <c r="AV34" s="37"/>
-      <c r="AW34" s="37"/>
-      <c r="AX34" s="37"/>
-      <c r="AY34" s="37"/>
-      <c r="AZ34" s="37"/>
-      <c r="BA34" s="37"/>
-      <c r="BB34" s="37"/>
-      <c r="BC34" s="37"/>
-      <c r="BD34" s="37"/>
-      <c r="BE34" s="37"/>
-      <c r="BF34" s="37"/>
-      <c r="BG34" s="37"/>
-      <c r="BH34" s="37"/>
-      <c r="BI34" s="37"/>
-      <c r="BJ34" s="37"/>
+      <c r="AR34" s="73"/>
+      <c r="AS34" s="73"/>
+      <c r="AT34" s="44"/>
+      <c r="AU34" s="44"/>
+      <c r="AV34" s="44"/>
+      <c r="AW34" s="44"/>
+      <c r="AX34" s="44"/>
+      <c r="AY34" s="44"/>
+      <c r="AZ34" s="44"/>
+      <c r="BA34" s="44"/>
+      <c r="BB34" s="44"/>
+      <c r="BC34" s="44"/>
+      <c r="BD34" s="44"/>
+      <c r="BE34" s="44"/>
+      <c r="BF34" s="44"/>
+      <c r="BG34" s="44"/>
+      <c r="BH34" s="44"/>
+      <c r="BI34" s="44"/>
+      <c r="BJ34" s="44"/>
       <c r="BK34" s="37"/>
       <c r="BL34">
         <v>2</v>
       </c>
-      <c r="BM34" s="37"/>
-      <c r="BN34" s="37"/>
-      <c r="BO34" s="37"/>
-      <c r="BP34" s="37"/>
-      <c r="BQ34" s="37"/>
-      <c r="BR34" s="37"/>
-      <c r="BS34" s="37"/>
-      <c r="BT34" s="37"/>
+      <c r="BM34" s="37">
+        <v>1</v>
+      </c>
+      <c r="BN34" s="37">
+        <v>2</v>
+      </c>
+      <c r="BO34" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="BP34" s="37">
+        <v>1</v>
+      </c>
+      <c r="BQ34" s="37">
+        <v>2</v>
+      </c>
+      <c r="BR34" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="BS34" s="37">
+        <v>1</v>
+      </c>
+      <c r="BT34" s="37">
+        <v>5</v>
+      </c>
       <c r="BU34" s="37"/>
-      <c r="BV34" s="37"/>
-      <c r="BW34" s="37"/>
-      <c r="BX34" s="37"/>
-      <c r="BY34" s="37"/>
-      <c r="BZ34" s="37"/>
-      <c r="CA34" s="37"/>
-      <c r="CB34" s="37"/>
-      <c r="CC34" s="37"/>
-      <c r="CD34" s="37"/>
-      <c r="CE34" s="37"/>
+      <c r="BV34" s="37">
+        <v>2</v>
+      </c>
+      <c r="BW34" s="37">
+        <v>3</v>
+      </c>
+      <c r="BX34" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="BY34" s="37">
+        <v>5</v>
+      </c>
+      <c r="BZ34" s="37">
+        <v>9</v>
+      </c>
+      <c r="CA34" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="CB34" s="37">
+        <v>3</v>
+      </c>
+      <c r="CC34" s="37">
+        <v>0</v>
+      </c>
+      <c r="CD34" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="CE34" s="37" t="s">
+        <v>200</v>
+      </c>
       <c r="CF34" s="37"/>
       <c r="CG34">
         <v>2</v>
@@ -19168,7 +19267,9 @@
       <c r="BS35" s="37"/>
       <c r="BT35" s="37"/>
       <c r="BU35" s="37"/>
-      <c r="BV35" s="37"/>
+      <c r="BV35" s="37" t="s">
+        <v>222</v>
+      </c>
       <c r="BW35" s="37"/>
       <c r="BX35" s="37"/>
       <c r="BY35" s="37"/>
@@ -19594,46 +19695,48 @@
       </c>
       <c r="B38" s="37"/>
       <c r="C38" s="37"/>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="F38" s="36" t="s">
+      <c r="F38" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="H38" s="36" t="s">
+      <c r="G38" s="37"/>
+      <c r="H38" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="I38" s="36" t="s">
+      <c r="I38" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="J38" s="36" t="s">
+      <c r="J38" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="K38" s="36" t="s">
+      <c r="K38" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="L38" s="36" t="s">
+      <c r="L38" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="M38" s="36" t="s">
+      <c r="M38" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="N38" s="36" t="s">
+      <c r="N38" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="P38" s="36" t="s">
+      <c r="O38" s="37"/>
+      <c r="P38" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="Q38" s="36" t="s">
+      <c r="Q38" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="R38" s="36" t="s">
+      <c r="R38" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="S38" s="36" t="s">
+      <c r="S38" s="37" t="s">
         <v>321</v>
       </c>
       <c r="T38" s="37"/>
@@ -20288,35 +20391,1529 @@
       </c>
     </row>
     <row r="42" spans="1:85" x14ac:dyDescent="0.35">
-      <c r="AW42">
-        <v>0</v>
-      </c>
-      <c r="AX42">
-        <v>1</v>
-      </c>
-      <c r="AY42">
-        <v>2</v>
-      </c>
-      <c r="AZ42">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="I42" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="J42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="K42" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="L42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="O42" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="P42" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="R42" s="37"/>
+      <c r="S42" s="37"/>
+      <c r="T42" s="37"/>
+      <c r="U42" s="37"/>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42" s="37"/>
+      <c r="X42" s="37"/>
+      <c r="Y42" s="37"/>
+      <c r="Z42" s="37"/>
+      <c r="AA42" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD42" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AE42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF42" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH42" s="37"/>
+      <c r="AI42" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ42" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="AK42" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AM42" s="37"/>
+      <c r="AN42" s="37"/>
+      <c r="AO42" s="37"/>
+      <c r="AP42" s="37"/>
+      <c r="AQ42">
+        <v>0</v>
+      </c>
+      <c r="AR42" s="37"/>
+      <c r="AS42" s="37"/>
+      <c r="AT42" s="37"/>
+      <c r="AU42" s="37"/>
+      <c r="AV42" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AX42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AY42" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AZ42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BA42" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BC42" s="37"/>
+      <c r="BD42" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="BE42" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="BF42" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="BG42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BH42" s="37"/>
+      <c r="BI42" s="37"/>
+      <c r="BJ42" s="37"/>
+      <c r="BK42" s="37"/>
+      <c r="BL42">
+        <v>0</v>
+      </c>
+      <c r="BM42" s="37"/>
+      <c r="BN42" s="37"/>
+      <c r="BO42" s="37"/>
+      <c r="BP42" s="37"/>
+      <c r="BQ42" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BR42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BS42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BT42" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="BU42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BV42" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BW42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BX42" s="37"/>
+      <c r="BY42" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="BZ42" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="CA42" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="CB42" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="CC42" s="37"/>
+      <c r="CD42" s="37"/>
+      <c r="CE42" s="37"/>
+      <c r="CF42" s="37"/>
+      <c r="CG42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37">
+        <v>1</v>
+      </c>
+      <c r="I43" s="38">
+        <v>2</v>
+      </c>
+      <c r="J43" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="K43" s="37">
         <v>3</v>
       </c>
-      <c r="BA42">
+      <c r="L43" s="38">
+        <v>0</v>
+      </c>
+      <c r="M43" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="N43" s="37">
+        <v>0</v>
+      </c>
+      <c r="O43" s="37">
+        <v>1</v>
+      </c>
+      <c r="P43" s="37"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="37"/>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37"/>
+      <c r="Y43" s="37"/>
+      <c r="Z43" s="37"/>
+      <c r="AA43" s="37"/>
+      <c r="AB43" s="37"/>
+      <c r="AC43" s="37">
+        <v>1</v>
+      </c>
+      <c r="AD43" s="38">
+        <v>2</v>
+      </c>
+      <c r="AE43" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF43" s="37">
+        <v>3</v>
+      </c>
+      <c r="AG43" s="38">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="AI43" s="37">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="37">
+        <v>1</v>
+      </c>
+      <c r="AK43" s="37"/>
+      <c r="AL43" s="37"/>
+      <c r="AM43" s="37"/>
+      <c r="AN43" s="37"/>
+      <c r="AO43" s="37"/>
+      <c r="AP43" s="37"/>
+      <c r="AQ43">
+        <v>1</v>
+      </c>
+      <c r="AR43" s="37"/>
+      <c r="AS43" s="37"/>
+      <c r="AT43" s="37"/>
+      <c r="AU43" s="37"/>
+      <c r="AV43" s="37"/>
+      <c r="AW43" s="37"/>
+      <c r="AX43" s="37">
+        <v>1</v>
+      </c>
+      <c r="AY43" s="38">
+        <v>2</v>
+      </c>
+      <c r="AZ43" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="BA43" s="37">
+        <v>3</v>
+      </c>
+      <c r="BB43" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC43" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="BD43" s="37">
+        <v>0</v>
+      </c>
+      <c r="BE43" s="37">
+        <v>1</v>
+      </c>
+      <c r="BF43" s="37"/>
+      <c r="BG43" s="37"/>
+      <c r="BH43" s="37"/>
+      <c r="BI43" s="37"/>
+      <c r="BJ43" s="37"/>
+      <c r="BK43" s="37"/>
+      <c r="BL43">
+        <v>1</v>
+      </c>
+      <c r="BM43" s="37"/>
+      <c r="BN43" s="37"/>
+      <c r="BO43" s="37"/>
+      <c r="BP43" s="37"/>
+      <c r="BQ43" s="37"/>
+      <c r="BR43" s="37">
+        <v>1</v>
+      </c>
+      <c r="BS43" s="37">
+        <v>1</v>
+      </c>
+      <c r="BT43" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="BU43" s="37">
+        <v>2</v>
+      </c>
+      <c r="BV43" s="37">
+        <v>8</v>
+      </c>
+      <c r="BW43" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="BX43" s="37">
+        <v>2</v>
+      </c>
+      <c r="BY43" s="37">
+        <v>0</v>
+      </c>
+      <c r="BZ43" s="37">
+        <v>1</v>
+      </c>
+      <c r="CA43" s="37">
+        <v>5</v>
+      </c>
+      <c r="CB43" s="37"/>
+      <c r="CC43" s="37"/>
+      <c r="CD43" s="37"/>
+      <c r="CE43" s="37"/>
+      <c r="CF43" s="37"/>
+      <c r="CG43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="I44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="37"/>
+      <c r="O44" s="37"/>
+      <c r="P44" s="37"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="37"/>
+      <c r="V44">
+        <v>2</v>
+      </c>
+      <c r="W44" s="37"/>
+      <c r="X44" s="37"/>
+      <c r="Y44" s="37"/>
+      <c r="Z44" s="37"/>
+      <c r="AA44" s="37"/>
+      <c r="AB44" s="37"/>
+      <c r="AC44" s="37"/>
+      <c r="AD44" s="37"/>
+      <c r="AE44" s="37"/>
+      <c r="AF44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AG44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH44" s="37"/>
+      <c r="AI44" s="37"/>
+      <c r="AJ44" s="37"/>
+      <c r="AK44" s="37"/>
+      <c r="AL44" s="37"/>
+      <c r="AM44" s="37"/>
+      <c r="AN44" s="37"/>
+      <c r="AO44" s="37"/>
+      <c r="AP44" s="37"/>
+      <c r="AQ44">
+        <v>2</v>
+      </c>
+      <c r="AR44" s="37"/>
+      <c r="AS44" s="37"/>
+      <c r="AT44" s="37"/>
+      <c r="AU44" s="37"/>
+      <c r="AV44" s="37"/>
+      <c r="AW44" s="37"/>
+      <c r="AX44" s="37"/>
+      <c r="AY44" s="37"/>
+      <c r="AZ44" s="37"/>
+      <c r="BA44" s="37"/>
+      <c r="BB44" s="37"/>
+      <c r="BC44" s="37"/>
+      <c r="BD44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="BE44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="BF44" s="37"/>
+      <c r="BG44" s="37"/>
+      <c r="BH44" s="37"/>
+      <c r="BI44" s="37"/>
+      <c r="BJ44" s="37"/>
+      <c r="BK44" s="37"/>
+      <c r="BL44">
+        <v>2</v>
+      </c>
+      <c r="BM44" s="37"/>
+      <c r="BN44" s="37"/>
+      <c r="BO44" s="37"/>
+      <c r="BP44" s="37"/>
+      <c r="BQ44" s="37"/>
+      <c r="BR44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="BS44" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="BT44" s="37"/>
+      <c r="BU44" s="37"/>
+      <c r="BV44" s="37"/>
+      <c r="BW44" s="37"/>
+      <c r="BX44" s="37"/>
+      <c r="BY44" s="37"/>
+      <c r="BZ44" s="37"/>
+      <c r="CA44" s="37"/>
+      <c r="CB44" s="37"/>
+      <c r="CC44" s="37"/>
+      <c r="CD44" s="37"/>
+      <c r="CE44" s="37"/>
+      <c r="CF44" s="37"/>
+      <c r="CG44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="G45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="H45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="K45" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="L45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="O45" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="P45" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q45" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45">
+        <v>3</v>
+      </c>
+      <c r="W45" s="37"/>
+      <c r="X45" s="37"/>
+      <c r="Y45" s="37"/>
+      <c r="Z45" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC45" s="37"/>
+      <c r="AD45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE45" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG45" s="37"/>
+      <c r="AH45" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI45" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="AJ45" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="AK45" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="AL45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AN45" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO45" s="37"/>
+      <c r="AP45" s="37"/>
+      <c r="AQ45">
+        <v>3</v>
+      </c>
+      <c r="AR45" s="37"/>
+      <c r="AS45" s="37"/>
+      <c r="AT45" s="37"/>
+      <c r="AU45" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AV45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AW45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AX45" s="37"/>
+      <c r="AY45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AZ45" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BA45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BB45" s="37"/>
+      <c r="BC45" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BD45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BE45" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="BF45" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="BG45" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BH45" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BI45" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="BJ45" s="37"/>
+      <c r="BK45" s="37"/>
+      <c r="BL45">
+        <v>3</v>
+      </c>
+      <c r="BM45" s="37"/>
+      <c r="BN45" s="37"/>
+      <c r="BO45" s="37"/>
+      <c r="BP45" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BQ45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BR45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BS45" s="37"/>
+      <c r="BT45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BU45" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BV45" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BW45" s="37"/>
+      <c r="BX45" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="BY45" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="BZ45" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="CA45" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="CB45" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="CC45" s="37"/>
+      <c r="CD45" s="37"/>
+      <c r="CE45" s="37"/>
+      <c r="CF45" s="37"/>
+      <c r="CG45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:85" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B46" s="39">
+        <v>0</v>
+      </c>
+      <c r="C46" s="39">
+        <v>1</v>
+      </c>
+      <c r="D46" s="39">
+        <v>2</v>
+      </c>
+      <c r="E46" s="39">
+        <v>3</v>
+      </c>
+      <c r="F46" s="39">
         <v>4</v>
       </c>
-      <c r="BB42">
+      <c r="G46" s="39">
         <v>5</v>
       </c>
-      <c r="BC42">
+      <c r="H46" s="39">
         <v>6</v>
       </c>
-      <c r="BD42">
+      <c r="I46" s="39">
         <v>7</v>
       </c>
-      <c r="BE42">
+      <c r="J46" s="39">
         <v>8</v>
       </c>
-      <c r="BF42">
+      <c r="K46" s="39">
         <v>9</v>
+      </c>
+      <c r="L46" s="39">
+        <v>10</v>
+      </c>
+      <c r="M46" s="39">
+        <v>11</v>
+      </c>
+      <c r="N46" s="39">
+        <v>12</v>
+      </c>
+      <c r="O46" s="39">
+        <v>13</v>
+      </c>
+      <c r="P46" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q46" s="39">
+        <v>15</v>
+      </c>
+      <c r="R46" s="39">
+        <v>16</v>
+      </c>
+      <c r="S46" s="39">
+        <v>17</v>
+      </c>
+      <c r="T46" s="39">
+        <v>18</v>
+      </c>
+      <c r="U46" s="39">
+        <v>19</v>
+      </c>
+      <c r="W46" s="39">
+        <v>0</v>
+      </c>
+      <c r="X46" s="39">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="39">
+        <v>2</v>
+      </c>
+      <c r="Z46" s="39">
+        <v>3</v>
+      </c>
+      <c r="AA46" s="39">
+        <v>4</v>
+      </c>
+      <c r="AB46" s="39">
+        <v>5</v>
+      </c>
+      <c r="AC46" s="39">
+        <v>6</v>
+      </c>
+      <c r="AD46" s="39">
+        <v>7</v>
+      </c>
+      <c r="AE46" s="39">
+        <v>8</v>
+      </c>
+      <c r="AF46" s="39">
+        <v>9</v>
+      </c>
+      <c r="AG46" s="39">
+        <v>10</v>
+      </c>
+      <c r="AH46" s="39">
+        <v>11</v>
+      </c>
+      <c r="AI46" s="39">
+        <v>12</v>
+      </c>
+      <c r="AJ46" s="39">
+        <v>13</v>
+      </c>
+      <c r="AK46" s="39">
+        <v>14</v>
+      </c>
+      <c r="AL46" s="39">
+        <v>15</v>
+      </c>
+      <c r="AM46" s="39">
+        <v>16</v>
+      </c>
+      <c r="AN46" s="39">
+        <v>17</v>
+      </c>
+      <c r="AO46" s="39">
+        <v>18</v>
+      </c>
+      <c r="AP46" s="39">
+        <v>19</v>
+      </c>
+      <c r="AR46" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS46" s="39">
+        <v>1</v>
+      </c>
+      <c r="AT46" s="39">
+        <v>2</v>
+      </c>
+      <c r="AU46" s="39">
+        <v>3</v>
+      </c>
+      <c r="AV46" s="39">
+        <v>4</v>
+      </c>
+      <c r="AW46" s="39">
+        <v>5</v>
+      </c>
+      <c r="AX46" s="39">
+        <v>6</v>
+      </c>
+      <c r="AY46" s="39">
+        <v>7</v>
+      </c>
+      <c r="AZ46" s="39">
+        <v>8</v>
+      </c>
+      <c r="BA46" s="39">
+        <v>9</v>
+      </c>
+      <c r="BB46" s="39">
+        <v>10</v>
+      </c>
+      <c r="BC46" s="39">
+        <v>11</v>
+      </c>
+      <c r="BD46" s="39">
+        <v>12</v>
+      </c>
+      <c r="BE46" s="39">
+        <v>13</v>
+      </c>
+      <c r="BF46" s="39">
+        <v>14</v>
+      </c>
+      <c r="BG46" s="39">
+        <v>15</v>
+      </c>
+      <c r="BH46" s="39">
+        <v>16</v>
+      </c>
+      <c r="BI46" s="39">
+        <v>17</v>
+      </c>
+      <c r="BJ46" s="39">
+        <v>18</v>
+      </c>
+      <c r="BK46" s="39">
+        <v>19</v>
+      </c>
+      <c r="BM46" s="39">
+        <v>0</v>
+      </c>
+      <c r="BN46" s="39">
+        <v>1</v>
+      </c>
+      <c r="BO46" s="39">
+        <v>2</v>
+      </c>
+      <c r="BP46" s="39">
+        <v>3</v>
+      </c>
+      <c r="BQ46" s="39">
+        <v>4</v>
+      </c>
+      <c r="BR46" s="39">
+        <v>5</v>
+      </c>
+      <c r="BS46" s="39">
+        <v>6</v>
+      </c>
+      <c r="BT46" s="39">
+        <v>7</v>
+      </c>
+      <c r="BU46" s="39">
+        <v>8</v>
+      </c>
+      <c r="BV46" s="39">
+        <v>9</v>
+      </c>
+      <c r="BW46" s="39">
+        <v>10</v>
+      </c>
+      <c r="BX46" s="39">
+        <v>11</v>
+      </c>
+      <c r="BY46" s="39">
+        <v>12</v>
+      </c>
+      <c r="BZ46" s="39">
+        <v>13</v>
+      </c>
+      <c r="CA46" s="39">
+        <v>14</v>
+      </c>
+      <c r="CB46" s="39">
+        <v>15</v>
+      </c>
+      <c r="CC46" s="39">
+        <v>16</v>
+      </c>
+      <c r="CD46" s="39">
+        <v>17</v>
+      </c>
+      <c r="CE46" s="39">
+        <v>18</v>
+      </c>
+      <c r="CF46" s="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37"/>
+      <c r="U47" s="37"/>
+      <c r="V47">
+        <v>0</v>
+      </c>
+      <c r="W47" s="37"/>
+      <c r="X47" s="37"/>
+      <c r="Y47" s="37"/>
+      <c r="Z47" s="37"/>
+      <c r="AA47" s="37"/>
+      <c r="AB47" s="37"/>
+      <c r="AC47" s="37"/>
+      <c r="AD47" s="37"/>
+      <c r="AE47" s="37"/>
+      <c r="AF47" s="37"/>
+      <c r="AG47" s="37"/>
+      <c r="AH47" s="37"/>
+      <c r="AI47" s="37"/>
+      <c r="AJ47" s="37"/>
+      <c r="AK47" s="37"/>
+      <c r="AL47" s="37"/>
+      <c r="AM47" s="37"/>
+      <c r="AN47" s="37"/>
+      <c r="AO47" s="37"/>
+      <c r="AP47" s="37"/>
+      <c r="AQ47">
+        <v>0</v>
+      </c>
+      <c r="AR47" s="37"/>
+      <c r="AS47" s="37"/>
+      <c r="AT47" s="37"/>
+      <c r="AU47" s="37"/>
+      <c r="AV47" s="37"/>
+      <c r="AW47" s="37"/>
+      <c r="AX47" s="37"/>
+      <c r="AY47" s="37"/>
+      <c r="AZ47" s="37"/>
+      <c r="BA47" s="37"/>
+      <c r="BB47" s="37"/>
+      <c r="BC47" s="37"/>
+      <c r="BD47" s="37"/>
+      <c r="BE47" s="37"/>
+      <c r="BF47" s="37"/>
+      <c r="BG47" s="37"/>
+      <c r="BH47" s="37"/>
+      <c r="BI47" s="37"/>
+      <c r="BJ47" s="37"/>
+      <c r="BK47" s="37"/>
+      <c r="BL47">
+        <v>0</v>
+      </c>
+      <c r="BM47" s="37"/>
+      <c r="BN47" s="37"/>
+      <c r="BO47" s="37"/>
+      <c r="BP47" s="37"/>
+      <c r="BQ47" s="37"/>
+      <c r="BR47" s="37"/>
+      <c r="BS47" s="37"/>
+      <c r="BT47" s="37"/>
+      <c r="BU47" s="37"/>
+      <c r="BV47" s="37"/>
+      <c r="BW47" s="37"/>
+      <c r="BX47" s="37"/>
+      <c r="BY47" s="37"/>
+      <c r="BZ47" s="37"/>
+      <c r="CA47" s="37"/>
+      <c r="CB47" s="37"/>
+      <c r="CC47" s="37"/>
+      <c r="CD47" s="37"/>
+      <c r="CE47" s="37"/>
+      <c r="CF47" s="37"/>
+      <c r="CG47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="37"/>
+      <c r="U48" s="37"/>
+      <c r="V48">
+        <v>1</v>
+      </c>
+      <c r="W48" s="37"/>
+      <c r="X48" s="37"/>
+      <c r="Y48" s="37"/>
+      <c r="Z48" s="37"/>
+      <c r="AA48" s="37"/>
+      <c r="AB48" s="37"/>
+      <c r="AC48" s="37"/>
+      <c r="AD48" s="38"/>
+      <c r="AE48" s="37"/>
+      <c r="AF48" s="37"/>
+      <c r="AG48" s="38"/>
+      <c r="AH48" s="37"/>
+      <c r="AI48" s="37"/>
+      <c r="AJ48" s="37"/>
+      <c r="AK48" s="37"/>
+      <c r="AL48" s="37"/>
+      <c r="AM48" s="37"/>
+      <c r="AN48" s="37"/>
+      <c r="AO48" s="37"/>
+      <c r="AP48" s="37"/>
+      <c r="AQ48">
+        <v>1</v>
+      </c>
+      <c r="AR48" s="37"/>
+      <c r="AS48" s="37"/>
+      <c r="AT48" s="37"/>
+      <c r="AU48" s="37"/>
+      <c r="AV48" s="37"/>
+      <c r="AW48" s="37"/>
+      <c r="AX48" s="37"/>
+      <c r="AY48" s="38"/>
+      <c r="AZ48" s="37"/>
+      <c r="BA48" s="37"/>
+      <c r="BB48" s="38"/>
+      <c r="BC48" s="37"/>
+      <c r="BD48" s="37"/>
+      <c r="BE48" s="37"/>
+      <c r="BF48" s="37"/>
+      <c r="BG48" s="37"/>
+      <c r="BH48" s="37"/>
+      <c r="BI48" s="37"/>
+      <c r="BJ48" s="37"/>
+      <c r="BK48" s="37"/>
+      <c r="BL48">
+        <v>1</v>
+      </c>
+      <c r="BM48" s="37"/>
+      <c r="BN48" s="37"/>
+      <c r="BO48" s="37"/>
+      <c r="BP48" s="37"/>
+      <c r="BQ48" s="37"/>
+      <c r="BR48" s="37"/>
+      <c r="BS48" s="37"/>
+      <c r="BT48" s="38"/>
+      <c r="BU48" s="37"/>
+      <c r="BV48" s="37"/>
+      <c r="BW48" s="38"/>
+      <c r="BX48" s="37"/>
+      <c r="BY48" s="37"/>
+      <c r="BZ48" s="37"/>
+      <c r="CA48" s="37"/>
+      <c r="CB48" s="37"/>
+      <c r="CC48" s="37"/>
+      <c r="CD48" s="37"/>
+      <c r="CE48" s="37"/>
+      <c r="CF48" s="37"/>
+      <c r="CG48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37"/>
+      <c r="U49" s="37"/>
+      <c r="V49">
+        <v>2</v>
+      </c>
+      <c r="W49" s="37"/>
+      <c r="X49" s="37"/>
+      <c r="Y49" s="37"/>
+      <c r="Z49" s="37"/>
+      <c r="AA49" s="37"/>
+      <c r="AB49" s="37"/>
+      <c r="AC49" s="37"/>
+      <c r="AD49" s="37"/>
+      <c r="AE49" s="37"/>
+      <c r="AF49" s="37"/>
+      <c r="AG49" s="37"/>
+      <c r="AH49" s="37"/>
+      <c r="AI49" s="37"/>
+      <c r="AJ49" s="37"/>
+      <c r="AK49" s="37"/>
+      <c r="AL49" s="37"/>
+      <c r="AM49" s="37"/>
+      <c r="AN49" s="37"/>
+      <c r="AO49" s="37"/>
+      <c r="AP49" s="37"/>
+      <c r="AQ49">
+        <v>2</v>
+      </c>
+      <c r="AR49" s="37"/>
+      <c r="AS49" s="37"/>
+      <c r="AT49" s="37"/>
+      <c r="AU49" s="37"/>
+      <c r="AV49" s="37"/>
+      <c r="AW49" s="37"/>
+      <c r="AX49" s="37"/>
+      <c r="AY49" s="37"/>
+      <c r="AZ49" s="37"/>
+      <c r="BA49" s="37"/>
+      <c r="BB49" s="37"/>
+      <c r="BC49" s="37"/>
+      <c r="BD49" s="37"/>
+      <c r="BE49" s="37"/>
+      <c r="BF49" s="37"/>
+      <c r="BG49" s="37"/>
+      <c r="BH49" s="37"/>
+      <c r="BI49" s="37"/>
+      <c r="BJ49" s="37"/>
+      <c r="BK49" s="37"/>
+      <c r="BL49">
+        <v>2</v>
+      </c>
+      <c r="BM49" s="37"/>
+      <c r="BN49" s="37"/>
+      <c r="BO49" s="37"/>
+      <c r="BP49" s="37"/>
+      <c r="BQ49" s="37"/>
+      <c r="BR49" s="37"/>
+      <c r="BS49" s="37"/>
+      <c r="BT49" s="37"/>
+      <c r="BU49" s="37"/>
+      <c r="BV49" s="37"/>
+      <c r="BW49" s="37"/>
+      <c r="BX49" s="37"/>
+      <c r="BY49" s="37"/>
+      <c r="BZ49" s="37"/>
+      <c r="CA49" s="37"/>
+      <c r="CB49" s="37"/>
+      <c r="CC49" s="37"/>
+      <c r="CD49" s="37"/>
+      <c r="CE49" s="37"/>
+      <c r="CF49" s="37"/>
+      <c r="CG49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="37"/>
+      <c r="U50" s="37"/>
+      <c r="V50">
+        <v>3</v>
+      </c>
+      <c r="W50" s="37"/>
+      <c r="X50" s="37"/>
+      <c r="Y50" s="37"/>
+      <c r="Z50" s="37"/>
+      <c r="AA50" s="37"/>
+      <c r="AB50" s="37"/>
+      <c r="AC50" s="37"/>
+      <c r="AD50" s="37"/>
+      <c r="AE50" s="37"/>
+      <c r="AF50" s="37"/>
+      <c r="AG50" s="37"/>
+      <c r="AH50" s="37"/>
+      <c r="AI50" s="37"/>
+      <c r="AJ50" s="37"/>
+      <c r="AK50" s="37"/>
+      <c r="AL50" s="37"/>
+      <c r="AM50" s="37"/>
+      <c r="AN50" s="37"/>
+      <c r="AO50" s="37"/>
+      <c r="AP50" s="37"/>
+      <c r="AQ50">
+        <v>3</v>
+      </c>
+      <c r="AR50" s="37"/>
+      <c r="AS50" s="37"/>
+      <c r="AT50" s="37"/>
+      <c r="AU50" s="37"/>
+      <c r="AV50" s="37"/>
+      <c r="AW50" s="37"/>
+      <c r="AX50" s="37"/>
+      <c r="AY50" s="37"/>
+      <c r="AZ50" s="37"/>
+      <c r="BA50" s="37"/>
+      <c r="BB50" s="37"/>
+      <c r="BC50" s="37"/>
+      <c r="BD50" s="37"/>
+      <c r="BE50" s="37"/>
+      <c r="BF50" s="37"/>
+      <c r="BG50" s="37"/>
+      <c r="BH50" s="37"/>
+      <c r="BI50" s="37"/>
+      <c r="BJ50" s="37"/>
+      <c r="BK50" s="37"/>
+      <c r="BL50">
+        <v>3</v>
+      </c>
+      <c r="BM50" s="37"/>
+      <c r="BN50" s="37"/>
+      <c r="BO50" s="37"/>
+      <c r="BP50" s="37"/>
+      <c r="BQ50" s="37"/>
+      <c r="BR50" s="37"/>
+      <c r="BS50" s="37"/>
+      <c r="BT50" s="37"/>
+      <c r="BU50" s="37"/>
+      <c r="BV50" s="37"/>
+      <c r="BW50" s="37"/>
+      <c r="BX50" s="37"/>
+      <c r="BY50" s="37"/>
+      <c r="BZ50" s="37"/>
+      <c r="CA50" s="37"/>
+      <c r="CB50" s="37"/>
+      <c r="CC50" s="37"/>
+      <c r="CD50" s="37"/>
+      <c r="CE50" s="37"/>
+      <c r="CF50" s="37"/>
+      <c r="CG50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:85" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B51" s="39">
+        <v>0</v>
+      </c>
+      <c r="C51" s="39">
+        <v>1</v>
+      </c>
+      <c r="D51" s="39">
+        <v>2</v>
+      </c>
+      <c r="E51" s="39">
+        <v>3</v>
+      </c>
+      <c r="F51" s="39">
+        <v>4</v>
+      </c>
+      <c r="G51" s="39">
+        <v>5</v>
+      </c>
+      <c r="H51" s="39">
+        <v>6</v>
+      </c>
+      <c r="I51" s="39">
+        <v>7</v>
+      </c>
+      <c r="J51" s="39">
+        <v>8</v>
+      </c>
+      <c r="K51" s="39">
+        <v>9</v>
+      </c>
+      <c r="L51" s="39">
+        <v>10</v>
+      </c>
+      <c r="M51" s="39">
+        <v>11</v>
+      </c>
+      <c r="N51" s="39">
+        <v>12</v>
+      </c>
+      <c r="O51" s="39">
+        <v>13</v>
+      </c>
+      <c r="P51" s="39">
+        <v>14</v>
+      </c>
+      <c r="Q51" s="39">
+        <v>15</v>
+      </c>
+      <c r="R51" s="39">
+        <v>16</v>
+      </c>
+      <c r="S51" s="39">
+        <v>17</v>
+      </c>
+      <c r="T51" s="39">
+        <v>18</v>
+      </c>
+      <c r="U51" s="39">
+        <v>19</v>
+      </c>
+      <c r="W51" s="39">
+        <v>0</v>
+      </c>
+      <c r="X51" s="39">
+        <v>1</v>
+      </c>
+      <c r="Y51" s="39">
+        <v>2</v>
+      </c>
+      <c r="Z51" s="39">
+        <v>3</v>
+      </c>
+      <c r="AA51" s="39">
+        <v>4</v>
+      </c>
+      <c r="AB51" s="39">
+        <v>5</v>
+      </c>
+      <c r="AC51" s="39">
+        <v>6</v>
+      </c>
+      <c r="AD51" s="39">
+        <v>7</v>
+      </c>
+      <c r="AE51" s="39">
+        <v>8</v>
+      </c>
+      <c r="AF51" s="39">
+        <v>9</v>
+      </c>
+      <c r="AG51" s="39">
+        <v>10</v>
+      </c>
+      <c r="AH51" s="39">
+        <v>11</v>
+      </c>
+      <c r="AI51" s="39">
+        <v>12</v>
+      </c>
+      <c r="AJ51" s="39">
+        <v>13</v>
+      </c>
+      <c r="AK51" s="39">
+        <v>14</v>
+      </c>
+      <c r="AL51" s="39">
+        <v>15</v>
+      </c>
+      <c r="AM51" s="39">
+        <v>16</v>
+      </c>
+      <c r="AN51" s="39">
+        <v>17</v>
+      </c>
+      <c r="AO51" s="39">
+        <v>18</v>
+      </c>
+      <c r="AP51" s="39">
+        <v>19</v>
+      </c>
+      <c r="AR51" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS51" s="39">
+        <v>1</v>
+      </c>
+      <c r="AT51" s="39">
+        <v>2</v>
+      </c>
+      <c r="AU51" s="39">
+        <v>3</v>
+      </c>
+      <c r="AV51" s="39">
+        <v>4</v>
+      </c>
+      <c r="AW51" s="39">
+        <v>5</v>
+      </c>
+      <c r="AX51" s="39">
+        <v>6</v>
+      </c>
+      <c r="AY51" s="39">
+        <v>7</v>
+      </c>
+      <c r="AZ51" s="39">
+        <v>8</v>
+      </c>
+      <c r="BA51" s="39">
+        <v>9</v>
+      </c>
+      <c r="BB51" s="39">
+        <v>10</v>
+      </c>
+      <c r="BC51" s="39">
+        <v>11</v>
+      </c>
+      <c r="BD51" s="39">
+        <v>12</v>
+      </c>
+      <c r="BE51" s="39">
+        <v>13</v>
+      </c>
+      <c r="BF51" s="39">
+        <v>14</v>
+      </c>
+      <c r="BG51" s="39">
+        <v>15</v>
+      </c>
+      <c r="BH51" s="39">
+        <v>16</v>
+      </c>
+      <c r="BI51" s="39">
+        <v>17</v>
+      </c>
+      <c r="BJ51" s="39">
+        <v>18</v>
+      </c>
+      <c r="BK51" s="39">
+        <v>19</v>
+      </c>
+      <c r="BM51" s="39">
+        <v>0</v>
+      </c>
+      <c r="BN51" s="39">
+        <v>1</v>
+      </c>
+      <c r="BO51" s="39">
+        <v>2</v>
+      </c>
+      <c r="BP51" s="39">
+        <v>3</v>
+      </c>
+      <c r="BQ51" s="39">
+        <v>4</v>
+      </c>
+      <c r="BR51" s="39">
+        <v>5</v>
+      </c>
+      <c r="BS51" s="39">
+        <v>6</v>
+      </c>
+      <c r="BT51" s="39">
+        <v>7</v>
+      </c>
+      <c r="BU51" s="39">
+        <v>8</v>
+      </c>
+      <c r="BV51" s="39">
+        <v>9</v>
+      </c>
+      <c r="BW51" s="39">
+        <v>10</v>
+      </c>
+      <c r="BX51" s="39">
+        <v>11</v>
+      </c>
+      <c r="BY51" s="39">
+        <v>12</v>
+      </c>
+      <c r="BZ51" s="39">
+        <v>13</v>
+      </c>
+      <c r="CA51" s="39">
+        <v>14</v>
+      </c>
+      <c r="CB51" s="39">
+        <v>15</v>
+      </c>
+      <c r="CC51" s="39">
+        <v>16</v>
+      </c>
+      <c r="CD51" s="39">
+        <v>17</v>
+      </c>
+      <c r="CE51" s="39">
+        <v>18</v>
+      </c>
+      <c r="CF51" s="39">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in the variables tempReadC[] and temReadF[] to have store the temperature readings outside the DS18B20_Read function.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Robbie</author>
+  </authors>
+  <commentList>
+    <comment ref="J55" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Robbie:
+AMPM will start here.  Will use the modifier "space" to add spaces here.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="338">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1010,13 +1035,43 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Column + 3</t>
+  </si>
+  <si>
+    <t>Column + 6</t>
+  </si>
+  <si>
+    <t>Column + 8</t>
+  </si>
+  <si>
+    <t>No Seconds</t>
+  </si>
+  <si>
+    <t>APM Display</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>APM w/Seconds</t>
+  </si>
+  <si>
+    <t>LCDTimeDisplay display variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1072,6 +1127,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1386,7 +1448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1469,6 +1531,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1502,8 +1567,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1824,12 +1895,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="A1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" t="s">
         <v>96</v>
       </c>
@@ -1992,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,12 +2077,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" t="s">
         <v>95</v>
       </c>
@@ -2218,13 +2289,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="19" t="s">
         <v>108</v>
       </c>
@@ -2254,7 +2325,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="66"/>
+      <c r="A3" s="67"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -2275,7 +2346,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="67"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -2296,7 +2367,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="64" t="s">
         <v>176</v>
       </c>
       <c r="B5" s="25">
@@ -2319,7 +2390,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -2340,7 +2411,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="64"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -2361,7 +2432,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="64"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -2382,7 +2453,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -2403,7 +2474,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="65"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -2424,7 +2495,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="64" t="s">
         <v>177</v>
       </c>
       <c r="B11" s="25">
@@ -2447,7 +2518,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="64"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -2468,7 +2539,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -2489,7 +2560,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -2510,7 +2581,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -2531,7 +2602,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="65"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -2552,7 +2623,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="64" t="s">
         <v>178</v>
       </c>
       <c r="B17" s="29">
@@ -2575,7 +2646,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -2596,7 +2667,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -2617,7 +2688,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -2638,7 +2709,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -2659,7 +2730,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="65"/>
+      <c r="A22" s="66"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -2680,7 +2751,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="64" t="s">
         <v>179</v>
       </c>
       <c r="B23" s="25">
@@ -2703,7 +2774,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="64"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -2724,7 +2795,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="64"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -2745,7 +2816,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -2766,7 +2837,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="64"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -2787,7 +2858,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="65"/>
+      <c r="A28" s="66"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -2808,7 +2879,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="64" t="s">
         <v>180</v>
       </c>
       <c r="B29" s="29">
@@ -2831,7 +2902,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="64"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -2852,7 +2923,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="64"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -2873,7 +2944,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="64"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -2894,7 +2965,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="64"/>
+      <c r="A33" s="65"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -2915,7 +2986,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="65"/>
+      <c r="A34" s="66"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -2936,7 +3007,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="64" t="s">
         <v>181</v>
       </c>
       <c r="B35" s="25">
@@ -2959,7 +3030,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="64"/>
+      <c r="A36" s="65"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -2980,7 +3051,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="64"/>
+      <c r="A37" s="65"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -3001,7 +3072,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="64"/>
+      <c r="A38" s="65"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -3022,7 +3093,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="64"/>
+      <c r="A39" s="65"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -3043,7 +3114,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="65"/>
+      <c r="A40" s="66"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -3064,7 +3135,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="63" t="s">
+      <c r="A41" s="64" t="s">
         <v>182</v>
       </c>
       <c r="B41" s="29">
@@ -3087,7 +3158,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="64"/>
+      <c r="A42" s="65"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -3108,7 +3179,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="64"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -3129,7 +3200,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="64"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -3150,7 +3221,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="64"/>
+      <c r="A45" s="65"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -3171,7 +3242,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="65"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -3192,7 +3263,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="63" t="s">
+      <c r="A47" s="64" t="s">
         <v>183</v>
       </c>
       <c r="B47" s="25">
@@ -3215,7 +3286,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="64"/>
+      <c r="A48" s="65"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -3236,7 +3307,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="64"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -3257,7 +3328,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="64"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -3278,7 +3349,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="64"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -3299,7 +3370,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="65"/>
+      <c r="A52" s="66"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -3358,8 +3429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z267"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4425,6 +4496,9 @@
         <f t="shared" si="2"/>
         <v>1110</v>
       </c>
+      <c r="M26" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27">
@@ -4458,6 +4532,12 @@
         <f t="shared" si="2"/>
         <v>1111</v>
       </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28">
@@ -4491,6 +4571,9 @@
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29">
@@ -4524,6 +4607,9 @@
         <f t="shared" si="2"/>
         <v>10001</v>
       </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30">
@@ -4557,6 +4643,9 @@
         <f t="shared" si="2"/>
         <v>10010</v>
       </c>
+      <c r="M30">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31">
@@ -4590,6 +4679,10 @@
         <f t="shared" si="2"/>
         <v>10011</v>
       </c>
+      <c r="M31">
+        <v>8</v>
+      </c>
+      <c r="N31" s="58"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32">
@@ -4623,8 +4716,11 @@
         <f t="shared" si="2"/>
         <v>10100</v>
       </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>0</v>
       </c>
@@ -4656,8 +4752,11 @@
         <f t="shared" si="2"/>
         <v>10101</v>
       </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>0</v>
       </c>
@@ -4689,8 +4788,11 @@
         <f t="shared" si="2"/>
         <v>10110</v>
       </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M34">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>0</v>
       </c>
@@ -4722,8 +4824,11 @@
         <f t="shared" si="2"/>
         <v>10111</v>
       </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>0</v>
       </c>
@@ -4755,8 +4860,11 @@
         <f t="shared" si="2"/>
         <v>11000</v>
       </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>0</v>
       </c>
@@ -4789,7 +4897,7 @@
         <v>11001</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>0</v>
       </c>
@@ -4822,7 +4930,7 @@
         <v>11010</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>0</v>
       </c>
@@ -4855,7 +4963,7 @@
         <v>11011</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>0</v>
       </c>
@@ -4888,7 +4996,7 @@
         <v>11100</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>0</v>
       </c>
@@ -4921,7 +5029,7 @@
         <v>11101</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>0</v>
       </c>
@@ -4954,7 +5062,7 @@
         <v>11110</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>0</v>
       </c>
@@ -4987,7 +5095,7 @@
         <v>11111</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>0</v>
       </c>
@@ -5020,7 +5128,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>0</v>
       </c>
@@ -5053,7 +5161,7 @@
         <v>100001</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>0</v>
       </c>
@@ -5086,7 +5194,7 @@
         <v>100010</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>0</v>
       </c>
@@ -5119,7 +5227,7 @@
         <v>100011</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>0</v>
       </c>
@@ -12385,11 +12493,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="BR34" sqref="BR34"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="X55" sqref="X55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -19064,8 +19172,8 @@
       <c r="AQ34">
         <v>2</v>
       </c>
-      <c r="AR34" s="73"/>
-      <c r="AS34" s="73"/>
+      <c r="AR34" s="62"/>
+      <c r="AS34" s="62"/>
       <c r="AT34" s="44"/>
       <c r="AU34" s="44"/>
       <c r="AV34" s="44"/>
@@ -20533,40 +20641,18 @@
       <c r="BN42" s="37"/>
       <c r="BO42" s="37"/>
       <c r="BP42" s="37"/>
-      <c r="BQ42" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="BR42" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="BS42" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="BT42" s="37" t="s">
-        <v>323</v>
-      </c>
-      <c r="BU42" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="BV42" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="BW42" s="37" t="s">
-        <v>192</v>
-      </c>
+      <c r="BQ42" s="37"/>
+      <c r="BR42" s="37"/>
+      <c r="BS42" s="37"/>
+      <c r="BT42" s="37"/>
+      <c r="BU42" s="37"/>
+      <c r="BV42" s="37"/>
+      <c r="BW42" s="37"/>
       <c r="BX42" s="37"/>
-      <c r="BY42" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="BZ42" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="CA42" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB42" s="37" t="s">
-        <v>192</v>
-      </c>
+      <c r="BY42" s="37"/>
+      <c r="BZ42" s="37"/>
+      <c r="CA42" s="37"/>
+      <c r="CB42" s="37"/>
       <c r="CC42" s="37"/>
       <c r="CD42" s="37"/>
       <c r="CE42" s="37"/>
@@ -20701,36 +20787,16 @@
       <c r="BO43" s="37"/>
       <c r="BP43" s="37"/>
       <c r="BQ43" s="37"/>
-      <c r="BR43" s="37">
-        <v>1</v>
-      </c>
-      <c r="BS43" s="37">
-        <v>1</v>
-      </c>
-      <c r="BT43" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="BU43" s="37">
-        <v>2</v>
-      </c>
-      <c r="BV43" s="37">
-        <v>8</v>
-      </c>
-      <c r="BW43" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="BX43" s="37">
-        <v>2</v>
-      </c>
-      <c r="BY43" s="37">
-        <v>0</v>
-      </c>
-      <c r="BZ43" s="37">
-        <v>1</v>
-      </c>
-      <c r="CA43" s="37">
-        <v>5</v>
-      </c>
+      <c r="BR43" s="37"/>
+      <c r="BS43" s="37"/>
+      <c r="BT43" s="38"/>
+      <c r="BU43" s="37"/>
+      <c r="BV43" s="37"/>
+      <c r="BW43" s="38"/>
+      <c r="BX43" s="37"/>
+      <c r="BY43" s="37"/>
+      <c r="BZ43" s="37"/>
+      <c r="CA43" s="37"/>
       <c r="CB43" s="37"/>
       <c r="CC43" s="37"/>
       <c r="CD43" s="37"/>
@@ -20830,12 +20896,8 @@
       <c r="BO44" s="37"/>
       <c r="BP44" s="37"/>
       <c r="BQ44" s="37"/>
-      <c r="BR44" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="BS44" s="37" t="s">
-        <v>209</v>
-      </c>
+      <c r="BR44" s="37"/>
+      <c r="BS44" s="37"/>
       <c r="BT44" s="37"/>
       <c r="BU44" s="37"/>
       <c r="BV44" s="37"/>
@@ -21001,41 +21063,19 @@
       <c r="BM45" s="37"/>
       <c r="BN45" s="37"/>
       <c r="BO45" s="37"/>
-      <c r="BP45" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="BQ45" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="BR45" s="37" t="s">
-        <v>193</v>
-      </c>
+      <c r="BP45" s="37"/>
+      <c r="BQ45" s="37"/>
+      <c r="BR45" s="37"/>
       <c r="BS45" s="37"/>
-      <c r="BT45" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="BU45" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="BV45" s="37" t="s">
-        <v>192</v>
-      </c>
+      <c r="BT45" s="37"/>
+      <c r="BU45" s="37"/>
+      <c r="BV45" s="37"/>
       <c r="BW45" s="37"/>
-      <c r="BX45" s="37" t="s">
-        <v>200</v>
-      </c>
-      <c r="BY45" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="BZ45" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="CA45" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB45" s="37" t="s">
-        <v>235</v>
-      </c>
+      <c r="BX45" s="37"/>
+      <c r="BY45" s="37"/>
+      <c r="BZ45" s="37"/>
+      <c r="CA45" s="37"/>
+      <c r="CB45" s="37"/>
       <c r="CC45" s="37"/>
       <c r="CD45" s="37"/>
       <c r="CE45" s="37"/>
@@ -21294,18 +21334,40 @@
       <c r="C47" s="37"/>
       <c r="D47" s="37"/>
       <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="37"/>
-      <c r="L47" s="37"/>
+      <c r="F47" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="I47" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="J47" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="K47" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="L47" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="M47" s="37"/>
-      <c r="N47" s="37"/>
-      <c r="O47" s="37"/>
-      <c r="P47" s="37"/>
-      <c r="Q47" s="37"/>
+      <c r="N47" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="O47" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="P47" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q47" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="R47" s="37"/>
       <c r="S47" s="37"/>
       <c r="T47" s="37"/>
@@ -21317,18 +21379,40 @@
       <c r="X47" s="37"/>
       <c r="Y47" s="37"/>
       <c r="Z47" s="37"/>
-      <c r="AA47" s="37"/>
-      <c r="AB47" s="37"/>
-      <c r="AC47" s="37"/>
-      <c r="AD47" s="37"/>
-      <c r="AE47" s="37"/>
-      <c r="AF47" s="37"/>
-      <c r="AG47" s="37"/>
+      <c r="AA47" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB47" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC47" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD47" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AE47" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF47" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG47" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="AH47" s="37"/>
-      <c r="AI47" s="37"/>
-      <c r="AJ47" s="37"/>
-      <c r="AK47" s="37"/>
-      <c r="AL47" s="37"/>
+      <c r="AI47" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ47" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="AK47" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL47" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="AM47" s="37"/>
       <c r="AN47" s="37"/>
       <c r="AO47" s="37"/>
@@ -21340,18 +21424,40 @@
       <c r="AS47" s="37"/>
       <c r="AT47" s="37"/>
       <c r="AU47" s="37"/>
-      <c r="AV47" s="37"/>
-      <c r="AW47" s="37"/>
-      <c r="AX47" s="37"/>
-      <c r="AY47" s="37"/>
-      <c r="AZ47" s="37"/>
-      <c r="BA47" s="37"/>
-      <c r="BB47" s="37"/>
+      <c r="AV47" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW47" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AX47" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AY47" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AZ47" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="BA47" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB47" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BC47" s="37"/>
-      <c r="BD47" s="37"/>
-      <c r="BE47" s="37"/>
-      <c r="BF47" s="37"/>
-      <c r="BG47" s="37"/>
+      <c r="BD47" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="BE47" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="BF47" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="BG47" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BH47" s="37"/>
       <c r="BI47" s="37"/>
       <c r="BJ47" s="37"/>
@@ -21391,17 +21497,37 @@
       <c r="C48" s="37"/>
       <c r="D48" s="37"/>
       <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="38"/>
-      <c r="M48" s="37"/>
+      <c r="F48" s="37">
+        <v>1</v>
+      </c>
+      <c r="G48" s="38">
+        <v>2</v>
+      </c>
+      <c r="H48" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="I48" s="37">
+        <v>3</v>
+      </c>
+      <c r="J48" s="38">
+        <v>0</v>
+      </c>
+      <c r="K48" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="L48" s="37">
+        <v>0</v>
+      </c>
+      <c r="M48" s="37">
+        <v>1</v>
+      </c>
       <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="37"/>
+      <c r="O48" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="P48" s="37" t="s">
+        <v>200</v>
+      </c>
       <c r="Q48" s="37"/>
       <c r="R48" s="37"/>
       <c r="S48" s="37"/>
@@ -21414,17 +21540,37 @@
       <c r="X48" s="37"/>
       <c r="Y48" s="37"/>
       <c r="Z48" s="37"/>
-      <c r="AA48" s="37"/>
-      <c r="AB48" s="37"/>
-      <c r="AC48" s="37"/>
-      <c r="AD48" s="38"/>
-      <c r="AE48" s="37"/>
-      <c r="AF48" s="37"/>
-      <c r="AG48" s="38"/>
-      <c r="AH48" s="37"/>
+      <c r="AA48" s="37">
+        <v>1</v>
+      </c>
+      <c r="AB48" s="38">
+        <v>2</v>
+      </c>
+      <c r="AC48" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD48" s="37">
+        <v>3</v>
+      </c>
+      <c r="AE48" s="38">
+        <v>0</v>
+      </c>
+      <c r="AF48" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG48" s="37">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="37">
+        <v>1</v>
+      </c>
       <c r="AI48" s="37"/>
-      <c r="AJ48" s="37"/>
-      <c r="AK48" s="37"/>
+      <c r="AJ48" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK48" s="37" t="s">
+        <v>200</v>
+      </c>
       <c r="AL48" s="37"/>
       <c r="AM48" s="37"/>
       <c r="AN48" s="37"/>
@@ -21437,17 +21583,37 @@
       <c r="AS48" s="37"/>
       <c r="AT48" s="37"/>
       <c r="AU48" s="37"/>
-      <c r="AV48" s="37"/>
-      <c r="AW48" s="37"/>
-      <c r="AX48" s="37"/>
-      <c r="AY48" s="38"/>
-      <c r="AZ48" s="37"/>
-      <c r="BA48" s="37"/>
-      <c r="BB48" s="38"/>
-      <c r="BC48" s="37"/>
+      <c r="AV48" s="37">
+        <v>1</v>
+      </c>
+      <c r="AW48" s="38">
+        <v>2</v>
+      </c>
+      <c r="AX48" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY48" s="37">
+        <v>3</v>
+      </c>
+      <c r="AZ48" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA48" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="BB48" s="37">
+        <v>0</v>
+      </c>
+      <c r="BC48" s="37">
+        <v>1</v>
+      </c>
       <c r="BD48" s="37"/>
-      <c r="BE48" s="37"/>
-      <c r="BF48" s="37"/>
+      <c r="BE48" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="BF48" s="37" t="s">
+        <v>200</v>
+      </c>
       <c r="BG48" s="37"/>
       <c r="BH48" s="37"/>
       <c r="BI48" s="37"/>
@@ -21488,8 +21654,12 @@
       <c r="C49" s="37"/>
       <c r="D49" s="37"/>
       <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
+      <c r="F49" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>209</v>
+      </c>
       <c r="H49" s="37"/>
       <c r="I49" s="37"/>
       <c r="J49" s="37"/>
@@ -21514,8 +21684,12 @@
       <c r="AA49" s="37"/>
       <c r="AB49" s="37"/>
       <c r="AC49" s="37"/>
-      <c r="AD49" s="37"/>
-      <c r="AE49" s="37"/>
+      <c r="AD49" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE49" s="37" t="s">
+        <v>209</v>
+      </c>
       <c r="AF49" s="37"/>
       <c r="AG49" s="37"/>
       <c r="AH49" s="37"/>
@@ -21540,8 +21714,12 @@
       <c r="AY49" s="37"/>
       <c r="AZ49" s="37"/>
       <c r="BA49" s="37"/>
-      <c r="BB49" s="37"/>
-      <c r="BC49" s="37"/>
+      <c r="BB49" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="BC49" s="37" t="s">
+        <v>209</v>
+      </c>
       <c r="BD49" s="37"/>
       <c r="BE49" s="37"/>
       <c r="BF49" s="37"/>
@@ -21585,18 +21763,38 @@
       <c r="C50" s="37"/>
       <c r="D50" s="37"/>
       <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
+      <c r="F50" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="G50" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="H50" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="37"/>
-      <c r="L50" s="37"/>
+      <c r="J50" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="K50" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="L50" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="M50" s="37"/>
-      <c r="N50" s="37"/>
-      <c r="O50" s="37"/>
-      <c r="P50" s="37"/>
-      <c r="Q50" s="37"/>
+      <c r="N50" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="O50" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="P50" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q50" s="37" t="s">
+        <v>197</v>
+      </c>
       <c r="R50" s="37"/>
       <c r="S50" s="37"/>
       <c r="T50" s="37"/>
@@ -21607,21 +21805,47 @@
       <c r="W50" s="37"/>
       <c r="X50" s="37"/>
       <c r="Y50" s="37"/>
-      <c r="Z50" s="37"/>
-      <c r="AA50" s="37"/>
-      <c r="AB50" s="37"/>
+      <c r="Z50" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA50" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB50" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="AC50" s="37"/>
-      <c r="AD50" s="37"/>
-      <c r="AE50" s="37"/>
-      <c r="AF50" s="37"/>
+      <c r="AD50" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE50" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF50" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="AG50" s="37"/>
-      <c r="AH50" s="37"/>
-      <c r="AI50" s="37"/>
-      <c r="AJ50" s="37"/>
-      <c r="AK50" s="37"/>
-      <c r="AL50" s="37"/>
-      <c r="AM50" s="37"/>
-      <c r="AN50" s="37"/>
+      <c r="AH50" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI50" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="AJ50" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="AK50" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="AL50" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM50" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AN50" s="37" t="s">
+        <v>220</v>
+      </c>
       <c r="AO50" s="37"/>
       <c r="AP50" s="37"/>
       <c r="AQ50">
@@ -21630,21 +21854,47 @@
       <c r="AR50" s="37"/>
       <c r="AS50" s="37"/>
       <c r="AT50" s="37"/>
-      <c r="AU50" s="37"/>
-      <c r="AV50" s="37"/>
-      <c r="AW50" s="37"/>
+      <c r="AU50" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AV50" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AW50" s="37" t="s">
+        <v>193</v>
+      </c>
       <c r="AX50" s="37"/>
-      <c r="AY50" s="37"/>
-      <c r="AZ50" s="37"/>
-      <c r="BA50" s="37"/>
+      <c r="AY50" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="AZ50" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="BA50" s="37" t="s">
+        <v>192</v>
+      </c>
       <c r="BB50" s="37"/>
-      <c r="BC50" s="37"/>
-      <c r="BD50" s="37"/>
-      <c r="BE50" s="37"/>
-      <c r="BF50" s="37"/>
-      <c r="BG50" s="37"/>
-      <c r="BH50" s="37"/>
-      <c r="BI50" s="37"/>
+      <c r="BC50" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="BD50" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="BE50" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="BF50" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="BG50" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="BH50" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="BI50" s="37" t="s">
+        <v>220</v>
+      </c>
       <c r="BJ50" s="37"/>
       <c r="BK50" s="37"/>
       <c r="BL50">
@@ -21916,9 +22166,156 @@
         <v>19</v>
       </c>
     </row>
+    <row r="52" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="D52" s="37">
+        <v>1</v>
+      </c>
+      <c r="E52" s="37">
+        <v>2</v>
+      </c>
+      <c r="F52" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="G52" s="37">
+        <v>5</v>
+      </c>
+      <c r="H52" s="37">
+        <v>9</v>
+      </c>
+      <c r="R52" s="36" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="53" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="C53" s="37">
+        <v>1</v>
+      </c>
+      <c r="D53" s="37">
+        <v>2</v>
+      </c>
+      <c r="E53" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F53" s="37">
+        <v>5</v>
+      </c>
+      <c r="G53" s="37">
+        <v>9</v>
+      </c>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="J53" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="R53" s="36" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="C54" s="37">
+        <v>1</v>
+      </c>
+      <c r="D54" s="38">
+        <v>2</v>
+      </c>
+      <c r="E54" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F54" s="37">
+        <v>3</v>
+      </c>
+      <c r="G54" s="38">
+        <v>0</v>
+      </c>
+      <c r="H54" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="I54" s="37">
+        <v>0</v>
+      </c>
+      <c r="J54" s="37">
+        <v>1</v>
+      </c>
+      <c r="R54" s="36" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="55" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="B55" s="37">
+        <v>1</v>
+      </c>
+      <c r="C55" s="38">
+        <v>2</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="E55" s="37">
+        <v>3</v>
+      </c>
+      <c r="F55" s="38">
+        <v>0</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="H55" s="37">
+        <v>0</v>
+      </c>
+      <c r="I55" s="37">
+        <v>1</v>
+      </c>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="L55" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="R55" s="36" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="56" spans="1:85" s="74" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="75" t="s">
+        <v>328</v>
+      </c>
+      <c r="C56" s="75"/>
+      <c r="D56" s="75" t="s">
+        <v>323</v>
+      </c>
+      <c r="E56" s="75" t="s">
+        <v>329</v>
+      </c>
+      <c r="F56" s="75"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="75" t="s">
+        <v>330</v>
+      </c>
+      <c r="I56" s="75"/>
+      <c r="J56" s="75" t="s">
+        <v>331</v>
+      </c>
+      <c r="K56" s="75"/>
+      <c r="L56" s="75"/>
+      <c r="M56" s="75"/>
+      <c r="N56" s="75"/>
+      <c r="O56" s="75"/>
+      <c r="P56" s="75"/>
+      <c r="Q56" s="75"/>
+      <c r="R56" s="75"/>
+      <c r="S56" s="75"/>
+      <c r="T56" s="75"/>
+      <c r="U56" s="75"/>
+      <c r="AR56" s="76"/>
+      <c r="AS56" s="76"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -21961,25 +22358,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="71" t="s">
+      <c r="L1" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="71" t="s">
+      <c r="N1" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="71" t="s">
+      <c r="O1" s="72" t="s">
         <v>83</v>
       </c>
     </row>
@@ -22000,13 +22397,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -22028,13 +22425,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -25163,14 +25560,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.44140625" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.77734375" customWidth="1"/>
+    <col min="6" max="10" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="50" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Tagging as v0.32  Added in the ability to log the 4 temperature sensors data to a SD Card.  The logger() function is used to log the data to logfile.  This is then flushed  to the SD Card after a time interval specified with the SDCARD_WRITE_INTERVAL.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="LCD Setups" sheetId="9" r:id="rId5"/>
     <sheet name="Menu Variables" sheetId="6" r:id="rId6"/>
     <sheet name="12 Hour" sheetId="10" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId8"/>
+    <sheet name="Timing" sheetId="12" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="333">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -797,72 +798,6 @@
     <t>if &gt; =12</t>
   </si>
   <si>
-    <t>Roadmap Generalized</t>
-  </si>
-  <si>
-    <t>Add a type to MenuNumSel and possibly rename it ot MenuSel since it wont just be dealing with Numbers</t>
-  </si>
-  <si>
-    <t>Finish out the Alarm functions</t>
-  </si>
-  <si>
-    <t>Add in Alarm Type</t>
-  </si>
-  <si>
-    <t>Make this usefull</t>
-  </si>
-  <si>
-    <t>Add in AlarmEnable/Disable to the AlarmOn/Off functions</t>
-  </si>
-  <si>
-    <t>Menu System Timeout</t>
-  </si>
-  <si>
-    <t>Add the ability for the menu system to timeout after being in it for a certain ammount of time</t>
-  </si>
-  <si>
-    <t>Add Alarm State reading and functionality</t>
-  </si>
-  <si>
-    <t>Continue to log sensors while in the menu</t>
-  </si>
-  <si>
-    <t>Set the date and time using the LCD screen</t>
-  </si>
-  <si>
-    <t>Add hardware and software support for Backlight brightness</t>
-  </si>
-  <si>
-    <t>Be able to address the sensors</t>
-  </si>
-  <si>
-    <t>Be able to calibrate the sensors</t>
-  </si>
-  <si>
-    <t>Add a flow meter to the project</t>
-  </si>
-  <si>
-    <t>calibrate the flow meter</t>
-  </si>
-  <si>
-    <t>display the flow on the LCD screen</t>
-  </si>
-  <si>
-    <t>be able to name the sensors according to the address</t>
-  </si>
-  <si>
-    <t>Assign the Alarms a relay to triger</t>
-  </si>
-  <si>
-    <t>Assign names to the alarms and make the display be able to select the alarms by name</t>
-  </si>
-  <si>
-    <t>Split the sysconfig menu and add a User Settings Menu</t>
-  </si>
-  <si>
-    <t>Next</t>
-  </si>
-  <si>
     <t>Time breakpoints brainstorming and visualization</t>
   </si>
   <si>
@@ -1065,6 +1000,57 @@
   </si>
   <si>
     <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t>loop()</t>
+  </si>
+  <si>
+    <t>poll menuMode to check to see if we should enter the menu</t>
+  </si>
+  <si>
+    <t>display the LCD Date</t>
+  </si>
+  <si>
+    <t>display the LCD Time</t>
+  </si>
+  <si>
+    <t>take a temp sensor reading</t>
+  </si>
+  <si>
+    <t>take a flow sensor reading</t>
+  </si>
+  <si>
+    <t>log sensor readings to the logfile</t>
+  </si>
+  <si>
+    <t>write the logfile to the SD card</t>
+  </si>
+  <si>
+    <t>4 sensor readings</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>total millis</t>
+  </si>
+  <si>
+    <t>log writing</t>
+  </si>
+  <si>
+    <t>SD Card writing</t>
+  </si>
+  <si>
+    <t>3 sensor readings</t>
+  </si>
+  <si>
+    <t>2 sensor readings</t>
+  </si>
+  <si>
+    <t>Date and Time Display</t>
   </si>
 </sst>
 </file>
@@ -1534,6 +1520,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1566,15 +1561,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1895,12 +1881,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="A1" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
       <c r="E1" t="s">
         <v>96</v>
       </c>
@@ -2063,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,12 +2063,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
       <c r="E1" t="s">
         <v>95</v>
       </c>
@@ -2165,13 +2151,13 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F7" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2201,13 +2187,13 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F10" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2215,7 +2201,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>8</v>
@@ -2226,13 +2212,13 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>316</v>
+        <v>294</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F12" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2273,7 +2259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2289,13 +2275,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="19" t="s">
         <v>108</v>
       </c>
@@ -2325,7 +2311,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="67"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -2346,7 +2332,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="68"/>
+      <c r="A4" s="71"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -2367,7 +2353,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="67" t="s">
         <v>176</v>
       </c>
       <c r="B5" s="25">
@@ -2390,7 +2376,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -2411,7 +2397,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="65"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -2432,7 +2418,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
+      <c r="A8" s="68"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -2453,7 +2439,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -2474,7 +2460,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="66"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -2495,7 +2481,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="67" t="s">
         <v>177</v>
       </c>
       <c r="B11" s="25">
@@ -2518,7 +2504,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -2539,7 +2525,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -2560,7 +2546,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="65"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -2581,7 +2567,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -2602,7 +2588,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="66"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -2623,7 +2609,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="67" t="s">
         <v>178</v>
       </c>
       <c r="B17" s="29">
@@ -2646,7 +2632,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
+      <c r="A18" s="68"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -2667,7 +2653,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="68"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -2688,7 +2674,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
+      <c r="A20" s="68"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -2709,7 +2695,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="68"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -2730,7 +2716,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="66"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -2751,7 +2737,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="67" t="s">
         <v>179</v>
       </c>
       <c r="B23" s="25">
@@ -2774,7 +2760,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -2795,7 +2781,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -2816,7 +2802,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -2837,7 +2823,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="68"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -2858,7 +2844,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="66"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -2879,7 +2865,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="67" t="s">
         <v>180</v>
       </c>
       <c r="B29" s="29">
@@ -2902,7 +2888,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="68"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -2923,7 +2909,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
+      <c r="A31" s="68"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -2944,7 +2930,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="68"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -2965,7 +2951,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="65"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -2986,7 +2972,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="66"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -3007,7 +2993,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="67" t="s">
         <v>181</v>
       </c>
       <c r="B35" s="25">
@@ -3030,7 +3016,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="65"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -3051,7 +3037,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="65"/>
+      <c r="A37" s="68"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -3072,7 +3058,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="65"/>
+      <c r="A38" s="68"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -3093,7 +3079,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="65"/>
+      <c r="A39" s="68"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -3114,7 +3100,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="66"/>
+      <c r="A40" s="69"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -3135,7 +3121,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="64" t="s">
+      <c r="A41" s="67" t="s">
         <v>182</v>
       </c>
       <c r="B41" s="29">
@@ -3158,7 +3144,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="65"/>
+      <c r="A42" s="68"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -3179,7 +3165,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="65"/>
+      <c r="A43" s="68"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -3200,7 +3186,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="65"/>
+      <c r="A44" s="68"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -3221,7 +3207,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="65"/>
+      <c r="A45" s="68"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -3242,7 +3228,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="66"/>
+      <c r="A46" s="69"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -3263,7 +3249,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="64" t="s">
+      <c r="A47" s="67" t="s">
         <v>183</v>
       </c>
       <c r="B47" s="25">
@@ -3286,7 +3272,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="65"/>
+      <c r="A48" s="68"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -3307,7 +3293,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="65"/>
+      <c r="A49" s="68"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -3328,7 +3314,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="65"/>
+      <c r="A50" s="68"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -3349,7 +3335,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="65"/>
+      <c r="A51" s="68"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -3370,7 +3356,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="66"/>
+      <c r="A52" s="69"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -3395,7 +3381,7 @@
         <v>150</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
       <c r="D53" s="60" t="s">
         <v>94</v>
@@ -3404,7 +3390,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="61" t="s">
-        <v>312</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3468,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="M1" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="U1" s="40" t="s">
         <v>223</v>
@@ -3790,7 +3776,7 @@
         <v>16</v>
       </c>
       <c r="N7" t="s">
-        <v>313</v>
+        <v>291</v>
       </c>
       <c r="U7" s="40">
         <v>5</v>
@@ -3900,7 +3886,7 @@
         <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="U9" s="40">
         <v>7</v>
@@ -4035,7 +4021,7 @@
         <v>10</v>
       </c>
       <c r="M14" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -4074,7 +4060,7 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -4113,13 +4099,13 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="O16" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="P16" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -4158,7 +4144,7 @@
         <v>2</v>
       </c>
       <c r="N17" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -4197,7 +4183,7 @@
         <v>4</v>
       </c>
       <c r="N18" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
@@ -4236,7 +4222,7 @@
         <v>8</v>
       </c>
       <c r="N19" s="58" t="s">
-        <v>310</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
@@ -4275,7 +4261,7 @@
         <v>16</v>
       </c>
       <c r="N20" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -4350,7 +4336,7 @@
         <v>64</v>
       </c>
       <c r="N22" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
@@ -4389,10 +4375,10 @@
         <v>128</v>
       </c>
       <c r="N23" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="O23" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
@@ -4497,7 +4483,7 @@
         <v>1110</v>
       </c>
       <c r="M26" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
@@ -4536,7 +4522,7 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
@@ -13981,7 +13967,7 @@
         <v>3</v>
       </c>
       <c r="BJ7" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK7" s="37" t="s">
         <v>228</v>
@@ -14028,7 +14014,7 @@
         <v>3</v>
       </c>
       <c r="CE7" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF7" s="37" t="s">
         <v>228</v>
@@ -14162,7 +14148,7 @@
         <v>3</v>
       </c>
       <c r="BJ8" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK8" s="37" t="s">
         <v>228</v>
@@ -14219,7 +14205,7 @@
         <v>3</v>
       </c>
       <c r="CE8" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF8" s="37" t="s">
         <v>228</v>
@@ -14329,7 +14315,7 @@
         <v>3</v>
       </c>
       <c r="BJ9" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK9" s="37" t="s">
         <v>228</v>
@@ -14368,7 +14354,7 @@
         <v>3</v>
       </c>
       <c r="CE9" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF9" s="37" t="s">
         <v>228</v>
@@ -14490,7 +14476,7 @@
         <v>3</v>
       </c>
       <c r="BJ10" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK10" s="37" t="s">
         <v>228</v>
@@ -14545,7 +14531,7 @@
         <v>3</v>
       </c>
       <c r="CE10" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF10" s="37" t="s">
         <v>228</v>
@@ -14949,7 +14935,7 @@
         <v>3</v>
       </c>
       <c r="BJ12" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK12" s="37" t="s">
         <v>228</v>
@@ -15002,7 +14988,7 @@
         <v>3</v>
       </c>
       <c r="CE12" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF12" s="37" t="s">
         <v>228</v>
@@ -15134,7 +15120,7 @@
         <v>3</v>
       </c>
       <c r="BJ13" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK13" s="37" t="s">
         <v>228</v>
@@ -15191,7 +15177,7 @@
         <v>3</v>
       </c>
       <c r="CE13" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF13" s="37" t="s">
         <v>228</v>
@@ -15301,7 +15287,7 @@
         <v>3</v>
       </c>
       <c r="BJ14" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK14" s="37" t="s">
         <v>228</v>
@@ -15340,7 +15326,7 @@
         <v>3</v>
       </c>
       <c r="CE14" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF14" s="37" t="s">
         <v>228</v>
@@ -15470,7 +15456,7 @@
         <v>3</v>
       </c>
       <c r="BJ15" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK15" s="37" t="s">
         <v>228</v>
@@ -15525,7 +15511,7 @@
         <v>3</v>
       </c>
       <c r="CE15" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="CF15" s="37" t="s">
         <v>228</v>
@@ -16751,7 +16737,7 @@
         <v>3</v>
       </c>
       <c r="T22" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U22" s="37" t="s">
         <v>228</v>
@@ -16808,7 +16794,7 @@
         <v>3</v>
       </c>
       <c r="AO22" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP22" s="37" t="s">
         <v>228</v>
@@ -16861,7 +16847,7 @@
         <v>3</v>
       </c>
       <c r="BJ22" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK22" s="37" t="s">
         <v>228</v>
@@ -16958,7 +16944,7 @@
         <v>3</v>
       </c>
       <c r="T23" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U23" s="37" t="s">
         <v>228</v>
@@ -17015,7 +17001,7 @@
         <v>3</v>
       </c>
       <c r="AO23" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP23" s="37" t="s">
         <v>228</v>
@@ -17072,7 +17058,7 @@
         <v>3</v>
       </c>
       <c r="BJ23" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK23" s="37" t="s">
         <v>228</v>
@@ -17153,7 +17139,7 @@
         <v>3</v>
       </c>
       <c r="T24" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U24" s="37" t="s">
         <v>228</v>
@@ -17192,7 +17178,7 @@
         <v>3</v>
       </c>
       <c r="AO24" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP24" s="37" t="s">
         <v>228</v>
@@ -17231,7 +17217,7 @@
         <v>3</v>
       </c>
       <c r="BJ24" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK24" s="37" t="s">
         <v>228</v>
@@ -17246,7 +17232,7 @@
       <c r="BQ24" s="37"/>
       <c r="BR24" s="37"/>
       <c r="BS24" s="37" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
       <c r="BT24" s="37" t="s">
         <v>192</v>
@@ -17332,7 +17318,7 @@
         <v>3</v>
       </c>
       <c r="T25" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U25" s="37" t="s">
         <v>228</v>
@@ -17387,7 +17373,7 @@
         <v>3</v>
       </c>
       <c r="AO25" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP25" s="37" t="s">
         <v>228</v>
@@ -17442,7 +17428,7 @@
         <v>3</v>
       </c>
       <c r="BJ25" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK25" s="37" t="s">
         <v>228</v>
@@ -17783,7 +17769,7 @@
         <v>3</v>
       </c>
       <c r="T27" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U27" s="37" t="s">
         <v>228</v>
@@ -17836,7 +17822,7 @@
         <v>3</v>
       </c>
       <c r="AO27" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP27" s="37" t="s">
         <v>228</v>
@@ -17883,7 +17869,7 @@
         <v>3</v>
       </c>
       <c r="BJ27" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK27" s="37" t="s">
         <v>228</v>
@@ -17984,7 +17970,7 @@
         <v>3</v>
       </c>
       <c r="T28" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U28" s="37" t="s">
         <v>228</v>
@@ -18041,7 +18027,7 @@
         <v>3</v>
       </c>
       <c r="AO28" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP28" s="37" t="s">
         <v>228</v>
@@ -18098,7 +18084,7 @@
         <v>3</v>
       </c>
       <c r="BJ28" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK28" s="37" t="s">
         <v>228</v>
@@ -18165,7 +18151,7 @@
         <v>3</v>
       </c>
       <c r="T29" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U29" s="37" t="s">
         <v>228</v>
@@ -18204,7 +18190,7 @@
         <v>3</v>
       </c>
       <c r="AO29" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP29" s="37" t="s">
         <v>228</v>
@@ -18243,7 +18229,7 @@
         <v>3</v>
       </c>
       <c r="BJ29" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK29" s="37" t="s">
         <v>228</v>
@@ -18326,7 +18312,7 @@
         <v>3</v>
       </c>
       <c r="T30" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="U30" s="37" t="s">
         <v>228</v>
@@ -18381,7 +18367,7 @@
         <v>3</v>
       </c>
       <c r="AO30" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="AP30" s="37" t="s">
         <v>228</v>
@@ -18436,7 +18422,7 @@
         <v>3</v>
       </c>
       <c r="BJ30" s="37" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="BK30" s="37" t="s">
         <v>228</v>
@@ -18810,7 +18796,7 @@
         <v>214</v>
       </c>
       <c r="BA32" s="37" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="BB32" s="37" t="s">
         <v>195</v>
@@ -18850,7 +18836,7 @@
       </c>
       <c r="BT32" s="37"/>
       <c r="BU32" s="37" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
       <c r="BV32" s="37" t="s">
         <v>214</v>
@@ -18971,13 +18957,13 @@
       <c r="AS33" s="37"/>
       <c r="AT33" s="37"/>
       <c r="AU33" s="37" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
       <c r="AV33" s="37" t="s">
         <v>210</v>
       </c>
       <c r="AW33" s="37" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="AX33" s="37" t="s">
         <v>214</v>
@@ -19086,7 +19072,7 @@
         <v>192</v>
       </c>
       <c r="E34" s="37" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="37" t="s">
@@ -19267,7 +19253,7 @@
         <v>192</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37" t="s">
@@ -19675,7 +19661,7 @@
         <v>193</v>
       </c>
       <c r="AD37" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="AE37" s="37" t="s">
         <v>193</v>
@@ -19720,7 +19706,7 @@
         <v>193</v>
       </c>
       <c r="AY37" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="AZ37" s="37" t="s">
         <v>193</v>
@@ -19765,7 +19751,7 @@
         <v>193</v>
       </c>
       <c r="BT37" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="BU37" s="37" t="s">
         <v>193</v>
@@ -19845,7 +19831,7 @@
         <v>206</v>
       </c>
       <c r="S38" s="37" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="T38" s="37"/>
       <c r="U38" s="37"/>
@@ -20004,7 +19990,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="37" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="N39" s="37"/>
       <c r="O39" s="37"/>
@@ -20516,7 +20502,7 @@
         <v>193</v>
       </c>
       <c r="I42" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="J42" s="37" t="s">
         <v>193</v>
@@ -20561,7 +20547,7 @@
         <v>193</v>
       </c>
       <c r="AD42" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="AE42" s="37" t="s">
         <v>193</v>
@@ -20606,7 +20592,7 @@
         <v>193</v>
       </c>
       <c r="AY42" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="AZ42" s="37" t="s">
         <v>193</v>
@@ -21344,7 +21330,7 @@
         <v>193</v>
       </c>
       <c r="I47" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="J47" s="37" t="s">
         <v>193</v>
@@ -21389,7 +21375,7 @@
         <v>193</v>
       </c>
       <c r="AD47" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="AE47" s="37" t="s">
         <v>193</v>
@@ -21434,7 +21420,7 @@
         <v>193</v>
       </c>
       <c r="AY47" s="37" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="AZ47" s="37" t="s">
         <v>193</v>
@@ -22183,7 +22169,7 @@
         <v>9</v>
       </c>
       <c r="R52" s="36" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
     </row>
     <row r="53" spans="1:85" x14ac:dyDescent="0.35">
@@ -22210,7 +22196,7 @@
         <v>200</v>
       </c>
       <c r="R53" s="36" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:85" x14ac:dyDescent="0.35">
@@ -22239,7 +22225,7 @@
         <v>1</v>
       </c>
       <c r="R54" s="36" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:85" x14ac:dyDescent="0.35">
@@ -22275,42 +22261,42 @@
         <v>200</v>
       </c>
       <c r="R55" s="36" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="56" spans="1:85" s="74" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="75" t="s">
-        <v>328</v>
-      </c>
-      <c r="C56" s="75"/>
-      <c r="D56" s="75" t="s">
-        <v>323</v>
-      </c>
-      <c r="E56" s="75" t="s">
-        <v>329</v>
-      </c>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="75" t="s">
-        <v>330</v>
-      </c>
-      <c r="I56" s="75"/>
-      <c r="J56" s="75" t="s">
-        <v>331</v>
-      </c>
-      <c r="K56" s="75"/>
-      <c r="L56" s="75"/>
-      <c r="M56" s="75"/>
-      <c r="N56" s="75"/>
-      <c r="O56" s="75"/>
-      <c r="P56" s="75"/>
-      <c r="Q56" s="75"/>
-      <c r="R56" s="75"/>
-      <c r="S56" s="75"/>
-      <c r="T56" s="75"/>
-      <c r="U56" s="75"/>
-      <c r="AR56" s="76"/>
-      <c r="AS56" s="76"/>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="56" spans="1:85" s="63" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="C56" s="64"/>
+      <c r="D56" s="64" t="s">
+        <v>301</v>
+      </c>
+      <c r="E56" s="64" t="s">
+        <v>307</v>
+      </c>
+      <c r="F56" s="64"/>
+      <c r="G56" s="64"/>
+      <c r="H56" s="64" t="s">
+        <v>308</v>
+      </c>
+      <c r="I56" s="64"/>
+      <c r="J56" s="64" t="s">
+        <v>309</v>
+      </c>
+      <c r="K56" s="64"/>
+      <c r="L56" s="64"/>
+      <c r="M56" s="64"/>
+      <c r="N56" s="64"/>
+      <c r="O56" s="64"/>
+      <c r="P56" s="64"/>
+      <c r="Q56" s="64"/>
+      <c r="R56" s="64"/>
+      <c r="S56" s="64"/>
+      <c r="T56" s="64"/>
+      <c r="U56" s="64"/>
+      <c r="AR56" s="65"/>
+      <c r="AS56" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22358,25 +22344,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="75" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="72" t="s">
+      <c r="N1" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="72" t="s">
+      <c r="O1" s="75" t="s">
         <v>83</v>
       </c>
     </row>
@@ -22397,13 +22383,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -22425,13 +22411,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -22470,7 +22456,7 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -22697,7 +22683,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -22759,7 +22745,7 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -22973,7 +22959,7 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -23019,7 +23005,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -23081,7 +23067,7 @@
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -23189,7 +23175,7 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
@@ -23262,7 +23248,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -23335,7 +23321,7 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -23443,7 +23429,7 @@
         <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -23551,7 +23537,7 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -23659,7 +23645,7 @@
         <v>0</v>
       </c>
       <c r="P37" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -23705,7 +23691,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -23742,7 +23728,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4">
@@ -23767,7 +23753,7 @@
         <v>0</v>
       </c>
       <c r="P40" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -23813,7 +23799,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -23850,7 +23836,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4">
@@ -23875,7 +23861,7 @@
         <v>0</v>
       </c>
       <c r="P43" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -23921,7 +23907,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -23958,7 +23944,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4">
@@ -23983,7 +23969,7 @@
         <v>0</v>
       </c>
       <c r="P46" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -24029,7 +24015,7 @@
         <v>7</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -24066,7 +24052,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="4">
@@ -24091,7 +24077,7 @@
         <v>0</v>
       </c>
       <c r="P49" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
@@ -25056,7 +25042,7 @@
         <v>4</v>
       </c>
       <c r="C80" s="57" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="D80" s="57"/>
       <c r="E80" s="57"/>
@@ -25146,7 +25132,7 @@
         <v>0</v>
       </c>
       <c r="P82" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="83" spans="4:16" x14ac:dyDescent="0.3">
@@ -25245,7 +25231,7 @@
         <v>0</v>
       </c>
       <c r="P85" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
     </row>
     <row r="86" spans="4:16" x14ac:dyDescent="0.3">
@@ -25285,7 +25271,7 @@
         <v>2</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>285</v>
+        <v>263</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -25344,7 +25330,7 @@
         <v>0</v>
       </c>
       <c r="P88" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
     </row>
     <row r="89" spans="4:16" x14ac:dyDescent="0.3">
@@ -25573,7 +25559,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="50" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="50" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="B1" s="51"/>
     </row>
@@ -25807,182 +25793,592 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B2">
+        <v>3736</v>
+      </c>
+      <c r="C2">
+        <v>10014</v>
+      </c>
+      <c r="D2">
+        <v>20015</v>
+      </c>
+      <c r="E2">
+        <v>30014</v>
+      </c>
+      <c r="F2">
+        <v>40014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3">
+        <v>4486</v>
+      </c>
+      <c r="C3">
+        <v>10764</v>
+      </c>
+      <c r="D3">
+        <v>20764</v>
+      </c>
+      <c r="E3">
+        <v>30764</v>
+      </c>
+      <c r="F3">
+        <v>40764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B4">
+        <f>B3-B2</f>
+        <v>750</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:F4" si="0">C3-C2</f>
+        <v>750</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>749</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>330</v>
+      </c>
+      <c r="F6">
+        <f>F4-F9</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B7">
+        <v>3599</v>
+      </c>
+      <c r="C7">
+        <v>10014</v>
+      </c>
+      <c r="D7">
+        <v>20015</v>
+      </c>
+      <c r="E7">
+        <v>30014</v>
+      </c>
+      <c r="F7">
+        <v>40014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8">
+        <v>4187</v>
+      </c>
+      <c r="C8">
+        <v>10602</v>
+      </c>
+      <c r="D8">
+        <v>20602</v>
+      </c>
+      <c r="E8">
+        <v>30602</v>
+      </c>
+      <c r="F8">
+        <v>40602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9">
+        <f>B8-B7</f>
+        <v>588</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9" si="1">C8-C7</f>
+        <v>588</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9" si="2">D8-D7</f>
+        <v>587</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9" si="3">E8-E7</f>
+        <v>588</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9" si="4">F8-F7</f>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>331</v>
+      </c>
+      <c r="F11">
+        <f>F9-F14</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12">
+        <v>3485</v>
+      </c>
+      <c r="C12">
+        <v>10014</v>
+      </c>
+      <c r="D12">
+        <v>20015</v>
+      </c>
+      <c r="E12">
+        <v>30014</v>
+      </c>
+      <c r="F12">
+        <v>40014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>326</v>
+      </c>
+      <c r="B13">
+        <v>3926</v>
+      </c>
+      <c r="C13">
+        <v>10455</v>
+      </c>
+      <c r="D13">
+        <v>20455</v>
+      </c>
+      <c r="E13">
+        <v>30454</v>
+      </c>
+      <c r="F13">
+        <v>40455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B14">
+        <f>B13-B12</f>
+        <v>441</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14" si="5">C13-C12</f>
+        <v>441</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14" si="6">D13-D12</f>
+        <v>440</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14" si="7">E13-E12</f>
+        <v>440</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14" si="8">F13-F12</f>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>331</v>
+      </c>
+      <c r="F16">
+        <f>F14-F19</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>325</v>
+      </c>
+      <c r="B17">
+        <v>3397</v>
+      </c>
+      <c r="C17">
+        <v>10014</v>
+      </c>
+      <c r="D17">
+        <v>20015</v>
+      </c>
+      <c r="E17">
+        <v>30014</v>
+      </c>
+      <c r="F17">
+        <v>40014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>326</v>
+      </c>
+      <c r="B18">
+        <v>3705</v>
+      </c>
+      <c r="C18">
+        <v>10322</v>
+      </c>
+      <c r="D18">
+        <v>20323</v>
+      </c>
+      <c r="E18">
+        <v>30322</v>
+      </c>
+      <c r="F18">
+        <v>40323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>327</v>
+      </c>
+      <c r="B19">
+        <f>B18-B17</f>
+        <v>308</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19" si="9">C18-C17</f>
+        <v>308</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19" si="10">D18-D17</f>
+        <v>308</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19" si="11">E18-E17</f>
+        <v>308</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19" si="12">F18-F17</f>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>325</v>
+      </c>
+      <c r="B22">
+        <v>4187</v>
+      </c>
+      <c r="C22">
+        <v>10602</v>
+      </c>
+      <c r="D22">
+        <v>20602</v>
+      </c>
+      <c r="E22">
+        <v>30602</v>
+      </c>
+      <c r="F22">
+        <v>40765</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B23">
+        <v>4196</v>
+      </c>
+      <c r="C23">
+        <v>10611</v>
+      </c>
+      <c r="D23">
+        <v>20611</v>
+      </c>
+      <c r="E23">
+        <v>30611</v>
+      </c>
+      <c r="F23">
+        <v>40774</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B24">
+        <f>B23-B22</f>
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:F24" si="13">C23-C22</f>
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>325</v>
+      </c>
+      <c r="B27">
+        <v>60777</v>
+      </c>
+      <c r="C27">
+        <v>130775</v>
+      </c>
+      <c r="D27">
+        <v>200774</v>
+      </c>
+      <c r="E27">
+        <v>260774</v>
+      </c>
+      <c r="F27">
+        <v>320774</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>326</v>
+      </c>
+      <c r="B28">
+        <v>60788</v>
+      </c>
+      <c r="C28">
+        <v>130787</v>
+      </c>
+      <c r="D28">
+        <v>200786</v>
+      </c>
+      <c r="E28">
+        <v>260787</v>
+      </c>
+      <c r="F28">
+        <v>320786</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>327</v>
+      </c>
+      <c r="B29">
+        <f>B28-B27</f>
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:F29" si="14">C28-C27</f>
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>325</v>
+      </c>
+      <c r="B32">
+        <v>5000</v>
+      </c>
+      <c r="C32">
+        <v>6000</v>
+      </c>
+      <c r="D32">
+        <v>7002</v>
+      </c>
+      <c r="E32">
+        <v>8000</v>
+      </c>
+      <c r="F32">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B33">
+        <v>5000</v>
+      </c>
+      <c r="C33">
+        <v>6000</v>
+      </c>
+      <c r="D33">
+        <v>7003</v>
+      </c>
+      <c r="E33">
+        <v>8000</v>
+      </c>
+      <c r="F33">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>326</v>
+      </c>
+      <c r="B34">
+        <v>5014</v>
+      </c>
+      <c r="C34">
+        <v>6014</v>
+      </c>
+      <c r="D34">
+        <v>7016</v>
+      </c>
+      <c r="E34">
+        <v>8014</v>
+      </c>
+      <c r="F34">
+        <v>9016</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>327</v>
+      </c>
+      <c r="B35">
+        <f>B34-B33</f>
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:F35" si="15">C34-C33</f>
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="15"/>
+        <v>13</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>269</v>
-      </c>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0</v>
-      </c>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>268</v>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v38.4  Finished up the time and date displaying on the 4.3" touchscreen.  It will basically display as the char lcd right now.  There is going to be problems with how the char lcd displays other items that use the function like the set date and time.  This will be fixed in a future version.  Added a menuMode reset just before the loop to prevent the menu from being called as soon as the loop starts.  Also added a read for the MCPA INTCAPA so that the interrupt that was triggered when the menu was called will be reset.  Changed the start up screen to use a sprintf just like the time and date display and added the option to it to choose which type to display to.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Robbie\My Documents\GitHub\Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Robbie\Documents\GitHub\Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Timing" sheetId="12" r:id="rId8"/>
     <sheet name="Sheet2" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1056,7 +1056,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12482,8 +12482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG56"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="X55" sqref="X55"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="BA23" sqref="AR23:BA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -16895,9 +16895,11 @@
       <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="37">
+        <v>1</v>
+      </c>
       <c r="C23" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>229</v>
@@ -17010,33 +17012,31 @@
         <v>1</v>
       </c>
       <c r="AR23" s="37"/>
-      <c r="AS23" s="37">
-        <v>1</v>
-      </c>
-      <c r="AT23" s="38" t="s">
+      <c r="AS23" s="38">
+        <v>1</v>
+      </c>
+      <c r="AT23" s="37" t="s">
         <v>229</v>
       </c>
       <c r="AU23" s="37">
-        <v>2</v>
-      </c>
-      <c r="AV23" s="37">
         <v>8</v>
       </c>
-      <c r="AW23" s="38" t="s">
+      <c r="AV23" s="38" t="s">
         <v>229</v>
       </c>
+      <c r="AW23" s="37">
+        <v>2</v>
+      </c>
       <c r="AX23" s="37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY23" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ23" s="37">
-        <v>1</v>
-      </c>
-      <c r="BA23" s="37">
         <v>5</v>
       </c>
+      <c r="BA23" s="44"/>
       <c r="BB23" s="37"/>
       <c r="BC23" s="37" t="s">
         <v>191</v>
@@ -25795,7 +25795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v38.6  Added the temp sensor readings to the 4.3" touchscreen.  Renamed DS18B20_Read() to ReadTempSensors().  Removed the ability to read multiple pins from the temperature sensors.  They will now only read 1 bus.  Started reformatting the strings for the sensors to prepare to print them to the LCD touchscreen.  Also renamed a few variables and defines for the sensors to make more sense.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -47,12 +47,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="J56" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Robbie:
+AMPM will start here.  Will use the modifier "space" to add spaces here.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="333">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1122,7 +1137,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1198,6 +1213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1434,7 +1455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1561,6 +1582,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2049,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="A13:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2221,21 +2245,6 @@
         <v>295</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>32</v>
-      </c>
-    </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>12</v>
@@ -2259,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12480,10 +12489,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG56"/>
+  <dimension ref="A1:CG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="BA23" sqref="AR23:BA23"/>
+    <sheetView topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="Y56" sqref="Y56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -22253,50 +22262,86 @@
       <c r="I55" s="37">
         <v>1</v>
       </c>
-      <c r="J55" s="37"/>
+      <c r="J55" s="37" t="s">
+        <v>211</v>
+      </c>
       <c r="K55" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="L55" s="37" t="s">
         <v>200</v>
       </c>
+      <c r="L55" s="77"/>
       <c r="R55" s="36" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:85" s="63" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="64" t="s">
+    <row r="56" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="B56" s="37">
+        <v>1</v>
+      </c>
+      <c r="C56" s="38">
+        <v>2</v>
+      </c>
+      <c r="D56" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="E56" s="37">
+        <v>3</v>
+      </c>
+      <c r="F56" s="38">
+        <v>0</v>
+      </c>
+      <c r="G56" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="H56" s="37">
+        <v>0</v>
+      </c>
+      <c r="I56" s="37">
+        <v>1</v>
+      </c>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="L56" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="R56" s="36" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="57" spans="1:85" s="63" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="64" t="s">
         <v>306</v>
       </c>
-      <c r="C56" s="64"/>
-      <c r="D56" s="64" t="s">
+      <c r="C57" s="64"/>
+      <c r="D57" s="64" t="s">
         <v>301</v>
       </c>
-      <c r="E56" s="64" t="s">
+      <c r="E57" s="64" t="s">
         <v>307</v>
       </c>
-      <c r="F56" s="64"/>
-      <c r="G56" s="64"/>
-      <c r="H56" s="64" t="s">
+      <c r="F57" s="64"/>
+      <c r="G57" s="64"/>
+      <c r="H57" s="64" t="s">
         <v>308</v>
       </c>
-      <c r="I56" s="64"/>
-      <c r="J56" s="64" t="s">
+      <c r="I57" s="64"/>
+      <c r="J57" s="64" t="s">
         <v>309</v>
       </c>
-      <c r="K56" s="64"/>
-      <c r="L56" s="64"/>
-      <c r="M56" s="64"/>
-      <c r="N56" s="64"/>
-      <c r="O56" s="64"/>
-      <c r="P56" s="64"/>
-      <c r="Q56" s="64"/>
-      <c r="R56" s="64"/>
-      <c r="S56" s="64"/>
-      <c r="T56" s="64"/>
-      <c r="U56" s="64"/>
-      <c r="AR56" s="65"/>
-      <c r="AS56" s="65"/>
+      <c r="K57" s="64"/>
+      <c r="L57" s="64"/>
+      <c r="M57" s="64"/>
+      <c r="N57" s="64"/>
+      <c r="O57" s="64"/>
+      <c r="P57" s="64"/>
+      <c r="Q57" s="64"/>
+      <c r="R57" s="64"/>
+      <c r="S57" s="64"/>
+      <c r="T57" s="64"/>
+      <c r="U57" s="64"/>
+      <c r="AR57" s="65"/>
+      <c r="AS57" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v39.1  Finished adding the relay status to the 4.3" touchscreen.  Updated the commenting on all relay functions as well.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -1660,6 +1660,7 @@
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1687,12 +1688,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1702,7 +1697,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2010,7 +2010,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2022,12 +2022,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
+      <c r="A1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
       <c r="E1" t="s">
         <v>96</v>
       </c>
@@ -2259,12 +2259,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
       <c r="E1" t="s">
         <v>95</v>
       </c>
@@ -2456,13 +2456,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="76"/>
       <c r="F1" s="19" t="s">
         <v>108</v>
       </c>
@@ -2492,7 +2492,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="71"/>
+      <c r="A3" s="72"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -2513,7 +2513,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="72"/>
+      <c r="A4" s="73"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -2534,7 +2534,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="69" t="s">
         <v>175</v>
       </c>
       <c r="B5" s="25">
@@ -2557,7 +2557,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="69"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -2578,7 +2578,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="69"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -2599,7 +2599,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="69"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -2620,7 +2620,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="69"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -2641,7 +2641,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="70"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -2662,7 +2662,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="69" t="s">
         <v>176</v>
       </c>
       <c r="B11" s="25">
@@ -2685,7 +2685,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -2706,7 +2706,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="69"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -2727,7 +2727,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="69"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
+      <c r="A15" s="70"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -2769,7 +2769,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="70"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -2790,7 +2790,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="69" t="s">
         <v>177</v>
       </c>
       <c r="B17" s="29">
@@ -2813,7 +2813,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="69"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -2834,7 +2834,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="69"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -2855,7 +2855,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="69"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -2876,7 +2876,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="69"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -2897,7 +2897,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="70"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -2918,7 +2918,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="69" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="25">
@@ -2941,7 +2941,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="69"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -2962,7 +2962,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="69"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -2983,7 +2983,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="69"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -3004,7 +3004,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="69"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -3025,7 +3025,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="70"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="69" t="s">
         <v>179</v>
       </c>
       <c r="B29" s="29">
@@ -3069,7 +3069,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="69"/>
+      <c r="A30" s="70"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -3090,7 +3090,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="69"/>
+      <c r="A31" s="70"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -3111,7 +3111,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="69"/>
+      <c r="A32" s="70"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -3132,7 +3132,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="69"/>
+      <c r="A33" s="70"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -3153,7 +3153,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="70"/>
+      <c r="A34" s="71"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -3174,7 +3174,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="68" t="s">
+      <c r="A35" s="69" t="s">
         <v>180</v>
       </c>
       <c r="B35" s="25">
@@ -3197,7 +3197,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="69"/>
+      <c r="A36" s="70"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -3218,7 +3218,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="69"/>
+      <c r="A37" s="70"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="69"/>
+      <c r="A38" s="70"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -3260,7 +3260,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="69"/>
+      <c r="A39" s="70"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -3281,7 +3281,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="70"/>
+      <c r="A40" s="71"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -3302,7 +3302,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="68" t="s">
+      <c r="A41" s="69" t="s">
         <v>181</v>
       </c>
       <c r="B41" s="29">
@@ -3325,7 +3325,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="69"/>
+      <c r="A42" s="70"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -3346,7 +3346,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="69"/>
+      <c r="A43" s="70"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -3367,7 +3367,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="69"/>
+      <c r="A44" s="70"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -3388,7 +3388,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="69"/>
+      <c r="A45" s="70"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -3409,7 +3409,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="70"/>
+      <c r="A46" s="71"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -3430,7 +3430,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="68" t="s">
+      <c r="A47" s="69" t="s">
         <v>182</v>
       </c>
       <c r="B47" s="25">
@@ -3453,7 +3453,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="69"/>
+      <c r="A48" s="70"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -3474,7 +3474,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="69"/>
+      <c r="A49" s="70"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -3495,7 +3495,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="69"/>
+      <c r="A50" s="70"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="69"/>
+      <c r="A51" s="70"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -3537,7 +3537,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="70"/>
+      <c r="A52" s="71"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -3596,7 +3596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:G44"/>
     </sheetView>
   </sheetViews>
@@ -3612,13 +3612,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
       <c r="F1" t="s">
         <v>333</v>
       </c>
@@ -3647,7 +3647,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="77" t="s">
         <v>343</v>
       </c>
       <c r="B3" s="25">
@@ -3668,7 +3668,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="79"/>
+      <c r="A4" s="78"/>
       <c r="B4" s="29">
         <v>152</v>
       </c>
@@ -3687,7 +3687,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="79"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="29">
         <v>153</v>
       </c>
@@ -3706,7 +3706,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="79"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="29">
         <v>154</v>
       </c>
@@ -3725,7 +3725,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="79"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="29">
         <v>155</v>
       </c>
@@ -3744,7 +3744,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="79"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="29">
         <v>156</v>
       </c>
@@ -3763,7 +3763,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="29">
         <v>157</v>
       </c>
@@ -3782,7 +3782,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="80"/>
+      <c r="A10" s="79"/>
       <c r="B10" s="22">
         <v>158</v>
       </c>
@@ -3801,7 +3801,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="77" t="s">
         <v>344</v>
       </c>
       <c r="B11" s="25">
@@ -3822,7 +3822,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="29">
         <v>160</v>
       </c>
@@ -3841,7 +3841,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="29">
         <v>161</v>
       </c>
@@ -3860,7 +3860,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="29">
         <v>162</v>
       </c>
@@ -3879,7 +3879,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="79"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="29">
         <v>163</v>
       </c>
@@ -3898,7 +3898,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="79"/>
+      <c r="A16" s="78"/>
       <c r="B16" s="29">
         <v>164</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="79"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="29">
         <v>165</v>
       </c>
@@ -3936,7 +3936,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="80"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="22">
         <v>166</v>
       </c>
@@ -3955,7 +3955,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="77" t="s">
         <v>345</v>
       </c>
       <c r="B19" s="25">
@@ -3976,7 +3976,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+      <c r="A20" s="78"/>
       <c r="B20" s="29">
         <v>168</v>
       </c>
@@ -3995,7 +3995,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+      <c r="A21" s="78"/>
       <c r="B21" s="29">
         <v>169</v>
       </c>
@@ -4014,7 +4014,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="79"/>
+      <c r="A22" s="78"/>
       <c r="B22" s="29">
         <v>170</v>
       </c>
@@ -4033,7 +4033,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="79"/>
+      <c r="A23" s="78"/>
       <c r="B23" s="29">
         <v>171</v>
       </c>
@@ -4052,7 +4052,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="79"/>
+      <c r="A24" s="78"/>
       <c r="B24" s="29">
         <v>172</v>
       </c>
@@ -4071,7 +4071,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="79"/>
+      <c r="A25" s="78"/>
       <c r="B25" s="29">
         <v>173</v>
       </c>
@@ -4090,7 +4090,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="80"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="22">
         <v>174</v>
       </c>
@@ -4109,7 +4109,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="77" t="s">
         <v>346</v>
       </c>
       <c r="B27" s="25">
@@ -4130,7 +4130,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="79"/>
+      <c r="A28" s="78"/>
       <c r="B28" s="29">
         <v>176</v>
       </c>
@@ -4149,7 +4149,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
+      <c r="A29" s="78"/>
       <c r="B29" s="29">
         <v>177</v>
       </c>
@@ -4168,7 +4168,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="79"/>
+      <c r="A30" s="78"/>
       <c r="B30" s="29">
         <v>178</v>
       </c>
@@ -4187,7 +4187,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="79"/>
+      <c r="A31" s="78"/>
       <c r="B31" s="29">
         <v>179</v>
       </c>
@@ -4206,7 +4206,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="79"/>
+      <c r="A32" s="78"/>
       <c r="B32" s="29">
         <v>180</v>
       </c>
@@ -4225,7 +4225,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="79"/>
+      <c r="A33" s="78"/>
       <c r="B33" s="29">
         <v>181</v>
       </c>
@@ -4244,7 +4244,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="80"/>
+      <c r="A34" s="79"/>
       <c r="B34" s="29">
         <v>182</v>
       </c>
@@ -4263,7 +4263,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="77" t="s">
         <v>349</v>
       </c>
       <c r="B35" s="25">
@@ -4279,12 +4279,12 @@
         <v>1</v>
       </c>
       <c r="F35" s="27"/>
-      <c r="G35" s="81" t="s">
+      <c r="G35" s="67" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="79"/>
+      <c r="A36" s="78"/>
       <c r="B36" s="29">
         <v>184</v>
       </c>
@@ -4303,7 +4303,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="79"/>
+      <c r="A37" s="78"/>
       <c r="B37" s="29">
         <v>185</v>
       </c>
@@ -4322,7 +4322,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="79"/>
+      <c r="A38" s="78"/>
       <c r="B38" s="29">
         <v>186</v>
       </c>
@@ -4341,7 +4341,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="79"/>
+      <c r="A39" s="78"/>
       <c r="B39" s="29">
         <v>187</v>
       </c>
@@ -4360,7 +4360,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="79"/>
+      <c r="A40" s="78"/>
       <c r="B40" s="29">
         <v>188</v>
       </c>
@@ -4379,7 +4379,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="79"/>
+      <c r="A41" s="78"/>
       <c r="B41" s="29">
         <v>189</v>
       </c>
@@ -4398,7 +4398,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="79"/>
+      <c r="A42" s="78"/>
       <c r="B42" s="29">
         <v>190</v>
       </c>
@@ -4417,7 +4417,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="79"/>
+      <c r="A43" s="78"/>
       <c r="B43" s="29">
         <v>191</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="80"/>
+      <c r="A44" s="79"/>
       <c r="B44" s="22">
         <v>192</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="78" t="s">
+      <c r="A45" s="77" t="s">
         <v>350</v>
       </c>
       <c r="B45" s="25">
@@ -4476,7 +4476,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="79"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="29">
         <v>194</v>
       </c>
@@ -4495,7 +4495,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="79"/>
+      <c r="A47" s="78"/>
       <c r="B47" s="29">
         <v>195</v>
       </c>
@@ -4514,7 +4514,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="79"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="29">
         <v>196</v>
       </c>
@@ -4533,7 +4533,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="79"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="29">
         <v>197</v>
       </c>
@@ -4552,7 +4552,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="79"/>
+      <c r="A50" s="78"/>
       <c r="B50" s="29">
         <v>198</v>
       </c>
@@ -4571,7 +4571,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="79"/>
+      <c r="A51" s="78"/>
       <c r="B51" s="29">
         <v>199</v>
       </c>
@@ -4590,7 +4590,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="79"/>
+      <c r="A52" s="78"/>
       <c r="B52" s="29">
         <v>200</v>
       </c>
@@ -4609,7 +4609,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="79"/>
+      <c r="A53" s="78"/>
       <c r="B53" s="29">
         <v>201</v>
       </c>
@@ -4628,7 +4628,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="80"/>
+      <c r="A54" s="79"/>
       <c r="B54" s="22">
         <v>202</v>
       </c>
@@ -4647,7 +4647,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="78" t="s">
+      <c r="A55" s="77" t="s">
         <v>351</v>
       </c>
       <c r="B55" s="25">
@@ -4668,7 +4668,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="79"/>
+      <c r="A56" s="78"/>
       <c r="B56" s="29">
         <v>204</v>
       </c>
@@ -4687,7 +4687,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="79"/>
+      <c r="A57" s="78"/>
       <c r="B57" s="29">
         <v>205</v>
       </c>
@@ -4706,7 +4706,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="79"/>
+      <c r="A58" s="78"/>
       <c r="B58" s="29">
         <v>206</v>
       </c>
@@ -4725,7 +4725,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="79"/>
+      <c r="A59" s="78"/>
       <c r="B59" s="29">
         <v>207</v>
       </c>
@@ -4744,7 +4744,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="79"/>
+      <c r="A60" s="78"/>
       <c r="B60" s="29">
         <v>208</v>
       </c>
@@ -4763,7 +4763,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="79"/>
+      <c r="A61" s="78"/>
       <c r="B61" s="29">
         <v>209</v>
       </c>
@@ -4782,7 +4782,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="79"/>
+      <c r="A62" s="78"/>
       <c r="B62" s="29">
         <v>210</v>
       </c>
@@ -4801,7 +4801,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="79"/>
+      <c r="A63" s="78"/>
       <c r="B63" s="29">
         <v>211</v>
       </c>
@@ -4820,7 +4820,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="80"/>
+      <c r="A64" s="79"/>
       <c r="B64" s="22">
         <v>212</v>
       </c>
@@ -4839,7 +4839,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="78" t="s">
+      <c r="A65" s="77" t="s">
         <v>352</v>
       </c>
       <c r="B65" s="25">
@@ -4860,7 +4860,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="79"/>
+      <c r="A66" s="78"/>
       <c r="B66" s="29">
         <v>214</v>
       </c>
@@ -4879,7 +4879,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="79"/>
+      <c r="A67" s="78"/>
       <c r="B67" s="29">
         <v>215</v>
       </c>
@@ -4898,7 +4898,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="79"/>
+      <c r="A68" s="78"/>
       <c r="B68" s="29">
         <v>216</v>
       </c>
@@ -4917,7 +4917,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="79"/>
+      <c r="A69" s="78"/>
       <c r="B69" s="29">
         <v>217</v>
       </c>
@@ -4936,7 +4936,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="79"/>
+      <c r="A70" s="78"/>
       <c r="B70" s="29">
         <v>218</v>
       </c>
@@ -4955,7 +4955,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="79"/>
+      <c r="A71" s="78"/>
       <c r="B71" s="29">
         <v>219</v>
       </c>
@@ -4974,7 +4974,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="79"/>
+      <c r="A72" s="78"/>
       <c r="B72" s="29">
         <v>220</v>
       </c>
@@ -4993,7 +4993,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="79"/>
+      <c r="A73" s="78"/>
       <c r="B73" s="29">
         <v>221</v>
       </c>
@@ -5012,7 +5012,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="80"/>
+      <c r="A74" s="79"/>
       <c r="B74" s="22">
         <v>222</v>
       </c>
@@ -5234,8 +5234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z267"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24199,25 +24199,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J1" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="76" t="s">
+      <c r="K1" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="M1" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="76" t="s">
+      <c r="N1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="76" t="s">
+      <c r="O1" s="80" t="s">
         <v>83</v>
       </c>
     </row>
@@ -24238,13 +24238,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -24266,13 +24266,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">

</xml_diff>

<commit_message>
v39.9  Fixed all issues that I had with displaying time editing in the menu.  Also added some delays to keep the previous button presses from triggering the next press.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Timing" sheetId="12" r:id="rId9"/>
     <sheet name="Sheet2" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -48,27 +48,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="J56" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Robbie:
-AMPM will start here.  Will use the modifier "space" to add spaces here.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="365">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1160,6 +1145,9 @@
   </si>
   <si>
     <t>char for storing a character for the sensor name</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -1796,6 +1784,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1831,6 +1836,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5234,7 +5256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -14299,10 +14321,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CG57"/>
+  <dimension ref="A1:CG64"/>
   <sheetViews>
-    <sheetView topLeftCell="B38" workbookViewId="0">
-      <selection activeCell="Y56" sqref="Y56"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -23326,13 +23348,13 @@
       <c r="M48" s="37">
         <v>1</v>
       </c>
-      <c r="N48" s="37"/>
+      <c r="N48" s="37" t="s">
+        <v>198</v>
+      </c>
       <c r="O48" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="P48" s="37" t="s">
         <v>199</v>
       </c>
+      <c r="P48" s="37"/>
       <c r="Q48" s="37"/>
       <c r="R48" s="37"/>
       <c r="S48" s="37"/>
@@ -23369,13 +23391,13 @@
       <c r="AH48" s="37">
         <v>1</v>
       </c>
-      <c r="AI48" s="37"/>
+      <c r="AI48" s="37" t="s">
+        <v>210</v>
+      </c>
       <c r="AJ48" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="AK48" s="37" t="s">
         <v>199</v>
       </c>
+      <c r="AK48" s="37"/>
       <c r="AL48" s="37"/>
       <c r="AM48" s="37"/>
       <c r="AN48" s="37"/>
@@ -23412,13 +23434,13 @@
       <c r="BC48" s="37">
         <v>1</v>
       </c>
-      <c r="BD48" s="37"/>
+      <c r="BD48" s="37" t="s">
+        <v>198</v>
+      </c>
       <c r="BE48" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="BF48" s="37" t="s">
         <v>199</v>
       </c>
+      <c r="BF48" s="37"/>
       <c r="BG48" s="37"/>
       <c r="BH48" s="37"/>
       <c r="BI48" s="37"/>
@@ -24108,11 +24130,10 @@
       <c r="I56" s="37">
         <v>1</v>
       </c>
-      <c r="J56" s="37"/>
+      <c r="J56" s="37" t="s">
+        <v>210</v>
+      </c>
       <c r="K56" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="L56" s="37" t="s">
         <v>199</v>
       </c>
       <c r="R56" s="36" t="s">
@@ -24152,6 +24173,170 @@
       <c r="U57" s="64"/>
       <c r="AR57" s="65"/>
       <c r="AS57" s="65"/>
+    </row>
+    <row r="58" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="D58" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="E58" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="G58" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="H58" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="I58" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="D59" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="E59" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="F59" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="G59" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="H59" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="I59" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="D60" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E60" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="F60" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="G60" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="H60" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="I60" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="J60" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="C61" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="D61" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="E61" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="G61" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="H61" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="I61" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="J61" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="K61" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="C62" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="E62" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="F62" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="G62" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="H62" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="I62" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="J62" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="D63" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="E63" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="F63" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="G63" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="H63" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="I63" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="C64" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="E64" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="F64" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="H64" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="I64" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="J64" s="36" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished up prototyping the menu buttons.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <sheet name="Menu Variables" sheetId="6" r:id="rId7"/>
     <sheet name="12 Hour" sheetId="10" r:id="rId8"/>
     <sheet name="Timing" sheetId="12" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId10"/>
+    <sheet name="Chart2" sheetId="16" r:id="rId10"/>
+    <sheet name="Chart1" sheetId="15" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="357">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -998,30 +1000,6 @@
   </si>
   <si>
     <t xml:space="preserve">No </t>
-  </si>
-  <si>
-    <t>loop()</t>
-  </si>
-  <si>
-    <t>poll menuMode to check to see if we should enter the menu</t>
-  </si>
-  <si>
-    <t>display the LCD Date</t>
-  </si>
-  <si>
-    <t>display the LCD Time</t>
-  </si>
-  <si>
-    <t>take a temp sensor reading</t>
-  </si>
-  <si>
-    <t>take a flow sensor reading</t>
-  </si>
-  <si>
-    <t>log sensor readings to the logfile</t>
-  </si>
-  <si>
-    <t>write the logfile to the SD card</t>
   </si>
   <si>
     <t>4 sensor readings</t>
@@ -1154,7 +1132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1217,6 +1195,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1305,7 +1290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1546,11 +1531,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1649,6 +1649,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1706,6 +1733,1586 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="987823712"/>
+        <c:axId val="987825792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="987823712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987825792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="987825792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987823712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="987638144"/>
+        <c:axId val="987639392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="987638144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987639392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="987639392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987638144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8661149" cy="6284614"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8667750" cy="6298406"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2044,12 +3651,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
+      <c r="A1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
       <c r="E1" t="s">
         <v>96</v>
       </c>
@@ -2210,56 +3817,317 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.21875" style="68" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="68" customWidth="1"/>
+    <col min="3" max="3" width="2.21875" style="68" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="68" customWidth="1"/>
+    <col min="5" max="5" width="2.21875" style="68" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" style="68" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" style="75" customWidth="1"/>
+    <col min="8" max="8" width="3.88671875" style="68" customWidth="1"/>
+    <col min="9" max="9" width="15" style="68" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" style="68" customWidth="1"/>
+    <col min="11" max="11" width="15" style="68" customWidth="1"/>
+    <col min="12" max="14" width="8.88671875" style="68"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>322</v>
+    <row r="1" spans="1:12" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="69">
+        <v>20</v>
+      </c>
+      <c r="B1" s="69">
+        <v>210</v>
+      </c>
+      <c r="C1" s="69">
+        <v>20</v>
+      </c>
+      <c r="D1" s="69">
+        <v>210</v>
+      </c>
+      <c r="E1" s="69">
+        <v>20</v>
+      </c>
+      <c r="F1" s="70">
+        <f>SUM(A1:E1)</f>
+        <v>480</v>
+      </c>
+      <c r="G1" s="74"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="69">
+        <v>135</v>
+      </c>
+      <c r="J1" s="69">
+        <v>210</v>
+      </c>
+      <c r="K1" s="69">
+        <v>135</v>
+      </c>
+      <c r="L1" s="68">
+        <f>SUM(I1:K1)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="69">
+        <v>40</v>
+      </c>
+      <c r="B2" s="71">
+        <v>40</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" s="74">
+        <v>20</v>
+      </c>
+      <c r="H2" s="76">
+        <f>20+40</f>
+        <v>60</v>
+      </c>
+      <c r="I2" s="69"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="69"/>
+    </row>
+    <row r="3" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="69">
+        <v>8</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+    </row>
+    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="69">
+        <v>40</v>
+      </c>
+      <c r="B4" s="71">
+        <v>40</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="G4" s="74">
+        <f>SUM(G2+48)</f>
+        <v>68</v>
+      </c>
+      <c r="H4" s="76">
+        <f>H2+48</f>
+        <v>108</v>
+      </c>
+      <c r="I4" s="69"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="69"/>
+    </row>
+    <row r="5" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="69">
+        <v>8</v>
+      </c>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+    </row>
+    <row r="6" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="69">
+        <v>40</v>
+      </c>
+      <c r="B6" s="71">
+        <v>40</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="G6" s="74">
+        <f>SUM(G4+48)</f>
+        <v>116</v>
+      </c>
+      <c r="H6" s="76">
+        <f>H4+48</f>
+        <v>156</v>
+      </c>
+      <c r="I6" s="69"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="69"/>
+    </row>
+    <row r="7" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="69">
+        <v>8</v>
+      </c>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+    </row>
+    <row r="8" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="69">
+        <v>40</v>
+      </c>
+      <c r="B8" s="71">
+        <v>40</v>
+      </c>
+      <c r="C8" s="69"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" s="74">
+        <f>SUM(G6+48)</f>
+        <v>164</v>
+      </c>
+      <c r="H8" s="76">
+        <f>H6+48</f>
+        <v>204</v>
+      </c>
+      <c r="I8" s="69"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="69"/>
+    </row>
+    <row r="9" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="69">
+        <v>8</v>
+      </c>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+    </row>
+    <row r="10" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="69">
+        <v>40</v>
+      </c>
+      <c r="B10" s="71">
+        <v>40</v>
+      </c>
+      <c r="C10" s="69"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70" t="s">
+        <v>217</v>
+      </c>
+      <c r="G10" s="74">
+        <f>SUM(G8+48)</f>
+        <v>212</v>
+      </c>
+      <c r="H10" s="76">
+        <f>H8+48</f>
+        <v>252</v>
+      </c>
+      <c r="I10" s="69"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="69"/>
+    </row>
+    <row r="11" spans="1:12" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="69">
+        <v>20</v>
+      </c>
+      <c r="B11" s="69">
+        <v>20</v>
+      </c>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="68">
+        <f>SUM(A1:A11)</f>
+        <v>272</v>
+      </c>
+      <c r="G12" s="74">
+        <f>SUM(G10+40+20)</f>
+        <v>272</v>
+      </c>
+      <c r="H12" s="76">
+        <f>H10+20</f>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="73">
+        <v>20</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="73">
+        <v>250</v>
+      </c>
+      <c r="H13" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="I13" s="68">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="72">
+        <f>20+210</f>
+        <v>230</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" s="72">
+        <v>460</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2281,12 +4149,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
       <c r="E1" t="s">
         <v>95</v>
       </c>
@@ -2478,18 +4346,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="76"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="85"/>
       <c r="F1" s="19" t="s">
         <v>108</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2514,7 +4382,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
+      <c r="A3" s="81"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -2535,7 +4403,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
+      <c r="A4" s="82"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -2556,7 +4424,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="78" t="s">
         <v>175</v>
       </c>
       <c r="B5" s="25">
@@ -2579,7 +4447,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="70"/>
+      <c r="A6" s="79"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -2600,7 +4468,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="70"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -2621,7 +4489,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="70"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -2642,7 +4510,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="70"/>
+      <c r="A9" s="79"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -2663,7 +4531,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="71"/>
+      <c r="A10" s="80"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -2684,7 +4552,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="78" t="s">
         <v>176</v>
       </c>
       <c r="B11" s="25">
@@ -2707,7 +4575,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -2728,7 +4596,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="70"/>
+      <c r="A13" s="79"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -2749,7 +4617,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="70"/>
+      <c r="A14" s="79"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -2770,7 +4638,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="70"/>
+      <c r="A15" s="79"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -2791,7 +4659,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="71"/>
+      <c r="A16" s="80"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -2812,7 +4680,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="78" t="s">
         <v>177</v>
       </c>
       <c r="B17" s="29">
@@ -2835,7 +4703,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="70"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -2856,7 +4724,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="70"/>
+      <c r="A19" s="79"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -2877,7 +4745,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="70"/>
+      <c r="A20" s="79"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -2898,7 +4766,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="70"/>
+      <c r="A21" s="79"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -2919,7 +4787,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="71"/>
+      <c r="A22" s="80"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -2940,7 +4808,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="78" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="25">
@@ -2963,7 +4831,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="70"/>
+      <c r="A24" s="79"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -2984,7 +4852,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="70"/>
+      <c r="A25" s="79"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -3005,7 +4873,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="70"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -3026,7 +4894,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="70"/>
+      <c r="A27" s="79"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -3047,7 +4915,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="71"/>
+      <c r="A28" s="80"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -3068,7 +4936,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="78" t="s">
         <v>179</v>
       </c>
       <c r="B29" s="29">
@@ -3091,7 +4959,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="70"/>
+      <c r="A30" s="79"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -3112,7 +4980,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="70"/>
+      <c r="A31" s="79"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -3133,7 +5001,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="70"/>
+      <c r="A32" s="79"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -3154,7 +5022,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="70"/>
+      <c r="A33" s="79"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -3175,7 +5043,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="71"/>
+      <c r="A34" s="80"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -3196,7 +5064,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="78" t="s">
         <v>180</v>
       </c>
       <c r="B35" s="25">
@@ -3219,7 +5087,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="70"/>
+      <c r="A36" s="79"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -3240,7 +5108,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="70"/>
+      <c r="A37" s="79"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -3261,7 +5129,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="70"/>
+      <c r="A38" s="79"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -3282,7 +5150,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="70"/>
+      <c r="A39" s="79"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -3303,7 +5171,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="71"/>
+      <c r="A40" s="80"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -3324,7 +5192,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="69" t="s">
+      <c r="A41" s="78" t="s">
         <v>181</v>
       </c>
       <c r="B41" s="29">
@@ -3347,7 +5215,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="70"/>
+      <c r="A42" s="79"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -3368,7 +5236,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="70"/>
+      <c r="A43" s="79"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -3389,7 +5257,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="70"/>
+      <c r="A44" s="79"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -3410,7 +5278,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="70"/>
+      <c r="A45" s="79"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -3431,7 +5299,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="71"/>
+      <c r="A46" s="80"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -3452,7 +5320,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="69" t="s">
+      <c r="A47" s="78" t="s">
         <v>182</v>
       </c>
       <c r="B47" s="25">
@@ -3475,7 +5343,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="70"/>
+      <c r="A48" s="79"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -3496,7 +5364,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="70"/>
+      <c r="A49" s="79"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -3517,7 +5385,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="70"/>
+      <c r="A50" s="79"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -3538,7 +5406,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="70"/>
+      <c r="A51" s="79"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -3559,7 +5427,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="71"/>
+      <c r="A52" s="80"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -3634,18 +5502,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
       <c r="F1" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="G1" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3669,14 +5537,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
-        <v>343</v>
+      <c r="A3" s="86" t="s">
+        <v>335</v>
       </c>
       <c r="B3" s="25">
         <v>151</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>94</v>
@@ -3686,16 +5554,16 @@
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="28" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="78"/>
+      <c r="A4" s="87"/>
       <c r="B4" s="29">
         <v>152</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>94</v>
@@ -3705,16 +5573,16 @@
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="78"/>
+      <c r="A5" s="87"/>
       <c r="B5" s="29">
         <v>153</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>94</v>
@@ -3724,16 +5592,16 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="78"/>
+      <c r="A6" s="87"/>
       <c r="B6" s="29">
         <v>154</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>94</v>
@@ -3743,16 +5611,16 @@
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="78"/>
+      <c r="A7" s="87"/>
       <c r="B7" s="29">
         <v>155</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>94</v>
@@ -3762,16 +5630,16 @@
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="78"/>
+      <c r="A8" s="87"/>
       <c r="B8" s="29">
         <v>156</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>94</v>
@@ -3781,16 +5649,16 @@
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="78"/>
+      <c r="A9" s="87"/>
       <c r="B9" s="29">
         <v>157</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>94</v>
@@ -3800,16 +5668,16 @@
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="79"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="22">
         <v>158</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>94</v>
@@ -3819,18 +5687,18 @@
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="32" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="77" t="s">
-        <v>344</v>
+      <c r="A11" s="86" t="s">
+        <v>336</v>
       </c>
       <c r="B11" s="25">
         <v>159</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>94</v>
@@ -3840,16 +5708,16 @@
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="28" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="78"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="29">
         <v>160</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>94</v>
@@ -3859,16 +5727,16 @@
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+      <c r="A13" s="87"/>
       <c r="B13" s="29">
         <v>161</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>94</v>
@@ -3878,16 +5746,16 @@
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="78"/>
+      <c r="A14" s="87"/>
       <c r="B14" s="29">
         <v>162</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>94</v>
@@ -3897,16 +5765,16 @@
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="78"/>
+      <c r="A15" s="87"/>
       <c r="B15" s="29">
         <v>163</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>94</v>
@@ -3916,16 +5784,16 @@
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="78"/>
+      <c r="A16" s="87"/>
       <c r="B16" s="29">
         <v>164</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>94</v>
@@ -3935,16 +5803,16 @@
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="78"/>
+      <c r="A17" s="87"/>
       <c r="B17" s="29">
         <v>165</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>94</v>
@@ -3954,16 +5822,16 @@
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="79"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="22">
         <v>166</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>94</v>
@@ -3973,18 +5841,18 @@
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="32" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
-        <v>345</v>
+      <c r="A19" s="86" t="s">
+        <v>337</v>
       </c>
       <c r="B19" s="25">
         <v>167</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>94</v>
@@ -3994,16 +5862,16 @@
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="28" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
+      <c r="A20" s="87"/>
       <c r="B20" s="29">
         <v>168</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>94</v>
@@ -4013,16 +5881,16 @@
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="78"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="29">
         <v>169</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>94</v>
@@ -4032,16 +5900,16 @@
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="78"/>
+      <c r="A22" s="87"/>
       <c r="B22" s="29">
         <v>170</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>94</v>
@@ -4051,16 +5919,16 @@
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="78"/>
+      <c r="A23" s="87"/>
       <c r="B23" s="29">
         <v>171</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>94</v>
@@ -4070,16 +5938,16 @@
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="78"/>
+      <c r="A24" s="87"/>
       <c r="B24" s="29">
         <v>172</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>94</v>
@@ -4089,16 +5957,16 @@
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="78"/>
+      <c r="A25" s="87"/>
       <c r="B25" s="29">
         <v>173</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>94</v>
@@ -4108,16 +5976,16 @@
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="79"/>
+      <c r="A26" s="88"/>
       <c r="B26" s="22">
         <v>174</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D26" s="31" t="s">
         <v>94</v>
@@ -4127,18 +5995,18 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="32" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="77" t="s">
-        <v>346</v>
+      <c r="A27" s="86" t="s">
+        <v>338</v>
       </c>
       <c r="B27" s="25">
         <v>175</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>94</v>
@@ -4148,16 +6016,16 @@
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="28" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="78"/>
+      <c r="A28" s="87"/>
       <c r="B28" s="29">
         <v>176</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>94</v>
@@ -4167,16 +6035,16 @@
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="78"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="29">
         <v>177</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>94</v>
@@ -4186,16 +6054,16 @@
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="78"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="29">
         <v>178</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>94</v>
@@ -4205,16 +6073,16 @@
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="78"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="29">
         <v>179</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>94</v>
@@ -4224,16 +6092,16 @@
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="78"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="29">
         <v>180</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>94</v>
@@ -4243,16 +6111,16 @@
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="78"/>
+      <c r="A33" s="87"/>
       <c r="B33" s="29">
         <v>181</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>94</v>
@@ -4262,16 +6130,16 @@
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="79"/>
+      <c r="A34" s="88"/>
       <c r="B34" s="29">
         <v>182</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>94</v>
@@ -4281,775 +6149,775 @@
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="30" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="77" t="s">
-        <v>349</v>
+      <c r="A35" s="86" t="s">
+        <v>341</v>
       </c>
       <c r="B35" s="25">
         <v>183</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E35" s="12">
         <v>1</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="67" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="78"/>
+      <c r="A36" s="87"/>
       <c r="B36" s="29">
         <v>184</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E36" s="11">
         <v>1</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="78"/>
+      <c r="A37" s="87"/>
       <c r="B37" s="29">
         <v>185</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E37" s="11">
         <v>1</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="78"/>
+      <c r="A38" s="87"/>
       <c r="B38" s="29">
         <v>186</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E38" s="11">
         <v>1</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="78"/>
+      <c r="A39" s="87"/>
       <c r="B39" s="29">
         <v>187</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E39" s="11">
         <v>1</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="78"/>
+      <c r="A40" s="87"/>
       <c r="B40" s="29">
         <v>188</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E40" s="11">
         <v>1</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="78"/>
+      <c r="A41" s="87"/>
       <c r="B41" s="29">
         <v>189</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E41" s="11">
         <v>1</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="78"/>
+      <c r="A42" s="87"/>
       <c r="B42" s="29">
         <v>190</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E42" s="11">
         <v>1</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="78"/>
+      <c r="A43" s="87"/>
       <c r="B43" s="29">
         <v>191</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E43" s="11">
         <v>1</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="79"/>
+      <c r="A44" s="88"/>
       <c r="B44" s="22">
         <v>192</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E44" s="13">
         <v>1</v>
       </c>
       <c r="F44" s="24"/>
       <c r="G44" s="32" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="77" t="s">
-        <v>350</v>
+      <c r="A45" s="86" t="s">
+        <v>342</v>
       </c>
       <c r="B45" s="25">
         <v>193</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E45" s="12">
         <v>1</v>
       </c>
       <c r="F45" s="27"/>
       <c r="G45" s="28" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="78"/>
+      <c r="A46" s="87"/>
       <c r="B46" s="29">
         <v>194</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E46" s="11">
         <v>1</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="78"/>
+      <c r="A47" s="87"/>
       <c r="B47" s="29">
         <v>195</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E47" s="11">
         <v>1</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="78"/>
+      <c r="A48" s="87"/>
       <c r="B48" s="29">
         <v>196</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E48" s="11">
         <v>1</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="78"/>
+      <c r="A49" s="87"/>
       <c r="B49" s="29">
         <v>197</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E49" s="11">
         <v>1</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="78"/>
+      <c r="A50" s="87"/>
       <c r="B50" s="29">
         <v>198</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E50" s="11">
         <v>1</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="78"/>
+      <c r="A51" s="87"/>
       <c r="B51" s="29">
         <v>199</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E51" s="11">
         <v>1</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="78"/>
+      <c r="A52" s="87"/>
       <c r="B52" s="29">
         <v>200</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E52" s="11">
         <v>1</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="78"/>
+      <c r="A53" s="87"/>
       <c r="B53" s="29">
         <v>201</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E53" s="11">
         <v>1</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="79"/>
+      <c r="A54" s="88"/>
       <c r="B54" s="22">
         <v>202</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E54" s="13">
         <v>1</v>
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="32" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="77" t="s">
-        <v>351</v>
+      <c r="A55" s="86" t="s">
+        <v>343</v>
       </c>
       <c r="B55" s="25">
         <v>203</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E55" s="12">
         <v>1</v>
       </c>
       <c r="F55" s="27"/>
       <c r="G55" s="28" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="78"/>
+      <c r="A56" s="87"/>
       <c r="B56" s="29">
         <v>204</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E56" s="11">
         <v>1</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="78"/>
+      <c r="A57" s="87"/>
       <c r="B57" s="29">
         <v>205</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E57" s="11">
         <v>1</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="78"/>
+      <c r="A58" s="87"/>
       <c r="B58" s="29">
         <v>206</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E58" s="11">
         <v>1</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="78"/>
+      <c r="A59" s="87"/>
       <c r="B59" s="29">
         <v>207</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E59" s="11">
         <v>1</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="78"/>
+      <c r="A60" s="87"/>
       <c r="B60" s="29">
         <v>208</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E60" s="11">
         <v>1</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="78"/>
+      <c r="A61" s="87"/>
       <c r="B61" s="29">
         <v>209</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E61" s="11">
         <v>1</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="78"/>
+      <c r="A62" s="87"/>
       <c r="B62" s="29">
         <v>210</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E62" s="11">
         <v>1</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="78"/>
+      <c r="A63" s="87"/>
       <c r="B63" s="29">
         <v>211</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E63" s="11">
         <v>1</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="79"/>
+      <c r="A64" s="88"/>
       <c r="B64" s="22">
         <v>212</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E64" s="13">
         <v>1</v>
       </c>
       <c r="F64" s="24"/>
       <c r="G64" s="32" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="77" t="s">
-        <v>352</v>
+      <c r="A65" s="86" t="s">
+        <v>344</v>
       </c>
       <c r="B65" s="25">
         <v>213</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E65" s="12">
         <v>1</v>
       </c>
       <c r="F65" s="27"/>
       <c r="G65" s="28" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="78"/>
+      <c r="A66" s="87"/>
       <c r="B66" s="29">
         <v>214</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E66" s="11">
         <v>1</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="78"/>
+      <c r="A67" s="87"/>
       <c r="B67" s="29">
         <v>215</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E67" s="11">
         <v>1</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="78"/>
+      <c r="A68" s="87"/>
       <c r="B68" s="29">
         <v>216</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E68" s="11">
         <v>1</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="78"/>
+      <c r="A69" s="87"/>
       <c r="B69" s="29">
         <v>217</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E69" s="11">
         <v>1</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="78"/>
+      <c r="A70" s="87"/>
       <c r="B70" s="29">
         <v>218</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E70" s="11">
         <v>1</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="78"/>
+      <c r="A71" s="87"/>
       <c r="B71" s="29">
         <v>219</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E71" s="11">
         <v>1</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="78"/>
+      <c r="A72" s="87"/>
       <c r="B72" s="29">
         <v>220</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E72" s="11">
         <v>1</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="78"/>
+      <c r="A73" s="87"/>
       <c r="B73" s="29">
         <v>221</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E73" s="11">
         <v>1</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="30" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="79"/>
+      <c r="A74" s="88"/>
       <c r="B74" s="22">
         <v>222</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E74" s="13">
         <v>1</v>
       </c>
       <c r="F74" s="24"/>
       <c r="G74" s="32" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -5057,7 +6925,7 @@
         <v>223</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -5065,7 +6933,7 @@
         <v>224</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -5073,7 +6941,7 @@
         <v>225</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -5081,7 +6949,7 @@
         <v>226</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -5089,7 +6957,7 @@
         <v>227</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -5097,7 +6965,7 @@
         <v>228</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">
@@ -14323,8 +16191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -24179,7 +26047,7 @@
         <v>190</v>
       </c>
       <c r="E58" s="36" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F58" s="36" t="s">
         <v>232</v>
@@ -24219,7 +26087,7 @@
         <v>193</v>
       </c>
       <c r="E60" s="36" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F60" s="36" t="s">
         <v>201</v>
@@ -24274,7 +26142,7 @@
         <v>204</v>
       </c>
       <c r="E62" s="36" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F62" s="36" t="s">
         <v>216</v>
@@ -24323,7 +26191,7 @@
         <v>193</v>
       </c>
       <c r="F64" s="36" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="G64" s="36" t="s">
         <v>216</v>
@@ -24384,25 +26252,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="80" t="s">
+      <c r="I1" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="80" t="s">
+      <c r="J1" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="80" t="s">
+      <c r="K1" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="80" t="s">
+      <c r="L1" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="80" t="s">
+      <c r="M1" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="80" t="s">
+      <c r="N1" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="80" t="s">
+      <c r="O1" s="89" t="s">
         <v>83</v>
       </c>
     </row>
@@ -24423,13 +26291,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -24451,13 +26319,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -27846,12 +29714,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B2">
         <v>3736</v>
@@ -27871,7 +29739,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B3">
         <v>4486</v>
@@ -27891,7 +29759,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B4">
         <f>B3-B2</f>
@@ -27916,7 +29784,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="F6">
         <f>F4-F9</f>
@@ -27925,7 +29793,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B7">
         <v>3599</v>
@@ -27945,7 +29813,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B8">
         <v>4187</v>
@@ -27965,7 +29833,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B9">
         <f>B8-B7</f>
@@ -27990,7 +29858,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="F11">
         <f>F9-F14</f>
@@ -27999,7 +29867,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B12">
         <v>3485</v>
@@ -28019,7 +29887,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B13">
         <v>3926</v>
@@ -28039,7 +29907,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B14">
         <f>B13-B12</f>
@@ -28064,7 +29932,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="F16">
         <f>F14-F19</f>
@@ -28073,7 +29941,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B17">
         <v>3397</v>
@@ -28093,7 +29961,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B18">
         <v>3705</v>
@@ -28113,7 +29981,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B19">
         <f>B18-B17</f>
@@ -28138,12 +30006,12 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B22">
         <v>4187</v>
@@ -28163,7 +30031,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B23">
         <v>4196</v>
@@ -28183,7 +30051,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B24">
         <f>B23-B22</f>
@@ -28208,12 +30076,12 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B27">
         <v>60777</v>
@@ -28233,7 +30101,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B28">
         <v>60788</v>
@@ -28253,7 +30121,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B29">
         <f>B28-B27</f>
@@ -28278,12 +30146,12 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B32">
         <v>5000</v>
@@ -28303,7 +30171,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B33">
         <v>5000</v>
@@ -28323,7 +30191,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B34">
         <v>5014</v>
@@ -28343,7 +30211,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B35">
         <f>B34-B33</f>

</xml_diff>

<commit_message>
v40.1 Still working on the touch menu.  Basic idea of how to print the buttons and text.  Still need to get the touch areas working and sending it to the proper functions to do stuff.   Defined arrays to easily find what the touch areas are for each button.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Timing" sheetId="12" r:id="rId9"/>
     <sheet name="Chart2" sheetId="16" r:id="rId10"/>
     <sheet name="Chart1" sheetId="15" r:id="rId11"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId12"/>
+    <sheet name="TFT Menu" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="359">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1126,13 +1126,19 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1198,6 +1204,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1550,7 +1563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1658,9 +1671,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1717,6 +1727,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3243,7 +3259,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3254,7 +3270,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3265,7 +3281,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661149" cy="6284614"/>
+    <xdr:ext cx="8648700" cy="6276975"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3292,7 +3308,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6298406"/>
+    <xdr:ext cx="8648700" cy="6276975"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3651,12 +3667,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
       <c r="E1" t="s">
         <v>96</v>
       </c>
@@ -3820,7 +3836,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3831,7 +3847,7 @@
     <col min="4" max="4" width="23.33203125" style="68" customWidth="1"/>
     <col min="5" max="5" width="2.21875" style="68" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" style="68" customWidth="1"/>
-    <col min="7" max="7" width="3.88671875" style="75" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" style="74" customWidth="1"/>
     <col min="8" max="8" width="3.88671875" style="68" customWidth="1"/>
     <col min="9" max="9" width="15" style="68" customWidth="1"/>
     <col min="10" max="10" width="23.33203125" style="68" customWidth="1"/>
@@ -3839,7 +3855,7 @@
     <col min="12" max="14" width="8.88671875" style="68"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69">
         <v>20</v>
       </c>
@@ -3859,8 +3875,12 @@
         <f>SUM(A1:E1)</f>
         <v>480</v>
       </c>
-      <c r="G1" s="74"/>
-      <c r="H1" s="70"/>
+      <c r="G1" s="73" t="s">
+        <v>357</v>
+      </c>
+      <c r="H1" s="70" t="s">
+        <v>358</v>
+      </c>
       <c r="I1" s="69">
         <v>135</v>
       </c>
@@ -3875,28 +3895,28 @@
         <v>480</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="69">
         <v>40</v>
       </c>
-      <c r="B2" s="71">
+      <c r="B2" s="90">
         <v>40</v>
       </c>
       <c r="C2" s="69"/>
-      <c r="D2" s="71"/>
+      <c r="D2" s="90"/>
       <c r="E2" s="69"/>
       <c r="F2" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="G2" s="74">
+      <c r="G2" s="73">
         <v>20</v>
       </c>
-      <c r="H2" s="76">
+      <c r="H2" s="75">
         <f>20+40</f>
         <v>60</v>
       </c>
       <c r="I2" s="69"/>
-      <c r="J2" s="71"/>
+      <c r="J2" s="90"/>
       <c r="K2" s="69"/>
     </row>
     <row r="3" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3908,7 +3928,7 @@
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
       <c r="F3" s="70"/>
-      <c r="G3" s="74"/>
+      <c r="G3" s="73"/>
       <c r="H3" s="70"/>
       <c r="I3" s="69"/>
       <c r="J3" s="69"/>
@@ -3918,25 +3938,29 @@
       <c r="A4" s="69">
         <v>40</v>
       </c>
-      <c r="B4" s="71">
-        <v>40</v>
+      <c r="B4" s="91">
+        <v>1</v>
       </c>
       <c r="C4" s="69"/>
-      <c r="D4" s="71"/>
+      <c r="D4" s="91">
+        <v>2</v>
+      </c>
       <c r="E4" s="69"/>
       <c r="F4" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="G4" s="74">
+      <c r="G4" s="73">
         <f>SUM(G2+48)</f>
         <v>68</v>
       </c>
-      <c r="H4" s="76">
+      <c r="H4" s="75">
         <f>H2+48</f>
         <v>108</v>
       </c>
       <c r="I4" s="69"/>
-      <c r="J4" s="71"/>
+      <c r="J4" s="91">
+        <v>1</v>
+      </c>
       <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3948,7 +3972,7 @@
       <c r="D5" s="69"/>
       <c r="E5" s="69"/>
       <c r="F5" s="70"/>
-      <c r="G5" s="74"/>
+      <c r="G5" s="73"/>
       <c r="H5" s="70"/>
       <c r="I5" s="69"/>
       <c r="J5" s="69"/>
@@ -3958,25 +3982,29 @@
       <c r="A6" s="69">
         <v>40</v>
       </c>
-      <c r="B6" s="71">
-        <v>40</v>
+      <c r="B6" s="91">
+        <v>3</v>
       </c>
       <c r="C6" s="69"/>
-      <c r="D6" s="71"/>
+      <c r="D6" s="91">
+        <v>4</v>
+      </c>
       <c r="E6" s="69"/>
       <c r="F6" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="73">
         <f>SUM(G4+48)</f>
         <v>116</v>
       </c>
-      <c r="H6" s="76">
+      <c r="H6" s="75">
         <f>H4+48</f>
         <v>156</v>
       </c>
       <c r="I6" s="69"/>
-      <c r="J6" s="71"/>
+      <c r="J6" s="91">
+        <v>2</v>
+      </c>
       <c r="K6" s="69"/>
     </row>
     <row r="7" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3988,7 +4016,7 @@
       <c r="D7" s="69"/>
       <c r="E7" s="69"/>
       <c r="F7" s="70"/>
-      <c r="G7" s="74"/>
+      <c r="G7" s="73"/>
       <c r="H7" s="70"/>
       <c r="I7" s="69"/>
       <c r="J7" s="69"/>
@@ -3998,25 +4026,29 @@
       <c r="A8" s="69">
         <v>40</v>
       </c>
-      <c r="B8" s="71">
-        <v>40</v>
+      <c r="B8" s="91">
+        <v>5</v>
       </c>
       <c r="C8" s="69"/>
-      <c r="D8" s="71"/>
+      <c r="D8" s="91">
+        <v>6</v>
+      </c>
       <c r="E8" s="69"/>
       <c r="F8" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="G8" s="74">
+      <c r="G8" s="73">
         <f>SUM(G6+48)</f>
         <v>164</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="75">
         <f>H6+48</f>
         <v>204</v>
       </c>
       <c r="I8" s="69"/>
-      <c r="J8" s="71"/>
+      <c r="J8" s="91">
+        <v>3</v>
+      </c>
       <c r="K8" s="69"/>
     </row>
     <row r="9" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4028,7 +4060,7 @@
       <c r="D9" s="69"/>
       <c r="E9" s="69"/>
       <c r="F9" s="70"/>
-      <c r="G9" s="74"/>
+      <c r="G9" s="73"/>
       <c r="H9" s="70"/>
       <c r="I9" s="69"/>
       <c r="J9" s="69"/>
@@ -4038,25 +4070,29 @@
       <c r="A10" s="69">
         <v>40</v>
       </c>
-      <c r="B10" s="71">
-        <v>40</v>
+      <c r="B10" s="91">
+        <v>7</v>
       </c>
       <c r="C10" s="69"/>
-      <c r="D10" s="71"/>
+      <c r="D10" s="91">
+        <v>8</v>
+      </c>
       <c r="E10" s="69"/>
       <c r="F10" s="70" t="s">
         <v>217</v>
       </c>
-      <c r="G10" s="74">
+      <c r="G10" s="73">
         <f>SUM(G8+48)</f>
         <v>212</v>
       </c>
-      <c r="H10" s="76">
+      <c r="H10" s="75">
         <f>H8+48</f>
         <v>252</v>
       </c>
       <c r="I10" s="69"/>
-      <c r="J10" s="71"/>
+      <c r="J10" s="91">
+        <v>4</v>
+      </c>
       <c r="K10" s="69"/>
     </row>
     <row r="11" spans="1:12" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4070,7 +4106,7 @@
       <c r="D11" s="69"/>
       <c r="E11" s="69"/>
       <c r="F11" s="70"/>
-      <c r="G11" s="74"/>
+      <c r="G11" s="73"/>
       <c r="H11" s="70"/>
       <c r="I11" s="69"/>
       <c r="J11" s="69"/>
@@ -4081,11 +4117,11 @@
         <f>SUM(A1:A11)</f>
         <v>272</v>
       </c>
-      <c r="G12" s="74">
+      <c r="G12" s="73">
         <f>SUM(G10+40+20)</f>
         <v>272</v>
       </c>
-      <c r="H12" s="76">
+      <c r="H12" s="75">
         <f>H10+20</f>
         <v>272</v>
       </c>
@@ -4094,19 +4130,25 @@
       <c r="A13" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="B13" s="73">
+      <c r="B13" s="72">
         <v>20</v>
       </c>
       <c r="C13" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="73">
+      <c r="D13" s="72">
         <v>250</v>
+      </c>
+      <c r="F13" s="68" t="s">
+        <v>357</v>
       </c>
       <c r="H13" s="68" t="s">
         <v>203</v>
       </c>
       <c r="I13" s="68">
+        <v>135</v>
+      </c>
+      <c r="J13" s="72">
         <v>135</v>
       </c>
     </row>
@@ -4114,15 +4156,21 @@
       <c r="A14" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="72">
+      <c r="B14" s="71">
         <f>20+210</f>
         <v>230</v>
       </c>
       <c r="C14" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="D14" s="72">
+      <c r="D14" s="71">
         <v>460</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>358</v>
+      </c>
+      <c r="J14" s="71">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -4149,12 +4197,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
       <c r="E1" t="s">
         <v>95</v>
       </c>
@@ -4346,13 +4394,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="85"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84"/>
       <c r="F1" s="19" t="s">
         <v>108</v>
       </c>
@@ -4382,7 +4430,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="81"/>
+      <c r="A3" s="80"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -4403,7 +4451,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="82"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -4424,7 +4472,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="77" t="s">
         <v>175</v>
       </c>
       <c r="B5" s="25">
@@ -4447,7 +4495,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="79"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -4468,7 +4516,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="79"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -4489,7 +4537,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="79"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -4510,7 +4558,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="79"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -4531,7 +4579,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="80"/>
+      <c r="A10" s="79"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -4552,7 +4600,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="77" t="s">
         <v>176</v>
       </c>
       <c r="B11" s="25">
@@ -4575,7 +4623,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="79"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -4596,7 +4644,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -4617,7 +4665,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -4638,7 +4686,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="79"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -4659,7 +4707,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="80"/>
+      <c r="A16" s="79"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -4680,7 +4728,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="77" t="s">
         <v>177</v>
       </c>
       <c r="B17" s="29">
@@ -4703,7 +4751,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="79"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -4724,7 +4772,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="79"/>
+      <c r="A19" s="78"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -4745,7 +4793,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+      <c r="A20" s="78"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -4766,7 +4814,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+      <c r="A21" s="78"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -4787,7 +4835,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="80"/>
+      <c r="A22" s="79"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -4808,7 +4856,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="77" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="25">
@@ -4831,7 +4879,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="79"/>
+      <c r="A24" s="78"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -4852,7 +4900,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="79"/>
+      <c r="A25" s="78"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -4873,7 +4921,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="79"/>
+      <c r="A26" s="78"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -4894,7 +4942,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="79"/>
+      <c r="A27" s="78"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -4915,7 +4963,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="80"/>
+      <c r="A28" s="79"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -4936,7 +4984,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="77" t="s">
         <v>179</v>
       </c>
       <c r="B29" s="29">
@@ -4959,7 +5007,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="79"/>
+      <c r="A30" s="78"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -4980,7 +5028,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="79"/>
+      <c r="A31" s="78"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -5001,7 +5049,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="79"/>
+      <c r="A32" s="78"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -5022,7 +5070,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="79"/>
+      <c r="A33" s="78"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -5043,7 +5091,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="80"/>
+      <c r="A34" s="79"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -5064,7 +5112,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="77" t="s">
         <v>180</v>
       </c>
       <c r="B35" s="25">
@@ -5087,7 +5135,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="79"/>
+      <c r="A36" s="78"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -5108,7 +5156,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="79"/>
+      <c r="A37" s="78"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -5129,7 +5177,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="79"/>
+      <c r="A38" s="78"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -5150,7 +5198,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="79"/>
+      <c r="A39" s="78"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -5171,7 +5219,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="80"/>
+      <c r="A40" s="79"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -5192,7 +5240,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="78" t="s">
+      <c r="A41" s="77" t="s">
         <v>181</v>
       </c>
       <c r="B41" s="29">
@@ -5215,7 +5263,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="79"/>
+      <c r="A42" s="78"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -5236,7 +5284,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="79"/>
+      <c r="A43" s="78"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -5257,7 +5305,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="79"/>
+      <c r="A44" s="78"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -5278,7 +5326,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="79"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -5299,7 +5347,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="80"/>
+      <c r="A46" s="79"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -5320,7 +5368,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="78" t="s">
+      <c r="A47" s="77" t="s">
         <v>182</v>
       </c>
       <c r="B47" s="25">
@@ -5343,7 +5391,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="79"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -5364,7 +5412,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="79"/>
+      <c r="A49" s="78"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -5385,7 +5433,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="79"/>
+      <c r="A50" s="78"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -5406,7 +5454,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="79"/>
+      <c r="A51" s="78"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -5427,7 +5475,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="80"/>
+      <c r="A52" s="79"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -5502,13 +5550,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
       <c r="F1" t="s">
         <v>325</v>
       </c>
@@ -5537,7 +5585,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="85" t="s">
         <v>335</v>
       </c>
       <c r="B3" s="25">
@@ -5558,7 +5606,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
+      <c r="A4" s="86"/>
       <c r="B4" s="29">
         <v>152</v>
       </c>
@@ -5577,7 +5625,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="87"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="29">
         <v>153</v>
       </c>
@@ -5596,7 +5644,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="87"/>
+      <c r="A6" s="86"/>
       <c r="B6" s="29">
         <v>154</v>
       </c>
@@ -5615,7 +5663,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="87"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="29">
         <v>155</v>
       </c>
@@ -5634,7 +5682,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="87"/>
+      <c r="A8" s="86"/>
       <c r="B8" s="29">
         <v>156</v>
       </c>
@@ -5653,7 +5701,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="87"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="29">
         <v>157</v>
       </c>
@@ -5672,7 +5720,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="88"/>
+      <c r="A10" s="87"/>
       <c r="B10" s="22">
         <v>158</v>
       </c>
@@ -5691,7 +5739,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="86" t="s">
+      <c r="A11" s="85" t="s">
         <v>336</v>
       </c>
       <c r="B11" s="25">
@@ -5712,7 +5760,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="87"/>
+      <c r="A12" s="86"/>
       <c r="B12" s="29">
         <v>160</v>
       </c>
@@ -5731,7 +5779,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="87"/>
+      <c r="A13" s="86"/>
       <c r="B13" s="29">
         <v>161</v>
       </c>
@@ -5750,7 +5798,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="87"/>
+      <c r="A14" s="86"/>
       <c r="B14" s="29">
         <v>162</v>
       </c>
@@ -5769,7 +5817,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="87"/>
+      <c r="A15" s="86"/>
       <c r="B15" s="29">
         <v>163</v>
       </c>
@@ -5788,7 +5836,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="87"/>
+      <c r="A16" s="86"/>
       <c r="B16" s="29">
         <v>164</v>
       </c>
@@ -5807,7 +5855,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="87"/>
+      <c r="A17" s="86"/>
       <c r="B17" s="29">
         <v>165</v>
       </c>
@@ -5826,7 +5874,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="88"/>
+      <c r="A18" s="87"/>
       <c r="B18" s="22">
         <v>166</v>
       </c>
@@ -5845,7 +5893,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="85" t="s">
         <v>337</v>
       </c>
       <c r="B19" s="25">
@@ -5866,7 +5914,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="87"/>
+      <c r="A20" s="86"/>
       <c r="B20" s="29">
         <v>168</v>
       </c>
@@ -5885,7 +5933,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="87"/>
+      <c r="A21" s="86"/>
       <c r="B21" s="29">
         <v>169</v>
       </c>
@@ -5904,7 +5952,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="87"/>
+      <c r="A22" s="86"/>
       <c r="B22" s="29">
         <v>170</v>
       </c>
@@ -5923,7 +5971,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="87"/>
+      <c r="A23" s="86"/>
       <c r="B23" s="29">
         <v>171</v>
       </c>
@@ -5942,7 +5990,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="87"/>
+      <c r="A24" s="86"/>
       <c r="B24" s="29">
         <v>172</v>
       </c>
@@ -5961,7 +6009,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="87"/>
+      <c r="A25" s="86"/>
       <c r="B25" s="29">
         <v>173</v>
       </c>
@@ -5980,7 +6028,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="88"/>
+      <c r="A26" s="87"/>
       <c r="B26" s="22">
         <v>174</v>
       </c>
@@ -5999,7 +6047,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="86" t="s">
+      <c r="A27" s="85" t="s">
         <v>338</v>
       </c>
       <c r="B27" s="25">
@@ -6020,7 +6068,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="87"/>
+      <c r="A28" s="86"/>
       <c r="B28" s="29">
         <v>176</v>
       </c>
@@ -6039,7 +6087,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="87"/>
+      <c r="A29" s="86"/>
       <c r="B29" s="29">
         <v>177</v>
       </c>
@@ -6058,7 +6106,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="87"/>
+      <c r="A30" s="86"/>
       <c r="B30" s="29">
         <v>178</v>
       </c>
@@ -6077,7 +6125,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="87"/>
+      <c r="A31" s="86"/>
       <c r="B31" s="29">
         <v>179</v>
       </c>
@@ -6096,7 +6144,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="87"/>
+      <c r="A32" s="86"/>
       <c r="B32" s="29">
         <v>180</v>
       </c>
@@ -6115,7 +6163,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="87"/>
+      <c r="A33" s="86"/>
       <c r="B33" s="29">
         <v>181</v>
       </c>
@@ -6134,7 +6182,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="88"/>
+      <c r="A34" s="87"/>
       <c r="B34" s="29">
         <v>182</v>
       </c>
@@ -6153,7 +6201,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="85" t="s">
         <v>341</v>
       </c>
       <c r="B35" s="25">
@@ -6174,7 +6222,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="87"/>
+      <c r="A36" s="86"/>
       <c r="B36" s="29">
         <v>184</v>
       </c>
@@ -6193,7 +6241,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="87"/>
+      <c r="A37" s="86"/>
       <c r="B37" s="29">
         <v>185</v>
       </c>
@@ -6212,7 +6260,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="87"/>
+      <c r="A38" s="86"/>
       <c r="B38" s="29">
         <v>186</v>
       </c>
@@ -6231,7 +6279,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="87"/>
+      <c r="A39" s="86"/>
       <c r="B39" s="29">
         <v>187</v>
       </c>
@@ -6250,7 +6298,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="87"/>
+      <c r="A40" s="86"/>
       <c r="B40" s="29">
         <v>188</v>
       </c>
@@ -6269,7 +6317,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="87"/>
+      <c r="A41" s="86"/>
       <c r="B41" s="29">
         <v>189</v>
       </c>
@@ -6288,7 +6336,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="87"/>
+      <c r="A42" s="86"/>
       <c r="B42" s="29">
         <v>190</v>
       </c>
@@ -6307,7 +6355,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="87"/>
+      <c r="A43" s="86"/>
       <c r="B43" s="29">
         <v>191</v>
       </c>
@@ -6326,7 +6374,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="88"/>
+      <c r="A44" s="87"/>
       <c r="B44" s="22">
         <v>192</v>
       </c>
@@ -6345,7 +6393,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="86" t="s">
+      <c r="A45" s="85" t="s">
         <v>342</v>
       </c>
       <c r="B45" s="25">
@@ -6366,7 +6414,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="87"/>
+      <c r="A46" s="86"/>
       <c r="B46" s="29">
         <v>194</v>
       </c>
@@ -6385,7 +6433,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="87"/>
+      <c r="A47" s="86"/>
       <c r="B47" s="29">
         <v>195</v>
       </c>
@@ -6404,7 +6452,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="87"/>
+      <c r="A48" s="86"/>
       <c r="B48" s="29">
         <v>196</v>
       </c>
@@ -6423,7 +6471,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="87"/>
+      <c r="A49" s="86"/>
       <c r="B49" s="29">
         <v>197</v>
       </c>
@@ -6442,7 +6490,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="87"/>
+      <c r="A50" s="86"/>
       <c r="B50" s="29">
         <v>198</v>
       </c>
@@ -6461,7 +6509,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="87"/>
+      <c r="A51" s="86"/>
       <c r="B51" s="29">
         <v>199</v>
       </c>
@@ -6480,7 +6528,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="87"/>
+      <c r="A52" s="86"/>
       <c r="B52" s="29">
         <v>200</v>
       </c>
@@ -6499,7 +6547,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="87"/>
+      <c r="A53" s="86"/>
       <c r="B53" s="29">
         <v>201</v>
       </c>
@@ -6518,7 +6566,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="88"/>
+      <c r="A54" s="87"/>
       <c r="B54" s="22">
         <v>202</v>
       </c>
@@ -6537,7 +6585,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="86" t="s">
+      <c r="A55" s="85" t="s">
         <v>343</v>
       </c>
       <c r="B55" s="25">
@@ -6558,7 +6606,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="87"/>
+      <c r="A56" s="86"/>
       <c r="B56" s="29">
         <v>204</v>
       </c>
@@ -6577,7 +6625,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="87"/>
+      <c r="A57" s="86"/>
       <c r="B57" s="29">
         <v>205</v>
       </c>
@@ -6596,7 +6644,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="87"/>
+      <c r="A58" s="86"/>
       <c r="B58" s="29">
         <v>206</v>
       </c>
@@ -6615,7 +6663,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="87"/>
+      <c r="A59" s="86"/>
       <c r="B59" s="29">
         <v>207</v>
       </c>
@@ -6634,7 +6682,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="87"/>
+      <c r="A60" s="86"/>
       <c r="B60" s="29">
         <v>208</v>
       </c>
@@ -6653,7 +6701,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="87"/>
+      <c r="A61" s="86"/>
       <c r="B61" s="29">
         <v>209</v>
       </c>
@@ -6672,7 +6720,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="87"/>
+      <c r="A62" s="86"/>
       <c r="B62" s="29">
         <v>210</v>
       </c>
@@ -6691,7 +6739,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="87"/>
+      <c r="A63" s="86"/>
       <c r="B63" s="29">
         <v>211</v>
       </c>
@@ -6710,7 +6758,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="88"/>
+      <c r="A64" s="87"/>
       <c r="B64" s="22">
         <v>212</v>
       </c>
@@ -6729,7 +6777,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="86" t="s">
+      <c r="A65" s="85" t="s">
         <v>344</v>
       </c>
       <c r="B65" s="25">
@@ -6750,7 +6798,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="87"/>
+      <c r="A66" s="86"/>
       <c r="B66" s="29">
         <v>214</v>
       </c>
@@ -6769,7 +6817,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="87"/>
+      <c r="A67" s="86"/>
       <c r="B67" s="29">
         <v>215</v>
       </c>
@@ -6788,7 +6836,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="87"/>
+      <c r="A68" s="86"/>
       <c r="B68" s="29">
         <v>216</v>
       </c>
@@ -6807,7 +6855,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="87"/>
+      <c r="A69" s="86"/>
       <c r="B69" s="29">
         <v>217</v>
       </c>
@@ -6826,7 +6874,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="87"/>
+      <c r="A70" s="86"/>
       <c r="B70" s="29">
         <v>218</v>
       </c>
@@ -6845,7 +6893,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="87"/>
+      <c r="A71" s="86"/>
       <c r="B71" s="29">
         <v>219</v>
       </c>
@@ -6864,7 +6912,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="87"/>
+      <c r="A72" s="86"/>
       <c r="B72" s="29">
         <v>220</v>
       </c>
@@ -6883,7 +6931,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="87"/>
+      <c r="A73" s="86"/>
       <c r="B73" s="29">
         <v>221</v>
       </c>
@@ -6902,7 +6950,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="88"/>
+      <c r="A74" s="87"/>
       <c r="B74" s="22">
         <v>222</v>
       </c>
@@ -16191,7 +16239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG64"/>
   <sheetViews>
-    <sheetView topLeftCell="B43" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
@@ -26252,25 +26300,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="I1" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="89" t="s">
+      <c r="J1" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="89" t="s">
+      <c r="K1" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="89" t="s">
+      <c r="M1" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="89" t="s">
+      <c r="N1" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="89" t="s">
+      <c r="O1" s="88" t="s">
         <v>83</v>
       </c>
     </row>
@@ -26291,13 +26339,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -26319,13 +26367,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">

</xml_diff>

<commit_message>
v40.1  Started getting the buttons to call specific functions.
</commit_message>
<xml_diff>
--- a/EEPROM Addressing.xlsx
+++ b/EEPROM Addressing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7572" windowHeight="2628" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Non User Settings" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,8 @@
     <sheet name="Menu Variables" sheetId="6" r:id="rId7"/>
     <sheet name="12 Hour" sheetId="10" r:id="rId8"/>
     <sheet name="Timing" sheetId="12" r:id="rId9"/>
-    <sheet name="Chart2" sheetId="16" r:id="rId10"/>
-    <sheet name="Chart1" sheetId="15" r:id="rId11"/>
-    <sheet name="TFT Menu" sheetId="11" r:id="rId12"/>
+    <sheet name="TFT Menu" sheetId="11" r:id="rId10"/>
+    <sheet name="Menu Entries" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="422">
   <si>
     <t>NON USER SETTINGS</t>
   </si>
@@ -1132,6 +1131,195 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>Old Menu</t>
+  </si>
+  <si>
+    <t>Useer Setup</t>
+  </si>
+  <si>
+    <t>Celcius</t>
+  </si>
+  <si>
+    <t>No Dec</t>
+  </si>
+  <si>
+    <t>Set Temp Read Delay</t>
+  </si>
+  <si>
+    <t>B Light Brightness</t>
+  </si>
+  <si>
+    <t>Set BL Brightness</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Set Date and Time</t>
+  </si>
+  <si>
+    <t>Flow Sensor On/Off</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Sensor Addr Setup</t>
+  </si>
+  <si>
+    <t>Address Sens</t>
+  </si>
+  <si>
+    <t>Sensor Setup</t>
+  </si>
+  <si>
+    <t>Flow Calib</t>
+  </si>
+  <si>
+    <t>Calibrate Flow Sensor</t>
+  </si>
+  <si>
+    <t>Set Min Flow</t>
+  </si>
+  <si>
+    <t>Disable Flow Sensor</t>
+  </si>
+  <si>
+    <t>System Setup</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Temp Sensors</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>Exit Erase EEPROM</t>
+  </si>
+  <si>
+    <t>Calibrate</t>
+  </si>
+  <si>
+    <t>{ "User Setup",</t>
+  </si>
+  <si>
+    <t>MENU_ITEM Main_Menu[] = {</t>
+  </si>
+  <si>
+    <t>{ "Brightness",</t>
+  </si>
+  <si>
+    <t>{ "Time Format",</t>
+  </si>
+  <si>
+    <t>{ "Display Sec",</t>
+  </si>
+  <si>
+    <t>{ "Set Date/Time",</t>
+  </si>
+  <si>
+    <t>{ "Back",</t>
+  </si>
+  <si>
+    <t>{ TimerSetup",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 1",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 2",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 3",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 4",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 5",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 6",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 7",</t>
+  </si>
+  <si>
+    <t>{ "Set Timer 8",</t>
+  </si>
+  <si>
+    <t>{ SensorSetup</t>
+  </si>
+  <si>
+    <t>{ "Temp Unit",</t>
+  </si>
+  <si>
+    <t>{ "Precision",</t>
+  </si>
+  <si>
+    <t>{ "Read Delay",</t>
+  </si>
+  <si>
+    <t>{ "Sensor Names",</t>
+  </si>
+  <si>
+    <t>{ "Calib Temp 1",</t>
+  </si>
+  <si>
+    <t>{ "Calib Temp 2",</t>
+  </si>
+  <si>
+    <t>{ "Calib Temp 3",</t>
+  </si>
+  <si>
+    <t>{ "Calib Temp 4",</t>
+  </si>
+  <si>
+    <t>{ Sensor Calib</t>
+  </si>
+  <si>
+    <t>{ System Setup</t>
+  </si>
+  <si>
+    <t>{ "Debugging",</t>
+  </si>
+  <si>
+    <t>{ "Erase EEPROM",</t>
+  </si>
+  <si>
+    <t>{ "Restore Defaults",</t>
+  </si>
+  <si>
+    <t>{ "On/Off",</t>
+  </si>
+  <si>
+    <t>{ "Calib Flow",</t>
+  </si>
+  <si>
+    <t>{ "Set Min Flow",</t>
+  </si>
+  <si>
+    <t>{ Setup Flow</t>
+  </si>
+  <si>
+    <t>135-60</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1686,6 +1874,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1728,12 +1923,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,1586 +1939,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="987823712"/>
-        <c:axId val="987825792"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="987823712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="987825792"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="987825792"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="987823712"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="987638144"/>
-        <c:axId val="987639392"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="987638144"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="987639392"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="987639392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="987638144"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8648700" cy="6276975"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8648700" cy="6276975"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3667,12 +2277,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
+      <c r="A1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
       <c r="E1" t="s">
         <v>96</v>
       </c>
@@ -3836,7 +2446,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3899,11 +2509,11 @@
       <c r="A2" s="69">
         <v>40</v>
       </c>
-      <c r="B2" s="90">
+      <c r="B2" s="76">
         <v>40</v>
       </c>
       <c r="C2" s="69"/>
-      <c r="D2" s="90"/>
+      <c r="D2" s="76"/>
       <c r="E2" s="69"/>
       <c r="F2" s="70" t="s">
         <v>217</v>
@@ -3916,7 +2526,7 @@
         <v>60</v>
       </c>
       <c r="I2" s="69"/>
-      <c r="J2" s="90"/>
+      <c r="J2" s="76"/>
       <c r="K2" s="69"/>
     </row>
     <row r="3" spans="1:12" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3938,11 +2548,11 @@
       <c r="A4" s="69">
         <v>40</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="77">
         <v>1</v>
       </c>
       <c r="C4" s="69"/>
-      <c r="D4" s="91">
+      <c r="D4" s="77">
         <v>2</v>
       </c>
       <c r="E4" s="69"/>
@@ -3958,7 +2568,7 @@
         <v>108</v>
       </c>
       <c r="I4" s="69"/>
-      <c r="J4" s="91">
+      <c r="J4" s="77">
         <v>1</v>
       </c>
       <c r="K4" s="69"/>
@@ -3982,11 +2592,11 @@
       <c r="A6" s="69">
         <v>40</v>
       </c>
-      <c r="B6" s="91">
+      <c r="B6" s="77">
         <v>3</v>
       </c>
       <c r="C6" s="69"/>
-      <c r="D6" s="91">
+      <c r="D6" s="77">
         <v>4</v>
       </c>
       <c r="E6" s="69"/>
@@ -4002,7 +2612,7 @@
         <v>156</v>
       </c>
       <c r="I6" s="69"/>
-      <c r="J6" s="91">
+      <c r="J6" s="77">
         <v>2</v>
       </c>
       <c r="K6" s="69"/>
@@ -4026,11 +2636,11 @@
       <c r="A8" s="69">
         <v>40</v>
       </c>
-      <c r="B8" s="91">
+      <c r="B8" s="77">
         <v>5</v>
       </c>
       <c r="C8" s="69"/>
-      <c r="D8" s="91">
+      <c r="D8" s="77">
         <v>6</v>
       </c>
       <c r="E8" s="69"/>
@@ -4046,7 +2656,7 @@
         <v>204</v>
       </c>
       <c r="I8" s="69"/>
-      <c r="J8" s="91">
+      <c r="J8" s="77">
         <v>3</v>
       </c>
       <c r="K8" s="69"/>
@@ -4070,11 +2680,11 @@
       <c r="A10" s="69">
         <v>40</v>
       </c>
-      <c r="B10" s="91">
+      <c r="B10" s="77">
         <v>7</v>
       </c>
       <c r="C10" s="69"/>
-      <c r="D10" s="91">
+      <c r="D10" s="77">
         <v>8</v>
       </c>
       <c r="E10" s="69"/>
@@ -4090,7 +2700,7 @@
         <v>252</v>
       </c>
       <c r="I10" s="69"/>
-      <c r="J10" s="91">
+      <c r="J10" s="77">
         <v>4</v>
       </c>
       <c r="K10" s="69"/>
@@ -4151,6 +2761,9 @@
       <c r="J13" s="72">
         <v>135</v>
       </c>
+      <c r="K13" s="68" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="68" t="s">
@@ -4176,6 +2789,587 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K74"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D4" s="78">
+        <v>42705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="93" t="s">
+        <v>364</v>
+      </c>
+      <c r="C6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="93" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>366</v>
+      </c>
+      <c r="D8" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="93" t="s">
+        <v>369</v>
+      </c>
+      <c r="C10" t="s">
+        <v>370</v>
+      </c>
+      <c r="D10" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="93" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>372</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>372</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="C16" t="s">
+        <v>372</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="C17" t="s">
+        <v>372</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="93" t="s">
+        <v>272</v>
+      </c>
+      <c r="C18" t="s">
+        <v>372</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="93" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" t="s">
+        <v>372</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>374</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>374</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>374</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>374</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="93" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>386</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>386</v>
+      </c>
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>386</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>386</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="93" t="s">
+        <v>376</v>
+      </c>
+      <c r="C30" t="s">
+        <v>377</v>
+      </c>
+      <c r="D30" t="s">
+        <v>378</v>
+      </c>
+      <c r="E30" t="s">
+        <v>379</v>
+      </c>
+      <c r="F30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="93" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" t="s">
+        <v>381</v>
+      </c>
+      <c r="E32" t="s">
+        <v>382</v>
+      </c>
+      <c r="F32" t="s">
+        <v>383</v>
+      </c>
+      <c r="G32" t="s">
+        <v>185</v>
+      </c>
+      <c r="H32" t="s">
+        <v>384</v>
+      </c>
+      <c r="I32" t="s">
+        <v>290</v>
+      </c>
+      <c r="J32" t="s">
+        <v>189</v>
+      </c>
+      <c r="K32" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="93" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" t="s">
+        <v>385</v>
+      </c>
+      <c r="D33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="93" t="s">
+        <v>262</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>262</v>
+      </c>
+      <c r="F34" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="93" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="93" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="93" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="93" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="93" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="93" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="93" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C49" s="93" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C50" s="93" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C51" s="93" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="93" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C53" s="93" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C55" s="93" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C56" s="93" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C57" s="93" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C58" s="93" t="s">
+        <v>407</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>393</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>412</v>
+      </c>
+      <c r="D60" s="44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C61" s="93" t="s">
+        <v>408</v>
+      </c>
+      <c r="D61" s="44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C62" s="93" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C63" s="93" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C64" s="93" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C67" s="93" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C68" s="93" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C71" s="93" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C72" s="93" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C73" s="93" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>393</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4197,12 +3391,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
       <c r="E1" t="s">
         <v>95</v>
       </c>
@@ -4394,13 +3588,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="87"/>
       <c r="F1" s="19" t="s">
         <v>108</v>
       </c>
@@ -4430,7 +3624,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="80"/>
+      <c r="A3" s="83"/>
       <c r="B3" s="25">
         <v>100</v>
       </c>
@@ -4451,7 +3645,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="81"/>
+      <c r="A4" s="84"/>
       <c r="B4" s="29">
         <v>101</v>
       </c>
@@ -4472,7 +3666,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="80" t="s">
         <v>175</v>
       </c>
       <c r="B5" s="25">
@@ -4495,7 +3689,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="78"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="29">
         <v>103</v>
       </c>
@@ -4516,7 +3710,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="78"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="29">
         <v>104</v>
       </c>
@@ -4537,7 +3731,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="78"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="29">
         <v>105</v>
       </c>
@@ -4558,7 +3752,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="78"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="29">
         <v>106</v>
       </c>
@@ -4579,7 +3773,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="79"/>
+      <c r="A10" s="82"/>
       <c r="B10" s="22">
         <v>107</v>
       </c>
@@ -4600,7 +3794,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="80" t="s">
         <v>176</v>
       </c>
       <c r="B11" s="25">
@@ -4623,7 +3817,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="78"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="29">
         <v>109</v>
       </c>
@@ -4644,7 +3838,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="29">
         <v>110</v>
       </c>
@@ -4665,7 +3859,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="78"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="29">
         <v>111</v>
       </c>
@@ -4686,7 +3880,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="78"/>
+      <c r="A15" s="81"/>
       <c r="B15" s="29">
         <v>112</v>
       </c>
@@ -4707,7 +3901,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="79"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="22">
         <v>113</v>
       </c>
@@ -4728,7 +3922,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="80" t="s">
         <v>177</v>
       </c>
       <c r="B17" s="29">
@@ -4751,7 +3945,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="78"/>
+      <c r="A18" s="81"/>
       <c r="B18" s="29">
         <v>115</v>
       </c>
@@ -4772,7 +3966,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="78"/>
+      <c r="A19" s="81"/>
       <c r="B19" s="29">
         <v>116</v>
       </c>
@@ -4793,7 +3987,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="78"/>
+      <c r="A20" s="81"/>
       <c r="B20" s="29">
         <v>117</v>
       </c>
@@ -4814,7 +4008,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="78"/>
+      <c r="A21" s="81"/>
       <c r="B21" s="29">
         <v>118</v>
       </c>
@@ -4835,7 +4029,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="79"/>
+      <c r="A22" s="82"/>
       <c r="B22" s="29">
         <v>119</v>
       </c>
@@ -4856,7 +4050,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="80" t="s">
         <v>178</v>
       </c>
       <c r="B23" s="25">
@@ -4879,7 +4073,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="78"/>
+      <c r="A24" s="81"/>
       <c r="B24" s="29">
         <v>121</v>
       </c>
@@ -4900,7 +4094,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="78"/>
+      <c r="A25" s="81"/>
       <c r="B25" s="29">
         <v>122</v>
       </c>
@@ -4921,7 +4115,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="78"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="29">
         <v>123</v>
       </c>
@@ -4942,7 +4136,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="78"/>
+      <c r="A27" s="81"/>
       <c r="B27" s="29">
         <v>124</v>
       </c>
@@ -4963,7 +4157,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="79"/>
+      <c r="A28" s="82"/>
       <c r="B28" s="22">
         <v>125</v>
       </c>
@@ -4984,7 +4178,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="80" t="s">
         <v>179</v>
       </c>
       <c r="B29" s="29">
@@ -5007,7 +4201,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="78"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="29">
         <v>127</v>
       </c>
@@ -5028,7 +4222,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="78"/>
+      <c r="A31" s="81"/>
       <c r="B31" s="29">
         <v>128</v>
       </c>
@@ -5049,7 +4243,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="78"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="29">
         <v>129</v>
       </c>
@@ -5070,7 +4264,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="78"/>
+      <c r="A33" s="81"/>
       <c r="B33" s="29">
         <v>130</v>
       </c>
@@ -5091,7 +4285,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="79"/>
+      <c r="A34" s="82"/>
       <c r="B34" s="29">
         <v>131</v>
       </c>
@@ -5112,7 +4306,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="80" t="s">
         <v>180</v>
       </c>
       <c r="B35" s="25">
@@ -5135,7 +4329,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="78"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="29">
         <v>133</v>
       </c>
@@ -5156,7 +4350,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="78"/>
+      <c r="A37" s="81"/>
       <c r="B37" s="29">
         <v>134</v>
       </c>
@@ -5177,7 +4371,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="78"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="29">
         <v>135</v>
       </c>
@@ -5198,7 +4392,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="78"/>
+      <c r="A39" s="81"/>
       <c r="B39" s="29">
         <v>136</v>
       </c>
@@ -5219,7 +4413,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="79"/>
+      <c r="A40" s="82"/>
       <c r="B40" s="22">
         <v>137</v>
       </c>
@@ -5240,7 +4434,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="77" t="s">
+      <c r="A41" s="80" t="s">
         <v>181</v>
       </c>
       <c r="B41" s="29">
@@ -5263,7 +4457,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="78"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="29">
         <v>139</v>
       </c>
@@ -5284,7 +4478,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="78"/>
+      <c r="A43" s="81"/>
       <c r="B43" s="29">
         <v>140</v>
       </c>
@@ -5305,7 +4499,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="78"/>
+      <c r="A44" s="81"/>
       <c r="B44" s="29">
         <v>141</v>
       </c>
@@ -5326,7 +4520,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="78"/>
+      <c r="A45" s="81"/>
       <c r="B45" s="29">
         <v>142</v>
       </c>
@@ -5347,7 +4541,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="79"/>
+      <c r="A46" s="82"/>
       <c r="B46" s="29">
         <v>143</v>
       </c>
@@ -5368,7 +4562,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="77" t="s">
+      <c r="A47" s="80" t="s">
         <v>182</v>
       </c>
       <c r="B47" s="25">
@@ -5391,7 +4585,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="78"/>
+      <c r="A48" s="81"/>
       <c r="B48" s="29">
         <v>145</v>
       </c>
@@ -5412,7 +4606,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="78"/>
+      <c r="A49" s="81"/>
       <c r="B49" s="29">
         <v>146</v>
       </c>
@@ -5433,7 +4627,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="78"/>
+      <c r="A50" s="81"/>
       <c r="B50" s="29">
         <v>147</v>
       </c>
@@ -5454,7 +4648,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="78"/>
+      <c r="A51" s="81"/>
       <c r="B51" s="29">
         <v>148</v>
       </c>
@@ -5475,7 +4669,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="79"/>
+      <c r="A52" s="82"/>
       <c r="B52" s="22">
         <v>149</v>
       </c>
@@ -5550,13 +4744,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
       <c r="F1" t="s">
         <v>325</v>
       </c>
@@ -5585,7 +4779,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="88" t="s">
         <v>335</v>
       </c>
       <c r="B3" s="25">
@@ -5606,7 +4800,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="29">
         <v>152</v>
       </c>
@@ -5625,7 +4819,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="86"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="29">
         <v>153</v>
       </c>
@@ -5644,7 +4838,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="86"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="29">
         <v>154</v>
       </c>
@@ -5663,7 +4857,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="86"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="29">
         <v>155</v>
       </c>
@@ -5682,7 +4876,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="29">
         <v>156</v>
       </c>
@@ -5701,7 +4895,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="86"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="29">
         <v>157</v>
       </c>
@@ -5720,7 +4914,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="87"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="22">
         <v>158</v>
       </c>
@@ -5739,7 +4933,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="88" t="s">
         <v>336</v>
       </c>
       <c r="B11" s="25">
@@ -5760,7 +4954,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
+      <c r="A12" s="89"/>
       <c r="B12" s="29">
         <v>160</v>
       </c>
@@ -5779,7 +4973,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="86"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="29">
         <v>161</v>
       </c>
@@ -5798,7 +4992,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
+      <c r="A14" s="89"/>
       <c r="B14" s="29">
         <v>162</v>
       </c>
@@ -5817,7 +5011,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="86"/>
+      <c r="A15" s="89"/>
       <c r="B15" s="29">
         <v>163</v>
       </c>
@@ -5836,7 +5030,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
+      <c r="A16" s="89"/>
       <c r="B16" s="29">
         <v>164</v>
       </c>
@@ -5855,7 +5049,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="86"/>
+      <c r="A17" s="89"/>
       <c r="B17" s="29">
         <v>165</v>
       </c>
@@ -5874,7 +5068,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="87"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="22">
         <v>166</v>
       </c>
@@ -5893,7 +5087,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="85" t="s">
+      <c r="A19" s="88" t="s">
         <v>337</v>
       </c>
       <c r="B19" s="25">
@@ -5914,7 +5108,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
+      <c r="A20" s="89"/>
       <c r="B20" s="29">
         <v>168</v>
       </c>
@@ -5933,7 +5127,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="86"/>
+      <c r="A21" s="89"/>
       <c r="B21" s="29">
         <v>169</v>
       </c>
@@ -5952,7 +5146,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="86"/>
+      <c r="A22" s="89"/>
       <c r="B22" s="29">
         <v>170</v>
       </c>
@@ -5971,7 +5165,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="86"/>
+      <c r="A23" s="89"/>
       <c r="B23" s="29">
         <v>171</v>
       </c>
@@ -5990,7 +5184,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="86"/>
+      <c r="A24" s="89"/>
       <c r="B24" s="29">
         <v>172</v>
       </c>
@@ -6009,7 +5203,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="86"/>
+      <c r="A25" s="89"/>
       <c r="B25" s="29">
         <v>173</v>
       </c>
@@ -6028,7 +5222,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="87"/>
+      <c r="A26" s="90"/>
       <c r="B26" s="22">
         <v>174</v>
       </c>
@@ -6047,7 +5241,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="85" t="s">
+      <c r="A27" s="88" t="s">
         <v>338</v>
       </c>
       <c r="B27" s="25">
@@ -6068,7 +5262,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="86"/>
+      <c r="A28" s="89"/>
       <c r="B28" s="29">
         <v>176</v>
       </c>
@@ -6087,7 +5281,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="86"/>
+      <c r="A29" s="89"/>
       <c r="B29" s="29">
         <v>177</v>
       </c>
@@ -6106,7 +5300,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="86"/>
+      <c r="A30" s="89"/>
       <c r="B30" s="29">
         <v>178</v>
       </c>
@@ -6125,7 +5319,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="86"/>
+      <c r="A31" s="89"/>
       <c r="B31" s="29">
         <v>179</v>
       </c>
@@ -6144,7 +5338,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="86"/>
+      <c r="A32" s="89"/>
       <c r="B32" s="29">
         <v>180</v>
       </c>
@@ -6163,7 +5357,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="86"/>
+      <c r="A33" s="89"/>
       <c r="B33" s="29">
         <v>181</v>
       </c>
@@ -6182,7 +5376,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="87"/>
+      <c r="A34" s="90"/>
       <c r="B34" s="29">
         <v>182</v>
       </c>
@@ -6201,7 +5395,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="88" t="s">
         <v>341</v>
       </c>
       <c r="B35" s="25">
@@ -6222,7 +5416,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="86"/>
+      <c r="A36" s="89"/>
       <c r="B36" s="29">
         <v>184</v>
       </c>
@@ -6241,7 +5435,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="86"/>
+      <c r="A37" s="89"/>
       <c r="B37" s="29">
         <v>185</v>
       </c>
@@ -6260,7 +5454,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="86"/>
+      <c r="A38" s="89"/>
       <c r="B38" s="29">
         <v>186</v>
       </c>
@@ -6279,7 +5473,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="86"/>
+      <c r="A39" s="89"/>
       <c r="B39" s="29">
         <v>187</v>
       </c>
@@ -6298,7 +5492,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="86"/>
+      <c r="A40" s="89"/>
       <c r="B40" s="29">
         <v>188</v>
       </c>
@@ -6317,7 +5511,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="86"/>
+      <c r="A41" s="89"/>
       <c r="B41" s="29">
         <v>189</v>
       </c>
@@ -6336,7 +5530,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="86"/>
+      <c r="A42" s="89"/>
       <c r="B42" s="29">
         <v>190</v>
       </c>
@@ -6355,7 +5549,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="86"/>
+      <c r="A43" s="89"/>
       <c r="B43" s="29">
         <v>191</v>
       </c>
@@ -6374,7 +5568,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="87"/>
+      <c r="A44" s="90"/>
       <c r="B44" s="22">
         <v>192</v>
       </c>
@@ -6393,7 +5587,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="85" t="s">
+      <c r="A45" s="88" t="s">
         <v>342</v>
       </c>
       <c r="B45" s="25">
@@ -6414,7 +5608,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="86"/>
+      <c r="A46" s="89"/>
       <c r="B46" s="29">
         <v>194</v>
       </c>
@@ -6433,7 +5627,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="86"/>
+      <c r="A47" s="89"/>
       <c r="B47" s="29">
         <v>195</v>
       </c>
@@ -6452,7 +5646,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="86"/>
+      <c r="A48" s="89"/>
       <c r="B48" s="29">
         <v>196</v>
       </c>
@@ -6471,7 +5665,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="86"/>
+      <c r="A49" s="89"/>
       <c r="B49" s="29">
         <v>197</v>
       </c>
@@ -6490,7 +5684,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="86"/>
+      <c r="A50" s="89"/>
       <c r="B50" s="29">
         <v>198</v>
       </c>
@@ -6509,7 +5703,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="86"/>
+      <c r="A51" s="89"/>
       <c r="B51" s="29">
         <v>199</v>
       </c>
@@ -6528,7 +5722,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="86"/>
+      <c r="A52" s="89"/>
       <c r="B52" s="29">
         <v>200</v>
       </c>
@@ -6547,7 +5741,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="86"/>
+      <c r="A53" s="89"/>
       <c r="B53" s="29">
         <v>201</v>
       </c>
@@ -6566,7 +5760,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="87"/>
+      <c r="A54" s="90"/>
       <c r="B54" s="22">
         <v>202</v>
       </c>
@@ -6585,7 +5779,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="85" t="s">
+      <c r="A55" s="88" t="s">
         <v>343</v>
       </c>
       <c r="B55" s="25">
@@ -6606,7 +5800,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="86"/>
+      <c r="A56" s="89"/>
       <c r="B56" s="29">
         <v>204</v>
       </c>
@@ -6625,7 +5819,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="86"/>
+      <c r="A57" s="89"/>
       <c r="B57" s="29">
         <v>205</v>
       </c>
@@ -6644,7 +5838,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="86"/>
+      <c r="A58" s="89"/>
       <c r="B58" s="29">
         <v>206</v>
       </c>
@@ -6663,7 +5857,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="86"/>
+      <c r="A59" s="89"/>
       <c r="B59" s="29">
         <v>207</v>
       </c>
@@ -6682,7 +5876,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="86"/>
+      <c r="A60" s="89"/>
       <c r="B60" s="29">
         <v>208</v>
       </c>
@@ -6701,7 +5895,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="86"/>
+      <c r="A61" s="89"/>
       <c r="B61" s="29">
         <v>209</v>
       </c>
@@ -6720,7 +5914,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="86"/>
+      <c r="A62" s="89"/>
       <c r="B62" s="29">
         <v>210</v>
       </c>
@@ -6739,7 +5933,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="86"/>
+      <c r="A63" s="89"/>
       <c r="B63" s="29">
         <v>211</v>
       </c>
@@ -6758,7 +5952,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="87"/>
+      <c r="A64" s="90"/>
       <c r="B64" s="22">
         <v>212</v>
       </c>
@@ -6777,7 +5971,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="85" t="s">
+      <c r="A65" s="88" t="s">
         <v>344</v>
       </c>
       <c r="B65" s="25">
@@ -6798,7 +5992,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="86"/>
+      <c r="A66" s="89"/>
       <c r="B66" s="29">
         <v>214</v>
       </c>
@@ -6817,7 +6011,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="86"/>
+      <c r="A67" s="89"/>
       <c r="B67" s="29">
         <v>215</v>
       </c>
@@ -6836,7 +6030,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="86"/>
+      <c r="A68" s="89"/>
       <c r="B68" s="29">
         <v>216</v>
       </c>
@@ -6855,7 +6049,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="86"/>
+      <c r="A69" s="89"/>
       <c r="B69" s="29">
         <v>217</v>
       </c>
@@ -6874,7 +6068,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="86"/>
+      <c r="A70" s="89"/>
       <c r="B70" s="29">
         <v>218</v>
       </c>
@@ -6893,7 +6087,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="86"/>
+      <c r="A71" s="89"/>
       <c r="B71" s="29">
         <v>219</v>
       </c>
@@ -6912,7 +6106,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="86"/>
+      <c r="A72" s="89"/>
       <c r="B72" s="29">
         <v>220</v>
       </c>
@@ -6931,7 +6125,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="86"/>
+      <c r="A73" s="89"/>
       <c r="B73" s="29">
         <v>221</v>
       </c>
@@ -6950,7 +6144,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="87"/>
+      <c r="A74" s="90"/>
       <c r="B74" s="22">
         <v>222</v>
       </c>
@@ -26300,25 +25494,25 @@
       <c r="H1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="88" t="s">
+      <c r="I1" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="91" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="88" t="s">
+      <c r="K1" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="88" t="s">
+      <c r="L1" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="88" t="s">
+      <c r="M1" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="88" t="s">
+      <c r="N1" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="88" t="s">
+      <c r="O1" s="91" t="s">
         <v>83</v>
       </c>
     </row>
@@ -26339,13 +25533,13 @@
       <c r="H2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
       <c r="P2" t="s">
         <v>84</v>
       </c>
@@ -26367,13 +25561,13 @@
       <c r="H3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5">

</xml_diff>